<commit_message>
added code for backup policy assignment thru tf
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="159">
   <si>
     <t>Regional</t>
   </si>
@@ -506,6 +506,12 @@
   </si>
   <si>
     <t>Allow group $ to manage instance-family in compartment *</t>
+  </si>
+  <si>
+    <t>Backup Policy</t>
+  </si>
+  <si>
+    <t>Gold</t>
   </si>
 </sst>
 </file>
@@ -670,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -723,6 +729,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1442,7 +1452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1925,10 +1935,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1942,12 +1952,12 @@
     <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>87</v>
       </c>
@@ -1978,8 +1988,11 @@
       <c r="J1" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2010,9 +2023,12 @@
       <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
     </row>
   </sheetData>
@@ -2022,10 +2038,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2038,7 +2054,7 @@
     <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -2057,8 +2073,11 @@
       <c r="F1" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2077,8 +2096,11 @@
       <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2086,7 +2108,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2094,7 +2116,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
updated to check for null vaules in CD3 for baseNetwork Creation
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="157">
   <si>
     <t>Regional</t>
   </si>
@@ -86,9 +86,6 @@
     <t>iscsi</t>
   </si>
   <si>
-    <t>nonprod_compartment_ocid</t>
-  </si>
-  <si>
     <t>qa-app</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
   </si>
   <si>
     <t>10.110.255.226,10.110.255.227</t>
-  </si>
-  <si>
-    <t>ntk_compartment_ocid</t>
   </si>
   <si>
     <t>PHXHub-VCN</t>
@@ -702,6 +696,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -729,10 +727,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1040,7 +1034,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,74 +1045,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>96</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -1153,58 +1147,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1241,74 +1235,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="A1" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1324,7 +1318,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1340,7 +1334,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1392,50 +1386,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="1"/>
     </row>
@@ -1466,50 +1460,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="E3" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -1518,13 +1512,13 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1537,22 +1531,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1560,16 +1554,16 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1585,7 +1579,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,30 +1629,30 @@
         <v>12</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="H2" s="1">
         <v>4</v>
@@ -1667,30 +1661,33 @@
         <v>100</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="H3" s="1">
         <v>2</v>
@@ -1699,7 +1696,10 @@
         <v>100</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1746,45 +1746,45 @@
   <sheetData>
     <row r="1" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -1796,16 +1796,16 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1884,10 +1884,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
@@ -1898,33 +1898,33 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1937,8 +1937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,37 +1959,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2000,31 +2000,31 @@
         <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2040,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,25 +2056,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>157</v>
+        <v>152</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2094,10 +2094,10 @@
         <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>158</v>
+        <v>99</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2148,209 +2148,209 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="19" t="s">
+      <c r="D2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="E2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="9" t="s">
+      <c r="E3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="10" t="s">
+      <c r="E4" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="11" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="10" t="s">
-        <v>73</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="12"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="12"/>
       <c r="D8" s="1"/>
       <c r="E8" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="12"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="12"/>
       <c r="D10" s="1"/>
       <c r="E10" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="20"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="12"/>
       <c r="D11" s="1"/>
       <c r="E11" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="20"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="12"/>
       <c r="D12" s="1"/>
       <c r="E12" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="20"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="20"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="10"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="20"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="10"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="20"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="1"/>
       <c r="E16" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="21"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="10"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F17" s="1"/>
     </row>

</xml_diff>

<commit_message>
updated attach tags code for instances and block vols
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -16,15 +16,17 @@
     <sheet name="Instances" sheetId="4" r:id="rId7"/>
     <sheet name="BlockVols" sheetId="5" r:id="rId8"/>
     <sheet name="Tags" sheetId="6" r:id="rId9"/>
-    <sheet name="AddRouteRules" sheetId="11" r:id="rId10"/>
-    <sheet name="AddSecRules" sheetId="12" r:id="rId11"/>
+    <sheet name="TagServer" sheetId="13" r:id="rId10"/>
+    <sheet name="TagVolume" sheetId="14" r:id="rId11"/>
+    <sheet name="AddRouteRules" sheetId="11" r:id="rId12"/>
+    <sheet name="AddSecRules" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="167">
   <si>
     <t>Regional</t>
   </si>
@@ -506,6 +508,36 @@
   </si>
   <si>
     <t>Gold</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Shruthi</t>
+  </si>
+  <si>
+    <t>Demo=True</t>
+  </si>
+  <si>
+    <t>Windows2012R2=True</t>
+  </si>
+  <si>
+    <t>HubPublicSub=True</t>
+  </si>
+  <si>
+    <t>dev=True</t>
+  </si>
+  <si>
+    <t>Lakshmi</t>
+  </si>
+  <si>
+    <t>VolumeName</t>
+  </si>
+  <si>
+    <t>Shruthi_disk2</t>
+  </si>
+  <si>
+    <t>Lakshmi_disk2</t>
   </si>
 </sst>
 </file>
@@ -670,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -727,6 +759,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1132,6 +1168,143 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1213,7 +1386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
@@ -1937,7 +2110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated to add dns_label for vcn and subnet
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="171">
   <si>
     <t>Regional</t>
   </si>
@@ -541,6 +541,15 @@
   </si>
   <si>
     <t>WindowsLatest</t>
+  </si>
+  <si>
+    <t>dns_label</t>
+  </si>
+  <si>
+    <t>phxhub</t>
+  </si>
+  <si>
+    <t>phxad</t>
   </si>
 </sst>
 </file>
@@ -705,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -766,6 +775,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1752,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1773,7 +1783,7 @@
     <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1807,8 +1817,11 @@
       <c r="K1" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1842,8 +1855,11 @@
       <c r="K2" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -1878,19 +1894,19 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1900,10 +1916,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,9 +1934,10 @@
     <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>152</v>
       </c>
@@ -1951,8 +1968,11 @@
       <c r="J1" s="6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1983,8 +2003,11 @@
       <c r="J2" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1996,7 +2019,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2008,7 +2031,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2020,7 +2043,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2113,7 +2136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated code for overwrite route rules and few other changes
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="172">
   <si>
     <t>Regional</t>
   </si>
@@ -552,13 +552,16 @@
   </si>
   <si>
     <t>phxad</t>
+  </si>
+  <si>
+    <t>VCN Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,6 +598,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -716,7 +725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -777,6 +786,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1561,79 +1573,107 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>128</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="13" t="s">
         <v>147</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to add comments row for each sheet
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="14"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="181">
   <si>
     <t>Regional</t>
   </si>
@@ -198,9 +198,6 @@
     <t>TagNamespace</t>
   </si>
   <si>
-    <t>RyderApplication</t>
-  </si>
-  <si>
     <t>OS</t>
   </si>
   <si>
@@ -237,9 +234,6 @@
     <t>qa</t>
   </si>
   <si>
-    <t>ACS</t>
-  </si>
-  <si>
     <t>OL76</t>
   </si>
   <si>
@@ -249,13 +243,7 @@
     <t>dr</t>
   </si>
   <si>
-    <t>AD</t>
-  </si>
-  <si>
     <t>prod</t>
-  </si>
-  <si>
-    <t>NFS</t>
   </si>
   <si>
     <t>dr-db-clnt</t>
@@ -521,12 +509,6 @@
     <t>Demo=True</t>
   </si>
   <si>
-    <t>Windows2012R2=True</t>
-  </si>
-  <si>
-    <t>HubPublicSub=True</t>
-  </si>
-  <si>
     <t>dev=True</t>
   </si>
   <si>
@@ -555,6 +537,51 @@
   </si>
   <si>
     <t>VCN Name</t>
+  </si>
+  <si>
+    <t># VCN names should be unique; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars</t>
+  </si>
+  <si>
+    <t># subnet names should be unique; All fields are mandatory for each subnet except dns_label for which the default value issubnet_name truncated to 15 chars</t>
+  </si>
+  <si>
+    <t># DHCP option is created in the same compartment as the VCN; Whichever DHCP option name you have mentioned in the Subnets Sheet should be defined here in this sheet;  if server_type is CustomDnsServer then you should not leave custom_dns_server column empty</t>
+  </si>
+  <si>
+    <t># Make sure to enter exact name in attached_to_instance column as entered in Hostname of Instances sheet;Backup Policy column can be left blank at the timeof block vol creation and can be filled up later on while attaching backup policy to the boot abd block volumes together;</t>
+  </si>
+  <si>
+    <t>#Template will be picked upon from template folder based on  OS column; Backup Policy column can be left blank at the time of instance creation and can be filled up later on while attaching backup policy to the boot abd block volumes together;ssh-key-var-name is the name of variable defined in variable.tf file containing SSH key to be pushed to the server</t>
+  </si>
+  <si>
+    <t># Horizontal row specifies the TagNameSpace Names to be created; Vertical row under each TagNameSpace represnts Keys in that tagnamespace; Enter compartment name in which  all tagnamespaces and keys will be created</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>Windows2012=True</t>
+  </si>
+  <si>
+    <t>Windows2012=</t>
+  </si>
+  <si>
+    <t>Demo=</t>
+  </si>
+  <si>
+    <t>qa-dmz=</t>
+  </si>
+  <si>
+    <t>qa-app=true</t>
+  </si>
+  <si>
+    <t>qa-dmz=true</t>
+  </si>
+  <si>
+    <t>#Hostname represents instance to which tagging needs tp be assigned; It should match the one entered in instances sheet. Enter TagKey=TagValue for each tagnamespace;  tagValue can be left empty also</t>
+  </si>
+  <si>
+    <t>#VolumeName represents instance to which tagging needs tp be assigned; It should match the one entered in BlockVols sheet. Enter TagKey=TagValue for each tagnamespace;  tagValue can be left empty also</t>
   </si>
 </sst>
 </file>
@@ -632,7 +659,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -694,15 +721,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -721,11 +739,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -760,16 +815,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -781,14 +839,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1108,74 +1175,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="A1" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -1195,137 +1262,170 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="18" t="s">
+    <row r="1" spans="1:5" s="19" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E2" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>161</v>
+        <v>173</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>176</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>162</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="20" t="s">
+    <row r="1" spans="1:5" s="19" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E2" s="20" t="s">
         <v>56</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C3" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>162</v>
+      <c r="B4" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1347,39 +1447,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1387,18 +1487,18 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1417,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,56 +1536,56 @@
   <sheetData>
     <row r="1" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+        <v>144</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1493,16 +1593,16 @@
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1518,7 +1618,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1534,7 +1634,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1591,22 +1691,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>121</v>
+        <v>124</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1619,7 +1719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
@@ -1634,46 +1734,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="N1" s="31" t="s">
-        <v>121</v>
+      <c r="M1" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1696,50 +1796,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" s="23"/>
+      <c r="A1" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B7" s="1"/>
     </row>
@@ -1770,50 +1870,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="A1" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -1822,13 +1922,13 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1841,22 +1941,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1864,16 +1964,16 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1886,10 +1986,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1907,91 +2007,69 @@
     <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="33"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="1">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1">
-        <v>100</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>169</v>
+      <c r="K2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>31</v>
@@ -2000,13 +2078,13 @@
         <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H3" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I3" s="1">
         <v>100</v>
@@ -2015,10 +2093,48 @@
         <v>30</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>93</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>100</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
     <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2029,10 +2145,40 @@
     <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
     <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2040,10 +2186,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,88 +2207,90 @@
     <col min="11" max="11" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+    </row>
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="15" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="K2" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="21" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="K3" s="21" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -2183,7 +2331,23 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2191,10 +2355,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,38 +2370,30 @@
     <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2245,16 +2401,36 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
       </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2262,10 +2438,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,91 +2460,121 @@
     <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="G2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="I2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="b">
+      <c r="E3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
+      <c r="J3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2381,59 +2587,62 @@
     <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="19" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>302</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1">
-        <v>302</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -2451,248 +2660,266 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C2" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="8" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="26" t="s">
+      <c r="C3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="35"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="9" t="s">
+      <c r="D4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="1" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="35"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="12" t="s">
-        <v>73</v>
-      </c>
+      <c r="A6" s="35"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="12"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="27"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="12"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="11" t="s">
-        <v>76</v>
+      <c r="E8" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="27"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="12"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>77</v>
+      <c r="E9" s="11" t="s">
+        <v>72</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="12"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="11" t="s">
-        <v>33</v>
+      <c r="E10" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="27"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="12"/>
       <c r="D11" s="1"/>
       <c r="E11" s="11" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="27"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="12"/>
       <c r="D12" s="1"/>
       <c r="E12" s="11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>81</v>
+      <c r="E14" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="27"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="10"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="27"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="10"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="11" t="s">
-        <v>83</v>
+      <c r="E16" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="28"/>
       <c r="C17" s="10"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>84</v>
+      <c r="E17" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="F17" s="1"/>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="35"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:B17"/>
-    <mergeCell ref="A2:A17"/>
+  <mergeCells count="3">
+    <mergeCell ref="B3:B18"/>
+    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="https://console.us-ashburn-1.oraclecloud.com/a/identity/tag-namespaces/ocid1.tagnamespace.oc1..aaaaaaaa77lkexyrq5t4gpuirhdetct5psrmbouinhad2s5soycj4jyimlwq/tag-definitions/ocid1.tagdefinition.oc1..aaaaaaaavfzlvfl6ndwskbl5nn2k6kz55kgjrad6x6vniyjopngwgc627vbq"/>
-    <hyperlink ref="E10" r:id="rId2" display="https://console.us-ashburn-1.oraclecloud.com/identity/tag-namespaces/ocid1.tagnamespace.oc1..aaaaaaaadzgtve7ubdqntcnzs5etayvagxt35lgjiroopapcjuppphlgka6a/tag-definitions/ocid1.tagdefinition.oc1..aaaaaaaalrrujpcabyq3c4lq6h3dc2fbs42w23t5pigyv5dep3w236eadraa"/>
-    <hyperlink ref="E11" r:id="rId3" display="https://console.us-ashburn-1.oraclecloud.com/identity/tag-namespaces/ocid1.tagnamespace.oc1..aaaaaaaadzgtve7ubdqntcnzs5etayvagxt35lgjiroopapcjuppphlgka6a/tag-definitions/ocid1.tagdefinition.oc1..aaaaaaaalrrujpcabyq3c4lq6h3dc2fbs42w23t5pigyv5dep3w236eadraa"/>
-    <hyperlink ref="E12" r:id="rId4" display="https://console.us-ashburn-1.oraclecloud.com/identity/tag-namespaces/ocid1.tagnamespace.oc1..aaaaaaaadzgtve7ubdqntcnzs5etayvagxt35lgjiroopapcjuppphlgka6a/tag-definitions/ocid1.tagdefinition.oc1..aaaaaaaalrrujpcabyq3c4lq6h3dc2fbs42w23t5pigyv5dep3w236eadraa"/>
-    <hyperlink ref="E13" r:id="rId5" display="https://console.us-ashburn-1.oraclecloud.com/identity/tag-namespaces/ocid1.tagnamespace.oc1..aaaaaaaadzgtve7ubdqntcnzs5etayvagxt35lgjiroopapcjuppphlgka6a/tag-definitions/ocid1.tagdefinition.oc1..aaaaaaaalrrujpcabyq3c4lq6h3dc2fbs42w23t5pigyv5dep3w236eadraa"/>
+    <hyperlink ref="D4" r:id="rId1" display="https://console.us-ashburn-1.oraclecloud.com/a/identity/tag-namespaces/ocid1.tagnamespace.oc1..aaaaaaaa77lkexyrq5t4gpuirhdetct5psrmbouinhad2s5soycj4jyimlwq/tag-definitions/ocid1.tagdefinition.oc1..aaaaaaaavfzlvfl6ndwskbl5nn2k6kz55kgjrad6x6vniyjopngwgc627vbq"/>
+    <hyperlink ref="E11" r:id="rId2" display="https://console.us-ashburn-1.oraclecloud.com/identity/tag-namespaces/ocid1.tagnamespace.oc1..aaaaaaaadzgtve7ubdqntcnzs5etayvagxt35lgjiroopapcjuppphlgka6a/tag-definitions/ocid1.tagdefinition.oc1..aaaaaaaalrrujpcabyq3c4lq6h3dc2fbs42w23t5pigyv5dep3w236eadraa"/>
+    <hyperlink ref="E12" r:id="rId3" display="https://console.us-ashburn-1.oraclecloud.com/identity/tag-namespaces/ocid1.tagnamespace.oc1..aaaaaaaadzgtve7ubdqntcnzs5etayvagxt35lgjiroopapcjuppphlgka6a/tag-definitions/ocid1.tagdefinition.oc1..aaaaaaaalrrujpcabyq3c4lq6h3dc2fbs42w23t5pigyv5dep3w236eadraa"/>
+    <hyperlink ref="E13" r:id="rId4" display="https://console.us-ashburn-1.oraclecloud.com/identity/tag-namespaces/ocid1.tagnamespace.oc1..aaaaaaaadzgtve7ubdqntcnzs5etayvagxt35lgjiroopapcjuppphlgka6a/tag-definitions/ocid1.tagdefinition.oc1..aaaaaaaalrrujpcabyq3c4lq6h3dc2fbs42w23t5pigyv5dep3w236eadraa"/>
+    <hyperlink ref="E14" r:id="rId5" display="https://console.us-ashburn-1.oraclecloud.com/identity/tag-namespaces/ocid1.tagnamespace.oc1..aaaaaaaadzgtve7ubdqntcnzs5etayvagxt35lgjiroopapcjuppphlgka6a/tag-definitions/ocid1.tagdefinition.oc1..aaaaaaaalrrujpcabyq3c4lq6h3dc2fbs42w23t5pigyv5dep3w236eadraa"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OCI Infra Automation Release v2.0
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="210">
   <si>
     <t>Regional</t>
   </si>
@@ -605,6 +605,85 @@
   </si>
   <si>
     <t>10.110.0.0/16</t>
+  </si>
+  <si>
+    <t># DHCP option is created in the same compartment as the VCN; Whichever DHCP option name(case-sensitie) you have mentioned in the Subnets Sheet should be defined here in this sheet; server_type field is also case-sensitive.  if server_type is CustomDnsServer then you should not leave custom_dns_server column empty</t>
+  </si>
+  <si>
+    <t>VCN Peering
+comma seperated VCNs on right column are peered with VCN on left column
+LPGs and rules are created based on this section; 
+eg: Mention Hub VCN name on left side and all spoke VCN names peered with it on right side</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Default Securoty List for PHXHub-VCN</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>0.0.0.0/0</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new  rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
+This sheet will only add new rules to theSecurity Lists; You can also edit Default Security List for a VCN- Mention subnet name as 'Default Security List for &lt;vcn_name&gt;'
+'SecRulesinOCI' sheet would be used for overwrite of all sec rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
+VCN Name and Compartment Name fields in this sheet are just for informational purpose right now; would be used in future when we allow same subnet names across VCNs</t>
+  </si>
+  <si>
+    <t>egress</t>
+  </si>
+  <si>
+    <t>10.20.30.40/32</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn
+vcn_name should be same as enterd in VCNs sheet;
+Route Rules for IGW, NGW and SGW would be created based on parameter values: configure_igw, configure_ngw and configure_sgw respectively for each subnet. The condition is the respectove component should hae been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
+</t>
+  </si>
+  <si>
+    <t># Leave Parent Compartment empty or mention root if it is under root;
+Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
+Compartment Name is mandatory field
+Compartments, Groups, Policies will be created in Home Region So while executing setUpOCI, Enter Region as your tenancy's Home Region for Compartment Creation</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
+Group Name is mandatory field
+Enter Region as your tenancy's Home Region for Group Creation</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new
+ rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
+This sheet will only add new rules to the route tables; 'RouteRulesinOCI' sheet would be used for overwrite of all route rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
+VCN Name and Compartment Name fields in this sheet are just for informational purpose right now; would be used in future when we allow same subnet names across VCNs
+Enter Route Destination Object as either the OCID of component or  the name of component- &lt;vcn_name&gt;_igw|&lt;vcn_name&gt;_lpg|&lt;vcn_name&gt;|ngw|&lt;vcn_name&gt;|drg|&lt;vcn_name&gt;_sgw</t>
+  </si>
+  <si>
+    <t>PHXHub-VCN_igw</t>
+  </si>
+  <si>
+    <t># Horizontal row specifies the TagNameSpace Names to be created; Vertical row under each TagNameSpace represnts Keys in that tagnamespace; Enter compartment name in which  all tagnamespaces and keys will be created;
+Enter Region as your tenancy's Home Region for Tags Creation</t>
+  </si>
+  <si>
+    <t>$ and * in PolicyStatements would be replaced by PolicyStatementGroup and PolicyStatementCompartment respectively;If Compartment Name is left empty or mentioned 'root', policy will be created in root compartment;
+# Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
+Enter Region as your tenancy's Home Region for Policy Creation</t>
+  </si>
+  <si>
+    <t>regions</t>
+  </si>
+  <si>
+    <t>Ashburn,Phoenix</t>
   </si>
   <si>
     <r>
@@ -765,79 +844,28 @@
       <t xml:space="preserve"> represents whether you want to add Ping rules for peered VCNs; useful for network related testing
 </t>
     </r>
-  </si>
-  <si>
-    <t># DHCP option is created in the same compartment as the VCN; Whichever DHCP option name(case-sensitie) you have mentioned in the Subnets Sheet should be defined here in this sheet; server_type field is also case-sensitive.  if server_type is CustomDnsServer then you should not leave custom_dns_server column empty</t>
-  </si>
-  <si>
-    <t>VCN Peering
-comma seperated VCNs on right column are peered with VCN on left column
-LPGs and rules are created based on this section; 
-eg: Mention Hub VCN name on left side and all spoke VCN names peered with it on right side</t>
-  </si>
-  <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>Default Securoty List for PHXHub-VCN</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>0.0.0.0/0</t>
-  </si>
-  <si>
-    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new  rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
-This sheet will only add new rules to theSecurity Lists; You can also edit Default Security List for a VCN- Mention subnet name as 'Default Security List for &lt;vcn_name&gt;'
-'SecRulesinOCI' sheet would be used for overwrite of all sec rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
-VCN Name and Compartment Name fields in this sheet are just for informational purpose right now; would be used in future when we allow same subnet names across VCNs</t>
-  </si>
-  <si>
-    <t>egress</t>
-  </si>
-  <si>
-    <t>10.20.30.40/32</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">regions </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">represents regions client's tenancy is subscribed to and plan to build infra for;accepts comma seperated list
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn
-vcn_name should be same as enterd in VCNs sheet;
-Route Rules for IGW, NGW and SGW would be created based on parameter values: configure_igw, configure_ngw and configure_sgw respectively for each subnet. The condition is the respectove component should hae been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
-</t>
-  </si>
-  <si>
-    <t># Leave Parent Compartment empty or mention root if it is under root;
-Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
-Compartment Name is mandatory field
-Compartments, Groups, Policies will be created in Home Region So while executing setUpOCI, Enter Region as your tenancy's Home Region for Compartment Creation</t>
-  </si>
-  <si>
-    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
-Group Name is mandatory field
-Enter Region as your tenancy's Home Region for Group Creation</t>
-  </si>
-  <si>
-    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new
- rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
-This sheet will only add new rules to the route tables; 'RouteRulesinOCI' sheet would be used for overwrite of all route rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
-VCN Name and Compartment Name fields in this sheet are just for informational purpose right now; would be used in future when we allow same subnet names across VCNs
-Enter Route Destination Object as either the OCID of component or  the name of component- &lt;vcn_name&gt;_igw|&lt;vcn_name&gt;_lpg|&lt;vcn_name&gt;|ngw|&lt;vcn_name&gt;|drg|&lt;vcn_name&gt;_sgw</t>
-  </si>
-  <si>
-    <t>PHXHub-VCN_igw</t>
-  </si>
-  <si>
-    <t># Horizontal row specifies the TagNameSpace Names to be created; Vertical row under each TagNameSpace represnts Keys in that tagnamespace; Enter compartment name in which  all tagnamespaces and keys will be created;
-Enter Region as your tenancy's Home Region for Tags Creation</t>
-  </si>
-  <si>
-    <t>$ and * in PolicyStatements would be replaced by PolicyStatementGroup and PolicyStatementCompartment respectively;If Compartment Name is left empty or mentioned 'root', policy will be created in root compartment;
-# Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
-Enter Region as your tenancy's Home Region for Policy Creation</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -915,7 +943,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1030,11 +1058,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1122,6 +1159,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1442,7 +1481,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1562,7 +1601,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="18" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -2031,7 +2070,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -2082,7 +2121,7 @@
         <v>119</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>120</v>
@@ -2162,7 +2201,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -2266,19 +2305,19 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>135</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2298,10 +2337,10 @@
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G5" s="1" t="b">
         <v>0</v>
@@ -2310,7 +2349,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2548,7 +2587,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="29"/>
@@ -2621,7 +2660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
@@ -2637,7 +2676,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -2789,7 +2828,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -3020,10 +3059,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3033,9 +3072,9 @@
     <col min="3" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="222.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="B1" s="34"/>
     </row>
@@ -3097,32 +3136,40 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="B10" s="36"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="36"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>180</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3154,7 +3201,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -3319,7 +3366,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -3472,7 +3519,7 @@
         <v>182</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Added NSG feature Modified setUpOCI to accept properties file instead of user input on cmd prompt
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <sheet name="AddSecRules" sheetId="12" r:id="rId14"/>
     <sheet name="RouteRulesinOCI" sheetId="16" r:id="rId15"/>
     <sheet name="SecRulesinOCI" sheetId="17" r:id="rId16"/>
+    <sheet name="NSGs" sheetId="19" r:id="rId17"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="239">
   <si>
     <t>Regional</t>
   </si>
@@ -506,9 +507,6 @@
   </si>
   <si>
     <t># Make sure to enter exact name in attached_to_instance column as entered in Hostname of Instances sheet;Backup Policy column can be left blank at the timeof block vol creation and can be filled up later on while attaching backup policy to the boot abd block volumes together;</t>
-  </si>
-  <si>
-    <t>#Template will be picked upon from template folder based on  OS column; Backup Policy column can be left blank at the time of instance creation and can be filled up later on while attaching backup policy to the boot abd block volumes together;ssh-key-var-name is the name of variable defined in variable.tf file containing SSH key to be pushed to the server</t>
   </si>
   <si>
     <t>Demo</t>
@@ -867,12 +865,102 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>NSGName</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>SourceType</t>
+  </si>
+  <si>
+    <t>DestType</t>
+  </si>
+  <si>
+    <t>Demo1</t>
+  </si>
+  <si>
+    <t>ASH-VCN1</t>
+  </si>
+  <si>
+    <t>ash-vcn1-nsg</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>cidr</t>
+  </si>
+  <si>
+    <t>172.0.0.0/8</t>
+  </si>
+  <si>
+    <t>icmp</t>
+  </si>
+  <si>
+    <t>ASH-Hub-VCN</t>
+  </si>
+  <si>
+    <t>ash-hub-nsg1</t>
+  </si>
+  <si>
+    <t>nsg</t>
+  </si>
+  <si>
+    <t>ash-hub-nsg2</t>
+  </si>
+  <si>
+    <t>OCICtoOCI</t>
+  </si>
+  <si>
+    <t>PHX-Hub-VCN</t>
+  </si>
+  <si>
+    <t>phx-hub-nsg1</t>
+  </si>
+  <si>
+    <t>10.116.0.0/16</t>
+  </si>
+  <si>
+    <t>udp</t>
+  </si>
+  <si>
+    <t>173.0.0.0/8</t>
+  </si>
+  <si>
+    <t>phx-hub-nsg2</t>
+  </si>
+  <si>
+    <t>PHX-VCN1</t>
+  </si>
+  <si>
+    <t>phx-vcn1-nsg</t>
+  </si>
+  <si>
+    <t>10.117.2.0/24</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>oci-phx-objectstorage</t>
+  </si>
+  <si>
+    <t>NSGs</t>
+  </si>
+  <si>
+    <t>#Template will be picked upon from template folder based on  OS column; Backup Policy column can be left blank at the time of instance creation and can be filled up later on while attaching backup policy to the boot abd block volumes together;ssh-key-var-name is the name of variable defined in variable.tf file containing SSH key to be pushed to the server; NSGs column accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG</t>
+  </si>
+  <si>
+    <t>Valid values for sourcetype or destinationtype are: cidr(for CIDR_BLOCK), nsg(for NETWORK_SECURITY_GROUP) and service(for SERVICE_CIDR_BLOCK)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -914,6 +1002,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1071,7 +1165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1114,6 +1208,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1159,8 +1258,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1480,16 +1584,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="A1" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>86</v>
@@ -1503,7 +1607,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>89</v>
@@ -1515,7 +1619,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>91</v>
@@ -1525,7 +1629,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>92</v>
@@ -1539,7 +1643,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>94</v>
@@ -1600,19 +1704,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="18" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="A1" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>138</v>
@@ -1634,13 +1738,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>182</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="40" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -1657,9 +1761,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="38"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="9" t="s">
         <v>58</v>
       </c>
@@ -1674,11 +1778,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="38"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>62</v>
@@ -1691,9 +1795,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="38"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="10"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
@@ -1704,9 +1808,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="38"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="12"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
@@ -1715,9 +1819,9 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="38"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="41"/>
       <c r="D8" s="12"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
@@ -1726,9 +1830,9 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="38"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="41"/>
       <c r="D9" s="12"/>
       <c r="E9" s="1"/>
       <c r="F9" s="11" t="s">
@@ -1737,9 +1841,9 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="38"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="12"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
@@ -1748,9 +1852,9 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="38"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="12"/>
       <c r="E11" s="1"/>
       <c r="F11" s="11" t="s">
@@ -1759,9 +1863,9 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="38"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="12"/>
       <c r="E12" s="1"/>
       <c r="F12" s="11" t="s">
@@ -1770,9 +1874,9 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="38"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="12"/>
       <c r="E13" s="1"/>
       <c r="F13" s="11" t="s">
@@ -1781,9 +1885,9 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="38"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="41"/>
       <c r="D14" s="12"/>
       <c r="E14" s="1"/>
       <c r="F14" s="11" t="s">
@@ -1792,9 +1896,9 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="38"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="10"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
@@ -1803,9 +1907,9 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="38"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="10"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
@@ -1814,9 +1918,9 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="38"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="10"/>
       <c r="E17" s="1"/>
       <c r="F17" s="11" t="s">
@@ -1825,9 +1929,9 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="39"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="10"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
@@ -1873,18 +1977,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="18" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="A1" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>77</v>
@@ -1904,7 +2008,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>144</v>
@@ -1913,10 +2017,10 @@
         <v>145</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>146</v>
@@ -1924,19 +2028,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>147</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>146</v>
@@ -1969,18 +2073,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="18" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="A1" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>148</v>
@@ -2000,7 +2104,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>149</v>
@@ -2009,10 +2113,10 @@
         <v>145</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>146</v>
@@ -2020,19 +2124,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>150</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>146</v>
@@ -2069,22 +2173,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="A1" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>112</v>
@@ -2110,7 +2214,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2121,7 +2225,7 @@
         <v>119</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>120</v>
@@ -2132,7 +2236,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2200,27 +2304,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
+      <c r="A1" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>112</v>
@@ -2267,7 +2371,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2300,24 +2404,24 @@
     </row>
     <row r="4" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>135</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2329,7 +2433,7 @@
     </row>
     <row r="5" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2337,10 +2441,10 @@
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G5" s="1" t="b">
         <v>0</v>
@@ -2349,7 +2453,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2434,7 +2538,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>112</v>
@@ -2487,7 +2591,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>112</v>
@@ -2567,6 +2671,737 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:Q1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="18" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="K3" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I4" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I5" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1">
+        <v>22</v>
+      </c>
+      <c r="O5" s="1">
+        <v>22</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="K6" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="I7" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="K8" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I9" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I10" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I11" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I12" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="K13" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I14" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I15" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I16" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K17" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="K18" s="46" t="s">
+        <v>232</v>
+      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2586,15 +3421,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
+      <c r="A1" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>86</v>
@@ -2605,7 +3440,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>98</v>
@@ -2616,7 +3451,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>100</v>
@@ -2627,7 +3462,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>102</v>
@@ -2675,19 +3510,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
+      <c r="A1" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>86</v>
@@ -2710,7 +3545,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>104</v>
@@ -2755,7 +3590,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>108</v>
@@ -2807,7 +3642,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2827,25 +3662,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32"/>
+      <c r="A1" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -2886,13 +3721,13 @@
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>26</v>
@@ -2927,7 +3762,7 @@
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>30</v>
@@ -2966,13 +3801,13 @@
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>26</v>
@@ -2987,7 +3822,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I5" s="3">
         <v>2</v>
@@ -3002,7 +3837,7 @@
         <v>89</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3061,8 +3896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3073,48 +3908,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="222.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1" s="34"/>
+      <c r="A1" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="37"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>167</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>27</v>
@@ -3122,7 +3957,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>26</v>
@@ -3130,40 +3965,40 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="B10" s="44" t="s">
-        <v>208</v>
-      </c>
     </row>
     <row r="11" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" s="36"/>
+      <c r="A11" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="39"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -3200,19 +4035,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
+      <c r="A1" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
     </row>
     <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3260,7 +4095,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -3365,13 +4200,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="A1" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3437,10 +4272,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,25 +4295,26 @@
     <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="32"/>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>77</v>
@@ -3513,13 +4349,16 @@
       <c r="L2" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -3551,8 +4390,11 @@
       <c r="L3" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3565,12 +4407,12 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C6" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3596,20 +4438,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="18" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>37</v>
@@ -3635,7 +4477,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>149</v>

</xml_diff>

<commit_message>
Added support for specifying names for VCN components(excel LPGs) as well as route tables and security lists.
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="243">
   <si>
     <t>Regional</t>
   </si>
@@ -42,18 +42,6 @@
   </si>
   <si>
     <t>vcn_cidr</t>
-  </si>
-  <si>
-    <t>drg_required(y|n)</t>
-  </si>
-  <si>
-    <t>igw_required(y|n)</t>
-  </si>
-  <si>
-    <t>ngw_required(y|n)</t>
-  </si>
-  <si>
-    <t>sgw_required(y|n)</t>
   </si>
   <si>
     <t>hub_spoke_none</t>
@@ -470,16 +458,6 @@
     <t>10.20.30.40/32</t>
   </si>
   <si>
-    <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn
-vcn_name should be same as enterd in VCNs sheet;
-Route Rules for IGW, NGW and SGW would be created based on parameter values: configure_igw, configure_ngw and configure_sgw respectively for each subnet. The condition is the respectove component should hae been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
-</t>
-  </si>
-  <si>
     <t># Leave Parent Compartment empty or mention root if it is under root;
 Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
 Compartment Name is mandatory field
@@ -491,13 +469,6 @@
 Enter Region as your tenancy's Home Region for Group Creation</t>
   </si>
   <si>
-    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new
- rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
-This sheet will only add new rules to the route tables; 'RouteRulesinOCI' sheet would be used for overwrite of all route rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
-VCN Name and Compartment Name fields in this sheet are just for informational purpose right now; would be used in future when we allow same subnet names across VCNs
-Enter Route Destination Object as either the OCID of component or  the name of component- &lt;vcn_name&gt;_igw|&lt;vcn_name&gt;_lpg|&lt;vcn_name&gt;|ngw|&lt;vcn_name&gt;|drg|&lt;vcn_name&gt;_sgw</t>
-  </si>
-  <si>
     <t># Horizontal row specifies the TagNameSpace Names to be created; Vertical row under each TagNameSpace represnts Keys in that tagnamespace; Enter compartment name in which  all tagnamespaces and keys will be created;
 Enter Region as your tenancy's Home Region for Tags Creation</t>
   </si>
@@ -718,9 +689,6 @@
   </si>
   <si>
     <t>prod=True</t>
-  </si>
-  <si>
-    <t>ASHHub-VCN_igw</t>
   </si>
   <si>
     <t>Default Security List for ASHHub-VCN</t>
@@ -927,6 +895,103 @@
       <t xml:space="preserve">represents regions client's tenancy is subscribed to and plan to build infra for;accepts comma seperated list; case insensitive; (allowed values: ashburn, phoenix, london, frankfurt, toronto, tokyo, seoul, mumbai)
 </t>
     </r>
+  </si>
+  <si>
+    <t>drg_required</t>
+  </si>
+  <si>
+    <t>igw_required</t>
+  </si>
+  <si>
+    <t>ngw_required</t>
+  </si>
+  <si>
+    <t>sgw_required</t>
+  </si>
+  <si>
+    <t>PHX-DRG</t>
+  </si>
+  <si>
+    <t>ASH-DRG</t>
+  </si>
+  <si>
+    <t>ashprodNGW</t>
+  </si>
+  <si>
+    <t>ashprodIGW</t>
+  </si>
+  <si>
+    <t>ngw:ashprodNGW</t>
+  </si>
+  <si>
+    <t>ngw:PHXNonProd-VCN_ngw</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new
+ rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
+This sheet will only add new rules to the route tables; 'RouteRulesinOCI' sheet would be used for overwrite of all route rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
+VCN Name and Compartment Name fields in this sheet are just for informational purpose right now; would be used in future when we allow same subnet names across VCNs
+Enter Route Destination Object as either the OCID of component or  name of component- spcify name as igw:&lt;IGWName&gt;, ngw:&lt;NGWName&gt;, sgw:&lt;SGWName&gt;, drg:&lt;DRGName&gt;, lpg:&lt;LPGName&gt;</t>
+  </si>
+  <si>
+    <t>route_table_name</t>
+  </si>
+  <si>
+    <t>seclist_name</t>
+  </si>
+  <si>
+    <t>devqa_seclist</t>
+  </si>
+  <si>
+    <t>proddr_seclist</t>
+  </si>
+  <si>
+    <t>phx_rt</t>
+  </si>
+  <si>
+    <t>ash_rt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn
+vcn_name should be same as enterd in VCNs sheet;
+Route Rules for IGW, NGW and SGW would be created based on parameter values: configure_igw, configure_ngw and configure_sgw respectively for each subnet. The condition is the respective component should have been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
+You can specify names for route tables and Scurity Lists; subnets can share same route table and seclist depending upon name specified; If left blank, default name which is subnet name would be used for that route table as well as security list.
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars;
+Valid Values for columns D,E,F,G:   y|n|&lt;component_name&gt; ie mention 'n' when a component(like IGW) is not required to be configured(like for PHXHub-VCN), specify name of the component- component will be configured with the mentioned name(eg PHX-DRG for the DRG in PHXHub-VCN) and mention 'y' if component needs to be configured with default name ie &lt;vcnname&gt;_ngw(eg PHXNonProd-VCN_ngw)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Not possible to specify names for LPGs
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Subnet Name/RouteTable Name</t>
+  </si>
+  <si>
+    <t>SubnetName/SecurityListName</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1226,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1221,6 +1285,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1541,96 +1608,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
+      <c r="A1" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1638,7 +1705,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1676,208 +1743,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="17" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="A1" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="D3" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="42"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="9"/>
       <c r="E5" s="1"/>
       <c r="F5" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="42"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="9"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="11"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="42"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="41"/>
       <c r="D8" s="11"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="42"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="41"/>
       <c r="D9" s="11"/>
       <c r="E9" s="1"/>
       <c r="F9" s="10"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="42"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="11"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="42"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="11"/>
       <c r="E11" s="1"/>
       <c r="F11" s="10"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="42"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="11"/>
       <c r="E12" s="1"/>
       <c r="F12" s="10"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="42"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="11"/>
       <c r="E13" s="1"/>
       <c r="F13" s="10"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="42"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="41"/>
       <c r="D14" s="11"/>
       <c r="E14" s="1"/>
       <c r="F14" s="10"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="42"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="9"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="42"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="9"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="42"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="9"/>
       <c r="E17" s="1"/>
       <c r="F17" s="10"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="43"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="9"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1914,73 +1981,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="A1" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2010,73 +2077,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="A1" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>215</v>
-      </c>
       <c r="E3" s="17" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2089,10 +2156,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,7 +2167,7 @@
     <col min="1" max="1" width="9.140625" style="17"/>
     <col min="2" max="2" width="11.7109375" style="17" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="17"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="86.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
@@ -2109,41 +2176,41 @@
     <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+    <row r="1" spans="1:10" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>84</v>
-      </c>
       <c r="G2" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="20"/>
@@ -2151,43 +2218,43 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="22" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="22" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2195,17 +2262,39 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="D5" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2220,8 +2309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,91 +2330,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
+      <c r="A1" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>97</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -2341,24 +2430,24 @@
     </row>
     <row r="4" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2370,18 +2459,18 @@
     </row>
     <row r="5" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G5" s="1" t="b">
         <v>0</v>
@@ -2390,7 +2479,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2399,7 +2488,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2475,25 +2564,25 @@
   <sheetData>
     <row r="1" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>84</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="20"/>
@@ -2528,83 +2617,83 @@
   <sheetData>
     <row r="1" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>97</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>101</v>
       </c>
       <c r="P1" s="12"/>
       <c r="Q1" s="20"/>
       <c r="R1" s="20"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2634,108 +2723,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
+      <c r="A1" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F2" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="I2" s="29" t="s">
+      <c r="N2" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="K2" s="20" t="s">
+      <c r="O2" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q2" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="30"/>
+      <c r="I3" s="29"/>
       <c r="J3" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>161</v>
+        <v>153</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>154</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2746,31 +2835,31 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>138</v>
+        <v>149</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>134</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -2787,31 +2876,31 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="K5" s="30" t="s">
-        <v>158</v>
+        <v>149</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>151</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2822,31 +2911,31 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>224</v>
+        <v>150</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>216</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -2882,66 +2971,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="33"/>
+      <c r="A1" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2974,57 +3063,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="36"/>
+      <c r="A1" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>79</v>
+      <c r="A2" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -3034,13 +3123,13 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3054,25 +3143,25 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3081,16 +3170,16 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3106,7 +3195,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3125,26 +3214,26 @@
     <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36"/>
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -3153,60 +3242,60 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>226</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I3" s="1">
         <v>3</v>
@@ -3215,39 +3304,39 @@
         <v>200</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="I4" s="1">
         <v>3</v>
@@ -3256,37 +3345,37 @@
         <v>200</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>227</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I5" s="3">
         <v>3</v>
@@ -3295,39 +3384,39 @@
         <v>200</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="I6" s="3">
         <v>3</v>
@@ -3336,15 +3425,15 @@
         <v>200</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3398,8 +3487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:B13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3410,97 +3499,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>229</v>
-      </c>
-      <c r="B1" s="38"/>
+      <c r="A1" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="37"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>150</v>
+      <c r="A10" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="40"/>
+      <c r="A11" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="39"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3515,10 +3604,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3530,74 +3619,83 @@
     <col min="5" max="5" width="24.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="8" max="9" width="18.42578125" style="17" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-    </row>
-    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+    </row>
+    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -3606,33 +3704,37 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -3641,33 +3743,37 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>20</v>
+        <v>183</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
@@ -3676,33 +3782,37 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>20</v>
+        <v>183</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>0</v>
@@ -3711,33 +3821,35 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>0</v>
@@ -3746,33 +3858,39 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>21</v>
+        <v>183</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>0</v>
@@ -3781,24 +3899,28 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>20</v>
+        <v>183</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3810,8 +3932,10 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -3823,8 +3947,10 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -3836,8 +3962,10 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -3849,10 +3977,12 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3877,96 +4007,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="A1" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>23</v>
+      <c r="A6" s="30" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>195</v>
+        <v>14</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>188</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -4004,221 +4134,221 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36"/>
+      <c r="A1" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="H2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="J2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="N3" s="22"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -4249,93 +4379,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="17" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="A1" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C3" s="1">
         <v>150</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C4" s="1">
         <v>150</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added support for FSS through cd3 as well as csv and configured older version of terraform for panda execution
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -18,20 +18,21 @@
     <sheet name="AddSecRules" sheetId="12" r:id="rId9"/>
     <sheet name="RouteRulesinOCI" sheetId="16" r:id="rId10"/>
     <sheet name="SecRulesinOCI" sheetId="17" r:id="rId11"/>
-    <sheet name="DedicatedVMHosts" sheetId="20" r:id="rId12"/>
-    <sheet name="Instances" sheetId="4" r:id="rId13"/>
-    <sheet name="BlockVols" sheetId="5" r:id="rId14"/>
-    <sheet name="Tags" sheetId="6" r:id="rId15"/>
-    <sheet name="TagServer" sheetId="13" r:id="rId16"/>
-    <sheet name="TagVolume" sheetId="14" r:id="rId17"/>
-    <sheet name="NSGs" sheetId="19" r:id="rId18"/>
+    <sheet name="NSGs" sheetId="19" r:id="rId12"/>
+    <sheet name="DedicatedVMHosts" sheetId="20" r:id="rId13"/>
+    <sheet name="Instances" sheetId="4" r:id="rId14"/>
+    <sheet name="BlockVols" sheetId="5" r:id="rId15"/>
+    <sheet name="FSS" sheetId="21" r:id="rId16"/>
+    <sheet name="Tags" sheetId="6" r:id="rId17"/>
+    <sheet name="TagServer" sheetId="13" r:id="rId18"/>
+    <sheet name="TagVolume" sheetId="14" r:id="rId19"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="272">
   <si>
     <t>Regional</t>
   </si>
@@ -1044,11 +1045,72 @@
       <t>Please use different names for route tables/seclists across VCNs</t>
     </r>
   </si>
+  <si>
+    <t>MountTarget Name</t>
+  </si>
+  <si>
+    <t>MountTarget IP</t>
+  </si>
+  <si>
+    <t>MountTarget Hostname</t>
+  </si>
+  <si>
+    <t>FSS Name</t>
+  </si>
+  <si>
+    <t>Availability Domain</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>sourceCIDR</t>
+  </si>
+  <si>
+    <t>GID</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>IDSquash (NONE|ALL|ROOT)</t>
+  </si>
+  <si>
+    <t>Access (READ_ONLY|READ_WRITE)</t>
+  </si>
+  <si>
+    <t>require_ps_port (true|false)</t>
+  </si>
+  <si>
+    <t>Max FSS inodes</t>
+  </si>
+  <si>
+    <t>Max FSS Capacity (in bytes)</t>
+  </si>
+  <si>
+    <t>Demo1</t>
+  </si>
+  <si>
+    <t>/fss/</t>
+  </si>
+  <si>
+    <t>FSS1</t>
+  </si>
+  <si>
+    <t>MT1</t>
+  </si>
+  <si>
+    <t>MountTarget SubnetName</t>
+  </si>
+  <si>
+    <t>Columns: Region, Compartment Name, Availability Domain, MountTarget Name, MountTarget SubnetName, FSS name, Path are mandatory.
+Default value for sourceCIDR- 0.0.0.0/0, Access- READ_ONLY, GID- 65534, UID- 65534, IDSquash- NONE and require_ps_port- false</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1241,7 +1303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1292,6 +1354,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1322,6 +1390,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1336,9 +1413,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1650,23 +1724,23 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="14.54296875" customWidth="1"/>
+    <col min="3" max="3" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>126</v>
       </c>
@@ -1680,7 +1754,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
@@ -1692,7 +1766,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>127</v>
       </c>
@@ -1704,7 +1778,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>127</v>
       </c>
@@ -1718,7 +1792,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>127</v>
       </c>
@@ -1732,7 +1806,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>127</v>
       </c>
@@ -1746,7 +1820,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>62</v>
       </c>
@@ -1754,7 +1828,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>63</v>
       </c>
@@ -1762,7 +1836,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1784,21 +1858,21 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="19.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="19.26953125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="17" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" style="17" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>126</v>
       </c>
@@ -1838,20 +1912,20 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="11.7109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="17"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="17"/>
-    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="11.7265625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="17"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1796875" style="17"/>
+    <col min="17" max="17" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>126</v>
       </c>
@@ -1901,31 +1975,31 @@
       <c r="Q1" s="20"/>
       <c r="R1" s="20"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="23"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="23"/>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
@@ -1938,32 +2012,287 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
+        <v>123</v>
+      </c>
+      <c r="O4" s="1">
+        <v>123</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
         <v>248</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>126</v>
       </c>
@@ -1983,7 +2312,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>128</v>
       </c>
@@ -2001,7 +2330,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>127</v>
       </c>
@@ -2021,7 +2350,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>62</v>
       </c>
@@ -2031,7 +2360,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>127</v>
       </c>
@@ -2059,7 +2388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
@@ -2067,43 +2396,43 @@
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" customWidth="1"/>
+    <col min="11" max="11" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="36"/>
-    </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="38"/>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>126</v>
       </c>
@@ -2147,7 +2476,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
@@ -2186,7 +2515,7 @@
       </c>
       <c r="O3" s="22"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>128</v>
       </c>
@@ -2228,7 +2557,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>127</v>
       </c>
@@ -2272,7 +2601,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>128</v>
       </c>
@@ -2322,7 +2651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -2330,30 +2659,30 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1"/>
+    <col min="7" max="7" width="26.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="17" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:8" s="17" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-    </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>126</v>
       </c>
@@ -2379,7 +2708,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
@@ -2405,7 +2734,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>128</v>
       </c>
@@ -2431,7 +2760,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2441,7 +2770,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2459,7 +2788,225 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="8.36328125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="7.7265625" style="17" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" customWidth="1"/>
+    <col min="13" max="13" width="12.26953125" customWidth="1"/>
+    <col min="16" max="16" width="11.1796875" customWidth="1"/>
+    <col min="17" max="17" width="10.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+    </row>
+    <row r="2" spans="1:17" s="32" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="N2" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="O2" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q2" s="33" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -2467,27 +3014,27 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="17" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:7" s="17" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>126</v>
       </c>
@@ -2510,14 +3057,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="47" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -2533,10 +3080,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="43"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="8" t="s">
         <v>204</v>
       </c>
@@ -2550,10 +3097,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="43"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="9"/>
       <c r="E5" s="1"/>
       <c r="F5" s="10" t="s">
@@ -2563,10 +3110,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="43"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="9"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
@@ -2576,109 +3123,109 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="43"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="11"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="43"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="11"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="43"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="11"/>
       <c r="E9" s="1"/>
       <c r="F9" s="10"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="43"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="11"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="43"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="11"/>
       <c r="E11" s="1"/>
       <c r="F11" s="10"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="43"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="11"/>
       <c r="E12" s="1"/>
       <c r="F12" s="10"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="43"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="11"/>
       <c r="E13" s="1"/>
       <c r="F13" s="10"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="43"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="11"/>
       <c r="E14" s="1"/>
       <c r="F14" s="10"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="43"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="50"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="9"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="43"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="50"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="9"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="43"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="50"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="9"/>
       <c r="E17" s="1"/>
       <c r="F17" s="10"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="44"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="50"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="9"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2696,7 +3243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -2704,27 +3251,27 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="17" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:6" s="17" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>126</v>
       </c>
@@ -2744,7 +3291,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>127</v>
       </c>
@@ -2764,7 +3311,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>128</v>
       </c>
@@ -2792,7 +3339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -2800,27 +3347,27 @@
       <selection activeCell="C3" sqref="C3:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="17" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:6" s="17" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>126</v>
       </c>
@@ -2840,7 +3387,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>127</v>
       </c>
@@ -2860,7 +3407,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>128</v>
       </c>
@@ -2885,261 +3432,6 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1">
-        <v>123</v>
-      </c>
-      <c r="O4" s="1">
-        <v>123</v>
-      </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:Q1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3151,21 +3443,21 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="33"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="35"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>126</v>
       </c>
@@ -3176,7 +3468,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
@@ -3187,7 +3479,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>127</v>
       </c>
@@ -3198,7 +3490,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>127</v>
       </c>
@@ -3209,14 +3501,14 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>63</v>
       </c>
@@ -3240,28 +3532,28 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="36"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="38"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>126</v>
       </c>
@@ -3284,7 +3576,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
@@ -3305,7 +3597,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3320,7 +3612,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3329,7 +3621,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>127</v>
       </c>
@@ -3352,7 +3644,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3365,7 +3657,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -3386,40 +3678,40 @@
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36"/>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="38"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>126</v>
       </c>
@@ -3460,7 +3752,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>128</v>
       </c>
@@ -3501,7 +3793,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>128</v>
       </c>
@@ -3540,7 +3832,7 @@
       </c>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>127</v>
       </c>
@@ -3581,7 +3873,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>127</v>
       </c>
@@ -3619,20 +3911,20 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -3646,9 +3938,9 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -3679,20 +3971,20 @@
       <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" style="17" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="32.26953125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:2" ht="238.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="38"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="40"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>116</v>
       </c>
@@ -3700,7 +3992,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>118</v>
       </c>
@@ -3708,25 +4000,25 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>123</v>
       </c>
@@ -3734,7 +4026,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="21" t="s">
         <v>124</v>
       </c>
@@ -3742,7 +4034,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
         <v>125</v>
       </c>
@@ -3750,7 +4042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>142</v>
       </c>
@@ -3758,13 +4050,13 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+    <row r="11" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="40"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="42"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>164</v>
       </c>
@@ -3772,7 +4064,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>15</v>
       </c>
@@ -3794,44 +4086,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="18.42578125" style="17" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.453125" customWidth="1"/>
+    <col min="6" max="6" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.453125" style="17" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:13" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-    </row>
-    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+    </row>
+    <row r="2" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>101</v>
       </c>
@@ -3872,7 +4164,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -3911,7 +4203,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -3950,7 +4242,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -3989,7 +4281,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -4026,7 +4318,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
@@ -4067,7 +4359,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
@@ -4106,7 +4398,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>62</v>
       </c>
@@ -4123,7 +4415,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4138,7 +4430,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4153,7 +4445,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -4185,25 +4477,25 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-    </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+    </row>
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -4220,7 +4512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4234,7 +4526,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -4248,7 +4540,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>165</v>
       </c>
@@ -4265,7 +4557,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
@@ -4282,7 +4574,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -4304,35 +4596,35 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="11.7109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="17"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="86.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="17" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="11.7265625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="17"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="86.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" style="17" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:10" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>126</v>
       </c>
@@ -4358,7 +4650,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
@@ -4380,7 +4672,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>128</v>
       </c>
@@ -4402,7 +4694,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>128</v>
       </c>
@@ -4424,7 +4716,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
@@ -4455,42 +4747,42 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="11.7109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="17"/>
-    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="11.7265625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="17"/>
+    <col min="4" max="4" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>126</v>
       </c>
@@ -4537,7 +4829,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
@@ -4570,7 +4862,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>127</v>
       </c>
@@ -4599,7 +4891,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>128</v>
       </c>
@@ -4628,7 +4920,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
@@ -4645,7 +4937,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -4659,7 +4951,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>

</xml_diff>

<commit_message>
Added LBR, ADW/ATP, DBSystem Modified panda to add only boot volume of 1.5 TB. remove mounting for block volume(variables.yml); Moved panda creation to outside of oraclemigration coz of TF issue; used latest tf version for panda.tf also Added support for createOCSWork.py to be able to run from linux machine also
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="11" activeTab="18"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -23,16 +23,19 @@
     <sheet name="Instances" sheetId="4" r:id="rId14"/>
     <sheet name="BlockVols" sheetId="5" r:id="rId15"/>
     <sheet name="FSS" sheetId="21" r:id="rId16"/>
-    <sheet name="Tags" sheetId="6" r:id="rId17"/>
-    <sheet name="TagServer" sheetId="13" r:id="rId18"/>
-    <sheet name="TagVolume" sheetId="14" r:id="rId19"/>
+    <sheet name="LBR" sheetId="22" r:id="rId17"/>
+    <sheet name="Tags" sheetId="6" r:id="rId18"/>
+    <sheet name="TagServer" sheetId="13" r:id="rId19"/>
+    <sheet name="TagVolume" sheetId="14" r:id="rId20"/>
+    <sheet name="ADW_ATP" sheetId="24" r:id="rId21"/>
+    <sheet name="Database" sheetId="25" r:id="rId22"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="373">
   <si>
     <t>Regional</t>
   </si>
@@ -1062,12 +1065,355 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>LBR Name</t>
+  </si>
+  <si>
+    <t>LBR Subnets</t>
+  </si>
+  <si>
+    <t>Listener Port</t>
+  </si>
+  <si>
+    <t>Backend HealthCheck
+Port</t>
+  </si>
+  <si>
+    <t>Is Private(True|False)</t>
+  </si>
+  <si>
+    <t>Backend
+ServerName:Port</t>
+  </si>
+  <si>
+    <t>LBR Hostname</t>
+  </si>
+  <si>
+    <t>my_lbr</t>
+  </si>
+  <si>
+    <t>Backend
+Policy(LEAST_CONNECTIONS|ROUND_ROBIN|IP_HASH)</t>
+  </si>
+  <si>
+    <t>HTTP</t>
+  </si>
+  <si>
+    <t>Shape(100Mbps|400Mbps|8000Mbps</t>
+  </si>
+  <si>
+    <t>Backend HealthCheck
+Protocol
+(HTTP|TCP)</t>
+  </si>
+  <si>
+    <t>Backend HealthCheck URL</t>
+  </si>
+  <si>
+    <t>400Mbps</t>
+  </si>
+  <si>
+    <t>10.111.1.4:80,Test2:81</t>
+  </si>
+  <si>
+    <t>IP_HASH</t>
+  </si>
+  <si>
+    <t>/welcome.html</t>
+  </si>
+  <si>
+    <t>app.example.com</t>
+  </si>
+  <si>
+    <t>UseSSL (y|n)</t>
+  </si>
+  <si>
+    <t>Public Cert</t>
+  </si>
+  <si>
+    <t>CA Cert</t>
+  </si>
+  <si>
+    <t>Private Key</t>
+  </si>
+  <si>
+    <t>Passphrase</t>
+  </si>
+  <si>
+    <t>OCICtoOCI</t>
+  </si>
+  <si>
+    <t>D:\\certificate.pem</t>
+  </si>
+  <si>
+    <t>D:\\key.pem</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DB Name: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Should Not be more than 14 character | Should contain only AlphaNumeric Characters</t>
+    </r>
+  </si>
+  <si>
+    <t>Display Name</t>
+  </si>
+  <si>
+    <t>DB Name</t>
+  </si>
+  <si>
+    <t>Admin Password</t>
+  </si>
+  <si>
+    <t>CPU Count</t>
+  </si>
+  <si>
+    <t>Size in TB</t>
+  </si>
+  <si>
+    <t>ADW or ATP</t>
+  </si>
+  <si>
+    <t>ADW_23_9_CD3</t>
+  </si>
+  <si>
+    <t>ADWAc3</t>
+  </si>
+  <si>
+    <t>Rajvilla#6330</t>
+  </si>
+  <si>
+    <t>ADW</t>
+  </si>
+  <si>
+    <t>ATP_23_9_CD3</t>
+  </si>
+  <si>
+    <t>ATPAc3</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>ADW_23_9_CD3_P</t>
+  </si>
+  <si>
+    <t>ADWPc3</t>
+  </si>
+  <si>
+    <t>ATP_23_9_CD3_p</t>
+  </si>
+  <si>
+    <t>ATPPc3</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>ATP_23_9_CD3_t</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>ATP_23_9_CD3_m</t>
+  </si>
+  <si>
+    <t>Subnet name</t>
+  </si>
+  <si>
+    <t>Name your DB system</t>
+  </si>
+  <si>
+    <t>CPU Core</t>
+  </si>
+  <si>
+    <t>Total node count</t>
+  </si>
+  <si>
+    <t>Oracle database software edition</t>
+  </si>
+  <si>
+    <t>Database Size (GB)</t>
+  </si>
+  <si>
+    <t>Database Disk Redundancy</t>
+  </si>
+  <si>
+    <t>Choose a license type</t>
+  </si>
+  <si>
+    <t>Hostname prefix</t>
+  </si>
+  <si>
+    <t>Database name</t>
+  </si>
+  <si>
+    <t>Database version</t>
+  </si>
+  <si>
+    <r>
+      <t>PDB name (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Optional)</t>
+    </r>
+  </si>
+  <si>
+    <t>Database username</t>
+  </si>
+  <si>
+    <t>Database admin password</t>
+  </si>
+  <si>
+    <t>Select workload type</t>
+  </si>
+  <si>
+    <t>Enable Automatic Backups</t>
+  </si>
+  <si>
+    <t>Experimentation</t>
+  </si>
+  <si>
+    <t>DBSUBNET1</t>
+  </si>
+  <si>
+    <t>RACDB2cd</t>
+  </si>
+  <si>
+    <t>VM.Standard2.24</t>
+  </si>
+  <si>
+    <t>ENTERPRISE_EDITION_EXTREME_PERFORMANCE</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>LICENSE_INCLUDED</t>
+  </si>
+  <si>
+    <t>RACDB2</t>
+  </si>
+  <si>
+    <t>CDB1</t>
+  </si>
+  <si>
+    <t>12.1.0.2</t>
+  </si>
+  <si>
+    <t>pdb1</t>
+  </si>
+  <si>
+    <t>opc</t>
+  </si>
+  <si>
+    <t>BEstrO0ng_#12</t>
+  </si>
+  <si>
+    <t>OLTP</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>EXADB1cd</t>
+  </si>
+  <si>
+    <t>VM.Standard2.2</t>
+  </si>
+  <si>
+    <t>ENTERPRISE_EDITION</t>
+  </si>
+  <si>
+    <t>EXADB1</t>
+  </si>
+  <si>
+    <t>CDB2</t>
+  </si>
+  <si>
+    <t>pdb2</t>
+  </si>
+  <si>
+    <t>DSS</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>AD3</t>
+  </si>
+  <si>
+    <t>TESTDB3cd</t>
+  </si>
+  <si>
+    <t>VM.Standard2.1</t>
+  </si>
+  <si>
+    <t>TESTDB3</t>
+  </si>
+  <si>
+    <t>CDB3</t>
+  </si>
+  <si>
+    <t>pdb3</t>
+  </si>
+  <si>
+    <t>OCIC2OCI</t>
+  </si>
+  <si>
+    <t>EXADB1cdphx</t>
+  </si>
+  <si>
+    <t>TESTDB3cdphx</t>
+  </si>
+  <si>
+    <t>TESTDB3cdtrt</t>
+  </si>
+  <si>
+    <t>TESTDB3cdmum</t>
+  </si>
+  <si>
+    <t>#Description</t>
+  </si>
+  <si>
+    <t>Listener Protocol (HTTP|TCP)</t>
+  </si>
+  <si>
+    <t>LBR Subnets: specify a single regional subnet name (recommended) or two comma seperated subnet names(AD specific) for public Load Balancer and provide a single subnet(Regional or AD specific) for Private load Balancer- subnets names should be same as defined in Subnets tab, Backend ServerName:Port- specify comma separated list of servernames:ports(either specify server name as same name defined in Instances sheet or specify the IP address); LBR Hostname can be null, all other fields are mandatory; Backend HealthCheck URL is required if Backend HealthCheck Protocol is HTTP; If you want to create an HTTPS Listener, please specify ListenerProtocol as HTTP and UseSSL as y; As of now allows only one BackendSet, One Listener and one Hostname for each LBR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode=";;;**"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1102,6 +1448,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1259,7 +1612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1316,23 +1669,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1349,16 +1726,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1680,12 +2066,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -1980,25 +2366,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
@@ -2230,14 +2616,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="50" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -2362,22 +2748,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="37"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="47"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -2618,16 +3004,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="17" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -2740,7 +3126,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2760,25 +3146,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="50" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
     </row>
     <row r="2" spans="1:17" s="32" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
@@ -2955,6 +3341,183 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="17"/>
+    <col min="2" max="2" width="12.54296875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="17"/>
+    <col min="4" max="4" width="12.1796875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.90625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" style="17" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" style="17" customWidth="1"/>
+    <col min="11" max="11" width="13.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.08984375" style="17" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" style="17"/>
+    <col min="14" max="14" width="15.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.26953125" style="17" customWidth="1"/>
+    <col min="16" max="16" width="14.6328125" style="17" customWidth="1"/>
+    <col min="17" max="17" width="8.7265625" style="17"/>
+    <col min="18" max="18" width="11.36328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.36328125" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="50" t="s">
+        <v>372</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+    </row>
+    <row r="2" spans="1:19" s="17" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>371</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="N2" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="O2" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="P2" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q2" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="R2" s="34" t="s">
+        <v>293</v>
+      </c>
+      <c r="S2" s="34" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="J3" s="1">
+        <v>80</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="M3" s="1">
+        <v>443</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="S3" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:S1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2971,15 +3534,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="17" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -3005,13 +3568,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="53" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -3028,9 +3591,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="42"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="8" t="s">
         <v>204</v>
       </c>
@@ -3045,9 +3608,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="42"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="9"/>
       <c r="E5" s="1"/>
       <c r="F5" s="10" t="s">
@@ -3058,9 +3621,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="44"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="42"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="9"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
@@ -3071,108 +3634,108 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="44"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="11"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="42"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="54"/>
       <c r="D8" s="11"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="42"/>
+      <c r="A9" s="56"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="11"/>
       <c r="E9" s="1"/>
       <c r="F9" s="10"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="44"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="42"/>
+      <c r="A10" s="56"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="11"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="44"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="42"/>
+      <c r="A11" s="56"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="11"/>
       <c r="E11" s="1"/>
       <c r="F11" s="10"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="44"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="42"/>
+      <c r="A12" s="56"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="11"/>
       <c r="E12" s="1"/>
       <c r="F12" s="10"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="42"/>
+      <c r="A13" s="56"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="54"/>
       <c r="D13" s="11"/>
       <c r="E13" s="1"/>
       <c r="F13" s="10"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="42"/>
+      <c r="A14" s="56"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="54"/>
       <c r="D14" s="11"/>
       <c r="E14" s="1"/>
       <c r="F14" s="10"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="44"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="42"/>
+      <c r="A15" s="56"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="9"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="42"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="54"/>
       <c r="D16" s="9"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="42"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="54"/>
       <c r="D17" s="9"/>
       <c r="E17" s="1"/>
       <c r="F17" s="10"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="43"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="55"/>
       <c r="D18" s="9"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -3190,7 +3753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -3209,14 +3772,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -3275,102 +3838,6 @@
         <v>210</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="9.1796875" style="17"/>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="17" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="F4" s="17" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3398,11 +3865,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -3468,6 +3935,871 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" style="17"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="17" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="58" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="60"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>303</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="F3" s="35">
+        <v>1</v>
+      </c>
+      <c r="G3" s="35">
+        <v>1</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>309</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="F4" s="35">
+        <v>1</v>
+      </c>
+      <c r="G4" s="35">
+        <v>1</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>312</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>313</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="F5" s="35">
+        <v>1</v>
+      </c>
+      <c r="G5" s="35">
+        <v>1</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="F6" s="35">
+        <v>1</v>
+      </c>
+      <c r="G6" s="35">
+        <v>1</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="F7" s="35">
+        <v>1</v>
+      </c>
+      <c r="G7" s="35">
+        <v>1</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="35" t="s">
+        <v>318</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>319</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1</v>
+      </c>
+      <c r="G8" s="35">
+        <v>1</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="42" customWidth="1"/>
+    <col min="13" max="13" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.08984375" customWidth="1"/>
+    <col min="15" max="15" width="8.6328125" customWidth="1"/>
+    <col min="16" max="16" width="10.08984375" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="61" t="s">
+        <v>370</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="63"/>
+    </row>
+    <row r="2" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>322</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>323</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>324</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>326</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>327</v>
+      </c>
+      <c r="M2" s="39" t="s">
+        <v>328</v>
+      </c>
+      <c r="N2" s="40" t="s">
+        <v>329</v>
+      </c>
+      <c r="O2" s="40" t="s">
+        <v>330</v>
+      </c>
+      <c r="P2" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q2" s="40" t="s">
+        <v>332</v>
+      </c>
+      <c r="R2" s="39" t="s">
+        <v>333</v>
+      </c>
+      <c r="S2" s="40" t="s">
+        <v>334</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>338</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="G3" s="38">
+        <v>1</v>
+      </c>
+      <c r="H3" s="38">
+        <v>1</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>340</v>
+      </c>
+      <c r="J3" s="38">
+        <v>256</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="L3" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="M3" s="38" t="s">
+        <v>343</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>344</v>
+      </c>
+      <c r="O3" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="P3" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q3" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="R3" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="S3" s="38" t="s">
+        <v>349</v>
+      </c>
+      <c r="T3" s="38" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>351</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>352</v>
+      </c>
+      <c r="G4" s="38">
+        <v>1</v>
+      </c>
+      <c r="H4" s="38">
+        <v>1</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="J4" s="38">
+        <v>256</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="L4" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="M4" s="38" t="s">
+        <v>354</v>
+      </c>
+      <c r="N4" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="O4" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="P4" s="38" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q4" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="R4" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="S4" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="T4" s="38" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>359</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>360</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="G5" s="38">
+        <v>1</v>
+      </c>
+      <c r="H5" s="38">
+        <v>1</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="J5" s="38">
+        <v>256</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="L5" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="M5" s="38" t="s">
+        <v>362</v>
+      </c>
+      <c r="N5" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="O5" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="P5" s="38" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q5" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="R5" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="S5" s="38" t="s">
+        <v>349</v>
+      </c>
+      <c r="T5" s="38" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>365</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>366</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>352</v>
+      </c>
+      <c r="G6" s="38">
+        <v>1</v>
+      </c>
+      <c r="H6" s="38">
+        <v>1</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="J6" s="38">
+        <v>256</v>
+      </c>
+      <c r="K6" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="L6" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="M6" s="38" t="s">
+        <v>354</v>
+      </c>
+      <c r="N6" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="O6" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="P6" s="38" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q6" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="R6" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="S6" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="T6" s="38" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>359</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>367</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="G7" s="38">
+        <v>1</v>
+      </c>
+      <c r="H7" s="38">
+        <v>1</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="J7" s="38">
+        <v>256</v>
+      </c>
+      <c r="K7" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="L7" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="M7" s="38" t="s">
+        <v>362</v>
+      </c>
+      <c r="N7" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="O7" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="P7" s="38" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q7" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="R7" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="S7" s="38" t="s">
+        <v>349</v>
+      </c>
+      <c r="T7" s="38" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>359</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>368</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="G8" s="38">
+        <v>1</v>
+      </c>
+      <c r="H8" s="38">
+        <v>1</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="J8" s="38">
+        <v>256</v>
+      </c>
+      <c r="K8" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="L8" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="M8" s="38" t="s">
+        <v>362</v>
+      </c>
+      <c r="N8" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="O8" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="P8" s="38" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q8" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="R8" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="S8" s="38" t="s">
+        <v>349</v>
+      </c>
+      <c r="T8" s="38" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>359</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>369</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="G9" s="38">
+        <v>1</v>
+      </c>
+      <c r="H9" s="38">
+        <v>1</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="J9" s="38">
+        <v>256</v>
+      </c>
+      <c r="K9" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="L9" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="M9" s="38" t="s">
+        <v>362</v>
+      </c>
+      <c r="N9" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="O9" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="P9" s="38" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q9" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="R9" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="S9" s="38" t="s">
+        <v>349</v>
+      </c>
+      <c r="T9" s="38" t="s">
+        <v>358</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:T1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3490,15 +4822,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="37"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
@@ -3642,21 +4974,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="45" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="37"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="47"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3926,10 +5258,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="238.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="48" t="s">
         <v>271</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="49"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -3998,10 +5330,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="37"/>
+      <c r="B11" s="47"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -4054,21 +5386,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -4434,13 +5766,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -4558,15 +5890,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -4711,23 +6043,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
updated FSS code to inlude multi FSS and multi MT scenarios
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -37,12 +37,12 @@
     <definedName name="Shape_Option">#REF!</definedName>
     <definedName name="Shape_Option_DB">[1]Database!$B$10:$J$10</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="391">
   <si>
     <t>Regional</t>
   </si>
@@ -852,12 +852,6 @@
   </si>
   <si>
     <t>Max FSS Capacity (in bytes)</t>
-  </si>
-  <si>
-    <t>Demo1</t>
-  </si>
-  <si>
-    <t>/fss/</t>
   </si>
   <si>
     <t>FSS1</t>
@@ -1464,11 +1458,56 @@
     <t>mumbai</t>
   </si>
   <si>
+    <t>MT2</t>
+  </si>
+  <si>
+    <t>HUB_SERVICES_SN</t>
+  </si>
+  <si>
+    <t>FSS3</t>
+  </si>
+  <si>
+    <t>/fss3/</t>
+  </si>
+  <si>
+    <t>10.0.0.0/8</t>
+  </si>
+  <si>
+    <t>READ_ONLY</t>
+  </si>
+  <si>
+    <t>/fss1/</t>
+  </si>
+  <si>
+    <t>MT3</t>
+  </si>
+  <si>
+    <t>11.0.0.0/8</t>
+  </si>
+  <si>
+    <t>READ_WRITE</t>
+  </si>
+  <si>
+    <t>FSS2</t>
+  </si>
+  <si>
+    <t>/fss2/</t>
+  </si>
+  <si>
+    <t>MT4</t>
+  </si>
+  <si>
+    <t>FSS4</t>
+  </si>
+  <si>
+    <t>/fss4/</t>
+  </si>
+  <si>
     <t>Columns: Region, Compartment Name, Availability Domain, MountTarget Name, MountTarget SubnetName, FSS name, Path are mandatory.
-Default value for sourceCIDR- 0.0.0.0/0, Access- READ_ONLY, GID- 65534, UID- 65534, IDSquash- NONE and require_ps_port- false
+Default value for columns if left blank: sourceCIDR- 0.0.0.0/0, Access- READ_ONLY, GID- 65534, UID- 65534, IDSquash- NONE and require_ps_port- false
 Mount target IP, FSS Capacity, FSS Inodes will take default values from OCI if left blank
-This will create one Mount target for one FSS
-Choose distinct names for Mount Targets and FSS</t>
+Resources will be created based on MountTargetName and FSSName columns.
+Below sample data shows example of  multiple FSS(FSS1 and FSS2) using single MT(MT1) , 1 FSS(FSS3) using multiple MTs(MT2 and MT3) and also 1 FSS(FSS4) using 1 MT(MT4)</t>
   </si>
 </sst>
 </file>
@@ -2980,7 +3019,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -3354,7 +3393,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:Q1"/>
@@ -3376,9 +3415,9 @@
     <col min="17" max="17" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -3411,7 +3450,7 @@
         <v>248</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>249</v>
@@ -3450,31 +3489,31 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>262</v>
+        <v>292</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>242</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>376</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>263</v>
+        <v>381</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -3483,20 +3522,32 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>376</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -3504,62 +3555,133 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+    <row r="5" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>376</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+    <row r="6" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>376</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>380</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+    <row r="7" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>376</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>389</v>
+      </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3603,7 +3725,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -3632,55 +3754,55 @@
         <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>360</v>
+      </c>
+      <c r="M2" s="33" t="s">
         <v>271</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>281</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="N2" s="33" t="s">
         <v>275</v>
       </c>
-      <c r="G2" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>279</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>282</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>362</v>
-      </c>
-      <c r="M2" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="N2" s="33" t="s">
-        <v>277</v>
-      </c>
       <c r="O2" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="P2" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q2" s="34" t="s">
         <v>289</v>
       </c>
-      <c r="P2" s="34" t="s">
+      <c r="R2" s="34" t="s">
         <v>290</v>
       </c>
-      <c r="Q2" s="34" t="s">
+      <c r="S2" s="34" t="s">
         <v>291</v>
-      </c>
-      <c r="R2" s="34" t="s">
-        <v>292</v>
-      </c>
-      <c r="S2" s="34" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -3688,13 +3810,13 @@
         <v>128</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>171</v>
@@ -3703,38 +3825,38 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J3" s="1">
         <v>80</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="M3" s="1">
         <v>443</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="S3" s="1"/>
     </row>
@@ -4285,7 +4407,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="64" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -4303,22 +4425,22 @@
         <v>76</v>
       </c>
       <c r="C2" s="37" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>297</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="F2" s="37" t="s">
         <v>298</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="G2" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="H2" s="37" t="s">
         <v>300</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>301</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -4326,16 +4448,16 @@
         <v>127</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C3" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>303</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>304</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>305</v>
       </c>
       <c r="F3" s="36">
         <v>1</v>
@@ -4344,7 +4466,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -4352,16 +4474,16 @@
         <v>127</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F4" s="36">
         <v>1</v>
@@ -4370,7 +4492,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -4378,16 +4500,16 @@
         <v>128</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F5" s="36">
         <v>1</v>
@@ -4396,7 +4518,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -4404,16 +4526,16 @@
         <v>128</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F6" s="36">
         <v>1</v>
@@ -4422,24 +4544,24 @@
         <v>1</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="36" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F7" s="36">
         <v>1</v>
@@ -4448,24 +4570,24 @@
         <v>1</v>
       </c>
       <c r="H7" s="36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F8" s="36">
         <v>1</v>
@@ -4474,7 +4596,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -4513,7 +4635,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="40" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="67" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="68"/>
@@ -4544,61 +4666,61 @@
         <v>76</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>53</v>
       </c>
       <c r="G2" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="I2" s="41" t="s">
         <v>320</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="J2" s="41" t="s">
         <v>321</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="K2" s="41" t="s">
         <v>322</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="L2" s="44" t="s">
         <v>323</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="M2" s="41" t="s">
         <v>324</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="N2" s="41" t="s">
         <v>325</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="O2" s="41" t="s">
         <v>326</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="P2" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="Q2" s="41" t="s">
         <v>328</v>
       </c>
-      <c r="P2" s="41" t="s">
+      <c r="R2" s="41" t="s">
         <v>329</v>
       </c>
-      <c r="Q2" s="41" t="s">
+      <c r="S2" s="41" t="s">
         <v>330</v>
       </c>
-      <c r="R2" s="41" t="s">
+      <c r="T2" s="41" t="s">
         <v>331</v>
       </c>
-      <c r="S2" s="41" t="s">
-        <v>332</v>
-      </c>
-      <c r="T2" s="41" t="s">
-        <v>333</v>
-      </c>
       <c r="U2" s="45" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
@@ -4606,19 +4728,19 @@
         <v>127</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D3" s="46" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G3" s="46">
         <v>1</v>
@@ -4627,40 +4749,40 @@
         <v>1</v>
       </c>
       <c r="I3" s="46" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J3" s="46">
         <v>256</v>
       </c>
       <c r="K3" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="L3" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="M3" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="N3" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="O3" s="46" t="s">
         <v>339</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="P3" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="Q3" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="P3" s="46" t="s">
+      <c r="R3" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="S3" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="T3" s="46" t="s">
         <v>344</v>
-      </c>
-      <c r="S3" s="46" t="s">
-        <v>345</v>
-      </c>
-      <c r="T3" s="46" t="s">
-        <v>346</v>
       </c>
       <c r="U3" s="46" t="s">
         <v>12</v>
@@ -4671,19 +4793,19 @@
         <v>127</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D4" s="46" t="s">
         <v>242</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F4" s="46" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G4" s="46">
         <v>1</v>
@@ -4692,40 +4814,40 @@
         <v>1</v>
       </c>
       <c r="I4" s="46" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J4" s="46">
         <v>256</v>
       </c>
       <c r="K4" s="46" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="L4" s="46" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M4" s="46" t="s">
+        <v>347</v>
+      </c>
+      <c r="N4" s="46" t="s">
+        <v>348</v>
+      </c>
+      <c r="O4" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="P4" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="N4" s="46" t="s">
+      <c r="Q4" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="R4" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="S4" s="46" t="s">
         <v>350</v>
       </c>
-      <c r="O4" s="46" t="s">
-        <v>341</v>
-      </c>
-      <c r="P4" s="46" t="s">
+      <c r="T4" s="46" t="s">
         <v>351</v>
-      </c>
-      <c r="Q4" s="46" t="s">
-        <v>343</v>
-      </c>
-      <c r="R4" s="46" t="s">
-        <v>344</v>
-      </c>
-      <c r="S4" s="46" t="s">
-        <v>352</v>
-      </c>
-      <c r="T4" s="46" t="s">
-        <v>353</v>
       </c>
       <c r="U4" s="46" t="s">
         <v>12</v>
@@ -4736,19 +4858,19 @@
         <v>128</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G5" s="46">
         <v>1</v>
@@ -4757,40 +4879,40 @@
         <v>1</v>
       </c>
       <c r="I5" s="46" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J5" s="46">
         <v>256</v>
       </c>
       <c r="K5" s="46" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="L5" s="46" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M5" s="46" t="s">
+        <v>354</v>
+      </c>
+      <c r="N5" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="O5" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="P5" s="46" t="s">
         <v>356</v>
       </c>
-      <c r="N5" s="46" t="s">
-        <v>357</v>
-      </c>
-      <c r="O5" s="46" t="s">
+      <c r="Q5" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="P5" s="46" t="s">
-        <v>358</v>
-      </c>
-      <c r="Q5" s="46" t="s">
+      <c r="R5" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="S5" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="R5" s="46" t="s">
-        <v>344</v>
-      </c>
-      <c r="S5" s="46" t="s">
-        <v>345</v>
-      </c>
       <c r="T5" s="46" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="U5" s="46" t="s">
         <v>12</v>
@@ -4801,16 +4923,16 @@
         <v>128</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D6" s="46" t="s">
         <v>242</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F6" s="46" t="s">
         <v>196</v>
@@ -4822,40 +4944,40 @@
         <v>1</v>
       </c>
       <c r="I6" s="46" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J6" s="46">
         <v>256</v>
       </c>
       <c r="K6" s="46" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="L6" s="46" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M6" s="46" t="s">
+        <v>347</v>
+      </c>
+      <c r="N6" s="46" t="s">
+        <v>348</v>
+      </c>
+      <c r="O6" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="P6" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="N6" s="46" t="s">
+      <c r="Q6" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="R6" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="S6" s="46" t="s">
         <v>350</v>
       </c>
-      <c r="O6" s="46" t="s">
-        <v>341</v>
-      </c>
-      <c r="P6" s="46" t="s">
+      <c r="T6" s="46" t="s">
         <v>351</v>
-      </c>
-      <c r="Q6" s="46" t="s">
-        <v>343</v>
-      </c>
-      <c r="R6" s="46" t="s">
-        <v>344</v>
-      </c>
-      <c r="S6" s="46" t="s">
-        <v>352</v>
-      </c>
-      <c r="T6" s="46" t="s">
-        <v>353</v>
       </c>
       <c r="U6" s="46" t="s">
         <v>12</v>
@@ -4863,22 +4985,22 @@
     </row>
     <row r="7" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="46" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F7" s="46" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G7" s="46">
         <v>1</v>
@@ -4887,40 +5009,40 @@
         <v>1</v>
       </c>
       <c r="I7" s="46" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J7" s="46">
         <v>256</v>
       </c>
       <c r="K7" s="46" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="L7" s="46" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M7" s="46" t="s">
+        <v>354</v>
+      </c>
+      <c r="N7" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="O7" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="P7" s="46" t="s">
         <v>356</v>
       </c>
-      <c r="N7" s="46" t="s">
-        <v>357</v>
-      </c>
-      <c r="O7" s="46" t="s">
+      <c r="Q7" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="P7" s="46" t="s">
-        <v>358</v>
-      </c>
-      <c r="Q7" s="46" t="s">
+      <c r="R7" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="S7" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="R7" s="46" t="s">
-        <v>344</v>
-      </c>
-      <c r="S7" s="46" t="s">
-        <v>345</v>
-      </c>
       <c r="T7" s="46" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="U7" s="46" t="s">
         <v>12</v>
@@ -4928,19 +5050,19 @@
     </row>
     <row r="8" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="46" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F8" s="46" t="s">
         <v>196</v>
@@ -4952,40 +5074,40 @@
         <v>1</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J8" s="46">
         <v>256</v>
       </c>
       <c r="K8" s="46" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="L8" s="46" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M8" s="46" t="s">
+        <v>354</v>
+      </c>
+      <c r="N8" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="O8" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="P8" s="46" t="s">
         <v>356</v>
       </c>
-      <c r="N8" s="46" t="s">
-        <v>357</v>
-      </c>
-      <c r="O8" s="46" t="s">
+      <c r="Q8" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="P8" s="46" t="s">
-        <v>358</v>
-      </c>
-      <c r="Q8" s="46" t="s">
+      <c r="R8" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="S8" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="R8" s="46" t="s">
-        <v>344</v>
-      </c>
-      <c r="S8" s="46" t="s">
-        <v>345</v>
-      </c>
       <c r="T8" s="46" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="U8" s="46" t="s">
         <v>12</v>
@@ -5184,7 +5306,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -5468,7 +5590,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="238.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B1" s="55"/>
     </row>
@@ -5596,7 +5718,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>

</xml_diff>

<commit_message>
Modified code for routes creation, Added support for common seclist to be created for subnets, Added support to add a new VCN, Added support for Mac to create OCSWorkVM
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="13" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="396">
   <si>
     <t>Regional</t>
   </si>
@@ -870,13 +870,6 @@
 Valid Values for columns D,E,F,G:   y|n|&lt;component_name&gt; ie mention 'n' when a component(like IGW) is not required to be configured(like for PHXHub-VCN), specify name of the component- component will be configured with the mentioned name(eg PHX-DRG for the DRG in PHXHub-VCN) and mention 'y' if component needs to be configured with default name ie &lt;vcnname&gt;_ngw(eg PHXNonProd-VCN_ngw)
 Note- Not possible to specify names for LPGs
 </t>
-  </si>
-  <si>
-    <t># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn
-vcn_name should be same as enterd in VCNs sheet;
-Route Rules for IGW, NGW and SGW would be created based on parameter values: configure_igw, configure_ngw and configure_sgw respectively for each subnet. The condition is the respective component should have been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
-You can specify names for route tables and Scurity Lists; subnets can share same route table and seclist depending upon name specified; If left blank, default name which is subnet name would be used for that route table as well as security list.
-Note- Please use different names for route tables/seclists across VCNs</t>
   </si>
   <si>
     <r>
@@ -1508,6 +1501,28 @@
 Mount target IP, FSS Capacity, FSS Inodes will take default values from OCI if left blank
 Resources will be created based on MountTargetName and FSSName columns.
 Below sample data shows example of  multiple FSS(FSS1 and FSS2) using single MT(MT1) , 1 FSS(FSS3) using multiple MTs(MT2 and MT3) and also 1 FSS(FSS4) using 1 MT(MT4)</t>
+  </si>
+  <si>
+    <t>RuleDescription</t>
+  </si>
+  <si>
+    <t>objectstorage</t>
+  </si>
+  <si>
+    <t>common_rules_phxprod</t>
+  </si>
+  <si>
+    <t>common_rules_ashprod</t>
+  </si>
+  <si>
+    <t># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn
+vcn_name should be same as enterd in VCNs sheet;
+Route Rules for IGW, NGW and SGW would be created based on parameter values: configure_igw, configure_ngw and configure_sgw respectively for each subnet. The condition is the respective component should have been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
+You can specify names for route tables and Scurity Lists; subnets can share same route table and seclist depending upon name specified; If left blank, default name which is subnet name would be used for that route table as well as security list. common_seclist_name column is also added to allow a seclist to be shared among multiple subnets
+Note- Please use different names for route tables/seclists across VCNs</t>
+  </si>
+  <si>
+    <t>common_seclist_name</t>
   </si>
 </sst>
 </file>
@@ -1777,7 +1792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1874,6 +1889,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1898,7 +1916,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2336,12 +2357,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -2615,10 +2636,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2633,30 +2654,32 @@
     <col min="10" max="10" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:18" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>126</v>
       </c>
@@ -2708,8 +2731,11 @@
       <c r="Q2" s="20" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R2" s="49" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
@@ -2745,8 +2771,11 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R3" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>127</v>
       </c>
@@ -2786,8 +2815,9 @@
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>128</v>
       </c>
@@ -2821,8 +2851,11 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R5" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>128</v>
       </c>
@@ -2858,10 +2891,11 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2886,14 +2920,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3018,22 +3052,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>265</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="54"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -3274,16 +3308,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="17" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3395,7 +3429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
@@ -3416,25 +3450,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
-        <v>390</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
+      <c r="A1" s="57" t="s">
+        <v>389</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
     </row>
     <row r="2" spans="1:17" s="32" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
@@ -3494,7 +3528,7 @@
         <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>242</v>
@@ -3503,7 +3537,7 @@
         <v>263</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -3513,7 +3547,7 @@
         <v>262</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -3527,7 +3561,7 @@
         <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>242</v>
@@ -3536,17 +3570,17 @@
         <v>263</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -3560,32 +3594,32 @@
         <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>378</v>
-      </c>
       <c r="L5" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>384</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -3597,32 +3631,32 @@
         <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -3634,26 +3668,26 @@
         <v>127</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>389</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -3724,27 +3758,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
-        <v>361</v>
-      </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
+      <c r="A1" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
     </row>
     <row r="2" spans="1:19" s="17" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
@@ -3754,55 +3788,55 @@
         <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="F2" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="I2" s="33" t="s">
         <v>279</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="J2" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="M2" s="33" t="s">
         <v>270</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G2" s="33" t="s">
+      <c r="N2" s="33" t="s">
         <v>274</v>
       </c>
-      <c r="H2" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>280</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>272</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>281</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>360</v>
-      </c>
-      <c r="M2" s="33" t="s">
-        <v>271</v>
-      </c>
-      <c r="N2" s="33" t="s">
-        <v>275</v>
-      </c>
       <c r="O2" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="P2" s="34" t="s">
         <v>287</v>
       </c>
-      <c r="P2" s="34" t="s">
+      <c r="Q2" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="Q2" s="34" t="s">
+      <c r="R2" s="34" t="s">
         <v>289</v>
       </c>
-      <c r="R2" s="34" t="s">
+      <c r="S2" s="34" t="s">
         <v>290</v>
-      </c>
-      <c r="S2" s="34" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -3810,13 +3844,13 @@
         <v>128</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>171</v>
@@ -3825,38 +3859,38 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J3" s="1">
         <v>80</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M3" s="1">
         <v>443</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="S3" s="1"/>
     </row>
@@ -3887,15 +3921,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="17" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -3921,13 +3955,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="61" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -3944,9 +3978,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="60"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="8" t="s">
         <v>204</v>
       </c>
@@ -3961,9 +3995,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="62"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="60"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="62"/>
       <c r="D5" s="9"/>
       <c r="E5" s="1"/>
       <c r="F5" s="10" t="s">
@@ -3974,9 +4008,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="62"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="60"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="9"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
@@ -3987,108 +4021,108 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="62"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="60"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="11"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="60"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="62"/>
       <c r="D8" s="11"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="62"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="60"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="62"/>
       <c r="D9" s="11"/>
       <c r="E9" s="1"/>
       <c r="F9" s="10"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="62"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="60"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="62"/>
       <c r="D10" s="11"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="62"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="60"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="62"/>
       <c r="D11" s="11"/>
       <c r="E11" s="1"/>
       <c r="F11" s="10"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="62"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="60"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="62"/>
       <c r="D12" s="11"/>
       <c r="E12" s="1"/>
       <c r="F12" s="10"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="62"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="60"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="62"/>
       <c r="D13" s="11"/>
       <c r="E13" s="1"/>
       <c r="F13" s="10"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="62"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="60"/>
+      <c r="A14" s="64"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="62"/>
       <c r="D14" s="11"/>
       <c r="E14" s="1"/>
       <c r="F14" s="10"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="62"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="60"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="62"/>
       <c r="D15" s="9"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="60"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="62"/>
       <c r="D16" s="9"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="62"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="60"/>
+      <c r="A17" s="64"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="62"/>
       <c r="D17" s="9"/>
       <c r="E17" s="1"/>
       <c r="F17" s="10"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="62"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="61"/>
+      <c r="A18" s="64"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="9"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -4125,14 +4159,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -4218,11 +4252,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -4310,14 +4344,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -4406,16 +4440,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
-        <v>362</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="66"/>
+      <c r="A1" s="66" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="68"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="37" t="s">
@@ -4425,22 +4459,22 @@
         <v>76</v>
       </c>
       <c r="C2" s="37" t="s">
+        <v>294</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>295</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="E2" s="39" t="s">
         <v>296</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="F2" s="37" t="s">
         <v>297</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="G2" s="37" t="s">
         <v>298</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="H2" s="37" t="s">
         <v>299</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -4448,16 +4482,16 @@
         <v>127</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="D3" s="36" t="s">
         <v>301</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="E3" s="38" t="s">
         <v>302</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>303</v>
       </c>
       <c r="F3" s="36">
         <v>1</v>
@@ -4466,7 +4500,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -4474,16 +4508,16 @@
         <v>127</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C4" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="D4" s="36" t="s">
         <v>305</v>
       </c>
-      <c r="D4" s="36" t="s">
-        <v>306</v>
-      </c>
       <c r="E4" s="38" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F4" s="36">
         <v>1</v>
@@ -4492,7 +4526,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -4500,16 +4534,16 @@
         <v>128</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C5" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="D5" s="36" t="s">
         <v>308</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>309</v>
-      </c>
       <c r="E5" s="38" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F5" s="36">
         <v>1</v>
@@ -4518,7 +4552,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -4526,16 +4560,16 @@
         <v>128</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="D6" s="36" t="s">
         <v>310</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>311</v>
-      </c>
       <c r="E6" s="38" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F6" s="36">
         <v>1</v>
@@ -4544,24 +4578,24 @@
         <v>1</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="36" t="s">
+        <v>311</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>291</v>
+      </c>
+      <c r="C7" s="36" t="s">
         <v>312</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>292</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>313</v>
-      </c>
       <c r="D7" s="36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F7" s="36">
         <v>1</v>
@@ -4570,24 +4604,24 @@
         <v>1</v>
       </c>
       <c r="H7" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>292</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>315</v>
-      </c>
       <c r="D8" s="36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F8" s="36">
         <v>1</v>
@@ -4596,7 +4630,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -4634,29 +4668,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="40" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
-        <v>369</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="69"/>
+      <c r="A1" s="69" t="s">
+        <v>368</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="71"/>
     </row>
     <row r="2" spans="1:21" s="36" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
@@ -4666,61 +4700,61 @@
         <v>76</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>53</v>
       </c>
       <c r="G2" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="H2" s="41" t="s">
         <v>318</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="I2" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="J2" s="41" t="s">
         <v>320</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="K2" s="41" t="s">
         <v>321</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="L2" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="M2" s="41" t="s">
         <v>323</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="N2" s="41" t="s">
         <v>324</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="O2" s="41" t="s">
         <v>325</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="P2" s="41" t="s">
         <v>326</v>
       </c>
-      <c r="P2" s="41" t="s">
+      <c r="Q2" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="Q2" s="41" t="s">
+      <c r="R2" s="41" t="s">
         <v>328</v>
       </c>
-      <c r="R2" s="41" t="s">
+      <c r="S2" s="41" t="s">
         <v>329</v>
       </c>
-      <c r="S2" s="41" t="s">
+      <c r="T2" s="41" t="s">
         <v>330</v>
       </c>
-      <c r="T2" s="41" t="s">
-        <v>331</v>
-      </c>
       <c r="U2" s="45" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
@@ -4728,19 +4762,19 @@
         <v>127</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D3" s="46" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G3" s="46">
         <v>1</v>
@@ -4749,40 +4783,40 @@
         <v>1</v>
       </c>
       <c r="I3" s="46" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J3" s="46">
         <v>256</v>
       </c>
       <c r="K3" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="L3" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="M3" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="N3" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="O3" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="P3" s="46" t="s">
         <v>339</v>
       </c>
-      <c r="P3" s="46" t="s">
+      <c r="Q3" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="R3" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="S3" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="S3" s="46" t="s">
+      <c r="T3" s="46" t="s">
         <v>343</v>
-      </c>
-      <c r="T3" s="46" t="s">
-        <v>344</v>
       </c>
       <c r="U3" s="46" t="s">
         <v>12</v>
@@ -4793,19 +4827,19 @@
         <v>127</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D4" s="46" t="s">
         <v>242</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F4" s="46" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G4" s="46">
         <v>1</v>
@@ -4814,40 +4848,40 @@
         <v>1</v>
       </c>
       <c r="I4" s="46" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J4" s="46">
         <v>256</v>
       </c>
       <c r="K4" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="L4" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="L4" s="46" t="s">
-        <v>336</v>
-      </c>
       <c r="M4" s="46" t="s">
+        <v>346</v>
+      </c>
+      <c r="N4" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="N4" s="46" t="s">
+      <c r="O4" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="P4" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="O4" s="46" t="s">
-        <v>339</v>
-      </c>
-      <c r="P4" s="46" t="s">
+      <c r="Q4" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="R4" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="S4" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="Q4" s="46" t="s">
-        <v>341</v>
-      </c>
-      <c r="R4" s="46" t="s">
-        <v>342</v>
-      </c>
-      <c r="S4" s="46" t="s">
+      <c r="T4" s="46" t="s">
         <v>350</v>
-      </c>
-      <c r="T4" s="46" t="s">
-        <v>351</v>
       </c>
       <c r="U4" s="46" t="s">
         <v>12</v>
@@ -4858,19 +4892,19 @@
         <v>128</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D5" s="46" t="s">
+        <v>351</v>
+      </c>
+      <c r="E5" s="46" t="s">
         <v>352</v>
       </c>
-      <c r="E5" s="46" t="s">
-        <v>353</v>
-      </c>
       <c r="F5" s="46" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G5" s="46">
         <v>1</v>
@@ -4879,40 +4913,40 @@
         <v>1</v>
       </c>
       <c r="I5" s="46" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J5" s="46">
         <v>256</v>
       </c>
       <c r="K5" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="L5" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="L5" s="46" t="s">
-        <v>336</v>
-      </c>
       <c r="M5" s="46" t="s">
+        <v>353</v>
+      </c>
+      <c r="N5" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="N5" s="46" t="s">
+      <c r="O5" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="P5" s="46" t="s">
         <v>355</v>
       </c>
-      <c r="O5" s="46" t="s">
-        <v>339</v>
-      </c>
-      <c r="P5" s="46" t="s">
-        <v>356</v>
-      </c>
       <c r="Q5" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="R5" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="R5" s="46" t="s">
+      <c r="S5" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="S5" s="46" t="s">
-        <v>343</v>
-      </c>
       <c r="T5" s="46" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="U5" s="46" t="s">
         <v>12</v>
@@ -4923,16 +4957,16 @@
         <v>128</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D6" s="46" t="s">
         <v>242</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F6" s="46" t="s">
         <v>196</v>
@@ -4944,40 +4978,40 @@
         <v>1</v>
       </c>
       <c r="I6" s="46" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J6" s="46">
         <v>256</v>
       </c>
       <c r="K6" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="L6" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="L6" s="46" t="s">
-        <v>336</v>
-      </c>
       <c r="M6" s="46" t="s">
+        <v>346</v>
+      </c>
+      <c r="N6" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="N6" s="46" t="s">
+      <c r="O6" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="P6" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="O6" s="46" t="s">
-        <v>339</v>
-      </c>
-      <c r="P6" s="46" t="s">
+      <c r="Q6" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="R6" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="S6" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="Q6" s="46" t="s">
-        <v>341</v>
-      </c>
-      <c r="R6" s="46" t="s">
-        <v>342</v>
-      </c>
-      <c r="S6" s="46" t="s">
+      <c r="T6" s="46" t="s">
         <v>350</v>
-      </c>
-      <c r="T6" s="46" t="s">
-        <v>351</v>
       </c>
       <c r="U6" s="46" t="s">
         <v>12</v>
@@ -4985,22 +5019,22 @@
     </row>
     <row r="7" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="46" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" s="47" t="s">
         <v>372</v>
       </c>
-      <c r="B7" s="46" t="s">
-        <v>332</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>373</v>
-      </c>
       <c r="D7" s="46" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F7" s="46" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G7" s="46">
         <v>1</v>
@@ -5009,40 +5043,40 @@
         <v>1</v>
       </c>
       <c r="I7" s="46" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J7" s="46">
         <v>256</v>
       </c>
       <c r="K7" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="L7" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="L7" s="46" t="s">
-        <v>336</v>
-      </c>
       <c r="M7" s="46" t="s">
+        <v>353</v>
+      </c>
+      <c r="N7" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="N7" s="46" t="s">
+      <c r="O7" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="P7" s="46" t="s">
         <v>355</v>
       </c>
-      <c r="O7" s="46" t="s">
-        <v>339</v>
-      </c>
-      <c r="P7" s="46" t="s">
-        <v>356</v>
-      </c>
       <c r="Q7" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="R7" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="R7" s="46" t="s">
+      <c r="S7" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="S7" s="46" t="s">
-        <v>343</v>
-      </c>
       <c r="T7" s="46" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="U7" s="46" t="s">
         <v>12</v>
@@ -5050,19 +5084,19 @@
     </row>
     <row r="8" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="46" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F8" s="46" t="s">
         <v>196</v>
@@ -5074,40 +5108,40 @@
         <v>1</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J8" s="46">
         <v>256</v>
       </c>
       <c r="K8" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="L8" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="L8" s="46" t="s">
-        <v>336</v>
-      </c>
       <c r="M8" s="46" t="s">
+        <v>353</v>
+      </c>
+      <c r="N8" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="N8" s="46" t="s">
+      <c r="O8" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="P8" s="46" t="s">
         <v>355</v>
       </c>
-      <c r="O8" s="46" t="s">
-        <v>339</v>
-      </c>
-      <c r="P8" s="46" t="s">
-        <v>356</v>
-      </c>
       <c r="Q8" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="R8" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="R8" s="46" t="s">
+      <c r="S8" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="S8" s="46" t="s">
-        <v>343</v>
-      </c>
       <c r="T8" s="46" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="U8" s="46" t="s">
         <v>12</v>
@@ -5153,15 +5187,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
@@ -5305,21 +5339,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="54"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -5589,10 +5623,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="238.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
-        <v>268</v>
-      </c>
-      <c r="B1" s="55"/>
+      <c r="A1" s="55" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="56"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -5661,10 +5695,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="53"/>
+      <c r="B11" s="54"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -5694,10 +5728,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5710,30 +5744,32 @@
     <col min="6" max="6" width="19.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="18.453125" style="17" customWidth="1"/>
-    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" customWidth="1"/>
-    <col min="12" max="12" width="11.1796875" customWidth="1"/>
-    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="10" max="10" width="26.36328125" style="36" customWidth="1"/>
+    <col min="11" max="11" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
-        <v>267</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-    </row>
-    <row r="2" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+    </row>
+    <row r="2" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>101</v>
       </c>
@@ -5762,19 +5798,22 @@
         <v>232</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -5800,20 +5839,21 @@
         <v>235</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="J3" s="13"/>
       <c r="K3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="19" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -5839,20 +5879,23 @@
       <c r="I4" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>16</v>
+      <c r="J4" s="1" t="s">
+        <v>392</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="L4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="N4" s="19" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -5878,20 +5921,23 @@
       <c r="I5" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>16</v>
+      <c r="J5" s="1" t="s">
+        <v>392</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="L5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="N5" s="19" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -5915,20 +5961,21 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="J6" s="1"/>
       <c r="K6" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="19" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
@@ -5956,20 +6003,23 @@
       <c r="I7" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="19" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
@@ -5995,20 +6045,23 @@
       <c r="I8" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="J8" s="6" t="s">
-        <v>16</v>
+      <c r="J8" s="1" t="s">
+        <v>393</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="L8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="N8" s="19" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>62</v>
       </c>
@@ -6024,8 +6077,9 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -6039,8 +6093,9 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -6054,8 +6109,9 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -6069,10 +6125,11 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6097,13 +6154,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -6221,15 +6278,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -6374,23 +6431,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
added support for same names of seclists/routetables across VCNs
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -458,12 +458,6 @@
     <t>0.0.0.0/0</t>
   </si>
   <si>
-    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new  rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
-This sheet will only add new rules to theSecurity Lists; You can also edit Default Security List for a VCN- Mention subnet name as 'Default Security List for &lt;vcn_name&gt;'
-'SecRulesinOCI' sheet would be used for overwrite of all sec rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
-VCN Name and Compartment Name fields in this sheet are just for informational purpose right now; would be used in future when we allow same subnet names across VCNs</t>
-  </si>
-  <si>
     <t>egress</t>
   </si>
   <si>
@@ -752,13 +746,6 @@
   </si>
   <si>
     <t>ngw:PHXNonProd-VCN_ngw</t>
-  </si>
-  <si>
-    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new
- rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
-This sheet will only add new rules to the route tables; 'RouteRulesinOCI' sheet would be used for overwrite of all route rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
-VCN Name and Compartment Name fields in this sheet are just for informational purpose right now; would be used in future when we allow same subnet names across VCNs
-Enter Route Destination Object as either the OCID of component or  name of component- spcify name as igw:&lt;IGWName&gt;, ngw:&lt;NGWName&gt;, sgw:&lt;SGWName&gt;, drg:&lt;DRGName&gt;, lpg:&lt;LPGName&gt;</t>
   </si>
   <si>
     <t>route_table_name</t>
@@ -1515,14 +1502,24 @@
     <t>common_rules_ashprod</t>
   </si>
   <si>
+    <t>common_seclist_name</t>
+  </si>
+  <si>
     <t># subnet names are unique and case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if left blank means subnet will use default dhcp options of the vcn
 vcn_name should be same as enterd in VCNs sheet;
 Route Rules for IGW, NGW and SGW would be created based on parameter values: configure_igw, configure_ngw and configure_sgw respectively for each subnet. The condition is the respective component should have been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
-You can specify names for route tables and Scurity Lists; subnets can share same route table and seclist depending upon name specified; If left blank, default name which is subnet name would be used for that route table as well as security list. common_seclist_name column is also added to allow a seclist to be shared among multiple subnets
-Note- Please use different names for route tables/seclists across VCNs</t>
-  </si>
-  <si>
-    <t>common_seclist_name</t>
+You can specify names for route tables and Scurity Lists; subnets can share same route table and seclist depending upon name specified; If left blank, default name which is subnet name would be used for that route table as well as security list. common_seclist_name column is also added to allow a seclist to be shared among multiple subnets</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new
+ rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
+This sheet will only add new rules to the route tables; 'RouteRulesinOCI' sheet would be used for overwrite of all route rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI
+Enter Route Destination Object as either the OCID of component or  name of component- spcify name as igw:&lt;IGWName&gt;, ngw:&lt;NGWName&gt;, sgw:&lt;SGWName&gt;, drg:&lt;DRGName&gt;, lpg:&lt;LPGName&gt;</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; or &lt;end&gt; will not be processed; While adding more rules, you should move previous ones to the below and insert new  rows at the beginning and Enter &lt;END&gt; so that old rules already added don’t get added again;
+This sheet will only add new rules to theSecurity Lists; You can also edit Default Security List for a VCN- Mention subnet name as 'Default Security List for &lt;vcn_name&gt;'
+'SecRulesinOCI' sheet would be used for overwrite of all sec rules in OCI; That means whatever is there in that sheet would be updated as it is in OCI</t>
   </si>
 </sst>
 </file>
@@ -2358,7 +2355,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -2395,10 +2392,10 @@
         <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2407,13 +2404,13 @@
         <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
@@ -2421,13 +2418,13 @@
         <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -2435,13 +2432,13 @@
         <v>127</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -2659,7 +2656,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -2690,10 +2687,10 @@
         <v>112</v>
       </c>
       <c r="D2" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>144</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>145</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>88</v>
@@ -2702,13 +2699,13 @@
         <v>89</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I2" s="28" t="s">
         <v>90</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>93</v>
@@ -2732,7 +2729,7 @@
         <v>97</v>
       </c>
       <c r="R2" s="49" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -2743,27 +2740,27 @@
         <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>133</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="29"/>
       <c r="J3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" s="29" t="s">
         <v>153</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>154</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2772,7 +2769,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -2783,10 +2780,10 @@
         <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>98</v>
@@ -2795,10 +2792,10 @@
         <v>99</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="I4" s="29" t="s">
         <v>134</v>
@@ -2828,22 +2825,22 @@
         <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>133</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="K5" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2852,7 +2849,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -2866,22 +2863,22 @@
         <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>98</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -2921,7 +2918,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -2954,17 +2951,17 @@
         <v>128</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -2972,19 +2969,19 @@
         <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -3002,19 +2999,19 @@
         <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -3053,7 +3050,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -3107,10 +3104,10 @@
         <v>104</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -3118,34 +3115,34 @@
         <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>109</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>105</v>
@@ -3157,41 +3154,41 @@
         <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>109</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>105</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
@@ -3205,37 +3202,37 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>105</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
@@ -3243,40 +3240,40 @@
         <v>128</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>105</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N6" s="1"/>
     </row>
@@ -3350,7 +3347,7 @@
         <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="1">
         <v>150</v>
@@ -3362,10 +3359,10 @@
         <v>132</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>105</v>
@@ -3376,7 +3373,7 @@
         <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="1">
         <v>150</v>
@@ -3385,13 +3382,13 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>105</v>
@@ -3451,7 +3448,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -3478,49 +3475,49 @@
         <v>76</v>
       </c>
       <c r="C2" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="L2" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>248</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>249</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>250</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>260</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="K2" s="33" t="s">
+      <c r="M2" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="N2" s="33" t="s">
         <v>253</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="O2" s="33" t="s">
         <v>254</v>
       </c>
-      <c r="M2" s="33" t="s">
-        <v>258</v>
-      </c>
-      <c r="N2" s="33" t="s">
+      <c r="P2" s="33" t="s">
         <v>255</v>
       </c>
-      <c r="O2" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="P2" s="33" t="s">
+      <c r="Q2" s="33" t="s">
         <v>257</v>
-      </c>
-      <c r="Q2" s="33" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
@@ -3528,26 +3525,26 @@
         <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -3561,26 +3558,26 @@
         <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -3594,32 +3591,32 @@
         <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -3631,32 +3628,32 @@
         <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -3668,26 +3665,26 @@
         <v>127</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -3759,7 +3756,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -3788,55 +3785,55 @@
         <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="M2" s="33" t="s">
         <v>268</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="N2" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="G2" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>279</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>271</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>280</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>359</v>
-      </c>
-      <c r="M2" s="33" t="s">
-        <v>270</v>
-      </c>
-      <c r="N2" s="33" t="s">
-        <v>274</v>
-      </c>
       <c r="O2" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="P2" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q2" s="34" t="s">
         <v>286</v>
       </c>
-      <c r="P2" s="34" t="s">
+      <c r="R2" s="34" t="s">
         <v>287</v>
       </c>
-      <c r="Q2" s="34" t="s">
+      <c r="S2" s="34" t="s">
         <v>288</v>
-      </c>
-      <c r="R2" s="34" t="s">
-        <v>289</v>
-      </c>
-      <c r="S2" s="34" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -3844,53 +3841,53 @@
         <v>128</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J3" s="1">
         <v>80</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="M3" s="1">
         <v>443</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S3" s="1"/>
     </row>
@@ -3922,7 +3919,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="17" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -3965,7 +3962,7 @@
         <v>40</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>41</v>
@@ -3982,7 +3979,7 @@
       <c r="B4" s="64"/>
       <c r="C4" s="62"/>
       <c r="D4" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>44</v>
@@ -4196,16 +4193,16 @@
         <v>132</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -4213,16 +4210,16 @@
         <v>128</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>107</v>
@@ -4253,7 +4250,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="51"/>
@@ -4299,7 +4296,7 @@
         <v>68</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -4378,19 +4375,19 @@
         <v>127</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -4398,16 +4395,16 @@
         <v>128</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>107</v>
@@ -4441,7 +4438,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="66" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -4459,22 +4456,22 @@
         <v>76</v>
       </c>
       <c r="C2" s="37" t="s">
+        <v>292</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>294</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="F2" s="37" t="s">
         <v>295</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="G2" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="H2" s="37" t="s">
         <v>297</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>298</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -4482,16 +4479,16 @@
         <v>127</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>300</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>301</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>302</v>
       </c>
       <c r="F3" s="36">
         <v>1</v>
@@ -4500,7 +4497,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -4508,16 +4505,16 @@
         <v>127</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F4" s="36">
         <v>1</v>
@@ -4526,7 +4523,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -4534,16 +4531,16 @@
         <v>128</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F5" s="36">
         <v>1</v>
@@ -4552,7 +4549,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -4560,16 +4557,16 @@
         <v>128</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F6" s="36">
         <v>1</v>
@@ -4578,24 +4575,24 @@
         <v>1</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="36" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F7" s="36">
         <v>1</v>
@@ -4604,24 +4601,24 @@
         <v>1</v>
       </c>
       <c r="H7" s="36" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F8" s="36">
         <v>1</v>
@@ -4630,7 +4627,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -4669,7 +4666,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="40" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="69" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B1" s="70"/>
       <c r="C1" s="70"/>
@@ -4700,61 +4697,61 @@
         <v>76</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>53</v>
       </c>
       <c r="G2" s="41" t="s">
+        <v>315</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>316</v>
+      </c>
+      <c r="I2" s="41" t="s">
         <v>317</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="J2" s="41" t="s">
         <v>318</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="K2" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="L2" s="44" t="s">
         <v>320</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="M2" s="41" t="s">
         <v>321</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="N2" s="41" t="s">
         <v>322</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="O2" s="41" t="s">
         <v>323</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="P2" s="41" t="s">
         <v>324</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="Q2" s="41" t="s">
         <v>325</v>
       </c>
-      <c r="P2" s="41" t="s">
+      <c r="R2" s="41" t="s">
         <v>326</v>
       </c>
-      <c r="Q2" s="41" t="s">
+      <c r="S2" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="R2" s="41" t="s">
+      <c r="T2" s="41" t="s">
         <v>328</v>
       </c>
-      <c r="S2" s="41" t="s">
-        <v>329</v>
-      </c>
-      <c r="T2" s="41" t="s">
-        <v>330</v>
-      </c>
       <c r="U2" s="45" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
@@ -4762,19 +4759,19 @@
         <v>127</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D3" s="46" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G3" s="46">
         <v>1</v>
@@ -4783,40 +4780,40 @@
         <v>1</v>
       </c>
       <c r="I3" s="46" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="J3" s="46">
         <v>256</v>
       </c>
       <c r="K3" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="L3" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="M3" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="N3" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="O3" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="P3" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="Q3" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="P3" s="46" t="s">
+      <c r="R3" s="46" t="s">
         <v>339</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="S3" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="T3" s="46" t="s">
         <v>341</v>
-      </c>
-      <c r="S3" s="46" t="s">
-        <v>342</v>
-      </c>
-      <c r="T3" s="46" t="s">
-        <v>343</v>
       </c>
       <c r="U3" s="46" t="s">
         <v>12</v>
@@ -4827,19 +4824,19 @@
         <v>127</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C4" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>240</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="F4" s="46" t="s">
         <v>363</v>
-      </c>
-      <c r="D4" s="46" t="s">
-        <v>242</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>344</v>
-      </c>
-      <c r="F4" s="46" t="s">
-        <v>365</v>
       </c>
       <c r="G4" s="46">
         <v>1</v>
@@ -4848,40 +4845,40 @@
         <v>1</v>
       </c>
       <c r="I4" s="46" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J4" s="46">
         <v>256</v>
       </c>
       <c r="K4" s="46" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L4" s="46" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M4" s="46" t="s">
+        <v>344</v>
+      </c>
+      <c r="N4" s="46" t="s">
+        <v>345</v>
+      </c>
+      <c r="O4" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="P4" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="N4" s="46" t="s">
+      <c r="Q4" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="R4" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="S4" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="O4" s="46" t="s">
-        <v>338</v>
-      </c>
-      <c r="P4" s="46" t="s">
+      <c r="T4" s="46" t="s">
         <v>348</v>
-      </c>
-      <c r="Q4" s="46" t="s">
-        <v>340</v>
-      </c>
-      <c r="R4" s="46" t="s">
-        <v>341</v>
-      </c>
-      <c r="S4" s="46" t="s">
-        <v>349</v>
-      </c>
-      <c r="T4" s="46" t="s">
-        <v>350</v>
       </c>
       <c r="U4" s="46" t="s">
         <v>12</v>
@@ -4892,19 +4889,19 @@
         <v>128</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G5" s="46">
         <v>1</v>
@@ -4913,40 +4910,40 @@
         <v>1</v>
       </c>
       <c r="I5" s="46" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J5" s="46">
         <v>256</v>
       </c>
       <c r="K5" s="46" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L5" s="46" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M5" s="46" t="s">
+        <v>351</v>
+      </c>
+      <c r="N5" s="46" t="s">
+        <v>352</v>
+      </c>
+      <c r="O5" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="P5" s="46" t="s">
         <v>353</v>
       </c>
-      <c r="N5" s="46" t="s">
-        <v>354</v>
-      </c>
-      <c r="O5" s="46" t="s">
+      <c r="Q5" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="P5" s="46" t="s">
-        <v>355</v>
-      </c>
-      <c r="Q5" s="46" t="s">
+      <c r="R5" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="S5" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="R5" s="46" t="s">
-        <v>341</v>
-      </c>
-      <c r="S5" s="46" t="s">
-        <v>342</v>
-      </c>
       <c r="T5" s="46" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="U5" s="46" t="s">
         <v>12</v>
@@ -4957,19 +4954,19 @@
         <v>128</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F6" s="46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G6" s="46">
         <v>1</v>
@@ -4978,40 +4975,40 @@
         <v>1</v>
       </c>
       <c r="I6" s="46" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J6" s="46">
         <v>256</v>
       </c>
       <c r="K6" s="46" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L6" s="46" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M6" s="46" t="s">
+        <v>344</v>
+      </c>
+      <c r="N6" s="46" t="s">
+        <v>345</v>
+      </c>
+      <c r="O6" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="P6" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="N6" s="46" t="s">
+      <c r="Q6" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="R6" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="S6" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="O6" s="46" t="s">
-        <v>338</v>
-      </c>
-      <c r="P6" s="46" t="s">
+      <c r="T6" s="46" t="s">
         <v>348</v>
-      </c>
-      <c r="Q6" s="46" t="s">
-        <v>340</v>
-      </c>
-      <c r="R6" s="46" t="s">
-        <v>341</v>
-      </c>
-      <c r="S6" s="46" t="s">
-        <v>349</v>
-      </c>
-      <c r="T6" s="46" t="s">
-        <v>350</v>
       </c>
       <c r="U6" s="46" t="s">
         <v>12</v>
@@ -5019,22 +5016,22 @@
     </row>
     <row r="7" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="46" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F7" s="46" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G7" s="46">
         <v>1</v>
@@ -5043,40 +5040,40 @@
         <v>1</v>
       </c>
       <c r="I7" s="46" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J7" s="46">
         <v>256</v>
       </c>
       <c r="K7" s="46" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L7" s="46" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M7" s="46" t="s">
+        <v>351</v>
+      </c>
+      <c r="N7" s="46" t="s">
+        <v>352</v>
+      </c>
+      <c r="O7" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="P7" s="46" t="s">
         <v>353</v>
       </c>
-      <c r="N7" s="46" t="s">
-        <v>354</v>
-      </c>
-      <c r="O7" s="46" t="s">
+      <c r="Q7" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="P7" s="46" t="s">
-        <v>355</v>
-      </c>
-      <c r="Q7" s="46" t="s">
+      <c r="R7" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="S7" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="R7" s="46" t="s">
-        <v>341</v>
-      </c>
-      <c r="S7" s="46" t="s">
-        <v>342</v>
-      </c>
       <c r="T7" s="46" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="U7" s="46" t="s">
         <v>12</v>
@@ -5084,22 +5081,22 @@
     </row>
     <row r="8" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="46" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F8" s="46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G8" s="46">
         <v>1</v>
@@ -5108,40 +5105,40 @@
         <v>1</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J8" s="46">
         <v>256</v>
       </c>
       <c r="K8" s="46" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L8" s="46" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M8" s="46" t="s">
+        <v>351</v>
+      </c>
+      <c r="N8" s="46" t="s">
+        <v>352</v>
+      </c>
+      <c r="O8" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="P8" s="46" t="s">
         <v>353</v>
       </c>
-      <c r="N8" s="46" t="s">
-        <v>354</v>
-      </c>
-      <c r="O8" s="46" t="s">
+      <c r="Q8" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="P8" s="46" t="s">
-        <v>355</v>
-      </c>
-      <c r="Q8" s="46" t="s">
+      <c r="R8" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="S8" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="R8" s="46" t="s">
-        <v>341</v>
-      </c>
-      <c r="S8" s="46" t="s">
-        <v>342</v>
-      </c>
       <c r="T8" s="46" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="U8" s="46" t="s">
         <v>12</v>
@@ -5188,7 +5185,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -5228,7 +5225,7 @@
         <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>71</v>
@@ -5273,7 +5270,7 @@
         <v>73</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>74</v>
@@ -5285,7 +5282,7 @@
         <v>68</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -5340,7 +5337,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -5366,16 +5363,16 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>4</v>
@@ -5407,7 +5404,7 @@
         <v>129</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
@@ -5445,7 +5442,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
@@ -5481,13 +5478,13 @@
         <v>127</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>17</v>
@@ -5514,7 +5511,7 @@
         <v>58</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -5522,10 +5519,10 @@
         <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -5534,10 +5531,10 @@
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>20</v>
@@ -5624,7 +5621,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="238.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="55" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B1" s="56"/>
     </row>
@@ -5688,10 +5685,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>142</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5702,10 +5699,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -5730,8 +5727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5753,7 +5750,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -5792,13 +5789,13 @@
         <v>35</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>32</v>
@@ -5821,10 +5818,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -5836,7 +5833,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="13"/>
@@ -5861,10 +5858,10 @@
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -5873,14 +5870,14 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>16</v>
@@ -5892,7 +5889,7 @@
         <v>17</v>
       </c>
       <c r="N4" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
@@ -5903,10 +5900,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
@@ -5915,14 +5912,14 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>16</v>
@@ -5934,7 +5931,7 @@
         <v>17</v>
       </c>
       <c r="N5" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
@@ -5942,13 +5939,13 @@
         <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>0</v>
@@ -5972,7 +5969,7 @@
         <v>17</v>
       </c>
       <c r="N6" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
@@ -5980,13 +5977,13 @@
         <v>58</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>0</v>
@@ -5995,16 +5992,16 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>16</v>
@@ -6016,7 +6013,7 @@
         <v>17</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
@@ -6024,13 +6021,13 @@
         <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>0</v>
@@ -6039,14 +6036,14 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>16</v>
@@ -6058,7 +6055,7 @@
         <v>17</v>
       </c>
       <c r="N8" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -6190,12 +6187,12 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>13</v>
@@ -6204,24 +6201,24 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.35">
@@ -6229,16 +6226,16 @@
         <v>19</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>187</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -6279,7 +6276,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="50" t="s">
-        <v>230</v>
+        <v>394</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -6302,7 +6299,7 @@
         <v>112</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>79</v>
@@ -6324,13 +6321,13 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>83</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>84</v>
@@ -6346,13 +6343,13 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>83</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>84</v>
@@ -6368,13 +6365,13 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>84</v>
@@ -6410,7 +6407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
@@ -6432,7 +6429,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>135</v>
+        <v>395</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -6460,7 +6457,7 @@
         <v>112</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>87</v>
@@ -6503,7 +6500,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>98</v>
@@ -6536,7 +6533,7 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>98</v>
@@ -6565,10 +6562,10 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>133</v>
@@ -6580,7 +6577,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>

</xml_diff>

<commit_message>
updated DB systems - seperate tabs for DB BM, VM and Exa
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="19" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -28,21 +28,28 @@
     <sheet name="TagServer" sheetId="13" r:id="rId19"/>
     <sheet name="TagVolume" sheetId="14" r:id="rId20"/>
     <sheet name="ADW_ATP" sheetId="24" r:id="rId21"/>
-    <sheet name="Database" sheetId="25" r:id="rId22"/>
+    <sheet name="DB_System_VM" sheetId="26" r:id="rId22"/>
+    <sheet name="DB_System_BM" sheetId="27" r:id="rId23"/>
+    <sheet name="DB_System_EXA" sheetId="28" r:id="rId24"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId23"/>
+    <externalReference r:id="rId25"/>
+    <externalReference r:id="rId26"/>
   </externalReferences>
   <definedNames>
+    <definedName name="Shape_Option" localSheetId="22">#REF!</definedName>
+    <definedName name="Shape_Option" localSheetId="23">#REF!</definedName>
+    <definedName name="Shape_Option" localSheetId="21">#REF!</definedName>
     <definedName name="Shape_Option">#REF!</definedName>
     <definedName name="Shape_Option_DB">[1]Database!$B$10:$J$10</definedName>
+    <definedName name="VM_Shapes">DB_System_VM!$Y$398:$Y$408</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="419">
   <si>
     <t>Regional</t>
   </si>
@@ -1241,12 +1248,6 @@
     <t>Enable Automatic Backups</t>
   </si>
   <si>
-    <t>Experimentation</t>
-  </si>
-  <si>
-    <t>RACDB2cd</t>
-  </si>
-  <si>
     <t>ENTERPRISE_EDITION_EXTREME_PERFORMANCE</t>
   </si>
   <si>
@@ -1280,15 +1281,9 @@
     <t>yes</t>
   </si>
   <si>
-    <t>EXADB1cd</t>
-  </si>
-  <si>
     <t>ENTERPRISE_EDITION</t>
   </si>
   <si>
-    <t>EXADB1</t>
-  </si>
-  <si>
     <t>CDB2</t>
   </si>
   <si>
@@ -1304,27 +1299,12 @@
     <t>AD3</t>
   </si>
   <si>
-    <t>TESTDB3cd</t>
-  </si>
-  <si>
-    <t>TESTDB3</t>
-  </si>
-  <si>
     <t>CDB3</t>
   </si>
   <si>
     <t>pdb3</t>
   </si>
   <si>
-    <t>EXADB1cdphx</t>
-  </si>
-  <si>
-    <t>TESTDB3cdtrt</t>
-  </si>
-  <si>
-    <t>TESTDB3cdmum</t>
-  </si>
-  <si>
     <t>Listener Protocol (HTTP|TCP)</t>
   </si>
   <si>
@@ -1337,12 +1317,6 @@
     <t>SSH Key</t>
   </si>
   <si>
-    <t>testk_sub_a</t>
-  </si>
-  <si>
-    <t>testk_sub_e</t>
-  </si>
-  <si>
     <t>VM.Standard2.4</t>
   </si>
   <si>
@@ -1350,86 +1324,6 @@
   </si>
   <si>
     <t>VM.Standard2.16</t>
-  </si>
-  <si>
-    <r>
-      <t>#for DB Systems, fill the sheet with required information, as suggested in 2 row headings | Select shape for Virtual machine, bare metal, EXADATA in "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>G</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" column and change CPU core and node count accordingly.  Type anything after &lt;END&gt; for testing. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Do not Modify "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Shape Option DB"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> row</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>testk_sub1_e</t>
-  </si>
-  <si>
-    <t>testk_sub1_a</t>
-  </si>
-  <si>
-    <t>toronto</t>
-  </si>
-  <si>
-    <t>Test_Subnet</t>
-  </si>
-  <si>
-    <t>mumbai</t>
   </si>
   <si>
     <t>MT2</t>
@@ -1521,6 +1415,126 @@
 comma seperated VCNs on right column are peered with VCN on left column
 LPGs and rules are created based on this section; 
 eg: Mention Hub VCN name on left side and all spoke VCN names peered with it on right side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#for DB Systems Virtual Machine, fill the sheet with required information, as suggested in 2 row headings | Select shape for Virtual Machine in "F" column and change Node Count accordingly | &lt;end&gt; or &lt;END&gt; is must | Type anything after&lt;end&gt; or &lt;END&gt; for testing.  | If VM DB System node count is "2" then Software edition must be "ENTERPRISE_EDITION_EXTREME_PERFORMANCE"  </t>
+  </si>
+  <si>
+    <t>Character Set</t>
+  </si>
+  <si>
+    <t>nCharacter Set</t>
+  </si>
+  <si>
+    <t>Recovery Windows in days</t>
+  </si>
+  <si>
+    <t>TestK_testk_sub_1</t>
+  </si>
+  <si>
+    <t>VMDB28</t>
+  </si>
+  <si>
+    <t>AL32UTF8</t>
+  </si>
+  <si>
+    <t>AL16UTF16</t>
+  </si>
+  <si>
+    <t>VMDB281</t>
+  </si>
+  <si>
+    <t>RACDB21</t>
+  </si>
+  <si>
+    <t>VMDB282</t>
+  </si>
+  <si>
+    <t>RACDB212</t>
+  </si>
+  <si>
+    <t>VM Shapes</t>
+  </si>
+  <si>
+    <t>VM.Standard2.1</t>
+  </si>
+  <si>
+    <t>VM.Standard2.2</t>
+  </si>
+  <si>
+    <t>VM.Standard2.24</t>
+  </si>
+  <si>
+    <t>VM.Standard1.1</t>
+  </si>
+  <si>
+    <t>VM.Standard1.2</t>
+  </si>
+  <si>
+    <t>VM.Standard1.4</t>
+  </si>
+  <si>
+    <t>VM.Standard1.8</t>
+  </si>
+  <si>
+    <t>VM.Standard1.16</t>
+  </si>
+  <si>
+    <t>BM.DenseIO1.36</t>
+  </si>
+  <si>
+    <t>BM.DenseIO2.52</t>
+  </si>
+  <si>
+    <t>BM Shape</t>
+  </si>
+  <si>
+    <t>BM36</t>
+  </si>
+  <si>
+    <t>BMDB136</t>
+  </si>
+  <si>
+    <t>BM52</t>
+  </si>
+  <si>
+    <t>BMDB252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#for DB Systems Bare Metal, fill the sheet with required information, as suggested in 2 row headings | Select shape for Bare Metal in "F" column and change CPU core and it should be a even (multiple of 2) value.  | &lt;end&gt; or &lt;END&gt; is must | Type anything after &lt;end&gt; or &lt;END&gt; for testing | FOR CPU CORES --&gt; BM.DenseIO1.36 - Specify a multiple of 2, from 2 to 36 | BM.DenseIO2.52 - Specify a multiple of 2, from 2 to 52 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#for DB Systems ExaData, fill the sheet with required information, as suggested in 2 row headings | Select shape for EXADATA in "F" column and change CPU core accordingly | &lt;end&gt; or &lt;END&gt; is must | Type anything after &lt;end&gt; or &lt;END&gt; for testing. | Software edition is ENTERPRISE_EDITION_EXTREME_PERFORMANCE by default | Node count is 2 by default | FOR CPU CORES --&gt; Exadata.Base.48 - Specify a multiple of 2, from 0 to 48 | Exadata.Quarter1.84 - Specify a multiple of 2, from 22 to 84 | Exadata.Half1.168 - Specify a multiple of 4, from 44 to 168 | Exadata.Full1.336 - Specify a multiple of 8, from 88 to 336 | Exadata.Quarter2.92 - Specify a multiple of 2, from 0 to 92 | Exadata.Half2.184 - Specify a multiple of 4, from 0 to 184 | Exadata.Full2.368 - Specify a multiple of 8, from 0 to 368 </t>
+  </si>
+  <si>
+    <t>Backup Subnet Name</t>
+  </si>
+  <si>
+    <t>TestK_testk_sub_2</t>
+  </si>
+  <si>
+    <t>EXADB21</t>
+  </si>
+  <si>
+    <t>EXA Shapes</t>
+  </si>
+  <si>
+    <t>Exadata.Quarter2.92</t>
+  </si>
+  <si>
+    <t>Exadata.Half2.184</t>
+  </si>
+  <si>
+    <t>Exadata.Full2.368</t>
+  </si>
+  <si>
+    <t>Exadata.Quarter1.84</t>
+  </si>
+  <si>
+    <t>Exadata.Half1.168</t>
+  </si>
+  <si>
+    <t>Exadata.Full1.336</t>
   </si>
 </sst>
 </file>
@@ -1530,7 +1544,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;**"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1575,13 +1589,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
@@ -1590,13 +1597,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1790,7 +1790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1869,11 +1869,11 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1883,12 +1883,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1956,6 +1956,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2048,6 +2049,63 @@
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="DB_System_VM"/>
+      <sheetName val="DB_System_EXA"/>
+      <sheetName val="Compartments"/>
+      <sheetName val="Groups"/>
+      <sheetName val="Policies"/>
+      <sheetName val="VCNs"/>
+      <sheetName val="VCN Info"/>
+      <sheetName val="Subnets"/>
+      <sheetName val="DHCP"/>
+      <sheetName val="AddRouteRules"/>
+      <sheetName val="AddSecRules"/>
+      <sheetName val="RouteRulesinOCI"/>
+      <sheetName val="SecRulesinOCI"/>
+      <sheetName val="NSGs"/>
+      <sheetName val="DedicatedVMHosts"/>
+      <sheetName val="Instances"/>
+      <sheetName val="BlockVols"/>
+      <sheetName val="FSS"/>
+      <sheetName val="LBR"/>
+      <sheetName val="Tags"/>
+      <sheetName val="TagServer"/>
+      <sheetName val="TagVolume"/>
+      <sheetName val="ADW_ATP"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2729,8 +2787,8 @@
       <c r="Q2" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="R2" s="49" t="s">
-        <v>387</v>
+      <c r="R2" s="48" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -2770,7 +2828,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>388</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -3449,7 +3507,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>386</v>
+        <v>369</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -3535,7 +3593,7 @@
         <v>260</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -3545,7 +3603,7 @@
         <v>259</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>377</v>
+        <v>360</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -3568,17 +3626,17 @@
         <v>260</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>381</v>
+        <v>364</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>382</v>
+        <v>365</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -3595,29 +3653,29 @@
         <v>288</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>379</v>
+        <v>362</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>380</v>
+        <v>363</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -3632,29 +3690,29 @@
         <v>288</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>371</v>
+        <v>354</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>376</v>
+        <v>359</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -3669,23 +3727,23 @@
         <v>288</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>384</v>
+        <v>367</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>385</v>
+        <v>368</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -3757,7 +3815,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -3813,7 +3871,7 @@
         <v>277</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="M2" s="33" t="s">
         <v>267</v>
@@ -4439,7 +4497,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="66" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -4641,33 +4699,44 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:Y408"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="35" customWidth="1"/>
-    <col min="13" max="13" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.08984375" customWidth="1"/>
-    <col min="15" max="15" width="8.6328125" customWidth="1"/>
-    <col min="16" max="16" width="10.08984375" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" customWidth="1"/>
-    <col min="19" max="19" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.453125" customWidth="1"/>
-    <col min="21" max="21" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="36"/>
+    <col min="2" max="2" width="13.36328125" style="36" customWidth="1"/>
+    <col min="3" max="3" width="20" style="36" customWidth="1"/>
+    <col min="4" max="4" width="14" style="36" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="15" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.7265625" style="36"/>
+    <col min="11" max="11" width="17.1796875" style="35" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7265625" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.08984375" style="36" customWidth="1"/>
+    <col min="14" max="14" width="8.6328125" style="36" customWidth="1"/>
+    <col min="15" max="15" width="10.08984375" style="36" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" style="36" customWidth="1"/>
+    <col min="17" max="17" width="8.7265625" style="36"/>
+    <col min="18" max="18" width="23.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.453125" style="36" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.453125" style="36" customWidth="1"/>
+    <col min="22" max="22" width="13.08984375" style="36" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.7265625" style="36"/>
+    <col min="25" max="25" width="18.26953125" style="36" customWidth="1"/>
+    <col min="26" max="16384" width="8.7265625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="40" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" s="40" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="69" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="B1" s="70"/>
       <c r="C1" s="70"/>
@@ -4688,9 +4757,11 @@
       <c r="R1" s="70"/>
       <c r="S1" s="70"/>
       <c r="T1" s="70"/>
-      <c r="U1" s="71"/>
-    </row>
-    <row r="2" spans="1:21" s="36" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="U1" s="70"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="71"/>
+    </row>
+    <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>126</v>
       </c>
@@ -4710,459 +4781,929 @@
         <v>53</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="J2" s="41" t="s">
-        <v>317</v>
-      </c>
-      <c r="K2" s="41" t="s">
         <v>318</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="K2" s="44" t="s">
         <v>319</v>
       </c>
+      <c r="L2" s="41" t="s">
+        <v>320</v>
+      </c>
       <c r="M2" s="41" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="N2" s="41" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="O2" s="41" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="P2" s="41" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Q2" s="41" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="R2" s="41" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="S2" s="41" t="s">
-        <v>326</v>
-      </c>
-      <c r="T2" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="U2" s="45" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="T2" s="45" t="s">
+        <v>350</v>
+      </c>
+      <c r="U2" s="41" t="s">
+        <v>380</v>
+      </c>
+      <c r="V2" s="41" t="s">
+        <v>381</v>
+      </c>
+      <c r="W2" s="41" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="46" t="s">
         <v>127</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>288</v>
       </c>
-      <c r="C3" s="47" t="s">
-        <v>361</v>
+      <c r="C3" s="1" t="s">
+        <v>383</v>
       </c>
       <c r="D3" s="46" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>329</v>
+        <v>384</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>362</v>
+        <v>394</v>
       </c>
       <c r="G3" s="46">
         <v>1</v>
       </c>
-      <c r="H3" s="46">
-        <v>1</v>
-      </c>
-      <c r="I3" s="46" t="s">
+      <c r="H3" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="I3" s="46">
+        <v>256</v>
+      </c>
+      <c r="J3" s="46" t="s">
+        <v>329</v>
+      </c>
+      <c r="K3" s="46" t="s">
         <v>330</v>
       </c>
-      <c r="J3" s="46">
-        <v>256</v>
-      </c>
-      <c r="K3" s="46" t="s">
+      <c r="L3" s="46" t="s">
         <v>331</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="M3" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="N3" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="O3" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="P3" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="P3" s="46" t="s">
+      <c r="Q3" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="R3" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="S3" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="S3" s="46" t="s">
-        <v>339</v>
-      </c>
       <c r="T3" s="46" t="s">
-        <v>340</v>
-      </c>
-      <c r="U3" s="46" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="U3" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="W3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="46" t="s">
         <v>127</v>
       </c>
       <c r="B4" s="46" t="s">
         <v>288</v>
       </c>
-      <c r="C4" s="47" t="s">
-        <v>360</v>
+      <c r="C4" s="1" t="s">
+        <v>383</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>239</v>
+        <v>11</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>341</v>
+        <v>387</v>
       </c>
       <c r="F4" s="46" t="s">
-        <v>362</v>
+        <v>194</v>
       </c>
       <c r="G4" s="46">
-        <v>1</v>
-      </c>
-      <c r="H4" s="46">
-        <v>1</v>
-      </c>
-      <c r="I4" s="46" t="s">
-        <v>342</v>
-      </c>
-      <c r="J4" s="46">
+        <v>2</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="I4" s="46">
         <v>256</v>
       </c>
+      <c r="J4" s="46" t="s">
+        <v>329</v>
+      </c>
       <c r="K4" s="46" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L4" s="46" t="s">
+        <v>388</v>
+      </c>
+      <c r="M4" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="M4" s="46" t="s">
-        <v>343</v>
-      </c>
       <c r="N4" s="46" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="O4" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="P4" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="P4" s="46" t="s">
-        <v>345</v>
-      </c>
       <c r="Q4" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="R4" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="R4" s="46" t="s">
+      <c r="S4" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="S4" s="46" t="s">
-        <v>346</v>
-      </c>
       <c r="T4" s="46" t="s">
-        <v>347</v>
-      </c>
-      <c r="U4" s="46" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="U4" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="W4" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="46" t="s">
         <v>288</v>
       </c>
-      <c r="C5" s="47" t="s">
-        <v>366</v>
+      <c r="C5" s="1" t="s">
+        <v>383</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>348</v>
+        <v>11</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>349</v>
+        <v>389</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>364</v>
+        <v>194</v>
       </c>
       <c r="G5" s="46">
-        <v>1</v>
-      </c>
-      <c r="H5" s="46">
-        <v>1</v>
-      </c>
-      <c r="I5" s="46" t="s">
-        <v>342</v>
-      </c>
-      <c r="J5" s="46">
+        <v>2</v>
+      </c>
+      <c r="H5" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="I5" s="46">
         <v>256</v>
       </c>
+      <c r="J5" s="46" t="s">
+        <v>329</v>
+      </c>
       <c r="K5" s="46" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L5" s="46" t="s">
+        <v>390</v>
+      </c>
+      <c r="M5" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="M5" s="46" t="s">
-        <v>350</v>
-      </c>
       <c r="N5" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="O5" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="P5" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q5" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="R5" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="S5" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="T5" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="W5" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="36"/>
+    </row>
+    <row r="397" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y397" s="72" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="398" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y398" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="399" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y399" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="400" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y400" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="O5" s="46" t="s">
-        <v>335</v>
-      </c>
-      <c r="P5" s="46" t="s">
-        <v>352</v>
-      </c>
-      <c r="Q5" s="46" t="s">
-        <v>337</v>
-      </c>
-      <c r="R5" s="46" t="s">
-        <v>338</v>
-      </c>
-      <c r="S5" s="46" t="s">
-        <v>339</v>
-      </c>
-      <c r="T5" s="46" t="s">
-        <v>347</v>
-      </c>
-      <c r="U5" s="46" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="46" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>288</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>367</v>
-      </c>
-      <c r="D6" s="46" t="s">
-        <v>239</v>
-      </c>
-      <c r="E6" s="46" t="s">
+    </row>
+    <row r="401" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y401" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="402" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y402" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="F6" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="G6" s="46">
-        <v>1</v>
-      </c>
-      <c r="H6" s="46">
-        <v>1</v>
-      </c>
-      <c r="I6" s="46" t="s">
-        <v>342</v>
-      </c>
-      <c r="J6" s="46">
-        <v>256</v>
-      </c>
-      <c r="K6" s="46" t="s">
-        <v>331</v>
-      </c>
-      <c r="L6" s="46" t="s">
-        <v>332</v>
-      </c>
-      <c r="M6" s="46" t="s">
-        <v>343</v>
-      </c>
-      <c r="N6" s="46" t="s">
-        <v>344</v>
-      </c>
-      <c r="O6" s="46" t="s">
-        <v>335</v>
-      </c>
-      <c r="P6" s="46" t="s">
-        <v>345</v>
-      </c>
-      <c r="Q6" s="46" t="s">
-        <v>337</v>
-      </c>
-      <c r="R6" s="46" t="s">
-        <v>338</v>
-      </c>
-      <c r="S6" s="46" t="s">
-        <v>346</v>
-      </c>
-      <c r="T6" s="46" t="s">
-        <v>347</v>
-      </c>
-      <c r="U6" s="46" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="46" t="s">
-        <v>368</v>
-      </c>
-      <c r="B7" s="46" t="s">
-        <v>328</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>369</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>348</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>354</v>
-      </c>
-      <c r="F7" s="46" t="s">
-        <v>363</v>
-      </c>
-      <c r="G7" s="46">
-        <v>1</v>
-      </c>
-      <c r="H7" s="46">
-        <v>1</v>
-      </c>
-      <c r="I7" s="46" t="s">
-        <v>342</v>
-      </c>
-      <c r="J7" s="46">
-        <v>256</v>
-      </c>
-      <c r="K7" s="46" t="s">
-        <v>331</v>
-      </c>
-      <c r="L7" s="46" t="s">
-        <v>332</v>
-      </c>
-      <c r="M7" s="46" t="s">
-        <v>350</v>
-      </c>
-      <c r="N7" s="46" t="s">
-        <v>351</v>
-      </c>
-      <c r="O7" s="46" t="s">
-        <v>335</v>
-      </c>
-      <c r="P7" s="46" t="s">
-        <v>352</v>
-      </c>
-      <c r="Q7" s="46" t="s">
-        <v>337</v>
-      </c>
-      <c r="R7" s="46" t="s">
-        <v>338</v>
-      </c>
-      <c r="S7" s="46" t="s">
-        <v>339</v>
-      </c>
-      <c r="T7" s="46" t="s">
-        <v>347</v>
-      </c>
-      <c r="U7" s="46" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="46" t="s">
-        <v>370</v>
-      </c>
-      <c r="B8" s="46" t="s">
-        <v>328</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>369</v>
-      </c>
-      <c r="D8" s="46" t="s">
-        <v>348</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>355</v>
-      </c>
-      <c r="F8" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="G8" s="46">
-        <v>1</v>
-      </c>
-      <c r="H8" s="46">
-        <v>1</v>
-      </c>
-      <c r="I8" s="46" t="s">
-        <v>342</v>
-      </c>
-      <c r="J8" s="46">
-        <v>256</v>
-      </c>
-      <c r="K8" s="46" t="s">
-        <v>331</v>
-      </c>
-      <c r="L8" s="46" t="s">
-        <v>332</v>
-      </c>
-      <c r="M8" s="46" t="s">
-        <v>350</v>
-      </c>
-      <c r="N8" s="46" t="s">
-        <v>351</v>
-      </c>
-      <c r="O8" s="46" t="s">
-        <v>335</v>
-      </c>
-      <c r="P8" s="46" t="s">
-        <v>352</v>
-      </c>
-      <c r="Q8" s="46" t="s">
-        <v>337</v>
-      </c>
-      <c r="R8" s="46" t="s">
-        <v>338</v>
-      </c>
-      <c r="S8" s="46" t="s">
-        <v>339</v>
-      </c>
-      <c r="T8" s="46" t="s">
-        <v>347</v>
-      </c>
-      <c r="U8" s="46" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="48" t="s">
-        <v>62</v>
+    </row>
+    <row r="403" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y403" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="404" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y404" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="405" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y405" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="406" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y406" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="407" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y407" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="408" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y408" s="1" t="s">
+        <v>399</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A1:W1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9">
-      <formula1>Shape_Option</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9">
-      <formula1>Shape_Option_DB</formula1>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F402">
+      <formula1>$Y$398:$Y$408</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y398"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="36"/>
+    <col min="2" max="2" width="13.36328125" style="36" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="36"/>
+    <col min="4" max="4" width="9.81640625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.7265625" style="36"/>
+    <col min="11" max="11" width="8.7265625" style="35" customWidth="1"/>
+    <col min="12" max="12" width="14.7265625" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.08984375" style="36" customWidth="1"/>
+    <col min="14" max="14" width="8.6328125" style="36" customWidth="1"/>
+    <col min="15" max="15" width="10.08984375" style="36" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" style="36" customWidth="1"/>
+    <col min="17" max="18" width="23.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.453125" style="36" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.453125" style="36" customWidth="1"/>
+    <col min="22" max="22" width="13.08984375" style="36" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.7265625" style="36"/>
+    <col min="25" max="25" width="14.90625" style="36" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.7265625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="40" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="69" t="s">
+        <v>407</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="70"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="70"/>
+      <c r="X1" s="49"/>
+    </row>
+    <row r="2" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>313</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>316</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="K2" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>320</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>321</v>
+      </c>
+      <c r="N2" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="O2" s="41" t="s">
+        <v>323</v>
+      </c>
+      <c r="P2" s="41" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q2" s="41" t="s">
+        <v>325</v>
+      </c>
+      <c r="R2" s="41" t="s">
+        <v>326</v>
+      </c>
+      <c r="S2" s="41" t="s">
+        <v>327</v>
+      </c>
+      <c r="T2" s="45" t="s">
+        <v>350</v>
+      </c>
+      <c r="U2" s="41" t="s">
+        <v>380</v>
+      </c>
+      <c r="V2" s="41" t="s">
+        <v>381</v>
+      </c>
+      <c r="W2" s="41" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A3" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>406</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>401</v>
+      </c>
+      <c r="G3" s="46">
+        <v>2</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="I3" s="46">
+        <v>256</v>
+      </c>
+      <c r="J3" s="46" t="s">
+        <v>329</v>
+      </c>
+      <c r="K3" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="L3" s="46" t="s">
+        <v>405</v>
+      </c>
+      <c r="M3" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="N3" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="O3" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="P3" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q3" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="R3" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="S3" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="T3" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="W3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>344</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>404</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>400</v>
+      </c>
+      <c r="G4" s="46">
+        <v>2</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="I4" s="46">
+        <v>256</v>
+      </c>
+      <c r="J4" s="46" t="s">
+        <v>329</v>
+      </c>
+      <c r="K4" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="L4" s="46" t="s">
+        <v>403</v>
+      </c>
+      <c r="M4" s="46" t="s">
+        <v>345</v>
+      </c>
+      <c r="N4" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="O4" s="46" t="s">
+        <v>346</v>
+      </c>
+      <c r="P4" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q4" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="R4" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="S4" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="T4" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="W4" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A5" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="36"/>
+    </row>
+    <row r="396" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y396" s="72" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="397" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y397" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="398" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y398" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:W1"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F396">
+      <formula1>$Y$397:$Y$398</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5">
+      <formula1>Shape_Option</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y402"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="36"/>
+    <col min="2" max="2" width="13.36328125" style="36" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" style="36" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.36328125" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.7265625" style="36"/>
+    <col min="11" max="11" width="17.1796875" style="35" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7265625" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.08984375" style="36" customWidth="1"/>
+    <col min="14" max="14" width="8.6328125" style="36" customWidth="1"/>
+    <col min="15" max="15" width="10.08984375" style="36" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" style="36" customWidth="1"/>
+    <col min="17" max="18" width="23.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" style="36" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.453125" style="36" customWidth="1"/>
+    <col min="22" max="22" width="13.08984375" style="36" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.7265625" style="36"/>
+    <col min="25" max="25" width="18.26953125" style="36" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.7265625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="40" customFormat="1" ht="93.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="69" t="s">
+        <v>408</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="70"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="71"/>
+    </row>
+    <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>409</v>
+      </c>
+      <c r="F2" s="43" t="s">
+        <v>313</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="K2" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>320</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>321</v>
+      </c>
+      <c r="N2" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="O2" s="41" t="s">
+        <v>323</v>
+      </c>
+      <c r="P2" s="41" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q2" s="41" t="s">
+        <v>325</v>
+      </c>
+      <c r="R2" s="41" t="s">
+        <v>326</v>
+      </c>
+      <c r="S2" s="41" t="s">
+        <v>327</v>
+      </c>
+      <c r="T2" s="45" t="s">
+        <v>350</v>
+      </c>
+      <c r="U2" s="41" t="s">
+        <v>380</v>
+      </c>
+      <c r="V2" s="41" t="s">
+        <v>381</v>
+      </c>
+      <c r="W2" s="41" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>411</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>352</v>
+      </c>
+      <c r="H3" s="46">
+        <v>2</v>
+      </c>
+      <c r="I3" s="46">
+        <v>256</v>
+      </c>
+      <c r="J3" s="46" t="s">
+        <v>329</v>
+      </c>
+      <c r="K3" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="L3" s="46" t="s">
+        <v>411</v>
+      </c>
+      <c r="M3" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="N3" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="O3" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="P3" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q3" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="R3" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="S3" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="T3" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="W3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="36"/>
+    </row>
+    <row r="395" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y395" s="72" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="396" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y396" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="397" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y397" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="398" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y398" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="399" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y399" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="400" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y400" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="401" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y401" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="402" spans="25:25" x14ac:dyDescent="0.35">
+      <c r="Y402" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:W1"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G395">
+      <formula1>$Y$396:$Y$402</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4">
+      <formula1>Shape_Option</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5609,7 +6150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
@@ -5694,7 +6235,7 @@
     </row>
     <row r="11" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="52" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="B11" s="54"/>
     </row>
@@ -5751,7 +6292,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -5796,7 +6337,7 @@
         <v>229</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>32</v>
@@ -5878,7 +6419,7 @@
         <v>230</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>389</v>
+        <v>372</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>16</v>
@@ -5920,7 +6461,7 @@
         <v>230</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>389</v>
+        <v>372</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>16</v>
@@ -6002,7 +6543,7 @@
         <v>231</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>16</v>
@@ -6044,7 +6585,7 @@
         <v>231</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>16</v>
@@ -6277,7 +6818,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="50" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -6408,8 +6949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6430,7 +6971,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>

</xml_diff>

<commit_message>
updated to sync with master: lpg in createOCSWork, instance sheet- subnet name,install older version of tf
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="19" activeTab="23"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId25"/>
-    <externalReference r:id="rId26"/>
   </externalReferences>
   <definedNames>
     <definedName name="Shape_Option" localSheetId="22">#REF!</definedName>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="423">
   <si>
     <t>Regional</t>
   </si>
@@ -849,9 +848,6 @@
   </si>
   <si>
     <t>MountTarget SubnetName</t>
-  </si>
-  <si>
-    <t>#Template will be picked upon from template folder based on  OS column; Backup Policy column can be left blank at the time of instance creation and can be filled up later on while attaching backup policy to the boot and block volumes together; Pub Address column represents whether public address needs to be assigned to the instance or not(TRUE|FALSE); ssh-key-var-name column accepts the name of variable defined in variables_&lt;region&gt;.tf file containing SSH key to be pushed to the server; NSGs column accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG; Leave DedicatedVMHost column blank if instance doesnt need to be launched on dedicated vm host</t>
   </si>
   <si>
     <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars;
@@ -1535,6 +1531,22 @@
   </si>
   <si>
     <t>Exadata.Full1.336</t>
+  </si>
+  <si>
+    <t>#Template will be picked upon from template folder based on  OS column; Backup Policy column can be left blank at the time of instance creation and can be filled up later on while attaching backup policy to the boot and block volumes together; Pub Address column represents whether public address needs to be assigned to the instance or not(TRUE|FALSE); ssh-key-var-name column accepts the name of variable defined in variables_&lt;region&gt;.tf file containing SSH key to be pushed to the server; NSGs column accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG; Leave DedicatedVMHost column blank if instance doesnt need to be launched on dedicated vm host
+#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
+  </si>
+  <si>
+    <t>ASHHub-VCN_ASHHub-VCN-subnet1</t>
+  </si>
+  <si>
+    <t>ASHProd-VCN_prod-subnet</t>
+  </si>
+  <si>
+    <t>PHXNonProd-VCN_dev-subnet</t>
+  </si>
+  <si>
+    <t>PHXHub-VCN_PHXHub-VCN-subnet1</t>
   </si>
 </sst>
 </file>
@@ -1890,6 +1902,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1956,7 +1969,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2049,63 +2061,6 @@
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="DB_System_VM"/>
-      <sheetName val="DB_System_EXA"/>
-      <sheetName val="Compartments"/>
-      <sheetName val="Groups"/>
-      <sheetName val="Policies"/>
-      <sheetName val="VCNs"/>
-      <sheetName val="VCN Info"/>
-      <sheetName val="Subnets"/>
-      <sheetName val="DHCP"/>
-      <sheetName val="AddRouteRules"/>
-      <sheetName val="AddSecRules"/>
-      <sheetName val="RouteRulesinOCI"/>
-      <sheetName val="SecRulesinOCI"/>
-      <sheetName val="NSGs"/>
-      <sheetName val="DedicatedVMHosts"/>
-      <sheetName val="Instances"/>
-      <sheetName val="BlockVols"/>
-      <sheetName val="FSS"/>
-      <sheetName val="LBR"/>
-      <sheetName val="Tags"/>
-      <sheetName val="TagServer"/>
-      <sheetName val="TagVolume"/>
-      <sheetName val="ADW_ATP"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2413,12 +2368,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="52"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -2714,26 +2669,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
@@ -2788,7 +2743,7 @@
         <v>97</v>
       </c>
       <c r="R2" s="48" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -2828,7 +2783,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -2976,14 +2931,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3085,8 +3040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3095,7 +3050,7 @@
     <col min="2" max="2" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7265625" customWidth="1"/>
+    <col min="5" max="5" width="31.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.7265625" bestFit="1" customWidth="1"/>
@@ -3107,23 +3062,23 @@
     <col min="14" max="14" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="54"/>
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="53" t="s">
+        <v>418</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="55"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -3183,7 +3138,7 @@
         <v>190</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>171</v>
+        <v>419</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
@@ -3222,7 +3177,7 @@
         <v>191</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>168</v>
+        <v>422</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
@@ -3264,7 +3219,7 @@
         <v>190</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>172</v>
+        <v>420</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
@@ -3308,7 +3263,7 @@
         <v>191</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>169</v>
+        <v>421</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>0</v>
@@ -3364,16 +3319,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="17" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3506,25 +3461,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
-        <v>369</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
+      <c r="A1" s="58" t="s">
+        <v>368</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
     </row>
     <row r="2" spans="1:17" s="32" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
@@ -3584,7 +3539,7 @@
         <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>239</v>
@@ -3593,7 +3548,7 @@
         <v>260</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -3603,7 +3558,7 @@
         <v>259</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -3617,7 +3572,7 @@
         <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>239</v>
@@ -3626,17 +3581,17 @@
         <v>260</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>365</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -3650,32 +3605,32 @@
         <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="L5" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>363</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -3687,32 +3642,32 @@
         <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>355</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>359</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -3724,26 +3679,26 @@
         <v>127</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>368</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -3814,27 +3769,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
-        <v>348</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
+      <c r="A1" s="58" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
     </row>
     <row r="2" spans="1:19" s="17" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
@@ -3844,55 +3799,55 @@
         <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="F2" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="I2" s="33" t="s">
         <v>275</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="J2" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="M2" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="G2" s="33" t="s">
+      <c r="N2" s="33" t="s">
         <v>270</v>
       </c>
-      <c r="H2" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>347</v>
-      </c>
-      <c r="M2" s="33" t="s">
-        <v>267</v>
-      </c>
-      <c r="N2" s="33" t="s">
-        <v>271</v>
-      </c>
       <c r="O2" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="P2" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="P2" s="34" t="s">
+      <c r="Q2" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="Q2" s="34" t="s">
+      <c r="R2" s="34" t="s">
         <v>285</v>
       </c>
-      <c r="R2" s="34" t="s">
+      <c r="S2" s="34" t="s">
         <v>286</v>
-      </c>
-      <c r="S2" s="34" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -3900,13 +3855,13 @@
         <v>128</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>169</v>
@@ -3915,38 +3870,38 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>280</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J3" s="1">
         <v>80</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M3" s="1">
         <v>443</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="S3" s="1"/>
     </row>
@@ -3977,15 +3932,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="17" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -4011,13 +3966,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="62" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -4034,9 +3989,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="62"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="8" t="s">
         <v>202</v>
       </c>
@@ -4051,9 +4006,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="64"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="62"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="63"/>
       <c r="D5" s="9"/>
       <c r="E5" s="1"/>
       <c r="F5" s="10" t="s">
@@ -4064,9 +4019,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="64"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="62"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="63"/>
       <c r="D6" s="9"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
@@ -4077,108 +4032,108 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="64"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="62"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="63"/>
       <c r="D7" s="11"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="64"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="62"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="63"/>
       <c r="D8" s="11"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="64"/>
-      <c r="B9" s="64"/>
-      <c r="C9" s="62"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="63"/>
       <c r="D9" s="11"/>
       <c r="E9" s="1"/>
       <c r="F9" s="10"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="64"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="62"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="63"/>
       <c r="D10" s="11"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="64"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="62"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="11"/>
       <c r="E11" s="1"/>
       <c r="F11" s="10"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="64"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="62"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="63"/>
       <c r="D12" s="11"/>
       <c r="E12" s="1"/>
       <c r="F12" s="10"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="64"/>
-      <c r="B13" s="64"/>
-      <c r="C13" s="62"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="63"/>
       <c r="D13" s="11"/>
       <c r="E13" s="1"/>
       <c r="F13" s="10"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="64"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="62"/>
+      <c r="A14" s="65"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="63"/>
       <c r="D14" s="11"/>
       <c r="E14" s="1"/>
       <c r="F14" s="10"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="64"/>
-      <c r="B15" s="64"/>
-      <c r="C15" s="62"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="9"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="64"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="62"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="63"/>
       <c r="D16" s="9"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="64"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="62"/>
+      <c r="A17" s="65"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="9"/>
       <c r="E17" s="1"/>
       <c r="F17" s="10"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="64"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="63"/>
+      <c r="A18" s="65"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="9"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -4215,14 +4170,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -4308,11 +4263,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -4400,14 +4355,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -4496,16 +4451,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="s">
-        <v>349</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="68"/>
+      <c r="A1" s="67" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="37" t="s">
@@ -4515,22 +4470,22 @@
         <v>76</v>
       </c>
       <c r="C2" s="37" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>291</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="E2" s="39" t="s">
         <v>292</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="F2" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="G2" s="37" t="s">
         <v>294</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="H2" s="37" t="s">
         <v>295</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -4538,16 +4493,16 @@
         <v>127</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="D3" s="36" t="s">
         <v>297</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="E3" s="38" t="s">
         <v>298</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>299</v>
       </c>
       <c r="F3" s="36">
         <v>1</v>
@@ -4556,7 +4511,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -4564,16 +4519,16 @@
         <v>127</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="36" t="s">
         <v>301</v>
       </c>
-      <c r="D4" s="36" t="s">
-        <v>302</v>
-      </c>
       <c r="E4" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F4" s="36">
         <v>1</v>
@@ -4582,7 +4537,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -4590,16 +4545,16 @@
         <v>128</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C5" s="36" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" s="36" t="s">
         <v>304</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>305</v>
-      </c>
       <c r="E5" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F5" s="36">
         <v>1</v>
@@ -4608,7 +4563,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -4616,16 +4571,16 @@
         <v>128</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C6" s="36" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="36" t="s">
         <v>306</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>307</v>
-      </c>
       <c r="E6" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F6" s="36">
         <v>1</v>
@@ -4634,24 +4589,24 @@
         <v>1</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="C7" s="36" t="s">
         <v>308</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>288</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>309</v>
-      </c>
       <c r="D7" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F7" s="36">
         <v>1</v>
@@ -4660,24 +4615,24 @@
         <v>1</v>
       </c>
       <c r="H7" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>310</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>288</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>311</v>
-      </c>
       <c r="D8" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F8" s="36">
         <v>1</v>
@@ -4686,7 +4641,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -4735,31 +4690,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="40" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="69" t="s">
-        <v>379</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="71"/>
+      <c r="A1" s="70" t="s">
+        <v>378</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="72"/>
     </row>
     <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
@@ -4769,67 +4724,67 @@
         <v>76</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>53</v>
       </c>
       <c r="G2" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="H2" s="41" t="s">
         <v>315</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="I2" s="41" t="s">
         <v>316</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="J2" s="41" t="s">
         <v>317</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="K2" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="K2" s="44" t="s">
+      <c r="L2" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="M2" s="41" t="s">
         <v>320</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="N2" s="41" t="s">
         <v>321</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="O2" s="41" t="s">
         <v>322</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="P2" s="41" t="s">
         <v>323</v>
       </c>
-      <c r="P2" s="41" t="s">
+      <c r="Q2" s="41" t="s">
         <v>324</v>
       </c>
-      <c r="Q2" s="41" t="s">
+      <c r="R2" s="41" t="s">
         <v>325</v>
       </c>
-      <c r="R2" s="41" t="s">
+      <c r="S2" s="41" t="s">
         <v>326</v>
       </c>
-      <c r="S2" s="41" t="s">
-        <v>327</v>
-      </c>
       <c r="T2" s="45" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="U2" s="41" t="s">
+        <v>379</v>
+      </c>
+      <c r="V2" s="41" t="s">
         <v>380</v>
       </c>
-      <c r="V2" s="41" t="s">
+      <c r="W2" s="41" t="s">
         <v>381</v>
-      </c>
-      <c r="W2" s="41" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
@@ -4837,67 +4792,67 @@
         <v>127</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D3" s="46" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G3" s="46">
         <v>1</v>
       </c>
       <c r="H3" s="46" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I3" s="46">
         <v>256</v>
       </c>
       <c r="J3" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="K3" s="46" t="s">
         <v>329</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="L3" s="46" t="s">
         <v>330</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="M3" s="46" t="s">
         <v>331</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="N3" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="O3" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="P3" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="P3" s="46" t="s">
+      <c r="Q3" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="R3" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="S3" s="46" t="s">
         <v>337</v>
-      </c>
-      <c r="S3" s="46" t="s">
-        <v>338</v>
       </c>
       <c r="T3" s="46" t="s">
         <v>12</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -4908,16 +4863,16 @@
         <v>127</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D4" s="46" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F4" s="46" t="s">
         <v>194</v>
@@ -4926,49 +4881,49 @@
         <v>2</v>
       </c>
       <c r="H4" s="46" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I4" s="46">
         <v>256</v>
       </c>
       <c r="J4" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="K4" s="46" t="s">
         <v>329</v>
       </c>
-      <c r="K4" s="46" t="s">
-        <v>330</v>
-      </c>
       <c r="L4" s="46" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M4" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="N4" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="N4" s="46" t="s">
+      <c r="O4" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="O4" s="46" t="s">
+      <c r="P4" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="P4" s="46" t="s">
+      <c r="Q4" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="Q4" s="46" t="s">
+      <c r="R4" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="R4" s="46" t="s">
+      <c r="S4" s="46" t="s">
         <v>337</v>
-      </c>
-      <c r="S4" s="46" t="s">
-        <v>338</v>
       </c>
       <c r="T4" s="46" t="s">
         <v>12</v>
       </c>
       <c r="U4" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="W4" s="1">
         <v>15</v>
@@ -4979,16 +4934,16 @@
         <v>127</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D5" s="46" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F5" s="46" t="s">
         <v>194</v>
@@ -4997,49 +4952,49 @@
         <v>2</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I5" s="46">
         <v>256</v>
       </c>
       <c r="J5" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="K5" s="46" t="s">
         <v>329</v>
       </c>
-      <c r="K5" s="46" t="s">
-        <v>330</v>
-      </c>
       <c r="L5" s="46" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M5" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="N5" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="N5" s="46" t="s">
+      <c r="O5" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="O5" s="46" t="s">
+      <c r="P5" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="P5" s="46" t="s">
+      <c r="Q5" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="Q5" s="46" t="s">
+      <c r="R5" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="R5" s="46" t="s">
+      <c r="S5" s="46" t="s">
         <v>337</v>
-      </c>
-      <c r="S5" s="46" t="s">
-        <v>338</v>
       </c>
       <c r="T5" s="46" t="s">
         <v>12</v>
       </c>
       <c r="U5" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="W5" s="1">
         <v>20</v>
@@ -5052,23 +5007,23 @@
       <c r="K6" s="36"/>
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
-      <c r="Y397" s="72" t="s">
-        <v>391</v>
+      <c r="Y397" s="50" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="399" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y399" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="400" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y400" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="401" spans="25:25" x14ac:dyDescent="0.35">
@@ -5078,37 +5033,37 @@
     </row>
     <row r="402" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y402" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="403" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y403" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="404" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y404" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="405" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y405" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="406" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y406" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="407" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y407" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="408" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y408" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -5162,31 +5117,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="40" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="69" t="s">
-        <v>407</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
+      <c r="A1" s="70" t="s">
+        <v>406</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
       <c r="X1" s="49"/>
     </row>
     <row r="2" spans="1:24" ht="29" x14ac:dyDescent="0.35">
@@ -5197,67 +5152,67 @@
         <v>76</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>53</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H2" s="41" t="s">
+        <v>315</v>
+      </c>
+      <c r="I2" s="41" t="s">
         <v>316</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="J2" s="41" t="s">
         <v>317</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="K2" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="K2" s="44" t="s">
+      <c r="L2" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="M2" s="41" t="s">
         <v>320</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="N2" s="41" t="s">
         <v>321</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="O2" s="41" t="s">
         <v>322</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="P2" s="41" t="s">
         <v>323</v>
       </c>
-      <c r="P2" s="41" t="s">
+      <c r="Q2" s="41" t="s">
         <v>324</v>
       </c>
-      <c r="Q2" s="41" t="s">
+      <c r="R2" s="41" t="s">
         <v>325</v>
       </c>
-      <c r="R2" s="41" t="s">
+      <c r="S2" s="41" t="s">
         <v>326</v>
       </c>
-      <c r="S2" s="41" t="s">
-        <v>327</v>
-      </c>
       <c r="T2" s="45" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="U2" s="41" t="s">
+        <v>379</v>
+      </c>
+      <c r="V2" s="41" t="s">
         <v>380</v>
       </c>
-      <c r="V2" s="41" t="s">
+      <c r="W2" s="41" t="s">
         <v>381</v>
-      </c>
-      <c r="W2" s="41" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
@@ -5265,67 +5220,67 @@
         <v>127</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D3" s="46" t="s">
         <v>239</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G3" s="46">
         <v>2</v>
       </c>
       <c r="H3" s="46" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I3" s="46">
         <v>256</v>
       </c>
       <c r="J3" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="K3" s="46" t="s">
         <v>329</v>
       </c>
-      <c r="K3" s="46" t="s">
-        <v>330</v>
-      </c>
       <c r="L3" s="46" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="M3" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="N3" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="O3" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="N3" s="46" t="s">
-        <v>333</v>
-      </c>
-      <c r="O3" s="46" t="s">
+      <c r="P3" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q3" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="R3" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="P3" s="46" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q3" s="46" t="s">
-        <v>336</v>
-      </c>
-      <c r="R3" s="46" t="s">
+      <c r="S3" s="46" t="s">
         <v>342</v>
-      </c>
-      <c r="S3" s="46" t="s">
-        <v>343</v>
       </c>
       <c r="T3" s="46" t="s">
         <v>12</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -5336,67 +5291,67 @@
         <v>128</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F4" s="46" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G4" s="46">
         <v>2</v>
       </c>
       <c r="H4" s="46" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I4" s="46">
         <v>256</v>
       </c>
       <c r="J4" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="K4" s="46" t="s">
         <v>329</v>
       </c>
-      <c r="K4" s="46" t="s">
-        <v>330</v>
-      </c>
       <c r="L4" s="46" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M4" s="46" t="s">
+        <v>344</v>
+      </c>
+      <c r="N4" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="O4" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="N4" s="46" t="s">
-        <v>333</v>
-      </c>
-      <c r="O4" s="46" t="s">
-        <v>346</v>
-      </c>
       <c r="P4" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q4" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="Q4" s="46" t="s">
+      <c r="R4" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="R4" s="46" t="s">
-        <v>337</v>
-      </c>
       <c r="S4" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="T4" s="46" t="s">
         <v>12</v>
       </c>
       <c r="U4" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="W4" s="1">
         <v>15</v>
@@ -5409,18 +5364,18 @@
       <c r="K5" s="36"/>
     </row>
     <row r="396" spans="25:25" x14ac:dyDescent="0.35">
-      <c r="Y396" s="72" t="s">
-        <v>402</v>
+      <c r="Y396" s="50" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y397" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -5443,7 +5398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y402"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -5476,31 +5431,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="40" customFormat="1" ht="93.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="69" t="s">
-        <v>408</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="71"/>
+      <c r="A1" s="70" t="s">
+        <v>407</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="72"/>
     </row>
     <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
@@ -5510,67 +5465,67 @@
         <v>76</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F2" s="43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>53</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I2" s="41" t="s">
+        <v>316</v>
+      </c>
+      <c r="J2" s="41" t="s">
         <v>317</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="K2" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="K2" s="44" t="s">
+      <c r="L2" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="M2" s="41" t="s">
         <v>320</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="N2" s="41" t="s">
         <v>321</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="O2" s="41" t="s">
         <v>322</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="P2" s="41" t="s">
         <v>323</v>
       </c>
-      <c r="P2" s="41" t="s">
+      <c r="Q2" s="41" t="s">
         <v>324</v>
       </c>
-      <c r="Q2" s="41" t="s">
+      <c r="R2" s="41" t="s">
         <v>325</v>
       </c>
-      <c r="R2" s="41" t="s">
+      <c r="S2" s="41" t="s">
         <v>326</v>
       </c>
-      <c r="S2" s="41" t="s">
-        <v>327</v>
-      </c>
       <c r="T2" s="45" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="U2" s="41" t="s">
+        <v>379</v>
+      </c>
+      <c r="V2" s="41" t="s">
         <v>380</v>
       </c>
-      <c r="V2" s="41" t="s">
+      <c r="W2" s="41" t="s">
         <v>381</v>
-      </c>
-      <c r="W2" s="41" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
@@ -5578,22 +5533,22 @@
         <v>127</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D3" s="46" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="F3" s="46" t="s">
         <v>410</v>
       </c>
-      <c r="F3" s="46" t="s">
-        <v>411</v>
-      </c>
       <c r="G3" s="46" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H3" s="46">
         <v>2</v>
@@ -5602,43 +5557,43 @@
         <v>256</v>
       </c>
       <c r="J3" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="K3" s="46" t="s">
         <v>329</v>
       </c>
-      <c r="K3" s="46" t="s">
-        <v>330</v>
-      </c>
       <c r="L3" s="46" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="M3" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="N3" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="N3" s="46" t="s">
+      <c r="O3" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="P3" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="P3" s="46" t="s">
+      <c r="Q3" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="R3" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="S3" s="46" t="s">
         <v>337</v>
-      </c>
-      <c r="S3" s="46" t="s">
-        <v>338</v>
       </c>
       <c r="T3" s="46" t="s">
         <v>12</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -5651,43 +5606,43 @@
       <c r="K4" s="36"/>
     </row>
     <row r="395" spans="25:25" x14ac:dyDescent="0.35">
-      <c r="Y395" s="72" t="s">
-        <v>412</v>
+      <c r="Y395" s="50" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="396" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y396" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y397" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="399" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y399" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="400" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y400" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="401" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y401" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="402" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y402" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -5726,15 +5681,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
@@ -5858,7 +5813,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5878,21 +5833,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
-        <v>263</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="54"/>
+      <c r="A1" s="53" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="55"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -6162,10 +6117,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="238.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
-        <v>264</v>
-      </c>
-      <c r="B1" s="56"/>
+      <c r="A1" s="56" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="57"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -6234,10 +6189,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="52" t="s">
-        <v>378</v>
-      </c>
-      <c r="B11" s="54"/>
+      <c r="A11" s="53" t="s">
+        <v>377</v>
+      </c>
+      <c r="B11" s="55"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -6270,7 +6225,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6291,22 +6246,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="103.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
-        <v>375</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
+      <c r="A1" s="53" t="s">
+        <v>374</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
     </row>
     <row r="2" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -6337,7 +6292,7 @@
         <v>229</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>32</v>
@@ -6419,7 +6374,7 @@
         <v>230</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>16</v>
@@ -6461,7 +6416,7 @@
         <v>230</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>16</v>
@@ -6543,7 +6498,7 @@
         <v>231</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>16</v>
@@ -6585,7 +6540,7 @@
         <v>231</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>16</v>
@@ -6693,13 +6648,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -6817,15 +6772,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
-        <v>376</v>
-      </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="A1" s="51" t="s">
+        <v>375</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -6970,23 +6925,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
-        <v>377</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
+      <c r="A1" s="58" t="s">
+        <v>376</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
Modified export rules code to add sheet formatting+ordering create_terraform_block_volumes.py - Modified to check int then str create_terraform_dhcp.py -  Modiified to allow empty search domain CD3-template.xlsx - change in db system header row Added new option to modify existing subnets ( subnet propertes) Modified panda so that it gets created in oraclemigration then fetched details using opc cli
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="17" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="7" r:id="rId1"/>
@@ -3040,7 +3040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E6"/>
     </sheetView>
   </sheetViews>
@@ -4656,8 +4656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y408"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5071,7 +5071,7 @@
     <mergeCell ref="A1:W1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F402">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F402">
       <formula1>$Y$398:$Y$408</formula1>
     </dataValidation>
   </dataValidations>
@@ -5085,7 +5085,7 @@
   <dimension ref="A1:Y398"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5398,8 +5398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y402"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Support for Non GreenField Tenancies - updated Added for dns_label as n
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="29" r:id="rId1"/>
@@ -1458,8 +1458,17 @@
     <t>seclist_names</t>
   </si>
   <si>
+    <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars.
+dns_label - if specified as n, DNS will not be enabled for the VCN
+Valid Values for columns E,F,G,H,I:   y|n|&lt;component_name&gt; ie mention 'n' when a component(like IGW) is not required to be configured(like for PHXHub-VCN), specify name of the component- component will be configured with the mentioned name(eg PHX-DRG for the DRG in PHXHub-VCN) and mention 'y' if component needs to be configured with default name ie &lt;vcnname&gt;_ngw(eg PHXNonProd-VCN_ngw)
+Note- For LPGs, specify comma seperated values based on number of LPGs required for each VCN. LPGs will be peered with other VCN LPGs in the order they are specified.
+Note- For column hub_spoke_peer_none - specify 'hub' if the VCN is a hub, specify 'spoke:&lt;hub vcn name&gt;' if VCN is a spoke of a hub VCN, specify 'peer:&lt;vcn name&gt;' if a VCN needs to be normal peered with some other VCN and specify 'none' in case it is none of these.
+</t>
+  </si>
+  <si>
     <t># subnet names are case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if
 left blank means subnet will use default dhcp options of the vcn.
+dns_label - if specified as n, DNS will not be enabled for the subnet
 vcn_name should be same as enterd in VCNs sheet.
 Initially Route Rules for IGW, NGW and SGW, On Prem and VCN peering for each subnet would be created based on parameter values: configure IGW route, configure NGW route and configure SGW route, configure OnPrem route and configure VCNPeering route respectively for each subnet. The condition is the respective component should have been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
 seclist_names - specify comma seperated names of SLs that needs to be attached to the subnet. If left blank, 1 seclist with name same as subnet name would be attached.  Specify n if you dont
@@ -1467,13 +1476,6 @@
 route_table_name - specify name of route table that needs to be attached to subnet. If left blank, route table with same name as subnet name would be attached. Specify n if you dont
  want any custom route table to be attached to the subnet.
 Subnets in a  VCN can share same route table and seclist depending upon name specified.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars.
-Valid Values for columns E,F,G,H,I:   y|n|&lt;component_name&gt; ie mention 'n' when a component(like IGW) is not required to be configured(like for PHXHub-VCN), specify name of the component- component will be configured with the mentioned name(eg PHX-DRG for the DRG in PHXHub-VCN) and mention 'y' if component needs to be configured with default name ie &lt;vcnname&gt;_ngw(eg PHXNonProd-VCN_ngw)
-Note- For LPGs, specify comma seperated values based on number of LPGs required for each VCN. LPGs will be peered with other VCN LPGs in the order they are specified.
-Note- For column hub_spoke_peer_none - specify 'hub' if the VCN is a hub, specify 'spoke:&lt;hub vcn name&gt;' if VCN is a spoke of a hub VCN, specify 'peer:&lt;vcn name&gt;' if a VCN needs to be normal peered with some other VCN and specify 'none' in case it is none of these.
-</t>
   </si>
 </sst>
 </file>
@@ -1842,11 +1844,23 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1878,19 +1892,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2325,23 +2327,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="32" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>415</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
     </row>
     <row r="2" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -2455,26 +2457,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
@@ -2717,14 +2719,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3247,25 +3249,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>409</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
     </row>
     <row r="2" spans="1:17" s="28" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
@@ -3555,27 +3557,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
     </row>
     <row r="2" spans="1:19" s="17" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
@@ -3718,15 +3720,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="17" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -3752,13 +3754,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="63" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -3775,9 +3777,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="60"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="8" t="s">
         <v>184</v>
       </c>
@@ -3792,9 +3794,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="62"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="60"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="64"/>
       <c r="D5" s="9"/>
       <c r="E5" s="1"/>
       <c r="F5" s="10" t="s">
@@ -3805,9 +3807,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="62"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="60"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="64"/>
       <c r="D6" s="9"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
@@ -3818,108 +3820,108 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="62"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="60"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="64"/>
       <c r="D7" s="11"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="60"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="11"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="62"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="60"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="64"/>
       <c r="D9" s="11"/>
       <c r="E9" s="1"/>
       <c r="F9" s="10"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="62"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="60"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="64"/>
       <c r="D10" s="11"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="62"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="60"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="64"/>
       <c r="D11" s="11"/>
       <c r="E11" s="1"/>
       <c r="F11" s="10"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="62"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="60"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="64"/>
       <c r="D12" s="11"/>
       <c r="E12" s="1"/>
       <c r="F12" s="10"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="62"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="60"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="64"/>
       <c r="D13" s="11"/>
       <c r="E13" s="1"/>
       <c r="F13" s="10"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="62"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="60"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="64"/>
       <c r="D14" s="11"/>
       <c r="E14" s="1"/>
       <c r="F14" s="10"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="62"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="60"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="64"/>
       <c r="D15" s="9"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="60"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="64"/>
       <c r="D16" s="9"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="62"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="60"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="64"/>
       <c r="D17" s="9"/>
       <c r="E17" s="1"/>
       <c r="F17" s="10"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="62"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="61"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="65"/>
       <c r="D18" s="9"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -4521,31 +4523,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="34" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="66"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="69"/>
     </row>
     <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
@@ -4948,31 +4950,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="34" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="68" t="s">
         <v>412</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
       <c r="X1" s="43"/>
     </row>
     <row r="2" spans="1:24" ht="29" x14ac:dyDescent="0.35">
@@ -5263,31 +5265,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="34" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="68" t="s">
         <v>413</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="66"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="69"/>
     </row>
     <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
@@ -5733,7 +5735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
@@ -5752,19 +5754,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="134" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
-        <v>418</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="69"/>
+      <c r="A1" s="53" t="s">
+        <v>417</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -6097,10 +6099,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="192.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="56" t="s">
         <v>395</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="57"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -6314,7 +6316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
@@ -6339,25 +6341,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="151" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
-        <v>417</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
+      <c r="A1" s="58" t="s">
+        <v>418</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
     </row>
     <row r="2" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -6824,15 +6826,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>414</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
     </row>
     <row r="2" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
Support for Non GreenField Tenancies - updated to create DRG without vcn name in TF var and updated policies to refernce comp using var. instead of oci
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="29" r:id="rId1"/>
@@ -1458,14 +1458,6 @@
     <t>seclist_names</t>
   </si>
   <si>
-    <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars.
-dns_label - if specified as n, DNS will not be enabled for the VCN
-Valid Values for columns E,F,G,H,I:   y|n|&lt;component_name&gt; ie mention 'n' when a component(like IGW) is not required to be configured(like for PHXHub-VCN), specify name of the component- component will be configured with the mentioned name(eg PHX-DRG for the DRG in PHXHub-VCN) and mention 'y' if component needs to be configured with default name ie &lt;vcnname&gt;_ngw(eg PHXNonProd-VCN_ngw)
-Note- For LPGs, specify comma seperated values based on number of LPGs required for each VCN. LPGs will be peered with other VCN LPGs in the order they are specified.
-Note- For column hub_spoke_peer_none - specify 'hub' if the VCN is a hub, specify 'spoke:&lt;hub vcn name&gt;' if VCN is a spoke of a hub VCN, specify 'peer:&lt;vcn name&gt;' if a VCN needs to be normal peered with some other VCN and specify 'none' in case it is none of these.
-</t>
-  </si>
-  <si>
     <t># subnet names are case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if
 left blank means subnet will use default dhcp options of the vcn.
 dns_label - if specified as n, DNS will not be enabled for the subnet; Make sure dns_label for VCN is enabled for its subnet DNS to be enabled.
@@ -1476,6 +1468,15 @@
 route_table_name - specify name of route table that needs to be attached to subnet. If left blank, route table with same name as subnet name would be attached. Specify n if you dont
  want any custom route table to be attached to the subnet.
 Subnets in a  VCN can share same route table and seclist depending upon name specified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars.
+dns_label - if specified as n, DNS will not be enabled for the VCN
+Valid Values for columns E,F,G,H,I:   y|n|&lt;component_name&gt; ie mention 'n' when a component(like IGW) is not required to be configured(like for PHXHub-VCN), specify name of the component- component will be configured with the mentioned name(eg PHX-DRG for the DRG in PHXHub-VCN) and mention 'y' if component needs to be configured with default name ie &lt;vcnname&gt;_ngw(eg PHXNonProd-VCN_ngw)
+Note- For DRG, if declaring multiple DRGs for a region, make sure to specify unique names.
+Note- For LPGs, specify comma seperated values based on number of LPGs required for each VCN. LPGs will be peered with other VCN LPGs in the order they are specified.
+Note- For column hub_spoke_peer_none - specify 'hub' if the VCN is a hub, specify 'spoke:&lt;hub vcn name&gt;' if VCN is a spoke of a hub VCN, specify 'peer:&lt;vcn name&gt;' if a VCN needs to be normal peered with some other VCN and specify 'none' in case it is none of these.
+</t>
   </si>
 </sst>
 </file>
@@ -5735,8 +5736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5753,9 +5754,9 @@
     <col min="10" max="10" width="21.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="134" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="145" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="53" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B1" s="54"/>
       <c r="C1" s="54"/>
@@ -6316,7 +6317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
@@ -6342,7 +6343,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>

</xml_diff>

<commit_message>
Support for Non GreenField Tenancies - updated
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="29" r:id="rId1"/>
@@ -1404,12 +1404,6 @@
     <t>SecListName</t>
   </si>
   <si>
-    <t>Automation Toolkit release verion- v5.0
-Tabs Afected: VCNs, VCN Info, DHCP, subnets
-Changes: Addition/Modification of columns
-Removal of 2 sheets: AddSecRules and AddRouteRules</t>
-  </si>
-  <si>
     <t>PHXVCN3</t>
   </si>
   <si>
@@ -1477,6 +1471,11 @@
 Note- For LPGs, specify comma seperated values based on number of LPGs required for each VCN. LPGs will be peered with other VCN LPGs in the order they are specified.
 Note- For column hub_spoke_peer_none - specify 'hub' if the VCN is a hub, specify 'spoke:&lt;hub vcn name&gt;' if VCN is a spoke of a hub VCN, specify 'peer:&lt;vcn name&gt;' if a VCN needs to be normal peered with some other VCN and specify 'none' in case it is none of these.
 </t>
+  </si>
+  <si>
+    <t>Automation Toolkit release verion- v6.0
+Tabs Affected: Subnets
+Major Feature - Support for NonGreenField Tenancies</t>
   </si>
 </sst>
 </file>
@@ -2287,8 +2286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2296,9 +2295,9 @@
     <col min="1" max="1" width="167.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
-        <v>403</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -2329,7 +2328,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="32" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -3251,7 +3250,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -3559,7 +3558,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -4525,7 +4524,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="34" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="68" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -4952,7 +4951,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="34" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="68" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -5267,7 +5266,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="34" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="68" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -5736,7 +5735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -5754,9 +5753,9 @@
     <col min="10" max="10" width="21.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="145" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="53" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B1" s="54"/>
       <c r="C1" s="54"/>
@@ -5898,10 +5897,10 @@
         <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -5946,10 +5945,10 @@
         <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>405</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
@@ -5964,7 +5963,7 @@
         <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>393</v>
@@ -6343,7 +6342,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -6391,7 +6390,7 @@
         <v>206</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>4</v>
@@ -6828,7 +6827,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>

</xml_diff>

<commit_message>
Added support for Flex shape for Instances, Modified Networking for compartment change
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="6" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="29" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="422">
   <si>
     <t>Regional</t>
   </si>
@@ -1213,10 +1213,6 @@
   </si>
   <si>
     <t>Exadata.Full1.336</t>
-  </si>
-  <si>
-    <t>#Template will be picked upon from template folder based on  OS column; Backup Policy column can be left blank at the time of instance creation and can be filled up later on while attaching backup policy to the boot and block volumes together; Pub Address column represents whether public address needs to be assigned to the instance or not(TRUE|FALSE); ssh-key-var-name column accepts the name of variable defined in variables_&lt;region&gt;.tf file containing SSH key to be pushed to the server; NSGs column accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG; Leave DedicatedVMHost column blank if instance doesnt need to be launched on dedicated vm host
-#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
   </si>
   <si>
     <t>ASHHub-VCN_ASHHub-VCN-subnet1</t>
@@ -1477,6 +1473,20 @@
 Tabs Affected: Subnets
 Major Feature - Support for NonGreenField Tenancies</t>
   </si>
+  <si>
+    <t>WindowsLatestFlex</t>
+  </si>
+  <si>
+    <t>VM.Standard.E3.Flex::5</t>
+  </si>
+  <si>
+    <t>LinuxLatestFlex</t>
+  </si>
+  <si>
+    <t>#Template will be picked upon from template folder based on  OS column; Backup Policy column can be left blank at the time of instance creation and can be filled up later on while attaching backup policy to the boot and block volumes together; Pub Address column represents whether public address needs to be assigned to the instance or not(TRUE|FALSE); ssh-key-var-name column accepts the name of variable defined in variables_&lt;region&gt;.tf file containing SSH key to be pushed to the server; NSGs column accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG; Leave DedicatedVMHost column blank if instance doesnt need to be launched on dedicated vm host
+#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
+#If shape is VM.Standard.E3.Flex then specify it as VM.Standard.E3.Flex::ocpus</t>
+  </si>
 </sst>
 </file>
 
@@ -1485,7 +1495,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;**"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1538,6 +1548,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1731,7 +1748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1895,6 +1912,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2297,7 +2315,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -2309,7 +2327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
@@ -2328,7 +2346,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="32" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -2357,7 +2375,7 @@
         <v>99</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>75</v>
@@ -2831,7 +2849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
@@ -2845,7 +2863,7 @@
     <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7265625" customWidth="1"/>
     <col min="10" max="10" width="16.81640625" customWidth="1"/>
     <col min="11" max="11" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
@@ -2855,7 +2873,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="50" t="s">
-        <v>379</v>
+        <v>421</v>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="51"/>
@@ -2929,7 +2947,7 @@
         <v>172</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
@@ -2954,7 +2972,7 @@
       </c>
       <c r="O3" s="21"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>111</v>
       </c>
@@ -2968,7 +2986,7 @@
         <v>173</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
@@ -2977,10 +2995,10 @@
         <v>174</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>176</v>
+        <v>418</v>
+      </c>
+      <c r="I4" s="70" t="s">
+        <v>419</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>9</v>
@@ -3010,7 +3028,7 @@
         <v>172</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
@@ -3040,7 +3058,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>111</v>
       </c>
@@ -3054,7 +3072,7 @@
         <v>173</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>0</v>
@@ -3063,10 +3081,10 @@
         <v>179</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>176</v>
+        <v>420</v>
+      </c>
+      <c r="I6" s="70" t="s">
+        <v>419</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>9</v>
@@ -3253,7 +3271,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -3561,7 +3579,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -4527,7 +4545,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="34" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="68" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -4954,7 +4972,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="34" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="68" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -5269,7 +5287,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="34" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="68" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -5758,7 +5776,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="53" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B1" s="54"/>
       <c r="C1" s="54"/>
@@ -5797,10 +5815,10 @@
         <v>201</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>97</v>
@@ -5870,7 +5888,7 @@
         <v>13</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -5882,10 +5900,10 @@
         <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>389</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -5900,10 +5918,10 @@
         <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -5915,10 +5933,10 @@
         <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
@@ -5933,10 +5951,10 @@
         <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>393</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -5948,10 +5966,10 @@
         <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>404</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
@@ -5966,10 +5984,10 @@
         <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -6037,7 +6055,7 @@
         <v>13</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -6103,7 +6121,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="192.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B1" s="57"/>
     </row>
@@ -6117,7 +6135,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>105</v>
@@ -6345,7 +6363,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -6393,25 +6411,25 @@
         <v>206</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="P2" s="14" t="s">
         <v>399</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>400</v>
       </c>
       <c r="Q2" s="14" t="s">
         <v>97</v>
@@ -6830,7 +6848,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="32" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -6851,7 +6869,7 @@
         <v>99</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Removed extra properties related to OCIC migration from ocswork.properties and created a mew Support for multiple Listeners in LBR
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="6" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="29" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="435">
   <si>
     <t>Regional</t>
   </si>
@@ -795,9 +795,6 @@
     <t>LBR Hostname</t>
   </si>
   <si>
-    <t>my_lbr</t>
-  </si>
-  <si>
     <t>Backend
 Policy(LEAST_CONNECTIONS|ROUND_ROBIN|IP_HASH)</t>
   </si>
@@ -817,9 +814,6 @@
   </si>
   <si>
     <t>400Mbps</t>
-  </si>
-  <si>
-    <t>10.111.1.4:80,Test2:81</t>
   </si>
   <si>
     <t>IP_HASH</t>
@@ -1423,10 +1417,6 @@
 Below sample data shows example of  multiple FSS(FSS1 and FSS2) using single MT(MT1) , 1 FSS(FSS3) using multiple MTs(MT2 and MT3) and also 1 FSS(FSS4) using 1 MT(MT4)</t>
   </si>
   <si>
-    <t>LBR Subnets: specify a single regional subnet name (recommended) or two comma seperated subnet names(AD specific) for public Load Balancer and provide a single subnet(Regional or AD specific) for Private load Balancer- subnets names should be same as defined in Subnets tab, Backend ServerName:Port- specify comma separated list of servernames:ports(either specify server name as same name defined in Instances sheet or specify the IP address); LBR Hostname can be null, all other fields are mandatory; Backend HealthCheck URL is required if Backend HealthCheck Protocol is HTTP; If you want to create an HTTPS Listener, please specify ListenerProtocol as HTTP and UseSSL as y; As of now allows only one BackendSet, One Listener and one Hostname for each LBR
-#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
-  </si>
-  <si>
     <t>#for DB Systems Virtual Machine, fill the sheet with required information, as suggested in 2 row headings | Select shape for Virtual Machine in "F" column and change Node Count accordingly | &lt;end&gt; or &lt;END&gt; is must | Type anything after&lt;end&gt; or &lt;END&gt; for testing.  | If VM DB System node count is "2" then Software edition must be "ENTERPRISE_EDITION_EXTREME_PERFORMANCE"  
 #Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
   </si>
@@ -1486,6 +1476,55 @@
     <t>#Template will be picked upon from template folder based on  OS column; Backup Policy column can be left blank at the time of instance creation and can be filled up later on while attaching backup policy to the boot and block volumes together; Pub Address column represents whether public address needs to be assigned to the instance or not(TRUE|FALSE); ssh-key-var-name column accepts the name of variable defined in variables_&lt;region&gt;.tf file containing SSH key to be pushed to the server; NSGs column accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG; Leave DedicatedVMHost column blank if instance doesnt need to be launched on dedicated vm host
 #Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
 #If shape is VM.Standard.E3.Flex then specify it as VM.Standard.E3.Flex::ocpus</t>
+  </si>
+  <si>
+    <t>ListenerName</t>
+  </si>
+  <si>
+    <t>listenr1</t>
+  </si>
+  <si>
+    <t>listenr2</t>
+  </si>
+  <si>
+    <t>my_lbr1</t>
+  </si>
+  <si>
+    <t>my_lbr2</t>
+  </si>
+  <si>
+    <t>100Mbps</t>
+  </si>
+  <si>
+    <t>PHXNonProd-VCN_qa-subnet</t>
+  </si>
+  <si>
+    <t>10.111.1.5:80,Test2:81</t>
+  </si>
+  <si>
+    <t>10.111.1.4:80,Test1:81</t>
+  </si>
+  <si>
+    <t>10.111.1.6:80</t>
+  </si>
+  <si>
+    <t>listenr</t>
+  </si>
+  <si>
+    <t>ROUND_ROBIN</t>
+  </si>
+  <si>
+    <t>TCP</t>
+  </si>
+  <si>
+    <t>app1.example.com</t>
+  </si>
+  <si>
+    <t>app2.example.com,app3.example.com</t>
+  </si>
+  <si>
+    <t>LBR Subnets: specify a single regional subnet name (recommended) or two comma seperated subnet names(AD specific) for public Load Balancer and provide a single subnet(Regional or AD specific) for Private load Balancer- subnets names should be same as defined in Subnets tab, Backend ServerName:Port- specify comma separated list of servernames:ports(either specify server name as same name defined in Instances sheet or specify the IP address); LBR Hostname can be null, all other fields are mandatory; Backend HealthCheck URL is required if Backend HealthCheck Protocol is HTTP; If you want to create an HTTPS Listener, please specify ListenerProtocol as HTTP and UseSSL as y; Allows multiple Listeners(seperate rows) per LBR and multiple Hostnames(comma seperated) per Listener
+#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
   </si>
 </sst>
 </file>
@@ -1846,6 +1885,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1912,7 +1952,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2315,7 +2354,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -2345,24 +2384,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="32" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
-        <v>413</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
+      <c r="A1" s="60" t="s">
+        <v>410</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
     </row>
     <row r="2" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -2375,7 +2414,7 @@
         <v>99</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>75</v>
@@ -2411,7 +2450,7 @@
         <v>85</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
@@ -2478,26 +2517,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
@@ -2552,7 +2591,7 @@
         <v>85</v>
       </c>
       <c r="R2" s="42" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -2592,7 +2631,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -2740,14 +2779,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -2849,7 +2888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
@@ -2872,22 +2911,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
-        <v>421</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="52"/>
+      <c r="A1" s="51" t="s">
+        <v>418</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="53"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -2947,7 +2986,7 @@
         <v>172</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
@@ -2986,7 +3025,7 @@
         <v>173</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
@@ -2995,10 +3034,10 @@
         <v>174</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="I4" s="70" t="s">
-        <v>419</v>
+        <v>415</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>416</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>9</v>
@@ -3028,7 +3067,7 @@
         <v>172</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
@@ -3072,7 +3111,7 @@
         <v>173</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>0</v>
@@ -3081,10 +3120,10 @@
         <v>179</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="I6" s="70" t="s">
-        <v>419</v>
+        <v>417</v>
+      </c>
+      <c r="I6" s="48" t="s">
+        <v>416</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>9</v>
@@ -3128,16 +3167,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="17" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3270,25 +3309,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
-        <v>407</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
+      <c r="A1" s="60" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
     </row>
     <row r="2" spans="1:17" s="28" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
@@ -3348,7 +3387,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>214</v>
@@ -3357,7 +3396,7 @@
         <v>235</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -3367,7 +3406,7 @@
         <v>234</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -3381,7 +3420,7 @@
         <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>214</v>
@@ -3390,17 +3429,17 @@
         <v>235</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -3414,32 +3453,32 @@
         <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -3451,32 +3490,32 @@
         <v>110</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>330</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -3488,26 +3527,26 @@
         <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -3548,10 +3587,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:S1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3560,47 +3599,49 @@
     <col min="2" max="2" width="12.54296875" style="17" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" style="17"/>
     <col min="4" max="4" width="12.1796875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="19.26953125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" style="28" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.54296875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.90625" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.08984375" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" style="17" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" style="17" customWidth="1"/>
-    <col min="11" max="11" width="13.54296875" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.08984375" style="17" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" style="17"/>
-    <col min="14" max="14" width="15.81640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.26953125" style="17" customWidth="1"/>
-    <col min="16" max="16" width="14.6328125" style="17" customWidth="1"/>
-    <col min="17" max="17" width="8.7265625" style="17"/>
-    <col min="18" max="18" width="11.36328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.36328125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="19.54296875" style="32" customWidth="1"/>
+    <col min="8" max="8" width="19.90625" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.26953125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="12.1796875" style="17" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.08984375" style="17" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="17"/>
+    <col min="15" max="15" width="15.81640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.26953125" style="17" customWidth="1"/>
+    <col min="17" max="17" width="14.6328125" style="17" customWidth="1"/>
+    <col min="18" max="18" width="8.7265625" style="17"/>
+    <col min="19" max="19" width="11.36328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.36328125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
-        <v>408</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-    </row>
-    <row r="2" spans="1:19" s="17" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="60" t="s">
+        <v>434</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+    </row>
+    <row r="2" spans="1:20" s="17" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
         <v>109</v>
       </c>
@@ -3611,112 +3652,228 @@
         <v>237</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>247</v>
-      </c>
-      <c r="E2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>238</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="H2" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="H2" s="29" t="s">
-        <v>245</v>
-      </c>
       <c r="I2" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="L2" s="29" t="s">
         <v>248</v>
       </c>
-      <c r="J2" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>319</v>
-      </c>
       <c r="M2" s="29" t="s">
+        <v>317</v>
+      </c>
+      <c r="N2" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="P2" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q2" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="R2" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="P2" s="30" t="s">
+      <c r="S2" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="Q2" s="30" t="s">
+      <c r="T2" s="30" t="s">
         <v>257</v>
       </c>
-      <c r="R2" s="30" t="s">
-        <v>258</v>
-      </c>
-      <c r="S2" s="30" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:20" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>244</v>
+        <v>422</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>151</v>
+        <v>249</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>379</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K3" s="1">
+        <v>80</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="N3" s="1">
+        <v>443</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" s="32" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="F4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K4" s="1">
+        <v>80</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="N4" s="1">
+        <v>443</v>
+      </c>
+      <c r="O4" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" s="32" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>425</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="K5" s="1">
+        <v>80</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="N5" s="1">
+        <v>80</v>
+      </c>
+      <c r="O5" s="29" t="s">
         <v>252</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="J3" s="1">
-        <v>80</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="M3" s="1">
-        <v>443</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" s="29" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="S3" s="1"/>
+      <c r="P5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3741,15 +3898,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="17" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -3775,13 +3932,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="64" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -3798,9 +3955,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="66"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="64"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="8" t="s">
         <v>184</v>
       </c>
@@ -3815,9 +3972,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="66"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="64"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="65"/>
       <c r="D5" s="9"/>
       <c r="E5" s="1"/>
       <c r="F5" s="10" t="s">
@@ -3828,9 +3985,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="66"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="64"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="9"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
@@ -3841,108 +3998,108 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="66"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="64"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="65"/>
       <c r="D7" s="11"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="66"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="64"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="65"/>
       <c r="D8" s="11"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="66"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="64"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="65"/>
       <c r="D9" s="11"/>
       <c r="E9" s="1"/>
       <c r="F9" s="10"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="66"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="64"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="65"/>
       <c r="D10" s="11"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="66"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="64"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="11"/>
       <c r="E11" s="1"/>
       <c r="F11" s="10"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="66"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="64"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="65"/>
       <c r="D12" s="11"/>
       <c r="E12" s="1"/>
       <c r="F12" s="10"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="66"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="64"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="65"/>
       <c r="D13" s="11"/>
       <c r="E13" s="1"/>
       <c r="F13" s="10"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="64"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="65"/>
       <c r="D14" s="11"/>
       <c r="E14" s="1"/>
       <c r="F14" s="10"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="66"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="64"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="65"/>
       <c r="D15" s="9"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="66"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="64"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="65"/>
       <c r="D16" s="9"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="66"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="64"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="65"/>
       <c r="D17" s="9"/>
       <c r="E17" s="1"/>
       <c r="F17" s="10"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="66"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="65"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="66"/>
       <c r="D18" s="9"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -3979,14 +4136,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -4075,14 +4232,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -4169,12 +4326,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="50"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -4305,16 +4462,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
-        <v>320</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="52"/>
+      <c r="A1" s="51" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="46" t="s">
@@ -4324,22 +4481,22 @@
         <v>69</v>
       </c>
       <c r="C2" s="46" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="E2" s="47" t="s">
         <v>263</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="F2" s="46" t="s">
         <v>264</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="G2" s="46" t="s">
         <v>265</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="H2" s="46" t="s">
         <v>266</v>
-      </c>
-      <c r="G2" s="46" t="s">
-        <v>267</v>
-      </c>
-      <c r="H2" s="46" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -4347,16 +4504,16 @@
         <v>110</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C3" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="E3" s="33" t="s">
         <v>269</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>270</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>271</v>
       </c>
       <c r="F3" s="32">
         <v>1</v>
@@ -4365,7 +4522,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -4373,16 +4530,16 @@
         <v>110</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F4" s="32">
         <v>1</v>
@@ -4391,7 +4548,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -4399,16 +4556,16 @@
         <v>111</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F5" s="32">
         <v>1</v>
@@ -4417,7 +4574,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -4425,16 +4582,16 @@
         <v>111</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F6" s="32">
         <v>1</v>
@@ -4443,24 +4600,24 @@
         <v>1</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F7" s="32">
         <v>1</v>
@@ -4469,24 +4626,24 @@
         <v>1</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F8" s="32">
         <v>1</v>
@@ -4495,7 +4652,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -4544,31 +4701,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="34" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="68" t="s">
-        <v>409</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="69"/>
+      <c r="A1" s="69" t="s">
+        <v>406</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="70"/>
     </row>
     <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
@@ -4578,67 +4735,67 @@
         <v>69</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D2" s="35" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F2" s="35" t="s">
         <v>46</v>
       </c>
       <c r="G2" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="I2" s="35" t="s">
         <v>287</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="J2" s="35" t="s">
         <v>288</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="K2" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="L2" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="M2" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="N2" s="35" t="s">
         <v>292</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="O2" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="P2" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="Q2" s="35" t="s">
         <v>295</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="R2" s="35" t="s">
         <v>296</v>
       </c>
-      <c r="Q2" s="35" t="s">
+      <c r="S2" s="35" t="s">
         <v>297</v>
       </c>
-      <c r="R2" s="35" t="s">
-        <v>298</v>
-      </c>
-      <c r="S2" s="35" t="s">
-        <v>299</v>
-      </c>
       <c r="T2" s="39" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="U2" s="35" t="s">
+        <v>340</v>
+      </c>
+      <c r="V2" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="W2" s="35" t="s">
         <v>342</v>
-      </c>
-      <c r="V2" s="35" t="s">
-        <v>343</v>
-      </c>
-      <c r="W2" s="35" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
@@ -4646,67 +4803,67 @@
         <v>110</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G3" s="40">
         <v>1</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I3" s="40">
         <v>256</v>
       </c>
       <c r="J3" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="K3" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="L3" s="40" t="s">
         <v>301</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="M3" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="N3" s="40" t="s">
         <v>303</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="O3" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="P3" s="40" t="s">
         <v>305</v>
       </c>
-      <c r="O3" s="40" t="s">
+      <c r="Q3" s="40" t="s">
         <v>306</v>
       </c>
-      <c r="P3" s="40" t="s">
+      <c r="R3" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="Q3" s="40" t="s">
+      <c r="S3" s="40" t="s">
         <v>308</v>
-      </c>
-      <c r="R3" s="40" t="s">
-        <v>309</v>
-      </c>
-      <c r="S3" s="40" t="s">
-        <v>310</v>
       </c>
       <c r="T3" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -4717,16 +4874,16 @@
         <v>110</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F4" s="40" t="s">
         <v>176</v>
@@ -4735,49 +4892,49 @@
         <v>2</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I4" s="40">
         <v>256</v>
       </c>
       <c r="J4" s="40" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K4" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="L4" s="40" t="s">
+        <v>348</v>
+      </c>
+      <c r="M4" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="L4" s="40" t="s">
-        <v>350</v>
-      </c>
-      <c r="M4" s="40" t="s">
+      <c r="N4" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="O4" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="N4" s="40" t="s">
+      <c r="P4" s="40" t="s">
         <v>305</v>
       </c>
-      <c r="O4" s="40" t="s">
+      <c r="Q4" s="40" t="s">
         <v>306</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="R4" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="Q4" s="40" t="s">
+      <c r="S4" s="40" t="s">
         <v>308</v>
-      </c>
-      <c r="R4" s="40" t="s">
-        <v>309</v>
-      </c>
-      <c r="S4" s="40" t="s">
-        <v>310</v>
       </c>
       <c r="T4" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W4" s="1">
         <v>15</v>
@@ -4788,16 +4945,16 @@
         <v>110</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F5" s="40" t="s">
         <v>176</v>
@@ -4806,49 +4963,49 @@
         <v>2</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I5" s="40">
         <v>256</v>
       </c>
       <c r="J5" s="40" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K5" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="L5" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="M5" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="L5" s="40" t="s">
-        <v>352</v>
-      </c>
-      <c r="M5" s="40" t="s">
+      <c r="N5" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="O5" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="N5" s="40" t="s">
+      <c r="P5" s="40" t="s">
         <v>305</v>
       </c>
-      <c r="O5" s="40" t="s">
+      <c r="Q5" s="40" t="s">
         <v>306</v>
       </c>
-      <c r="P5" s="40" t="s">
+      <c r="R5" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="Q5" s="40" t="s">
+      <c r="S5" s="40" t="s">
         <v>308</v>
-      </c>
-      <c r="R5" s="40" t="s">
-        <v>309</v>
-      </c>
-      <c r="S5" s="40" t="s">
-        <v>310</v>
       </c>
       <c r="T5" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W5" s="1">
         <v>20</v>
@@ -4862,22 +5019,22 @@
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y397" s="44" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="399" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y399" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="400" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y400" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="401" spans="25:25" x14ac:dyDescent="0.35">
@@ -4887,37 +5044,37 @@
     </row>
     <row r="402" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y402" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="403" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y403" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="404" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y404" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="405" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y405" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="406" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y406" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="407" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y407" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="408" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y408" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -4971,31 +5128,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="34" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="68" t="s">
-        <v>410</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
+      <c r="A1" s="69" t="s">
+        <v>407</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
       <c r="X1" s="43"/>
     </row>
     <row r="2" spans="1:24" ht="29" x14ac:dyDescent="0.35">
@@ -5006,67 +5163,67 @@
         <v>69</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D2" s="35" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F2" s="35" t="s">
         <v>46</v>
       </c>
       <c r="G2" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="H2" s="35" t="s">
         <v>286</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="I2" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="J2" s="35" t="s">
         <v>288</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="K2" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="L2" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="M2" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="N2" s="35" t="s">
         <v>292</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="O2" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="P2" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="Q2" s="35" t="s">
         <v>295</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="R2" s="35" t="s">
         <v>296</v>
       </c>
-      <c r="Q2" s="35" t="s">
+      <c r="S2" s="35" t="s">
         <v>297</v>
       </c>
-      <c r="R2" s="35" t="s">
-        <v>298</v>
-      </c>
-      <c r="S2" s="35" t="s">
-        <v>299</v>
-      </c>
       <c r="T2" s="39" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="U2" s="35" t="s">
+        <v>340</v>
+      </c>
+      <c r="V2" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="W2" s="35" t="s">
         <v>342</v>
-      </c>
-      <c r="V2" s="35" t="s">
-        <v>343</v>
-      </c>
-      <c r="W2" s="35" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
@@ -5074,67 +5231,67 @@
         <v>110</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>214</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G3" s="40">
         <v>2</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I3" s="40">
         <v>256</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K3" s="40" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="L3" s="40" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="M3" s="40" t="s">
+        <v>310</v>
+      </c>
+      <c r="N3" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="O3" s="40" t="s">
+        <v>311</v>
+      </c>
+      <c r="P3" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q3" s="40" t="s">
+        <v>306</v>
+      </c>
+      <c r="R3" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="N3" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="O3" s="40" t="s">
+      <c r="S3" s="40" t="s">
         <v>313</v>
-      </c>
-      <c r="P3" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="Q3" s="40" t="s">
-        <v>308</v>
-      </c>
-      <c r="R3" s="40" t="s">
-        <v>314</v>
-      </c>
-      <c r="S3" s="40" t="s">
-        <v>315</v>
       </c>
       <c r="T3" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -5145,67 +5302,67 @@
         <v>111</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G4" s="40">
         <v>2</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I4" s="40">
         <v>256</v>
       </c>
       <c r="J4" s="40" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K4" s="40" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="L4" s="40" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="M4" s="40" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N4" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="O4" s="40" t="s">
+        <v>316</v>
+      </c>
+      <c r="P4" s="40" t="s">
         <v>305</v>
       </c>
-      <c r="O4" s="40" t="s">
-        <v>318</v>
-      </c>
-      <c r="P4" s="40" t="s">
+      <c r="Q4" s="40" t="s">
+        <v>306</v>
+      </c>
+      <c r="R4" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="Q4" s="40" t="s">
-        <v>308</v>
-      </c>
-      <c r="R4" s="40" t="s">
-        <v>309</v>
-      </c>
       <c r="S4" s="40" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="T4" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W4" s="1">
         <v>15</v>
@@ -5219,17 +5376,17 @@
     </row>
     <row r="396" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y396" s="44" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y397" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -5286,31 +5443,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="34" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="68" t="s">
-        <v>411</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="69"/>
+      <c r="A1" s="69" t="s">
+        <v>408</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="70"/>
     </row>
     <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
@@ -5320,67 +5477,67 @@
         <v>69</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D2" s="35" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>46</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I2" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>288</v>
+      </c>
+      <c r="K2" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="L2" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="M2" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="N2" s="35" t="s">
         <v>292</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="O2" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="P2" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="Q2" s="35" t="s">
         <v>295</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="R2" s="35" t="s">
         <v>296</v>
       </c>
-      <c r="Q2" s="35" t="s">
+      <c r="S2" s="35" t="s">
         <v>297</v>
       </c>
-      <c r="R2" s="35" t="s">
-        <v>298</v>
-      </c>
-      <c r="S2" s="35" t="s">
-        <v>299</v>
-      </c>
       <c r="T2" s="39" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="U2" s="35" t="s">
+        <v>340</v>
+      </c>
+      <c r="V2" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="W2" s="35" t="s">
         <v>342</v>
-      </c>
-      <c r="V2" s="35" t="s">
-        <v>343</v>
-      </c>
-      <c r="W2" s="35" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
@@ -5388,22 +5545,22 @@
         <v>110</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H3" s="40">
         <v>2</v>
@@ -5412,43 +5569,43 @@
         <v>256</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K3" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>369</v>
+      </c>
+      <c r="M3" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="L3" s="40" t="s">
-        <v>371</v>
-      </c>
-      <c r="M3" s="40" t="s">
+      <c r="N3" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="O3" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="P3" s="40" t="s">
         <v>305</v>
       </c>
-      <c r="O3" s="40" t="s">
+      <c r="Q3" s="40" t="s">
         <v>306</v>
       </c>
-      <c r="P3" s="40" t="s">
+      <c r="R3" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="Q3" s="40" t="s">
+      <c r="S3" s="40" t="s">
         <v>308</v>
-      </c>
-      <c r="R3" s="40" t="s">
-        <v>309</v>
-      </c>
-      <c r="S3" s="40" t="s">
-        <v>310</v>
       </c>
       <c r="T3" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -5462,42 +5619,42 @@
     </row>
     <row r="395" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y395" s="44" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="396" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y396" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y397" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="399" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y399" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="400" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y400" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="401" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y401" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="402" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y402" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -5533,11 +5690,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="50"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -5625,15 +5782,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="53"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
@@ -5775,19 +5932,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
-        <v>416</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="55"/>
+      <c r="A1" s="54" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="56"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -5815,10 +5972,10 @@
         <v>201</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>97</v>
@@ -5888,7 +6045,7 @@
         <v>13</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -5900,10 +6057,10 @@
         <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -5918,10 +6075,10 @@
         <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -5933,10 +6090,10 @@
         <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
@@ -5951,10 +6108,10 @@
         <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -5966,10 +6123,10 @@
         <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
@@ -5984,10 +6141,10 @@
         <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -6055,7 +6212,7 @@
         <v>13</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -6120,10 +6277,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="192.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
-        <v>394</v>
-      </c>
-      <c r="B1" s="57"/>
+      <c r="A1" s="57" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" s="58"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -6135,7 +6292,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>105</v>
@@ -6152,7 +6309,7 @@
         <v>107</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.35">
@@ -6200,15 +6357,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -6338,7 +6495,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6362,25 +6519,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
-        <v>415</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
+      <c r="A1" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
     </row>
     <row r="2" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -6411,25 +6568,25 @@
         <v>206</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="14" t="s">
         <v>396</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="14" t="s">
         <v>397</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>398</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>399</v>
       </c>
       <c r="Q2" s="14" t="s">
         <v>97</v>
@@ -6847,16 +7004,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="32" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
-        <v>412</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
+      <c r="A1" s="60" t="s">
+        <v>409</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
     </row>
     <row r="2" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
@@ -6869,7 +7026,7 @@
         <v>99</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>72</v>
@@ -6881,7 +7038,7 @@
         <v>74</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>

</xml_diff>

<commit_message>
Removed extra properties related to OCIC migration from ocswork.properties and created a mew modified image ocid variable names and template names (removed latest)
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="29" r:id="rId1"/>
@@ -341,9 +341,6 @@
     <t>VolumeName</t>
   </si>
   <si>
-    <t>WindowsLatest</t>
-  </si>
-  <si>
     <t>dns_label</t>
   </si>
   <si>
@@ -418,10 +415,6 @@
 Enter Region as your tenancy's Home Region for Group Creation</t>
   </si>
   <si>
-    <t># Horizontal row specifies the TagNameSpace Names to be created; Vertical row under each TagNameSpace represnts Keys in that tagnamespace; Enter compartment name in which  all tagnamespaces and keys will be created;
-Enter Region as your tenancy's Home Region for Tags Creation</t>
-  </si>
-  <si>
     <t>$ and * in PolicyStatements would be replaced by PolicyStatementGroup and PolicyStatementCompartment respectively;If Compartment Name is left empty or mentioned 'root', policy will be created in root compartment;
 # Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
 Enter Region as your tenancy's Home Region for Policy Creation</t>
@@ -590,9 +583,6 @@
   </si>
   <si>
     <t>VM.Standard2.8</t>
-  </si>
-  <si>
-    <t>LinuxLatest</t>
   </si>
   <si>
     <t>10.219.1.1</t>
@@ -1464,13 +1454,7 @@
 Major Feature - Support for NonGreenField Tenancies</t>
   </si>
   <si>
-    <t>WindowsLatestFlex</t>
-  </si>
-  <si>
     <t>VM.Standard.E3.Flex::5</t>
-  </si>
-  <si>
-    <t>LinuxLatestFlex</t>
   </si>
   <si>
     <t>#Template will be picked upon from template folder based on  OS column; Backup Policy column can be left blank at the time of instance creation and can be filled up later on while attaching backup policy to the boot and block volumes together; Pub Address column represents whether public address needs to be assigned to the instance or not(TRUE|FALSE); ssh-key-var-name column accepts the name of variable defined in variables_&lt;region&gt;.tf file containing SSH key to be pushed to the server; NSGs column accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG; Leave DedicatedVMHost column blank if instance doesnt need to be launched on dedicated vm host
@@ -1525,6 +1509,22 @@
   <si>
     <t>LBR Subnets: specify a single regional subnet name (recommended) or two comma seperated subnet names(AD specific) for public Load Balancer and provide a single subnet(Regional or AD specific) for Private load Balancer- subnets names should be same as defined in Subnets tab, Backend ServerName:Port- specify comma separated list of servernames:ports(either specify server name as same name defined in Instances sheet or specify the IP address); LBR Hostname can be null, all other fields are mandatory; Backend HealthCheck URL is required if Backend HealthCheck Protocol is HTTP; If you want to create an HTTPS Listener, please specify ListenerProtocol as HTTP and UseSSL as y; Allows multiple Listeners(seperate rows) per LBR and multiple Hostnames(comma seperated) per Listener
 #Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>LinuxFlex</t>
+  </si>
+  <si>
+    <t>WindowsFlex</t>
+  </si>
+  <si>
+    <t># Horizontal row specifies the TagNameSpace Names to be created; Vertical column under each TagNameSpace represnts Keys in that tagnamespace; Enter compartment name in which  all tagnamespaces and keys will be created;
+Enter Region as your tenancy's Home Region for Tags Creation</t>
   </si>
 </sst>
 </file>
@@ -2343,7 +2343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -2354,7 +2354,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -2385,7 +2385,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="32" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -2405,16 +2405,16 @@
     </row>
     <row r="2" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>75</v>
@@ -2450,7 +2450,7 @@
         <v>85</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
@@ -2518,7 +2518,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="61" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -2540,19 +2540,19 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>76</v>
@@ -2561,13 +2561,13 @@
         <v>77</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I2" s="25" t="s">
         <v>78</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>81</v>
@@ -2591,38 +2591,38 @@
         <v>85</v>
       </c>
       <c r="R2" s="42" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="26"/>
       <c r="J3" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2631,21 +2631,21 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>86</v>
@@ -2654,13 +2654,13 @@
         <v>87</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -2678,7 +2678,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>51</v>
@@ -2687,22 +2687,22 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K5" s="26" t="s">
         <v>129</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>131</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2711,12 +2711,12 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>51</v>
@@ -2725,22 +2725,22 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="I6" s="26" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -2780,7 +2780,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>69</v>
@@ -2810,40 +2810,40 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -2858,22 +2858,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2889,7 +2889,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2912,7 +2912,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -2930,7 +2930,7 @@
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>40</v>
@@ -2966,45 +2966,45 @@
         <v>91</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>96</v>
+        <v>430</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>92</v>
@@ -3013,129 +3013,129 @@
     </row>
     <row r="4" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
       <c r="I4" s="48" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>92</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>177</v>
+        <v>431</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>92</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>417</v>
+        <v>432</v>
       </c>
       <c r="I6" s="48" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>92</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N6" s="1"/>
     </row>
@@ -3168,7 +3168,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="17" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>20</v>
@@ -3206,10 +3206,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C3" s="1">
         <v>150</v>
@@ -3218,13 +3218,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>92</v>
@@ -3232,10 +3232,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C4" s="1">
         <v>150</v>
@@ -3244,13 +3244,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>92</v>
@@ -3310,7 +3310,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B1" s="63"/>
       <c r="C1" s="63"/>
@@ -3331,82 +3331,82 @@
     </row>
     <row r="2" spans="1:17" s="28" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="N2" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>236</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>222</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>233</v>
-      </c>
-      <c r="I2" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="K2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="P2" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="M2" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="O2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
         <v>228</v>
-      </c>
-      <c r="P2" s="29" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q2" s="29" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -3417,29 +3417,29 @@
     </row>
     <row r="4" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -3450,35 +3450,35 @@
     </row>
     <row r="5" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -3487,35 +3487,35 @@
     </row>
     <row r="6" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>328</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -3524,29 +3524,29 @@
     </row>
     <row r="7" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -3589,7 +3589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
@@ -3619,7 +3619,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -3643,225 +3643,225 @@
     </row>
     <row r="2" spans="1:20" s="17" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="K2" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="I2" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>247</v>
-      </c>
-      <c r="K2" s="29" t="s">
+      <c r="L2" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="O2" s="29" t="s">
         <v>240</v>
       </c>
-      <c r="L2" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>317</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>239</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>243</v>
-      </c>
       <c r="P2" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q2" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="R2" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="S2" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="Q2" s="30" t="s">
+      <c r="T2" s="30" t="s">
         <v>254</v>
-      </c>
-      <c r="R2" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="S2" s="30" t="s">
-        <v>256</v>
-      </c>
-      <c r="T2" s="30" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="K3" s="1">
         <v>80</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N3" s="1">
         <v>443</v>
       </c>
       <c r="O3" s="29" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="Q3" s="29" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" s="32" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>426</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="K4" s="1">
         <v>80</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N4" s="1">
         <v>443</v>
       </c>
       <c r="O4" s="29" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="Q4" s="29" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="T4" s="1"/>
     </row>
     <row r="5" spans="1:20" s="32" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="K5" s="1">
         <v>80</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="N5" s="1">
         <v>80</v>
       </c>
       <c r="O5" s="29" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>14</v>
@@ -3899,7 +3899,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="17" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="68" t="s">
-        <v>120</v>
+        <v>434</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="68"/>
@@ -3910,7 +3910,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>88</v>
@@ -3933,7 +3933,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="67" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="67" t="s">
         <v>51</v>
@@ -3942,7 +3942,7 @@
         <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>34</v>
@@ -3959,7 +3959,7 @@
       <c r="B4" s="67"/>
       <c r="C4" s="65"/>
       <c r="D4" s="8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>37</v>
@@ -4137,7 +4137,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -4147,7 +4147,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>40</v>
@@ -4167,39 +4167,39 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>94</v>
@@ -4233,7 +4233,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="17" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -4243,7 +4243,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>95</v>
@@ -4263,39 +4263,39 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>94</v>
@@ -4327,7 +4327,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -4335,7 +4335,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>48</v>
@@ -4349,7 +4349,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>51</v>
@@ -4361,56 +4361,56 @@
     </row>
     <row r="4" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -4463,7 +4463,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -4475,45 +4475,45 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="46" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="G2" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="H2" s="46" t="s">
         <v>263</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>264</v>
-      </c>
-      <c r="G2" s="46" t="s">
-        <v>265</v>
-      </c>
-      <c r="H2" s="46" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F3" s="32">
         <v>1</v>
@@ -4522,24 +4522,24 @@
         <v>1</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F4" s="32">
         <v>1</v>
@@ -4548,24 +4548,24 @@
         <v>1</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F5" s="32">
         <v>1</v>
@@ -4574,24 +4574,24 @@
         <v>1</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F6" s="32">
         <v>1</v>
@@ -4600,24 +4600,24 @@
         <v>1</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F7" s="32">
         <v>1</v>
@@ -4626,24 +4626,24 @@
         <v>1</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F8" s="32">
         <v>1</v>
@@ -4652,7 +4652,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -4702,7 +4702,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="34" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="69" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -4729,141 +4729,141 @@
     </row>
     <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D2" s="35" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F2" s="35" t="s">
         <v>46</v>
       </c>
       <c r="G2" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2" s="35" t="s">
         <v>285</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="K2" s="38" t="s">
         <v>286</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="L2" s="35" t="s">
         <v>287</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="M2" s="35" t="s">
         <v>288</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="N2" s="35" t="s">
         <v>289</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="O2" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="P2" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="Q2" s="35" t="s">
         <v>292</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="R2" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="S2" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="Q2" s="35" t="s">
-        <v>295</v>
-      </c>
-      <c r="R2" s="35" t="s">
-        <v>296</v>
-      </c>
-      <c r="S2" s="35" t="s">
-        <v>297</v>
-      </c>
       <c r="T2" s="39" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="V2" s="35" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="W2" s="35" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G3" s="40">
         <v>1</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I3" s="40">
         <v>256</v>
       </c>
       <c r="J3" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="K3" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>298</v>
+      </c>
+      <c r="M3" s="40" t="s">
         <v>299</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="N3" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="O3" s="40" t="s">
         <v>301</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="P3" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="Q3" s="40" t="s">
         <v>303</v>
       </c>
-      <c r="O3" s="40" t="s">
+      <c r="R3" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="P3" s="40" t="s">
+      <c r="S3" s="40" t="s">
         <v>305</v>
-      </c>
-      <c r="Q3" s="40" t="s">
-        <v>306</v>
-      </c>
-      <c r="R3" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="S3" s="40" t="s">
-        <v>308</v>
       </c>
       <c r="T3" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -4871,70 +4871,70 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G4" s="40">
         <v>2</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I4" s="40">
         <v>256</v>
       </c>
       <c r="J4" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="K4" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="L4" s="40" t="s">
+        <v>345</v>
+      </c>
+      <c r="M4" s="40" t="s">
         <v>299</v>
       </c>
-      <c r="K4" s="40" t="s">
+      <c r="N4" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="L4" s="40" t="s">
-        <v>348</v>
-      </c>
-      <c r="M4" s="40" t="s">
+      <c r="O4" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="P4" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="N4" s="40" t="s">
+      <c r="Q4" s="40" t="s">
         <v>303</v>
       </c>
-      <c r="O4" s="40" t="s">
+      <c r="R4" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="S4" s="40" t="s">
         <v>305</v>
-      </c>
-      <c r="Q4" s="40" t="s">
-        <v>306</v>
-      </c>
-      <c r="R4" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="S4" s="40" t="s">
-        <v>308</v>
       </c>
       <c r="T4" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="W4" s="1">
         <v>15</v>
@@ -4942,70 +4942,70 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G5" s="40">
         <v>2</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I5" s="40">
         <v>256</v>
       </c>
       <c r="J5" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="K5" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="L5" s="40" t="s">
+        <v>347</v>
+      </c>
+      <c r="M5" s="40" t="s">
         <v>299</v>
       </c>
-      <c r="K5" s="40" t="s">
+      <c r="N5" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="L5" s="40" t="s">
-        <v>350</v>
-      </c>
-      <c r="M5" s="40" t="s">
+      <c r="O5" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="P5" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="N5" s="40" t="s">
+      <c r="Q5" s="40" t="s">
         <v>303</v>
       </c>
-      <c r="O5" s="40" t="s">
+      <c r="R5" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="P5" s="40" t="s">
+      <c r="S5" s="40" t="s">
         <v>305</v>
-      </c>
-      <c r="Q5" s="40" t="s">
-        <v>306</v>
-      </c>
-      <c r="R5" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="S5" s="40" t="s">
-        <v>308</v>
       </c>
       <c r="T5" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="W5" s="1">
         <v>20</v>
@@ -5019,62 +5019,62 @@
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y397" s="44" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="399" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y399" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="400" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y400" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="401" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y401" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="402" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y402" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="403" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y403" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="404" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y404" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="405" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y405" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="406" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y406" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="407" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y407" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="408" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y408" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -5129,7 +5129,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="34" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="69" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -5157,141 +5157,141 @@
     </row>
     <row r="2" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D2" s="35" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F2" s="35" t="s">
         <v>46</v>
       </c>
       <c r="G2" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="I2" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="J2" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="K2" s="38" t="s">
         <v>286</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="L2" s="35" t="s">
         <v>287</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="M2" s="35" t="s">
         <v>288</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="N2" s="35" t="s">
         <v>289</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="O2" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="P2" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="Q2" s="35" t="s">
         <v>292</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="R2" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="S2" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="Q2" s="35" t="s">
-        <v>295</v>
-      </c>
-      <c r="R2" s="35" t="s">
-        <v>296</v>
-      </c>
-      <c r="S2" s="35" t="s">
-        <v>297</v>
-      </c>
       <c r="T2" s="39" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="V2" s="35" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="W2" s="35" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G3" s="40">
         <v>2</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="I3" s="40">
         <v>256</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="K3" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>362</v>
+      </c>
+      <c r="M3" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="N3" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="L3" s="40" t="s">
-        <v>365</v>
-      </c>
-      <c r="M3" s="40" t="s">
+      <c r="O3" s="40" t="s">
+        <v>308</v>
+      </c>
+      <c r="P3" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q3" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="R3" s="40" t="s">
+        <v>309</v>
+      </c>
+      <c r="S3" s="40" t="s">
         <v>310</v>
-      </c>
-      <c r="N3" s="40" t="s">
-        <v>303</v>
-      </c>
-      <c r="O3" s="40" t="s">
-        <v>311</v>
-      </c>
-      <c r="P3" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q3" s="40" t="s">
-        <v>306</v>
-      </c>
-      <c r="R3" s="40" t="s">
-        <v>312</v>
-      </c>
-      <c r="S3" s="40" t="s">
-        <v>313</v>
       </c>
       <c r="T3" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -5299,70 +5299,70 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G4" s="40">
         <v>2</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="I4" s="40">
         <v>256</v>
       </c>
       <c r="J4" s="40" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="K4" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="L4" s="40" t="s">
+        <v>360</v>
+      </c>
+      <c r="M4" s="40" t="s">
+        <v>312</v>
+      </c>
+      <c r="N4" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="L4" s="40" t="s">
-        <v>363</v>
-      </c>
-      <c r="M4" s="40" t="s">
-        <v>315</v>
-      </c>
-      <c r="N4" s="40" t="s">
+      <c r="O4" s="40" t="s">
+        <v>313</v>
+      </c>
+      <c r="P4" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q4" s="40" t="s">
         <v>303</v>
       </c>
-      <c r="O4" s="40" t="s">
-        <v>316</v>
-      </c>
-      <c r="P4" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q4" s="40" t="s">
-        <v>306</v>
-      </c>
       <c r="R4" s="40" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="S4" s="40" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="T4" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="W4" s="1">
         <v>15</v>
@@ -5376,17 +5376,17 @@
     </row>
     <row r="396" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y396" s="44" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y397" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -5444,7 +5444,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="34" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="69" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -5471,96 +5471,96 @@
     </row>
     <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D2" s="35" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>46</v>
       </c>
       <c r="H2" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="I2" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="J2" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>286</v>
+      </c>
+      <c r="L2" s="35" t="s">
         <v>287</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="M2" s="35" t="s">
         <v>288</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="N2" s="35" t="s">
         <v>289</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="O2" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="P2" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="Q2" s="35" t="s">
         <v>292</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="R2" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="S2" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="Q2" s="35" t="s">
-        <v>295</v>
-      </c>
-      <c r="R2" s="35" t="s">
-        <v>296</v>
-      </c>
-      <c r="S2" s="35" t="s">
-        <v>297</v>
-      </c>
       <c r="T2" s="39" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="V2" s="35" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="W2" s="35" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="H3" s="40">
         <v>2</v>
@@ -5569,43 +5569,43 @@
         <v>256</v>
       </c>
       <c r="J3" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="K3" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>366</v>
+      </c>
+      <c r="M3" s="40" t="s">
         <v>299</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="N3" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="L3" s="40" t="s">
-        <v>369</v>
-      </c>
-      <c r="M3" s="40" t="s">
+      <c r="O3" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="P3" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="Q3" s="40" t="s">
         <v>303</v>
       </c>
-      <c r="O3" s="40" t="s">
+      <c r="R3" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="P3" s="40" t="s">
+      <c r="S3" s="40" t="s">
         <v>305</v>
-      </c>
-      <c r="Q3" s="40" t="s">
-        <v>306</v>
-      </c>
-      <c r="R3" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="S3" s="40" t="s">
-        <v>308</v>
       </c>
       <c r="T3" s="40" t="s">
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -5619,42 +5619,42 @@
     </row>
     <row r="395" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y395" s="44" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="396" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y396" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y397" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="399" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y399" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="400" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y400" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="401" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y401" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="402" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y402" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -5691,14 +5691,14 @@
   <sheetData>
     <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="50"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>48</v>
@@ -5709,7 +5709,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>57</v>
@@ -5720,7 +5720,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>59</v>
@@ -5731,13 +5731,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -5783,7 +5783,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -5794,7 +5794,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>48</v>
@@ -5817,13 +5817,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>64</v>
@@ -5862,13 +5862,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>67</v>
@@ -5880,7 +5880,7 @@
         <v>61</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -5933,7 +5933,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
@@ -5948,7 +5948,7 @@
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>88</v>
@@ -5960,30 +5960,30 @@
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>51</v>
@@ -5992,10 +5992,10 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
@@ -6013,12 +6013,12 @@
         <v>15</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>51</v>
@@ -6027,7 +6027,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -6045,22 +6045,22 @@
         <v>13</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -6075,25 +6075,25 @@
         <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
@@ -6108,25 +6108,25 @@
         <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
@@ -6141,28 +6141,28 @@
         <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>14</v>
@@ -6180,21 +6180,21 @@
         <v>15</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -6203,16 +6203,16 @@
         <v>14</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -6278,43 +6278,43 @@
   <sheetData>
     <row r="1" spans="1:2" ht="192.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B1" s="58"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
@@ -6322,10 +6322,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -6358,7 +6358,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -6369,7 +6369,7 @@
     </row>
     <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>88</v>
@@ -6392,7 +6392,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>51</v>
@@ -6407,18 +6407,18 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>10</v>
@@ -6427,35 +6427,35 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>51</v>
@@ -6464,16 +6464,16 @@
         <v>16</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -6520,7 +6520,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -6541,7 +6541,7 @@
     </row>
     <row r="2" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>88</v>
@@ -6565,36 +6565,36 @@
         <v>28</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="O2" s="14" t="s">
         <v>393</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="P2" s="14" t="s">
         <v>394</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>396</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>397</v>
-      </c>
       <c r="Q2" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>51</v>
@@ -6603,10 +6603,10 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>0</v>
@@ -6618,7 +6618,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="13" t="s">
@@ -6640,12 +6640,12 @@
         <v>13</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>51</v>
@@ -6654,10 +6654,10 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>0</v>
@@ -6666,11 +6666,11 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
@@ -6691,12 +6691,12 @@
         <v>14</v>
       </c>
       <c r="Q4" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>51</v>
@@ -6705,10 +6705,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>0</v>
@@ -6717,11 +6717,11 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>13</v>
@@ -6742,24 +6742,24 @@
         <v>13</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>0</v>
@@ -6791,24 +6791,24 @@
         <v>13</v>
       </c>
       <c r="Q6" s="19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>0</v>
@@ -6817,13 +6817,13 @@
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
@@ -6844,24 +6844,24 @@
         <v>14</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>0</v>
@@ -6870,11 +6870,11 @@
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>13</v>
@@ -6895,7 +6895,7 @@
         <v>13</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
@@ -7005,7 +7005,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="32" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -7017,16 +7017,16 @@
     </row>
     <row r="2" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>72</v>
@@ -7038,7 +7038,7 @@
         <v>74</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>

</xml_diff>

<commit_message>
Removed Regions field from CD3 template also. Added Release-Notes
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="29" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="402">
   <si>
     <t>Regional</t>
   </si>
@@ -388,12 +388,6 @@
     <t>$ and * in PolicyStatements would be replaced by PolicyStatementGroup and PolicyStatementCompartment respectively;If Compartment Name is left empty or mentioned 'root', policy will be created in root compartment;
 # Rows after &lt;END&gt; or &lt;end&gt; will not be processed;
 Enter Region as your tenancy's Home Region for Policy Creation</t>
-  </si>
-  <si>
-    <t>regions</t>
-  </si>
-  <si>
-    <t>Ashburn,Phoenix</t>
   </si>
   <si>
     <t>NSGName</t>
@@ -1020,6 +1014,302 @@
   </si>
   <si>
     <t>onprem_destinations</t>
+  </si>
+  <si>
+    <t>configure SGW route
+(n|object_storage|all_services)</t>
+  </si>
+  <si>
+    <t>configure NGW route
+(y|n)</t>
+  </si>
+  <si>
+    <t>configure IGW route (y|n)</t>
+  </si>
+  <si>
+    <t>configure OnPrem route (y|n)</t>
+  </si>
+  <si>
+    <t>configure VCNPeering
+route (y|n)</t>
+  </si>
+  <si>
+    <t>RouteTableName</t>
+  </si>
+  <si>
+    <t>SecListName</t>
+  </si>
+  <si>
+    <t>Columns: Region, Compartment Name, Availability Domain, MountTarget Name, MountTarget SubnetName, FSS name, Path are mandatory.
+Default value for columns if left blank: sourceCIDR- 0.0.0.0/0, Access- READ_ONLY, GID- 65534, UID- 65534, IDSquash- NONE and require_ps_port- false
+Mount target IP, FSS Capacity, FSS Inodes will take default values from OCI if left blank
+Resources will be created based on MountTargetName and FSSName columns.
+#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
+Below sample data shows example of  multiple FSS(FSS1 and FSS2) using single MT(MT1) , 1 FSS(FSS3) using multiple MTs(MT2 and MT3) and also 1 FSS(FSS4) using 1 MT(MT4)</t>
+  </si>
+  <si>
+    <t>#for DB Systems Virtual Machine, fill the sheet with required information, as suggested in 2 row headings | Select shape for Virtual Machine in "F" column and change Node Count accordingly | &lt;end&gt; or &lt;END&gt; is must | Type anything after&lt;end&gt; or &lt;END&gt; for testing.  | If VM DB System node count is "2" then Software edition must be "ENTERPRISE_EDITION_EXTREME_PERFORMANCE"  
+#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
+  </si>
+  <si>
+    <t>#for DB Systems Bare Metal, fill the sheet with required information, as suggested in 2 row headings | Select shape for Bare Metal in "F" column and change CPU core and it should be a even (multiple of 2) value.  | &lt;end&gt; or &lt;END&gt; is must | Type anything after &lt;end&gt; or &lt;END&gt; for testing | FOR CPU CORES --&gt; BM.DenseIO1.36 - Specify a multiple of 2, from 2 to 36 | BM.DenseIO2.52 - Specify a multiple of 2, from 2 to 52 
+#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
+  </si>
+  <si>
+    <t>#for DB Systems ExaData, fill the sheet with required information, as suggested in 2 row headings | Select shape for EXADATA in "F" column and change CPU core accordingly | &lt;end&gt; or &lt;END&gt; is must | Type anything after &lt;end&gt; or &lt;END&gt; for testing. | Software edition is ENTERPRISE_EDITION_EXTREME_PERFORMANCE by default | Node count is 2 by default | FOR CPU CORES --&gt; Exadata.Base.48 - Specify a multiple of 2, from 0 to 48 | Exadata.Quarter1.84 - Specify a multiple of 2, from 22 to 84 | Exadata.Half1.168 - Specify a multiple of 4, from 44 to 168 | Exadata.Full1.336 - Specify a multiple of 8, from 88 to 336 | Exadata.Quarter2.92 - Specify a multiple of 2, from 0 to 92 | Exadata.Half2.184 - Specify a multiple of 4, from 0 to 184 | Exadata.Full2.368 - Specify a multiple of 8, from 0 to 368 
+#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
+  </si>
+  <si>
+    <t>Route Rules will be exported here</t>
+  </si>
+  <si>
+    <t>SecRules will be exported here</t>
+  </si>
+  <si>
+    <t>seclist_names</t>
+  </si>
+  <si>
+    <t># subnet names are case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if
+left blank means subnet will use default dhcp options of the vcn.
+dns_label - if specified as n, DNS will not be enabled for the subnet; Make sure dns_label for VCN is enabled for its subnet DNS to be enabled.
+vcn_name should be same as enterd in VCNs sheet.
+Initially Route Rules for IGW, NGW and SGW, On Prem and VCN peering for each subnet would be created based on parameter values: configure IGW route, configure NGW route and configure SGW route, configure OnPrem route and configure VCNPeering route respectively for each subnet. The condition is the respective component should have been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
+seclist_names - specify comma seperated names of SLs that needs to be attached to the subnet. If left blank, 1 seclist with name same as subnet name would be attached.  Specify n if you dont
+want any custom security list to be attached to the subnet.
+route_table_name - specify name of route table that needs to be attached to subnet. If left blank, route table with same name as subnet name would be attached. Specify n if you dont
+ want any custom route table to be attached to the subnet.
+Subnets in a  VCN can share same route table and seclist depending upon name specified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars.
+dns_label - if specified as n, DNS will not be enabled for the VCN
+Valid Values for columns E,F,G,H,I:   y|n|&lt;component_name&gt; ie mention 'n' when a component(like IGW) is not required to be configured(like for PHXHub-VCN), specify name of the component- component will be configured with the mentioned name(eg PHX-DRG for the DRG in PHXHub-VCN) and mention 'y' if component needs to be configured with default name ie &lt;vcnname&gt;_ngw(eg PHXNonProd-VCN_ngw)
+Note- For DRG, if declaring multiple DRGs for a region, make sure to specify unique names.
+Note- For LPGs, specify comma seperated values based on number of LPGs required for each VCN. LPGs will be peered with other VCN LPGs in the order they are specified.
+Note- For column hub_spoke_peer_none - specify 'hub' if the VCN is a hub, specify 'spoke:&lt;hub vcn name&gt;' if VCN is a spoke of a hub VCN, specify 'peer:&lt;vcn name&gt;' if a VCN needs to be normal peered with some other VCN and specify 'none' in case it is none of these.
+</t>
+  </si>
+  <si>
+    <t>Automation Toolkit release verion- v6.0
+Tabs Affected: Subnets
+Major Feature - Support for NonGreenField Tenancies</t>
+  </si>
+  <si>
+    <t>VM.Standard.E3.Flex::5</t>
+  </si>
+  <si>
+    <t>#Template will be picked upon from template folder based on  OS column; Backup Policy column can be left blank at the time of instance creation and can be filled up later on while attaching backup policy to the boot and block volumes together; Pub Address column represents whether public address needs to be assigned to the instance or not(TRUE|FALSE); ssh-key-var-name column accepts the name of variable defined in variables_&lt;region&gt;.tf file containing SSH key to be pushed to the server; NSGs column accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG; Leave DedicatedVMHost column blank if instance doesnt need to be launched on dedicated vm host
+#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
+#If shape is VM.Standard.E3.Flex then specify it as VM.Standard.E3.Flex::ocpus</t>
+  </si>
+  <si>
+    <t>ListenerName</t>
+  </si>
+  <si>
+    <t>listenr1</t>
+  </si>
+  <si>
+    <t>listenr2</t>
+  </si>
+  <si>
+    <t>my_lbr1</t>
+  </si>
+  <si>
+    <t>my_lbr2</t>
+  </si>
+  <si>
+    <t>100Mbps</t>
+  </si>
+  <si>
+    <t>10.111.1.5:80,Test2:81</t>
+  </si>
+  <si>
+    <t>10.111.1.4:80,Test1:81</t>
+  </si>
+  <si>
+    <t>10.111.1.6:80</t>
+  </si>
+  <si>
+    <t>listenr</t>
+  </si>
+  <si>
+    <t>ROUND_ROBIN</t>
+  </si>
+  <si>
+    <t>TCP</t>
+  </si>
+  <si>
+    <t>app1.example.com</t>
+  </si>
+  <si>
+    <t>app2.example.com,app3.example.com</t>
+  </si>
+  <si>
+    <t>LBR Subnets: specify a single regional subnet name (recommended) or two comma seperated subnet names(AD specific) for public Load Balancer and provide a single subnet(Regional or AD specific) for Private load Balancer- subnets names should be same as defined in Subnets tab, Backend ServerName:Port- specify comma separated list of servernames:ports(either specify server name as same name defined in Instances sheet or specify the IP address); LBR Hostname can be null, all other fields are mandatory; Backend HealthCheck URL is required if Backend HealthCheck Protocol is HTTP; If you want to create an HTTPS Listener, please specify ListenerProtocol as HTTP and UseSSL as y; Allows multiple Listeners(seperate rows) per LBR and multiple Hostnames(comma seperated) per Listener
+#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
+  </si>
+  <si>
+    <t>LinuxFlex</t>
+  </si>
+  <si>
+    <t>WindowsFlex</t>
+  </si>
+  <si>
+    <t># Horizontal row specifies the TagNameSpace Names to be created; Vertical column under each TagNameSpace represnts Keys in that tagnamespace; Enter compartment name in which  all tagnamespaces and keys will be created;
+Enter Region as your tenancy's Home Region for Tags Creation</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Apps</t>
+  </si>
+  <si>
+    <t>EBS</t>
+  </si>
+  <si>
+    <t>Compartment for Common Network Objects</t>
+  </si>
+  <si>
+    <t>Compartment for EBS Network Resources</t>
+  </si>
+  <si>
+    <t>Compartment for other objects</t>
+  </si>
+  <si>
+    <t>NPR</t>
+  </si>
+  <si>
+    <t>PRD</t>
+  </si>
+  <si>
+    <t>Compartment for EBS-NPR Resources</t>
+  </si>
+  <si>
+    <t>Apps::EBS</t>
+  </si>
+  <si>
+    <t>Compartment for EBS other Resources</t>
+  </si>
+  <si>
+    <t>EBS_Admins</t>
+  </si>
+  <si>
+    <t>EBS admins</t>
+  </si>
+  <si>
+    <t>Hub Network Administrators</t>
+  </si>
+  <si>
+    <t>EBSInstancePolicy</t>
+  </si>
+  <si>
+    <t>PHXEBS-VCN</t>
+  </si>
+  <si>
+    <t>Network::EBS</t>
+  </si>
+  <si>
+    <t>TCC</t>
+  </si>
+  <si>
+    <t>Compartment for TCC Network Resources</t>
+  </si>
+  <si>
+    <t>Compartment for TCC other Resources</t>
+  </si>
+  <si>
+    <t>Compartment for TCC-PRD Resources</t>
+  </si>
+  <si>
+    <t>Apps::TCC</t>
+  </si>
+  <si>
+    <t>TCC_Admins</t>
+  </si>
+  <si>
+    <t>TCC admins</t>
+  </si>
+  <si>
+    <t>TCCInstancePolicy</t>
+  </si>
+  <si>
+    <t>Network::TCC</t>
+  </si>
+  <si>
+    <t>PHXTCC-VCN</t>
+  </si>
+  <si>
+    <t>lpgebs</t>
+  </si>
+  <si>
+    <t>lpgtcc</t>
+  </si>
+  <si>
+    <t>10.112.1.0/24</t>
+  </si>
+  <si>
+    <t>10.112.2.0/24</t>
+  </si>
+  <si>
+    <t>prd-subnet</t>
+  </si>
+  <si>
+    <t>10.112.3.0/24</t>
+  </si>
+  <si>
+    <t>dev_sl,common_sl</t>
+  </si>
+  <si>
+    <t>qa_sl,common_sl</t>
+  </si>
+  <si>
+    <t>prd_sl,common_sl</t>
+  </si>
+  <si>
+    <t>all_services</t>
+  </si>
+  <si>
+    <t>object_storage</t>
+  </si>
+  <si>
+    <t>ebs-nsg</t>
+  </si>
+  <si>
+    <t>tcc-nsg</t>
+  </si>
+  <si>
+    <t>EBSInstance</t>
+  </si>
+  <si>
+    <t>TCCInstance</t>
+  </si>
+  <si>
+    <t>DNS-Server-PhxHub</t>
+  </si>
+  <si>
+    <t>PHXEBS-VCN_qa-subnet</t>
+  </si>
+  <si>
+    <t>PHXTCC-VCN_prd-subnet</t>
+  </si>
+  <si>
+    <t>Apps::TCC::PRD</t>
+  </si>
+  <si>
+    <t>EBSInstance_Disk2</t>
+  </si>
+  <si>
+    <t>TCCInstance_Disk2</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>PHXEBS-VCN_dev-subnet</t>
+  </si>
+  <si>
+    <t>y,y</t>
   </si>
   <si>
     <r>
@@ -1111,19 +1401,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> represents naming convention; Mention y if you want to attachd AD and CIDR to object's display name; defaults to n
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">regions </t>
+      <t xml:space="preserve"> represents naming convention; Mention y if you want to attachd AD and CIDR to object's display name; defaults to n</t>
     </r>
     <r>
       <rPr>
@@ -1133,305 +1411,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">represents regions client's tenancy is subscribed to and plan to build infra for;accepts comma seperated list; case insensitive; (allowed values: ashburn, phoenix, london, frankfurt, toronto, tokyo, seoul, mumbai)
+      <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <t>configure SGW route
-(n|object_storage|all_services)</t>
-  </si>
-  <si>
-    <t>configure NGW route
-(y|n)</t>
-  </si>
-  <si>
-    <t>configure IGW route (y|n)</t>
-  </si>
-  <si>
-    <t>configure OnPrem route (y|n)</t>
-  </si>
-  <si>
-    <t>configure VCNPeering
-route (y|n)</t>
-  </si>
-  <si>
-    <t>RouteTableName</t>
-  </si>
-  <si>
-    <t>SecListName</t>
-  </si>
-  <si>
-    <t>Columns: Region, Compartment Name, Availability Domain, MountTarget Name, MountTarget SubnetName, FSS name, Path are mandatory.
-Default value for columns if left blank: sourceCIDR- 0.0.0.0/0, Access- READ_ONLY, GID- 65534, UID- 65534, IDSquash- NONE and require_ps_port- false
-Mount target IP, FSS Capacity, FSS Inodes will take default values from OCI if left blank
-Resources will be created based on MountTargetName and FSSName columns.
-#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
-Below sample data shows example of  multiple FSS(FSS1 and FSS2) using single MT(MT1) , 1 FSS(FSS3) using multiple MTs(MT2 and MT3) and also 1 FSS(FSS4) using 1 MT(MT4)</t>
-  </si>
-  <si>
-    <t>#for DB Systems Virtual Machine, fill the sheet with required information, as suggested in 2 row headings | Select shape for Virtual Machine in "F" column and change Node Count accordingly | &lt;end&gt; or &lt;END&gt; is must | Type anything after&lt;end&gt; or &lt;END&gt; for testing.  | If VM DB System node count is "2" then Software edition must be "ENTERPRISE_EDITION_EXTREME_PERFORMANCE"  
-#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
-  </si>
-  <si>
-    <t>#for DB Systems Bare Metal, fill the sheet with required information, as suggested in 2 row headings | Select shape for Bare Metal in "F" column and change CPU core and it should be a even (multiple of 2) value.  | &lt;end&gt; or &lt;END&gt; is must | Type anything after &lt;end&gt; or &lt;END&gt; for testing | FOR CPU CORES --&gt; BM.DenseIO1.36 - Specify a multiple of 2, from 2 to 36 | BM.DenseIO2.52 - Specify a multiple of 2, from 2 to 52 
-#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
-  </si>
-  <si>
-    <t>#for DB Systems ExaData, fill the sheet with required information, as suggested in 2 row headings | Select shape for EXADATA in "F" column and change CPU core accordingly | &lt;end&gt; or &lt;END&gt; is must | Type anything after &lt;end&gt; or &lt;END&gt; for testing. | Software edition is ENTERPRISE_EDITION_EXTREME_PERFORMANCE by default | Node count is 2 by default | FOR CPU CORES --&gt; Exadata.Base.48 - Specify a multiple of 2, from 0 to 48 | Exadata.Quarter1.84 - Specify a multiple of 2, from 22 to 84 | Exadata.Half1.168 - Specify a multiple of 4, from 44 to 168 | Exadata.Full1.336 - Specify a multiple of 8, from 88 to 336 | Exadata.Quarter2.92 - Specify a multiple of 2, from 0 to 92 | Exadata.Half2.184 - Specify a multiple of 4, from 0 to 184 | Exadata.Full2.368 - Specify a multiple of 8, from 0 to 368 
-#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
-  </si>
-  <si>
-    <t>Route Rules will be exported here</t>
-  </si>
-  <si>
-    <t>SecRules will be exported here</t>
-  </si>
-  <si>
-    <t>seclist_names</t>
-  </si>
-  <si>
-    <t># subnet names are case-sensitive across sheets; All fields are mandatory for each subnet except dns_label for which the default value is subnet_name truncated to 15 chars; dhcp_option_name field if
-left blank means subnet will use default dhcp options of the vcn.
-dns_label - if specified as n, DNS will not be enabled for the subnet; Make sure dns_label for VCN is enabled for its subnet DNS to be enabled.
-vcn_name should be same as enterd in VCNs sheet.
-Initially Route Rules for IGW, NGW and SGW, On Prem and VCN peering for each subnet would be created based on parameter values: configure IGW route, configure NGW route and configure SGW route, configure OnPrem route and configure VCNPeering route respectively for each subnet. The condition is the respective component should have been created for that using parameters: igw_required, ngw_required and sgw_required parameters in VCNs sheet.
-seclist_names - specify comma seperated names of SLs that needs to be attached to the subnet. If left blank, 1 seclist with name same as subnet name would be attached.  Specify n if you dont
-want any custom security list to be attached to the subnet.
-route_table_name - specify name of route table that needs to be attached to subnet. If left blank, route table with same name as subnet name would be attached. Specify n if you dont
- want any custom route table to be attached to the subnet.
-Subnets in a  VCN can share same route table and seclist depending upon name specified.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># VCN names should be unique and are case-sensitie across sheets; All fields are mandatory for each VCN except dns_label for which the default value is vcn_name truncated to 15 chars.
-dns_label - if specified as n, DNS will not be enabled for the VCN
-Valid Values for columns E,F,G,H,I:   y|n|&lt;component_name&gt; ie mention 'n' when a component(like IGW) is not required to be configured(like for PHXHub-VCN), specify name of the component- component will be configured with the mentioned name(eg PHX-DRG for the DRG in PHXHub-VCN) and mention 'y' if component needs to be configured with default name ie &lt;vcnname&gt;_ngw(eg PHXNonProd-VCN_ngw)
-Note- For DRG, if declaring multiple DRGs for a region, make sure to specify unique names.
-Note- For LPGs, specify comma seperated values based on number of LPGs required for each VCN. LPGs will be peered with other VCN LPGs in the order they are specified.
-Note- For column hub_spoke_peer_none - specify 'hub' if the VCN is a hub, specify 'spoke:&lt;hub vcn name&gt;' if VCN is a spoke of a hub VCN, specify 'peer:&lt;vcn name&gt;' if a VCN needs to be normal peered with some other VCN and specify 'none' in case it is none of these.
-</t>
-  </si>
-  <si>
-    <t>Automation Toolkit release verion- v6.0
-Tabs Affected: Subnets
-Major Feature - Support for NonGreenField Tenancies</t>
-  </si>
-  <si>
-    <t>VM.Standard.E3.Flex::5</t>
-  </si>
-  <si>
-    <t>#Template will be picked upon from template folder based on  OS column; Backup Policy column can be left blank at the time of instance creation and can be filled up later on while attaching backup policy to the boot and block volumes together; Pub Address column represents whether public address needs to be assigned to the instance or not(TRUE|FALSE); ssh-key-var-name column accepts the name of variable defined in variables_&lt;region&gt;.tf file containing SSH key to be pushed to the server; NSGs column accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG; Leave DedicatedVMHost column blank if instance doesnt need to be launched on dedicated vm host
-#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
-#If shape is VM.Standard.E3.Flex then specify it as VM.Standard.E3.Flex::ocpus</t>
-  </si>
-  <si>
-    <t>ListenerName</t>
-  </si>
-  <si>
-    <t>listenr1</t>
-  </si>
-  <si>
-    <t>listenr2</t>
-  </si>
-  <si>
-    <t>my_lbr1</t>
-  </si>
-  <si>
-    <t>my_lbr2</t>
-  </si>
-  <si>
-    <t>100Mbps</t>
-  </si>
-  <si>
-    <t>10.111.1.5:80,Test2:81</t>
-  </si>
-  <si>
-    <t>10.111.1.4:80,Test1:81</t>
-  </si>
-  <si>
-    <t>10.111.1.6:80</t>
-  </si>
-  <si>
-    <t>listenr</t>
-  </si>
-  <si>
-    <t>ROUND_ROBIN</t>
-  </si>
-  <si>
-    <t>TCP</t>
-  </si>
-  <si>
-    <t>app1.example.com</t>
-  </si>
-  <si>
-    <t>app2.example.com,app3.example.com</t>
-  </si>
-  <si>
-    <t>LBR Subnets: specify a single regional subnet name (recommended) or two comma seperated subnet names(AD specific) for public Load Balancer and provide a single subnet(Regional or AD specific) for Private load Balancer- subnets names should be same as defined in Subnets tab, Backend ServerName:Port- specify comma separated list of servernames:ports(either specify server name as same name defined in Instances sheet or specify the IP address); LBR Hostname can be null, all other fields are mandatory; Backend HealthCheck URL is required if Backend HealthCheck Protocol is HTTP; If you want to create an HTTPS Listener, please specify ListenerProtocol as HTTP and UseSSL as y; Allows multiple Listeners(seperate rows) per LBR and multiple Hostnames(comma seperated) per Listener
-#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
-  </si>
-  <si>
-    <t>LinuxFlex</t>
-  </si>
-  <si>
-    <t>WindowsFlex</t>
-  </si>
-  <si>
-    <t># Horizontal row specifies the TagNameSpace Names to be created; Vertical column under each TagNameSpace represnts Keys in that tagnamespace; Enter compartment name in which  all tagnamespaces and keys will be created;
-Enter Region as your tenancy's Home Region for Tags Creation</t>
-  </si>
-  <si>
-    <t>Network</t>
-  </si>
-  <si>
-    <t>Apps</t>
-  </si>
-  <si>
-    <t>EBS</t>
-  </si>
-  <si>
-    <t>Compartment for Common Network Objects</t>
-  </si>
-  <si>
-    <t>Compartment for EBS Network Resources</t>
-  </si>
-  <si>
-    <t>Compartment for other objects</t>
-  </si>
-  <si>
-    <t>NPR</t>
-  </si>
-  <si>
-    <t>PRD</t>
-  </si>
-  <si>
-    <t>Compartment for EBS-NPR Resources</t>
-  </si>
-  <si>
-    <t>Apps::EBS</t>
-  </si>
-  <si>
-    <t>Compartment for EBS other Resources</t>
-  </si>
-  <si>
-    <t>EBS_Admins</t>
-  </si>
-  <si>
-    <t>EBS admins</t>
-  </si>
-  <si>
-    <t>Hub Network Administrators</t>
-  </si>
-  <si>
-    <t>EBSInstancePolicy</t>
-  </si>
-  <si>
-    <t>PHXEBS-VCN</t>
-  </si>
-  <si>
-    <t>Network::EBS</t>
-  </si>
-  <si>
-    <t>TCC</t>
-  </si>
-  <si>
-    <t>Compartment for TCC Network Resources</t>
-  </si>
-  <si>
-    <t>Compartment for TCC other Resources</t>
-  </si>
-  <si>
-    <t>Compartment for TCC-PRD Resources</t>
-  </si>
-  <si>
-    <t>Apps::TCC</t>
-  </si>
-  <si>
-    <t>TCC_Admins</t>
-  </si>
-  <si>
-    <t>TCC admins</t>
-  </si>
-  <si>
-    <t>TCCInstancePolicy</t>
-  </si>
-  <si>
-    <t>Network::TCC</t>
-  </si>
-  <si>
-    <t>PHXTCC-VCN</t>
-  </si>
-  <si>
-    <t>lpgebs</t>
-  </si>
-  <si>
-    <t>lpgtcc</t>
-  </si>
-  <si>
-    <t>10.112.1.0/24</t>
-  </si>
-  <si>
-    <t>10.112.2.0/24</t>
-  </si>
-  <si>
-    <t>prd-subnet</t>
-  </si>
-  <si>
-    <t>10.112.3.0/24</t>
-  </si>
-  <si>
-    <t>dev_sl,common_sl</t>
-  </si>
-  <si>
-    <t>qa_sl,common_sl</t>
-  </si>
-  <si>
-    <t>prd_sl,common_sl</t>
-  </si>
-  <si>
-    <t>all_services</t>
-  </si>
-  <si>
-    <t>object_storage</t>
-  </si>
-  <si>
-    <t>ebs-nsg</t>
-  </si>
-  <si>
-    <t>tcc-nsg</t>
-  </si>
-  <si>
-    <t>EBSInstance</t>
-  </si>
-  <si>
-    <t>TCCInstance</t>
-  </si>
-  <si>
-    <t>DNS-Server-PhxHub</t>
-  </si>
-  <si>
-    <t>PHXEBS-VCN_qa-subnet</t>
-  </si>
-  <si>
-    <t>PHXTCC-VCN_prd-subnet</t>
-  </si>
-  <si>
-    <t>Apps::TCC::PRD</t>
-  </si>
-  <si>
-    <t>EBSInstance_Disk2</t>
-  </si>
-  <si>
-    <t>TCCInstance_Disk2</t>
-  </si>
-  <si>
-    <t>Linux</t>
-  </si>
-  <si>
-    <t>PHXEBS-VCN_dev-subnet</t>
-  </si>
-  <si>
-    <t>y,y</t>
   </si>
 </sst>
 </file>
@@ -2259,7 +2241,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="43" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -2290,7 +2272,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="30" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -2319,7 +2301,7 @@
         <v>89</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>66</v>
@@ -2355,7 +2337,7 @@
         <v>76</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="Q2" s="19"/>
       <c r="R2" s="19"/>
@@ -2423,7 +2405,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="16" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -2454,10 +2436,10 @@
         <v>89</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>67</v>
@@ -2466,13 +2448,13 @@
         <v>68</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>69</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>72</v>
@@ -2496,7 +2478,7 @@
         <v>76</v>
       </c>
       <c r="R2" s="40" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -2504,13 +2486,13 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>106</v>
@@ -2519,12 +2501,12 @@
         <v>104</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="24"/>
       <c r="J3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>105</v>
@@ -2542,13 +2524,13 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>77</v>
@@ -2557,13 +2539,13 @@
         <v>78</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="I4" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -2584,13 +2566,13 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>106</v>
@@ -2599,13 +2581,13 @@
         <v>104</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K5" s="24" t="s">
         <v>117</v>
-      </c>
-      <c r="K5" s="24" t="s">
-        <v>119</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2620,25 +2602,25 @@
         <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>77</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I6" s="24"/>
       <c r="J6" s="1"/>
@@ -2683,7 +2665,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -2716,17 +2698,17 @@
         <v>101</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -2783,7 +2765,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -2837,10 +2819,10 @@
         <v>82</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -2848,41 +2830,41 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>83</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -2890,38 +2872,38 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="I4" s="46" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="N4" s="1"/>
     </row>
@@ -2930,38 +2912,38 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="I5" s="46" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>83</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="N5" s="1"/>
     </row>
@@ -3035,7 +3017,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C3" s="1">
         <v>150</v>
@@ -3044,13 +3026,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>83</v>
@@ -3061,7 +3043,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C4" s="1">
         <v>150</v>
@@ -3070,13 +3052,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>83</v>
@@ -3136,7 +3118,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -3163,49 +3145,49 @@
         <v>60</v>
       </c>
       <c r="C2" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="L2" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="K2" s="27" t="s">
+      <c r="M2" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="N2" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="O2" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="M2" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="N2" s="27" t="s">
+      <c r="P2" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="O2" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="P2" s="27" t="s">
+      <c r="Q2" s="27" t="s">
         <v>167</v>
-      </c>
-      <c r="Q2" s="27" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -3213,26 +3195,26 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -3246,26 +3228,26 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -3279,32 +3261,32 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -3316,32 +3298,32 @@
         <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -3353,26 +3335,26 @@
         <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -3445,7 +3427,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -3475,58 +3457,58 @@
         <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="N2" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="O2" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="K2" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="M2" s="27" t="s">
-        <v>255</v>
-      </c>
-      <c r="N2" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="O2" s="27" t="s">
-        <v>181</v>
-      </c>
       <c r="P2" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="R2" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="Q2" s="28" t="s">
+      <c r="S2" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="T2" s="28" t="s">
         <v>193</v>
-      </c>
-      <c r="S2" s="28" t="s">
-        <v>194</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -3534,56 +3516,56 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K3" s="1">
         <v>80</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N3" s="1">
         <v>443</v>
       </c>
       <c r="O3" s="27" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="Q3" s="27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="T3" s="1"/>
     </row>
@@ -3592,56 +3574,56 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K4" s="1">
         <v>80</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N4" s="1">
         <v>443</v>
       </c>
       <c r="O4" s="27" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="Q4" s="27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="T4" s="1"/>
     </row>
@@ -3650,44 +3632,44 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>346</v>
       </c>
       <c r="K5" s="1">
         <v>80</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="N5" s="1">
         <v>80</v>
       </c>
       <c r="O5" s="27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>14</v>
@@ -3725,7 +3707,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="16" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="66" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -3764,7 +3746,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>32</v>
@@ -3778,7 +3760,7 @@
       <c r="B4" s="65"/>
       <c r="C4" s="63"/>
       <c r="D4" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>35</v>
@@ -3963,16 +3945,16 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -3980,13 +3962,13 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C4" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>142</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>85</v>
@@ -4048,16 +4030,16 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>141</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -4065,13 +4047,13 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C4" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>140</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>142</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>85</v>
@@ -4128,10 +4110,10 @@
         <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>356</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -4140,13 +4122,13 @@
         <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4154,13 +4136,13 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
@@ -4168,10 +4150,10 @@
         <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -4180,13 +4162,13 @@
         <v>100</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4194,13 +4176,13 @@
         <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4208,13 +4190,13 @@
         <v>100</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4222,13 +4204,13 @@
         <v>100</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -4279,7 +4261,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -4297,22 +4279,22 @@
         <v>60</v>
       </c>
       <c r="C2" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="F2" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="G2" s="44" t="s">
         <v>201</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="H2" s="44" t="s">
         <v>202</v>
-      </c>
-      <c r="G2" s="44" t="s">
-        <v>203</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -4320,16 +4302,16 @@
         <v>100</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C3" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="31" t="s">
         <v>205</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>207</v>
       </c>
       <c r="F3" s="30">
         <v>1</v>
@@ -4338,7 +4320,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -4346,16 +4328,16 @@
         <v>100</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F4" s="30">
         <v>1</v>
@@ -4364,7 +4346,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -4372,16 +4354,16 @@
         <v>101</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F5" s="30">
         <v>1</v>
@@ -4390,7 +4372,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -4398,16 +4380,16 @@
         <v>101</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F6" s="30">
         <v>1</v>
@@ -4416,24 +4398,24 @@
         <v>1</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="30" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F7" s="30">
         <v>1</v>
@@ -4442,24 +4424,24 @@
         <v>1</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="30" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F8" s="30">
         <v>1</v>
@@ -4468,7 +4450,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -4518,7 +4500,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="32" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="67" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -4551,67 +4533,67 @@
         <v>60</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D2" s="33" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>44</v>
       </c>
       <c r="G2" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="I2" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="J2" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="K2" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="L2" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="M2" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="N2" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="O2" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="P2" s="33" t="s">
         <v>230</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="Q2" s="33" t="s">
         <v>231</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="R2" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="Q2" s="33" t="s">
+      <c r="S2" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="R2" s="33" t="s">
-        <v>234</v>
-      </c>
-      <c r="S2" s="33" t="s">
-        <v>235</v>
-      </c>
       <c r="T2" s="37" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="U2" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="V2" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="W2" s="33" t="s">
         <v>276</v>
-      </c>
-      <c r="V2" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="W2" s="33" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
@@ -4619,67 +4601,67 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G3" s="38">
         <v>1</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I3" s="38">
         <v>256</v>
       </c>
       <c r="J3" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="L3" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="M3" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="N3" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="O3" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="P3" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="O3" s="38" t="s">
+      <c r="Q3" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="P3" s="38" t="s">
+      <c r="R3" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="Q3" s="38" t="s">
+      <c r="S3" s="38" t="s">
         <v>244</v>
-      </c>
-      <c r="R3" s="38" t="s">
-        <v>245</v>
-      </c>
-      <c r="S3" s="38" t="s">
-        <v>246</v>
       </c>
       <c r="T3" s="38" t="s">
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -4690,67 +4672,67 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G4" s="38">
         <v>2</v>
       </c>
       <c r="H4" s="38" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I4" s="38">
         <v>256</v>
       </c>
       <c r="J4" s="38" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K4" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="L4" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="M4" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="L4" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="M4" s="38" t="s">
+      <c r="N4" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="O4" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="N4" s="38" t="s">
+      <c r="P4" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="O4" s="38" t="s">
+      <c r="Q4" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="P4" s="38" t="s">
+      <c r="R4" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="Q4" s="38" t="s">
+      <c r="S4" s="38" t="s">
         <v>244</v>
-      </c>
-      <c r="R4" s="38" t="s">
-        <v>245</v>
-      </c>
-      <c r="S4" s="38" t="s">
-        <v>246</v>
       </c>
       <c r="T4" s="38" t="s">
         <v>9</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="W4" s="1">
         <v>15</v>
@@ -4764,62 +4746,62 @@
     </row>
     <row r="396" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y396" s="42" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y397" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="399" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y399" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="400" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y400" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="401" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y401" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="402" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y402" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="403" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y403" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="404" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y404" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="405" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y405" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="406" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y406" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="407" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y407" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -4874,7 +4856,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="32" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="67" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -4908,67 +4890,67 @@
         <v>60</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D2" s="33" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>44</v>
       </c>
       <c r="G2" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="H2" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="I2" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="J2" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="K2" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="L2" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="M2" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="N2" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="O2" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="P2" s="33" t="s">
         <v>230</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="Q2" s="33" t="s">
         <v>231</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="R2" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="Q2" s="33" t="s">
+      <c r="S2" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="R2" s="33" t="s">
-        <v>234</v>
-      </c>
-      <c r="S2" s="33" t="s">
-        <v>235</v>
-      </c>
       <c r="T2" s="37" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="U2" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="V2" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="W2" s="33" t="s">
         <v>276</v>
-      </c>
-      <c r="V2" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="W2" s="33" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
@@ -4976,67 +4958,67 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G3" s="38">
         <v>2</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I3" s="38">
         <v>256</v>
       </c>
       <c r="J3" s="38" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K3" s="38" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L3" s="38" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M3" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="O3" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="P3" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q3" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="R3" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="N3" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="O3" s="38" t="s">
+      <c r="S3" s="38" t="s">
         <v>249</v>
-      </c>
-      <c r="P3" s="38" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q3" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="R3" s="38" t="s">
-        <v>250</v>
-      </c>
-      <c r="S3" s="38" t="s">
-        <v>251</v>
       </c>
       <c r="T3" s="38" t="s">
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -5047,67 +5029,67 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G4" s="38">
         <v>2</v>
       </c>
       <c r="H4" s="38" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I4" s="38">
         <v>256</v>
       </c>
       <c r="J4" s="38" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K4" s="38" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L4" s="38" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M4" s="38" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N4" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="O4" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="P4" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="O4" s="38" t="s">
-        <v>254</v>
-      </c>
-      <c r="P4" s="38" t="s">
+      <c r="Q4" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="R4" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="Q4" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="R4" s="38" t="s">
-        <v>245</v>
-      </c>
       <c r="S4" s="38" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="T4" s="38" t="s">
         <v>9</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="W4" s="1">
         <v>15</v>
@@ -5121,17 +5103,17 @@
     </row>
     <row r="396" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y396" s="42" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y397" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -5189,7 +5171,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="32" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="67" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -5222,67 +5204,67 @@
         <v>60</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D2" s="33" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G2" s="33" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I2" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="K2" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="L2" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="M2" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="N2" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="O2" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="P2" s="33" t="s">
         <v>230</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="Q2" s="33" t="s">
         <v>231</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="R2" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="Q2" s="33" t="s">
+      <c r="S2" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="R2" s="33" t="s">
-        <v>234</v>
-      </c>
-      <c r="S2" s="33" t="s">
-        <v>235</v>
-      </c>
       <c r="T2" s="37" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="U2" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="V2" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="W2" s="33" t="s">
         <v>276</v>
-      </c>
-      <c r="V2" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="W2" s="33" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="29" x14ac:dyDescent="0.35">
@@ -5290,22 +5272,22 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H3" s="38">
         <v>2</v>
@@ -5314,43 +5296,43 @@
         <v>256</v>
       </c>
       <c r="J3" s="38" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K3" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>299</v>
+      </c>
+      <c r="M3" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="L3" s="38" t="s">
-        <v>301</v>
-      </c>
-      <c r="M3" s="38" t="s">
+      <c r="N3" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="O3" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="P3" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="O3" s="38" t="s">
+      <c r="Q3" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="P3" s="38" t="s">
+      <c r="R3" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="Q3" s="38" t="s">
+      <c r="S3" s="38" t="s">
         <v>244</v>
-      </c>
-      <c r="R3" s="38" t="s">
-        <v>245</v>
-      </c>
-      <c r="S3" s="38" t="s">
-        <v>246</v>
       </c>
       <c r="T3" s="38" t="s">
         <v>9</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="W3" s="1">
         <v>10</v>
@@ -5366,42 +5348,42 @@
     </row>
     <row r="395" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y395" s="42" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="396" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y396" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="397" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y397" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="398" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y398" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="399" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y399" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="400" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y400" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="401" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y401" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="402" spans="25:25" x14ac:dyDescent="0.35">
       <c r="Y402" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -5473,7 +5455,7 @@
         <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -5481,10 +5463,10 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -5492,10 +5474,10 @@
         <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -5602,7 +5584,7 @@
         <v>53</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -5610,10 +5592,10 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>58</v>
@@ -5622,10 +5604,10 @@
         <v>81</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -5633,10 +5615,10 @@
         <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>58</v>
@@ -5645,10 +5627,10 @@
         <v>81</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -5663,7 +5645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -5683,7 +5665,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -5710,22 +5692,22 @@
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>87</v>
@@ -5736,7 +5718,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -5745,7 +5727,7 @@
         <v>102</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
@@ -5757,7 +5739,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
@@ -5771,13 +5753,13 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -5792,10 +5774,10 @@
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -5804,13 +5786,13 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -5825,10 +5807,10 @@
         <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -5885,8 +5867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5898,7 +5880,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="192.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="55" t="s">
-        <v>315</v>
+        <v>401</v>
       </c>
       <c r="B1" s="56"/>
     </row>
@@ -5912,7 +5894,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>95</v>
@@ -5941,12 +5923,8 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6015,7 +5993,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -6027,10 +6005,10 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -6038,10 +6016,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>10</v>
@@ -6050,7 +6028,7 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
@@ -6058,19 +6036,19 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -6123,7 +6101,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -6168,28 +6146,28 @@
         <v>27</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="O2" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="P2" s="13" t="s">
         <v>317</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>320</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>87</v>
@@ -6200,16 +6178,16 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>0</v>
@@ -6221,14 +6199,14 @@
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="12" t="s">
         <v>13</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>13</v>
@@ -6249,16 +6227,16 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>0</v>
@@ -6275,7 +6253,7 @@
         <v>13</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>13</v>
@@ -6296,16 +6274,16 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>0</v>
@@ -6322,7 +6300,7 @@
         <v>13</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>13</v>
@@ -6343,16 +6321,16 @@
         <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>382</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>0</v>
@@ -6361,11 +6339,11 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>14</v>
@@ -6392,16 +6370,16 @@
         <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>0</v>
@@ -6410,11 +6388,11 @@
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
@@ -6441,16 +6419,16 @@
         <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>0</v>
@@ -6459,17 +6437,17 @@
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>14</v>
@@ -6592,7 +6570,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="30" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -6613,7 +6591,7 @@
         <v>89</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>63</v>
@@ -6625,7 +6603,7 @@
         <v>65</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>

</xml_diff>

<commit_message>
added sample data for multiple export options for FSS in CD3; Updated release version in CD3
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="9" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="29" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="403">
   <si>
     <t>Regional</t>
   </si>
@@ -1040,14 +1040,6 @@
     <t>SecListName</t>
   </si>
   <si>
-    <t>Columns: Region, Compartment Name, Availability Domain, MountTarget Name, MountTarget SubnetName, FSS name, Path are mandatory.
-Default value for columns if left blank: sourceCIDR- 0.0.0.0/0, Access- READ_ONLY, GID- 65534, UID- 65534, IDSquash- NONE and require_ps_port- false
-Mount target IP, FSS Capacity, FSS Inodes will take default values from OCI if left blank
-Resources will be created based on MountTargetName and FSSName columns.
-#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
-Below sample data shows example of  multiple FSS(FSS1 and FSS2) using single MT(MT1) , 1 FSS(FSS3) using multiple MTs(MT2 and MT3) and also 1 FSS(FSS4) using 1 MT(MT4)</t>
-  </si>
-  <si>
     <t>#for DB Systems Virtual Machine, fill the sheet with required information, as suggested in 2 row headings | Select shape for Virtual Machine in "F" column and change Node Count accordingly | &lt;end&gt; or &lt;END&gt; is must | Type anything after&lt;end&gt; or &lt;END&gt; for testing.  | If VM DB System node count is "2" then Software edition must be "ENTERPRISE_EDITION_EXTREME_PERFORMANCE"  
 #Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
   </si>
@@ -1088,11 +1080,6 @@
 Note- For LPGs, specify comma seperated values based on number of LPGs required for each VCN. LPGs will be peered with other VCN LPGs in the order they are specified.
 Note- For column hub_spoke_peer_none - specify 'hub' if the VCN is a hub, specify 'spoke:&lt;hub vcn name&gt;' if VCN is a spoke of a hub VCN, specify 'peer:&lt;vcn name&gt;' if a VCN needs to be normal peered with some other VCN and specify 'none' in case it is none of these.
 </t>
-  </si>
-  <si>
-    <t>Automation Toolkit release verion- v6.0
-Tabs Affected: Subnets
-Major Feature - Support for NonGreenField Tenancies</t>
   </si>
   <si>
     <t>VM.Standard.E3.Flex::5</t>
@@ -1414,6 +1401,22 @@
   <si>
     <t>LBR Subnets: specify a single regional subnet name (recommended) or two comma seperated subnet names(AD specific) for public Load Balancer and provide a single subnet(Regional or AD specific) for Private load Balancer- subnets names should be same as defined in Subnets tab, Backend ServerName:Port- specify comma separated list of servernames:ports(either specify server name as same name defined in Instances sheet or specify the IP address); LBR Hostname can be null, LBR Hostname is to be left empty if creating TCP listener; all other fields are mandatory; Backend HealthCheck URL is required if Backend HealthCheck Protocol is HTTP; If you want to create an HTTPS Listener, please specify ListenerProtocol as HTTP and UseSSL as y; Allows multiple Listeners(seperate rows) per LBR and multiple Hostnames(comma seperated) per Listener
 #Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;</t>
+  </si>
+  <si>
+    <t>20.20.20.20/32</t>
+  </si>
+  <si>
+    <t>Columns: Region, Compartment Name, Availability Domain, MountTarget Name, MountTarget SubnetName, FSS name, Path are mandatory.
+Default value for columns if left blank: sourceCIDR- 0.0.0.0/0, Access- READ_ONLY, GID- 65534, UID- 65534, IDSquash- NONE and require_ps_port- false
+Mount target IP, FSS Capacity, FSS Inodes will take default values from OCI if left blank
+Resources will be created based on MountTargetName and FSSName columns.
+#Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
+Below sample data shows example of  multiple FSS(FSS1 and FSS2) using single MT(MT1) , 1 FSS(FSS3) using multiple MTs(MT2 and MT3) and also 1 FSS(FSS4) using 1 MT(MT4); Also shows multiple export options</t>
+  </si>
+  <si>
+    <t>Automation Toolkit release verion- v6.1
+Tabs Affected: SecRulesinOCI, RouteRulesinOCI, FSS, LBR, Instances
+Major Feature - Support for Duplicate Compartment Names, New GIT Repo</t>
   </si>
 </sst>
 </file>
@@ -2230,8 +2233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2241,7 +2244,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="43" t="s">
-        <v>329</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -2272,7 +2275,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="30" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -2486,7 +2489,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -2524,7 +2527,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -2566,13 +2569,13 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>106</v>
@@ -2602,13 +2605,13 @@
         <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>77</v>
@@ -2698,7 +2701,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>151</v>
@@ -2765,7 +2768,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -2830,7 +2833,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -2848,7 +2851,7 @@
         <v>132</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>133</v>
@@ -2857,7 +2860,7 @@
         <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>83</v>
@@ -2872,7 +2875,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -2881,29 +2884,29 @@
         <v>130</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="I4" s="46" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="N4" s="1"/>
     </row>
@@ -2912,7 +2915,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -2921,29 +2924,29 @@
         <v>131</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I5" s="46" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>83</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="N5" s="1"/>
     </row>
@@ -3017,7 +3020,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C3" s="1">
         <v>150</v>
@@ -3026,13 +3029,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>134</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>83</v>
@@ -3043,7 +3046,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C4" s="1">
         <v>150</v>
@@ -3052,13 +3055,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>134</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>83</v>
@@ -3094,10 +3097,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3116,9 +3119,9 @@
     <col min="17" max="17" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="89.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>320</v>
+        <v>401</v>
       </c>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -3195,7 +3198,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>153</v>
@@ -3223,34 +3226,26 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>307</v>
-      </c>
+    <row r="4" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>268</v>
-      </c>
+      <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+        <v>264</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -3261,13 +3256,13 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>250</v>
+        <v>153</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>265</v>
+        <v>171</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>307</v>
@@ -3277,17 +3272,13 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>267</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -3298,13 +3289,13 @@
         <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>250</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>307</v>
@@ -3320,10 +3311,10 @@
         <v>261</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -3335,13 +3326,13 @@
         <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>250</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>307</v>
@@ -3351,38 +3342,75 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+        <v>261</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="30" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="27"/>
+        <v>101</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>307</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3397,7 +3425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -3427,7 +3455,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -3469,7 +3497,7 @@
         <v>177</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H2" s="27" t="s">
         <v>178</v>
@@ -3516,10 +3544,10 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>185</v>
@@ -3531,10 +3559,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>186</v>
@@ -3555,7 +3583,7 @@
         <v>443</v>
       </c>
       <c r="O3" s="27" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>13</v>
@@ -3574,10 +3602,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>185</v>
@@ -3589,13 +3617,13 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>181</v>
@@ -3613,7 +3641,7 @@
         <v>443</v>
       </c>
       <c r="O4" s="27" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>13</v>
@@ -3632,13 +3660,13 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>307</v>
@@ -3647,23 +3675,23 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>186</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K5" s="1">
         <v>80</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="N5" s="1">
         <v>80</v>
@@ -3707,7 +3735,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="16" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="66" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -3945,7 +3973,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>137</v>
@@ -3962,7 +3990,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>138</v>
@@ -4030,7 +4058,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>137</v>
@@ -4047,7 +4075,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>138</v>
@@ -4110,10 +4138,10 @@
         <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -4122,13 +4150,13 @@
         <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>353</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4136,13 +4164,13 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
@@ -4150,10 +4178,10 @@
         <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -4162,13 +4190,13 @@
         <v>100</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4176,13 +4204,13 @@
         <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4190,13 +4218,13 @@
         <v>100</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>368</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4204,13 +4232,13 @@
         <v>100</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -4500,7 +4528,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="32" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="67" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -4601,10 +4629,10 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>8</v>
@@ -4672,10 +4700,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>8</v>
@@ -4856,7 +4884,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="32" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="67" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -4958,10 +4986,10 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>153</v>
@@ -5029,10 +5057,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>250</v>
@@ -5171,7 +5199,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="32" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="67" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -5272,16 +5300,16 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F3" s="38" t="s">
         <v>299</v>
@@ -5455,7 +5483,7 @@
         <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -5463,10 +5491,10 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -5474,10 +5502,10 @@
         <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -5584,7 +5612,7 @@
         <v>53</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -5592,10 +5620,10 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>58</v>
@@ -5604,10 +5632,10 @@
         <v>81</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -5615,10 +5643,10 @@
         <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>58</v>
@@ -5627,10 +5655,10 @@
         <v>81</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -5665,7 +5693,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -5718,7 +5746,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -5739,7 +5767,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
@@ -5753,10 +5781,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>121</v>
@@ -5774,7 +5802,7 @@
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>310</v>
@@ -5786,10 +5814,10 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>311</v>
@@ -5807,7 +5835,7 @@
         <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>310</v>
@@ -5880,7 +5908,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="192.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="55" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B1" s="56"/>
     </row>
@@ -5993,7 +6021,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -6016,10 +6044,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>10</v>
@@ -6036,10 +6064,10 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>128</v>
@@ -6101,7 +6129,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -6149,7 +6177,7 @@
         <v>149</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>4</v>
@@ -6178,7 +6206,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -6206,7 +6234,7 @@
         <v>13</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>13</v>
@@ -6227,10 +6255,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>123</v>
@@ -6253,7 +6281,7 @@
         <v>13</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>13</v>
@@ -6274,10 +6302,10 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>124</v>
@@ -6300,7 +6328,7 @@
         <v>13</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>13</v>
@@ -6321,16 +6349,16 @@
         <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>0</v>
@@ -6343,7 +6371,7 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>14</v>
@@ -6370,16 +6398,16 @@
         <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>124</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>0</v>
@@ -6392,7 +6420,7 @@
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
@@ -6419,16 +6447,16 @@
         <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>0</v>
@@ -6441,13 +6469,13 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>14</v>
@@ -6570,7 +6598,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="30" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>

</xml_diff>

<commit_message>
updated Instances and ReleaseNotes
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="404">
   <si>
     <t>Regional</t>
   </si>
@@ -1132,12 +1132,6 @@
     <t>app2.example.com,app3.example.com</t>
   </si>
   <si>
-    <t>LinuxFlex</t>
-  </si>
-  <si>
-    <t>WindowsFlex</t>
-  </si>
-  <si>
     <t># Horizontal row specifies the TagNameSpace Names to be created; Vertical column under each TagNameSpace represnts Keys in that tagnamespace; Enter compartment name in which  all tagnamespaces and keys will be created;
 Enter Region as your tenancy's Home Region for Tags Creation</t>
   </si>
@@ -1266,9 +1260,6 @@
   </si>
   <si>
     <t>TCCInstance</t>
-  </si>
-  <si>
-    <t>DNS-Server-PhxHub</t>
   </si>
   <si>
     <t>PHXEBS-VCN_qa-subnet</t>
@@ -1414,9 +1405,21 @@
 Below sample data shows example of  multiple FSS(FSS1 and FSS2) using single MT(MT1) , 1 FSS(FSS3) using multiple MTs(MT2 and MT3) and also 1 FSS(FSS4) using 1 MT(MT4); Also shows multiple export options</t>
   </si>
   <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>LinuxLatest</t>
+  </si>
+  <si>
+    <t>DNS-Server1-PhxHub</t>
+  </si>
+  <si>
+    <t>DNS-Server2-PhxHub</t>
+  </si>
+  <si>
     <t>Automation Toolkit release verion- v6.1
-Tabs Affected: SecRulesinOCI, RouteRulesinOCI, FSS, LBR, Instances
-Major Feature - Support for Duplicate Compartment Names, New GIT Repo</t>
+Tabs Affected: SecRulesinOCI, RouteRulesinOCI, VCN Info, FSS, LBR, Instances
+Major Features - Support for Duplicate Compartment Names, New GIT Repo</t>
   </si>
 </sst>
 </file>
@@ -2244,7 +2247,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="43" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -2489,7 +2492,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -2527,7 +2530,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -2569,13 +2572,13 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>106</v>
@@ -2605,13 +2608,13 @@
         <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>77</v>
@@ -2701,7 +2704,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>151</v>
@@ -2742,10 +2745,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2833,13 +2836,13 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>307</v>
@@ -2851,16 +2854,16 @@
         <v>132</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>133</v>
+        <v>284</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>83</v>
@@ -2870,68 +2873,68 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>387</v>
+        <v>402</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>390</v>
+        <v>307</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="I4" s="46" t="s">
-        <v>328</v>
+        <v>400</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>284</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="N4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="1" t="s">
-        <v>344</v>
+        <v>399</v>
       </c>
       <c r="I5" s="46" t="s">
         <v>328</v>
@@ -2940,15 +2943,55 @@
         <v>9</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>392</v>
+        <v>351</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>83</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="N5" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="I6" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="N6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3020,7 +3063,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C3" s="1">
         <v>150</v>
@@ -3029,13 +3072,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>134</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>83</v>
@@ -3046,7 +3089,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C4" s="1">
         <v>150</v>
@@ -3055,13 +3098,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>134</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>83</v>
@@ -3121,7 +3164,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="89.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -3198,7 +3241,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>153</v>
@@ -3241,7 +3284,7 @@
         <v>264</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>267</v>
@@ -3256,7 +3299,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>153</v>
@@ -3289,7 +3332,7 @@
         <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>250</v>
@@ -3326,7 +3369,7 @@
         <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>250</v>
@@ -3363,7 +3406,7 @@
         <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>250</v>
@@ -3455,7 +3498,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -3544,7 +3587,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>333</v>
@@ -3602,7 +3645,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>333</v>
@@ -3660,7 +3703,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>334</v>
@@ -3735,7 +3778,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="16" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="66" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -3973,7 +4016,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>137</v>
@@ -3990,7 +4033,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>138</v>
@@ -4058,7 +4101,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>137</v>
@@ -4075,7 +4118,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>138</v>
@@ -4138,10 +4181,10 @@
         <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -4150,13 +4193,13 @@
         <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4164,13 +4207,13 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
@@ -4178,10 +4221,10 @@
         <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -4190,13 +4233,13 @@
         <v>100</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4204,13 +4247,13 @@
         <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>355</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4218,13 +4261,13 @@
         <v>100</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>366</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -4232,13 +4275,13 @@
         <v>100</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -4629,10 +4672,10 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>8</v>
@@ -4700,10 +4743,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>8</v>
@@ -4986,10 +5029,10 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>153</v>
@@ -5057,10 +5100,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>250</v>
@@ -5300,16 +5343,16 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F3" s="38" t="s">
         <v>299</v>
@@ -5483,7 +5526,7 @@
         <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -5491,10 +5534,10 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -5502,10 +5545,10 @@
         <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -5612,7 +5655,7 @@
         <v>53</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -5620,10 +5663,10 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>58</v>
@@ -5632,10 +5675,10 @@
         <v>81</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.35">
@@ -5643,10 +5686,10 @@
         <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>58</v>
@@ -5655,10 +5698,10 @@
         <v>81</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -5746,7 +5789,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -5767,7 +5810,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
@@ -5781,10 +5824,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>121</v>
@@ -5802,7 +5845,7 @@
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>310</v>
@@ -5814,10 +5857,10 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>311</v>
@@ -5835,7 +5878,7 @@
         <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>310</v>
@@ -5908,7 +5951,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="192.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="55" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B1" s="56"/>
     </row>
@@ -6021,7 +6064,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -6044,10 +6087,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>10</v>
@@ -6064,10 +6107,10 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>128</v>
@@ -6206,7 +6249,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -6234,7 +6277,7 @@
         <v>13</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>13</v>
@@ -6255,10 +6298,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>123</v>
@@ -6281,7 +6324,7 @@
         <v>13</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>13</v>
@@ -6302,10 +6345,10 @@
         <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>124</v>
@@ -6328,7 +6371,7 @@
         <v>13</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>13</v>
@@ -6349,16 +6392,16 @@
         <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>0</v>
@@ -6371,7 +6414,7 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>14</v>
@@ -6398,16 +6441,16 @@
         <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>124</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>0</v>
@@ -6420,7 +6463,7 @@
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
@@ -6447,16 +6490,16 @@
         <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>0</v>
@@ -6469,13 +6512,13 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
CD3 - Excel sheet updated for DB and FSS
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oci_develop\oci_tenancy\SetUpOCI_Via_TF\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ocifromnewgit\oci_tenancy\SetUpOCI_Via_TF\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8020" firstSheet="19" activeTab="25"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,11 @@
     <definedName name="Action_Values" localSheetId="17">'Rule Set Dropdown'!$A$2:$A$12</definedName>
     <definedName name="Allowed_Methods" localSheetId="17">'Rule Set Dropdown'!$B$2:$B$41</definedName>
     <definedName name="Attribute_Names" localSheetId="17">'Rule Set Dropdown'!$D$2:$D$5</definedName>
+    <definedName name="bm_shapes_drop">Database_Dropdown!$F$2:$F$3</definedName>
+    <definedName name="db_sersion_drop">Database_Dropdown!$C$2:$C$14</definedName>
+    <definedName name="exa_shapes_drop">Database_Dropdown!$E$2:$E$8</definedName>
     <definedName name="Header_Size">'Rule Set Dropdown'!$F$2:$F$6</definedName>
+    <definedName name="license_type_drop">Database_Dropdown!$G$2:$G$3</definedName>
     <definedName name="Match_Style" localSheetId="18">'Rule Set Dropdown'!$C$2:$C$6</definedName>
     <definedName name="Match_Style" localSheetId="17">'Rule Set Dropdown'!$C$2:$C$6</definedName>
     <definedName name="Response_Code">'Rule Set Dropdown'!$E$2:$E$7</definedName>
@@ -57,15 +61,18 @@
     <definedName name="Shape_Option" localSheetId="23">#REF!</definedName>
     <definedName name="Shape_Option">#REF!</definedName>
     <definedName name="Shape_Option_DB">[1]Database!$B$10:$J$10</definedName>
+    <definedName name="software_drop">Database_Dropdown!$B$2:$B$5</definedName>
     <definedName name="VM_Shapes" localSheetId="26">Database_Dropdown!$A$2:$A$12</definedName>
     <definedName name="VM_Shapes">DB_System_VM!$Y$397:$Y$407</definedName>
+    <definedName name="VM_shapes_drop">Database_Dropdown!$A$2:$A$12</definedName>
+    <definedName name="workload_drop">Database_Dropdown!$D$2:$D$3</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="555">
   <si>
     <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
 Leave "Parent Compartment" empty or mention 'root' if it is under 'root' compartment;
@@ -1826,6 +1833,9 @@
   </si>
   <si>
     <t>PHXEBS-VCN_dev-subnet</t>
+  </si>
+  <si>
+    <t>phx-nsg1,phx-nsg2</t>
   </si>
 </sst>
 </file>
@@ -2168,7 +2178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2307,7 +2317,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -2322,25 +2331,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyProtection="1">
@@ -2354,9 +2350,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2429,14 +2422,16 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2824,16 +2819,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="167.08984375" style="49" customWidth="1"/>
+    <col min="1" max="1" width="167.109375" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -2852,38 +2847,38 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="49" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" style="49" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" style="49" customWidth="1"/>
-    <col min="4" max="4" width="33.08984375" style="49" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.08984375" style="49" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="49" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="49" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" style="49" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="104"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="98"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -2945,52 +2940,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:T7"/>
+    <sheetView zoomScale="91" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.08984375" style="49" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.81640625" style="49" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="49" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" style="49" customWidth="1"/>
     <col min="11" max="11" width="19" style="49" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.08984375" style="49" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="106" t="s">
+    <row r="1" spans="1:20" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="107"/>
-      <c r="S1" s="107"/>
-      <c r="T1" s="107"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="101"/>
+      <c r="P1" s="101"/>
+      <c r="Q1" s="101"/>
+      <c r="R1" s="101"/>
+      <c r="S1" s="101"/>
+      <c r="T1" s="101"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
@@ -3045,14 +3040,14 @@
       <c r="R2" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="S2" s="95" t="s">
+      <c r="S2" s="89" t="s">
         <v>551</v>
       </c>
-      <c r="T2" s="95" t="s">
+      <c r="T2" s="89" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -3076,7 +3071,7 @@
       <c r="S3" s="50"/>
       <c r="T3" s="50"/>
     </row>
-    <row r="4" spans="1:20" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -3116,7 +3111,7 @@
       <c r="S4" s="50"/>
       <c r="T4" s="50"/>
     </row>
-    <row r="5" spans="1:20" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>6</v>
       </c>
@@ -3160,7 +3155,7 @@
       <c r="S5" s="50"/>
       <c r="T5" s="50"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>6</v>
       </c>
@@ -3198,7 +3193,7 @@
       <c r="S6" s="50"/>
       <c r="T6" s="50"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
         <v>6</v>
       </c>
@@ -3254,29 +3249,29 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.1796875" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" style="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="49" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="104"/>
-    </row>
-    <row r="2" spans="1:6" s="57" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="98"/>
+    </row>
+    <row r="2" spans="1:6" s="57" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
@@ -3296,7 +3291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -3306,7 +3301,7 @@
       <c r="E3" s="50"/>
       <c r="F3" s="50"/>
     </row>
-    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -3326,7 +3321,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>6</v>
       </c>
@@ -3346,7 +3341,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>6</v>
       </c>
@@ -3379,46 +3374,46 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView zoomScale="81" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="49" customWidth="1"/>
-    <col min="2" max="2" width="26.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" style="49" customWidth="1"/>
-    <col min="6" max="6" width="24.1796875" style="49" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.81640625" style="49" customWidth="1"/>
-    <col min="10" max="10" width="22.08984375" style="49" customWidth="1"/>
-    <col min="11" max="11" width="26.81640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" style="49" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" style="49" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.77734375" style="49" customWidth="1"/>
+    <col min="10" max="10" width="22.109375" style="49" customWidth="1"/>
+    <col min="11" max="11" width="26.77734375" style="49" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="49" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.1796875" style="49" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.21875" style="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="100.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:14" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="104"/>
-    </row>
-    <row r="2" spans="1:14" s="57" customFormat="1" ht="52.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="98"/>
+    </row>
+    <row r="2" spans="1:14" s="57" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
@@ -3462,7 +3457,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -3480,7 +3475,7 @@
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -3522,7 +3517,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>6</v>
       </c>
@@ -3562,7 +3557,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="59" t="s">
         <v>6</v>
       </c>
@@ -3602,7 +3597,7 @@
       </c>
       <c r="N6" s="50"/>
     </row>
-    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="59" t="s">
         <v>6</v>
       </c>
@@ -3659,30 +3654,30 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="49" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
     <col min="2" max="2" width="23" style="49" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" style="49" customWidth="1"/>
-    <col min="7" max="7" width="26.81640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" style="49" customWidth="1"/>
+    <col min="7" max="7" width="26.77734375" style="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="58.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="104"/>
-    </row>
-    <row r="2" spans="1:8" s="57" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="98"/>
+    </row>
+    <row r="2" spans="1:8" s="57" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -3708,7 +3703,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -3720,7 +3715,7 @@
       <c r="G3" s="50"/>
       <c r="H3" s="50"/>
     </row>
-    <row r="4" spans="1:8" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -3746,7 +3741,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>6</v>
       </c>
@@ -3783,50 +3778,52 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScale="89" workbookViewId="0">
-      <selection activeCell="E2" sqref="E1:E1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.453125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" style="49" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" style="49" customWidth="1"/>
-    <col min="5" max="5" width="20.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.90625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="49" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="49" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="49" customWidth="1"/>
     <col min="7" max="7" width="15" style="49" customWidth="1"/>
-    <col min="8" max="8" width="8.36328125" style="49" customWidth="1"/>
-    <col min="9" max="9" width="9.81640625" style="49" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="49" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" style="49" customWidth="1"/>
     <col min="10" max="10" width="16" style="49" customWidth="1"/>
-    <col min="11" max="11" width="19.1796875" style="49" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" style="49" customWidth="1"/>
-    <col min="13" max="13" width="12.1796875" style="49" customWidth="1"/>
-    <col min="14" max="14" width="17.08984375" style="49" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" style="49" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" style="49" customWidth="1"/>
+    <col min="12" max="12" width="7.77734375" style="49" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" style="49" customWidth="1"/>
+    <col min="14" max="14" width="17.109375" style="49" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" style="49" customWidth="1"/>
+    <col min="16" max="16" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:16" ht="84.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="104"/>
-    </row>
-    <row r="2" spans="1:15" s="3" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+    </row>
+    <row r="2" spans="1:16" s="3" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -3872,8 +3869,11 @@
       <c r="O2" s="14" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P2" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -3891,8 +3891,9 @@
       <c r="M3" s="50"/>
       <c r="N3" s="50"/>
       <c r="O3" s="50"/>
-    </row>
-    <row r="4" spans="1:15" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P3" s="50"/>
+    </row>
+    <row r="4" spans="1:16" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>6</v>
       </c>
@@ -3924,8 +3925,11 @@
       <c r="M4" s="32"/>
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P4" s="48" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="32"/>
       <c r="B5" s="50"/>
       <c r="C5" s="32"/>
@@ -3947,8 +3951,9 @@
       <c r="M5" s="32"/>
       <c r="N5" s="32"/>
       <c r="O5" s="32"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P5" s="50"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="32"/>
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
@@ -3969,8 +3974,9 @@
       <c r="M6" s="32"/>
       <c r="N6" s="32"/>
       <c r="O6" s="32"/>
-    </row>
-    <row r="7" spans="1:15" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P6" s="50"/>
+    </row>
+    <row r="7" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>6</v>
       </c>
@@ -4000,8 +4006,9 @@
       <c r="M7" s="32"/>
       <c r="N7" s="32"/>
       <c r="O7" s="32"/>
-    </row>
-    <row r="8" spans="1:15" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P7" s="50"/>
+    </row>
+    <row r="8" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>6</v>
       </c>
@@ -4035,8 +4042,11 @@
       <c r="M8" s="32"/>
       <c r="N8" s="32"/>
       <c r="O8" s="32"/>
-    </row>
-    <row r="9" spans="1:15" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P8" s="50" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
         <v>6</v>
       </c>
@@ -4070,8 +4080,9 @@
       <c r="M9" s="32"/>
       <c r="N9" s="32"/>
       <c r="O9" s="32"/>
-    </row>
-    <row r="10" spans="1:15" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P9" s="50"/>
+    </row>
+    <row r="10" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
         <v>6</v>
       </c>
@@ -4101,10 +4112,11 @@
       <c r="M10" s="32"/>
       <c r="N10" s="32"/>
       <c r="O10" s="32"/>
+      <c r="P10" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -4116,43 +4128,43 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.6328125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" style="49" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" style="49" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="49" customWidth="1"/>
-    <col min="6" max="6" width="18.90625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="49" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="49" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" style="49" customWidth="1"/>
     <col min="8" max="8" width="25" style="49" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" style="49" customWidth="1"/>
-    <col min="11" max="11" width="7.453125" style="49" customWidth="1"/>
-    <col min="13" max="13" width="28.1796875" style="49" customWidth="1"/>
-    <col min="14" max="14" width="13.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" style="49" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" style="49" customWidth="1"/>
+    <col min="13" max="13" width="28.21875" style="49" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+    <row r="1" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-    </row>
-    <row r="2" spans="1:15" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+    </row>
+    <row r="2" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
@@ -4199,7 +4211,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>5</v>
       </c>
@@ -4218,7 +4230,7 @@
       <c r="N3" s="50"/>
       <c r="O3" s="50"/>
     </row>
-    <row r="4" spans="1:15" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -4255,11 +4267,11 @@
       <c r="N4" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="O4" s="93" t="s">
+      <c r="O4" s="87" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -4282,7 +4294,7 @@
       <c r="N5" s="50"/>
       <c r="O5" s="50"/>
     </row>
-    <row r="6" spans="1:15" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>6</v>
       </c>
@@ -4339,46 +4351,46 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.1796875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" style="49" customWidth="1"/>
     <col min="3" max="3" width="11" style="49" customWidth="1"/>
-    <col min="4" max="5" width="10.90625" style="49" customWidth="1"/>
+    <col min="4" max="5" width="10.88671875" style="49" customWidth="1"/>
     <col min="6" max="6" width="18" style="49" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" style="49" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" style="49" customWidth="1"/>
-    <col min="9" max="9" width="11.90625" style="49" customWidth="1"/>
-    <col min="10" max="10" width="14.6328125" style="49" customWidth="1"/>
-    <col min="11" max="11" width="14.36328125" style="49" customWidth="1"/>
-    <col min="13" max="13" width="23.6328125" style="49" customWidth="1"/>
-    <col min="15" max="15" width="12.6328125" style="49" customWidth="1"/>
-    <col min="16" max="16" width="14.81640625" style="49" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" style="49" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" style="49" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" style="49" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="49" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="49" customWidth="1"/>
+    <col min="13" max="13" width="23.6640625" style="49" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" style="49" customWidth="1"/>
+    <col min="16" max="16" width="14.77734375" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+    <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="104"/>
-    </row>
-    <row r="2" spans="1:16" ht="58.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="98"/>
+    </row>
+    <row r="2" spans="1:16" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
@@ -4428,7 +4440,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -4448,7 +4460,7 @@
       <c r="O3" s="50"/>
       <c r="P3" s="50"/>
     </row>
-    <row r="4" spans="1:16" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -4496,7 +4508,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -4534,7 +4546,7 @@
       </c>
       <c r="P5" s="50"/>
     </row>
-    <row r="6" spans="1:16" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>6</v>
       </c>
@@ -4589,49 +4601,49 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="79" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.81640625" style="49" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" style="49" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" style="49" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" style="49" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" style="49" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" style="49" customWidth="1"/>
-    <col min="9" max="9" width="13.6328125" style="49" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" style="49" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" style="49" customWidth="1"/>
-    <col min="13" max="13" width="15.1796875" style="49" customWidth="1"/>
-    <col min="14" max="15" width="13.81640625" style="49" customWidth="1"/>
-    <col min="16" max="16" width="21.08984375" style="49" customWidth="1"/>
-    <col min="17" max="17" width="17.1796875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="49" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" style="49" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" style="49" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="49" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" style="49" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" style="49" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="49" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" style="49" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" style="49" customWidth="1"/>
+    <col min="13" max="13" width="15.21875" style="49" customWidth="1"/>
+    <col min="14" max="15" width="13.77734375" style="49" customWidth="1"/>
+    <col min="16" max="16" width="21.109375" style="49" customWidth="1"/>
+    <col min="17" max="17" width="17.21875" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="157.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="99" t="s">
+    <row r="1" spans="1:18" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="93" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="101"/>
-    </row>
-    <row r="2" spans="1:18" ht="58.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
+      <c r="R1" s="95"/>
+    </row>
+    <row r="2" spans="1:18" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -4687,7 +4699,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -4709,7 +4721,7 @@
       <c r="Q3" s="50"/>
       <c r="R3" s="50"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -4741,7 +4753,7 @@
       </c>
       <c r="R4" s="50"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -4763,7 +4775,7 @@
       <c r="Q5" s="50"/>
       <c r="R5" s="50"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="50"/>
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
@@ -4785,7 +4797,7 @@
       <c r="Q6" s="50"/>
       <c r="R6" s="50"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="50"/>
       <c r="B7" s="50"/>
       <c r="C7" s="50"/>
@@ -4807,7 +4819,7 @@
       <c r="Q7" s="50"/>
       <c r="R7" s="50"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="50"/>
       <c r="B8" s="50"/>
       <c r="C8" s="50"/>
@@ -4829,7 +4841,7 @@
       <c r="Q8" s="50"/>
       <c r="R8" s="50"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="50"/>
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
@@ -4855,7 +4867,7 @@
       <c r="Q9" s="50"/>
       <c r="R9" s="50"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
@@ -4883,7 +4895,7 @@
       <c r="Q10" s="50"/>
       <c r="R10" s="50"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="50"/>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
@@ -4917,7 +4929,7 @@
       <c r="Q11" s="50"/>
       <c r="R11" s="50"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="50"/>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
@@ -4951,7 +4963,7 @@
       <c r="Q12" s="50"/>
       <c r="R12" s="50"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
@@ -4977,7 +4989,7 @@
       <c r="Q13" s="50"/>
       <c r="R13" s="50"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50"/>
@@ -5003,7 +5015,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="50"/>
       <c r="B15" s="50"/>
       <c r="C15" s="50"/>
@@ -5027,7 +5039,7 @@
       <c r="Q15" s="50"/>
       <c r="R15" s="50"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="50"/>
       <c r="B16" s="50"/>
       <c r="C16" s="50"/>
@@ -5053,7 +5065,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="50"/>
       <c r="B17" s="50"/>
       <c r="C17" s="50"/>
@@ -5077,7 +5089,7 @@
       <c r="Q17" s="50"/>
       <c r="R17" s="50"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="50"/>
       <c r="B18" s="50"/>
       <c r="C18" s="50"/>
@@ -5103,7 +5115,7 @@
       <c r="Q18" s="50"/>
       <c r="R18" s="50"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="50"/>
       <c r="B19" s="50"/>
       <c r="C19" s="50"/>
@@ -5123,7 +5135,7 @@
       <c r="Q19" s="50"/>
       <c r="R19" s="50"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="50"/>
       <c r="B20" s="50"/>
       <c r="C20" s="50" t="s">
@@ -5149,7 +5161,7 @@
       <c r="Q20" s="50"/>
       <c r="R20" s="50"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="50"/>
       <c r="B21" s="50"/>
       <c r="C21" s="50"/>
@@ -5171,7 +5183,7 @@
       <c r="Q21" s="50"/>
       <c r="R21" s="50"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="50" t="s">
         <v>6</v>
       </c>
@@ -5201,7 +5213,7 @@
       <c r="Q22" s="50"/>
       <c r="R22" s="50"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="50"/>
       <c r="B23" s="50"/>
       <c r="C23" s="50"/>
@@ -5260,25 +5272,25 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.36328125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="26.08984375" style="49" customWidth="1"/>
-    <col min="4" max="4" width="20.08984375" style="49" customWidth="1"/>
-    <col min="6" max="6" width="28.6328125" style="49" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="49" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" style="49" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="49" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="57" customFormat="1" ht="82.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="99" t="s">
+    <row r="1" spans="1:6" s="57" customFormat="1" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="93" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="101"/>
-    </row>
-    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="95"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
@@ -5298,7 +5310,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -5308,7 +5320,7 @@
       <c r="E3" s="50"/>
       <c r="F3" s="50"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -5328,7 +5340,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -5342,7 +5354,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="50"/>
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
@@ -5358,7 +5370,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
         <v>6</v>
       </c>
@@ -5399,23 +5411,23 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="49" customWidth="1"/>
-    <col min="2" max="2" width="22.6328125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="40.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.54296875" style="49" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="57" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:4" s="57" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="98"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="92"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -5429,7 +5441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -5437,7 +5449,7 @@
       <c r="C3" s="33"/>
       <c r="D3" s="35"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -5449,7 +5461,7 @@
       </c>
       <c r="D4" s="50"/>
     </row>
-    <row r="5" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>6</v>
       </c>
@@ -5463,7 +5475,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>6</v>
       </c>
@@ -5477,7 +5489,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
         <v>6</v>
       </c>
@@ -5489,7 +5501,7 @@
       </c>
       <c r="D7" s="50"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
         <v>6</v>
       </c>
@@ -5503,7 +5515,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="50" t="s">
         <v>6</v>
       </c>
@@ -5517,7 +5529,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="50" t="s">
         <v>6</v>
       </c>
@@ -5531,7 +5543,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="50" t="s">
         <v>6</v>
       </c>
@@ -5559,40 +5571,40 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.54296875" style="49" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="49" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" style="49" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" style="49" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" style="49" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" style="49" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="49" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="49" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" style="49" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="49" customWidth="1"/>
     <col min="9" max="9" width="15" style="49" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" style="49" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="113.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="108" t="s">
+    <row r="1" spans="1:14" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="102" t="s">
         <v>272</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-    </row>
-    <row r="2" spans="1:14" ht="46.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+    </row>
+    <row r="2" spans="1:14" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -5636,7 +5648,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -5654,7 +5666,7 @@
       <c r="M3" s="50"/>
       <c r="N3" s="50"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -5686,11 +5698,11 @@
       <c r="M4" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="N4" s="94" t="s">
+      <c r="N4" s="88" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
       <c r="C5" s="50" t="s">
@@ -5714,7 +5726,7 @@
       <c r="M5" s="50"/>
       <c r="N5" s="50"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>6</v>
       </c>
@@ -5771,17 +5783,17 @@
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="28.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.453125" style="49" customWidth="1"/>
-    <col min="2" max="2" width="35.08984375" style="49" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="26.81640625" style="49" customWidth="1"/>
-    <col min="5" max="5" width="17.6328125" style="49" customWidth="1"/>
-    <col min="6" max="6" width="17.90625" style="49" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" style="49" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" style="49" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="49" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>284</v>
       </c>
@@ -5801,7 +5813,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>246</v>
       </c>
@@ -5821,7 +5833,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>250</v>
       </c>
@@ -5841,7 +5853,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>230</v>
       </c>
@@ -5861,7 +5873,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>223</v>
       </c>
@@ -5879,7 +5891,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>243</v>
       </c>
@@ -5892,7 +5904,7 @@
       </c>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>255</v>
       </c>
@@ -5901,7 +5913,7 @@
       </c>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>229</v>
       </c>
@@ -5909,7 +5921,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>234</v>
       </c>
@@ -5917,7 +5929,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>248</v>
       </c>
@@ -5925,7 +5937,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>253</v>
       </c>
@@ -5933,153 +5945,153 @@
         <v>298</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
       <c r="B12" s="36" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="36" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="36" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="36" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="36" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="36" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="36" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="36" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="36" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="36" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="36" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="36" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="36" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="36" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="36" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="28" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="36" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="36" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="30" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="36" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="36" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="32" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="36" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="36" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="36" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="36" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="36" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="36" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="38" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="36" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="36" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="40" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="36" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="41" spans="2:2" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="12"/>
     </row>
   </sheetData>
@@ -6093,38 +6105,38 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="19.1796875" style="49" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="49" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" style="49" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" style="49" customWidth="1"/>
-    <col min="6" max="6" width="22.36328125" style="49" customWidth="1"/>
-    <col min="7" max="7" width="21.6328125" style="49" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="19.21875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="49" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="49" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="49" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="49" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="49" customWidth="1"/>
     <col min="8" max="8" width="21" style="49" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="15.90625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
         <v>490</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="104"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="98"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
@@ -6156,7 +6168,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="56" t="s">
         <v>5</v>
       </c>
@@ -6170,7 +6182,7 @@
       <c r="I3" s="55"/>
       <c r="J3" s="56"/>
     </row>
-    <row r="4" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="63" t="s">
         <v>6</v>
       </c>
@@ -6200,7 +6212,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="63"/>
       <c r="B5" s="37"/>
       <c r="C5" s="38"/>
@@ -6222,7 +6234,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="63" t="s">
         <v>6</v>
       </c>
@@ -6242,7 +6254,7 @@
       <c r="I6" s="39"/>
       <c r="J6" s="40"/>
     </row>
-    <row r="7" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="63" t="s">
         <v>6</v>
       </c>
@@ -6264,7 +6276,7 @@
       <c r="I7" s="39"/>
       <c r="J7" s="40"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="63"/>
       <c r="B8" s="37"/>
       <c r="C8" s="38"/>
@@ -6278,7 +6290,7 @@
       <c r="I8" s="39"/>
       <c r="J8" s="40"/>
     </row>
-    <row r="9" spans="1:10" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="63" t="s">
         <v>6</v>
       </c>
@@ -6306,7 +6318,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="40"/>
       <c r="B10" s="37"/>
       <c r="C10" s="38"/>
@@ -6320,7 +6332,7 @@
       <c r="I10" s="39"/>
       <c r="J10" s="40"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="63"/>
       <c r="B11" s="37"/>
       <c r="C11" s="41"/>
@@ -6334,7 +6346,7 @@
       <c r="I11" s="39"/>
       <c r="J11" s="40"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="63"/>
       <c r="B12" s="37"/>
       <c r="C12" s="41"/>
@@ -6362,73 +6374,73 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.90625" style="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" style="49" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.90625" style="49"/>
+    <col min="3" max="3" width="16.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="49"/>
     <col min="8" max="8" width="11" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.90625" style="49"/>
+    <col min="9" max="16384" width="8.88671875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="58.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="110" t="s">
+    <row r="1" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="104" t="s">
         <v>495</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="112"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="66" t="s">
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="106"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="65" t="s">
         <v>351</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="65" t="s">
         <v>352</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="66" t="s">
         <v>353</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="65" t="s">
         <v>354</v>
       </c>
-      <c r="G2" s="66" t="s">
+      <c r="G2" s="65" t="s">
         <v>355</v>
       </c>
-      <c r="H2" s="66" t="s">
+      <c r="H2" s="65" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="70" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="69" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
       <c r="D3" s="50"/>
-      <c r="E3" s="68"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="50"/>
       <c r="G3" s="50"/>
       <c r="H3" s="50"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>357</v>
       </c>
@@ -6441,7 +6453,7 @@
       <c r="D4" s="50" t="s">
         <v>358</v>
       </c>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="67" t="s">
         <v>359</v>
       </c>
       <c r="F4" s="50">
@@ -6453,10 +6465,10 @@
       <c r="H4" s="50" t="s">
         <v>360</v>
       </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="65"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I4" s="70"/>
+      <c r="J4" s="64"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>357</v>
       </c>
@@ -6469,7 +6481,7 @@
       <c r="D5" s="50" t="s">
         <v>361</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="67" t="s">
         <v>359</v>
       </c>
       <c r="F5" s="50">
@@ -6481,8 +6493,8 @@
       <c r="H5" s="50" t="s">
         <v>362</v>
       </c>
-      <c r="I5" s="71"/>
-      <c r="J5" s="65"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6496,390 +6508,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="97" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="20.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.54296875" style="49"/>
-    <col min="3" max="3" width="31.26953125" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.54296875" style="49"/>
-    <col min="8" max="8" width="42" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.54296875" style="49"/>
-    <col min="10" max="10" width="23.54296875" style="49" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.1796875" style="81" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.54296875" style="49"/>
-    <col min="14" max="14" width="20.54296875" style="5"/>
-    <col min="15" max="18" width="20.54296875" style="49"/>
+    <col min="1" max="1" width="10.21875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="14" style="49" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="49" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" style="49" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="49" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="49" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" style="49" customWidth="1"/>
+    <col min="9" max="9" width="13" style="49" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" style="49" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="76" customWidth="1"/>
+    <col min="12" max="13" width="20.5546875" style="49"/>
+    <col min="14" max="14" width="20.5546875" style="5"/>
+    <col min="15" max="18" width="20.5546875" style="49"/>
     <col min="19" max="19" width="23" style="49" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="20.54296875" style="49"/>
-    <col min="23" max="23" width="23.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.54296875" style="49"/>
-    <col min="25" max="25" width="23.08984375" style="49" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="20.54296875" style="49"/>
+    <col min="20" max="22" width="20.5546875" style="49"/>
+    <col min="23" max="23" width="23.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.5546875" style="49"/>
+    <col min="25" max="25" width="23.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="20.5546875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="72" customFormat="1" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="113" t="s">
+    <row r="1" spans="1:23" s="71" customFormat="1" ht="101.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="104" t="s">
         <v>498</v>
-      </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="114"/>
-      <c r="R1" s="114"/>
-      <c r="S1" s="114"/>
-      <c r="T1" s="114"/>
-      <c r="U1" s="114"/>
-      <c r="V1" s="114"/>
-      <c r="W1" s="115"/>
-    </row>
-    <row r="2" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="73" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="74" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="73" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="75" t="s">
-        <v>499</v>
-      </c>
-      <c r="F2" s="73" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" s="73" t="s">
-        <v>500</v>
-      </c>
-      <c r="H2" s="73" t="s">
-        <v>501</v>
-      </c>
-      <c r="I2" s="73" t="s">
-        <v>502</v>
-      </c>
-      <c r="J2" s="73" t="s">
-        <v>503</v>
-      </c>
-      <c r="K2" s="76" t="s">
-        <v>504</v>
-      </c>
-      <c r="L2" s="73" t="s">
-        <v>505</v>
-      </c>
-      <c r="M2" s="73" t="s">
-        <v>506</v>
-      </c>
-      <c r="N2" s="77" t="s">
-        <v>507</v>
-      </c>
-      <c r="O2" s="73" t="s">
-        <v>508</v>
-      </c>
-      <c r="P2" s="73" t="s">
-        <v>509</v>
-      </c>
-      <c r="Q2" s="73" t="s">
-        <v>510</v>
-      </c>
-      <c r="R2" s="73" t="s">
-        <v>511</v>
-      </c>
-      <c r="S2" s="73" t="s">
-        <v>512</v>
-      </c>
-      <c r="T2" s="78" t="s">
-        <v>364</v>
-      </c>
-      <c r="U2" s="73" t="s">
-        <v>365</v>
-      </c>
-      <c r="V2" s="73" t="s">
-        <v>366</v>
-      </c>
-      <c r="W2" s="73" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A3" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A4" s="79" t="s">
-        <v>357</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>416</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>553</v>
-      </c>
-      <c r="D4" s="79" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="79" t="s">
-        <v>514</v>
-      </c>
-      <c r="F4" s="79" t="s">
-        <v>386</v>
-      </c>
-      <c r="G4" s="79">
-        <v>2</v>
-      </c>
-      <c r="H4" s="79" t="s">
-        <v>370</v>
-      </c>
-      <c r="I4" s="79">
-        <v>256</v>
-      </c>
-      <c r="J4" s="79" t="s">
-        <v>371</v>
-      </c>
-      <c r="K4" s="79" t="s">
-        <v>372</v>
-      </c>
-      <c r="L4" s="79" t="s">
-        <v>515</v>
-      </c>
-      <c r="M4" s="79" t="s">
-        <v>373</v>
-      </c>
-      <c r="N4" s="80" t="s">
-        <v>516</v>
-      </c>
-      <c r="O4" s="79" t="s">
-        <v>375</v>
-      </c>
-      <c r="P4" s="79" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q4" s="79" t="s">
-        <v>377</v>
-      </c>
-      <c r="R4" s="79" t="s">
-        <v>378</v>
-      </c>
-      <c r="S4" s="79" t="b">
-        <v>1</v>
-      </c>
-      <c r="T4" s="79" t="s">
-        <v>119</v>
-      </c>
-      <c r="U4" s="50" t="s">
-        <v>379</v>
-      </c>
-      <c r="V4" s="50" t="s">
-        <v>380</v>
-      </c>
-      <c r="W4" s="50">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A5" s="79" t="s">
-        <v>357</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>416</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>368</v>
-      </c>
-      <c r="D5" s="79" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="79" t="s">
-        <v>517</v>
-      </c>
-      <c r="F5" s="79" t="s">
-        <v>389</v>
-      </c>
-      <c r="G5" s="79">
-        <v>2</v>
-      </c>
-      <c r="H5" s="79" t="s">
-        <v>395</v>
-      </c>
-      <c r="I5" s="79">
-        <v>256</v>
-      </c>
-      <c r="J5" s="79" t="s">
-        <v>371</v>
-      </c>
-      <c r="K5" s="79" t="s">
-        <v>518</v>
-      </c>
-      <c r="L5" s="79" t="s">
-        <v>519</v>
-      </c>
-      <c r="M5" s="79" t="s">
-        <v>396</v>
-      </c>
-      <c r="N5" s="80" t="s">
-        <v>520</v>
-      </c>
-      <c r="O5" s="79" t="s">
-        <v>397</v>
-      </c>
-      <c r="P5" s="79" t="s">
-        <v>521</v>
-      </c>
-      <c r="Q5" s="79" t="s">
-        <v>377</v>
-      </c>
-      <c r="R5" s="79" t="s">
-        <v>378</v>
-      </c>
-      <c r="S5" s="79" t="b">
-        <v>0</v>
-      </c>
-      <c r="T5" s="79" t="s">
-        <v>119</v>
-      </c>
-      <c r="U5" s="50" t="s">
-        <v>379</v>
-      </c>
-      <c r="V5" s="50" t="s">
-        <v>380</v>
-      </c>
-      <c r="W5" s="50">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:W1"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" sqref="F2"/>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$A$2:$A$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>F3:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$B$2:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>H3:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$G$2:$G$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>K3:K1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$C$2:$C$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>N3:N1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$D$2:$D$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>R3:R1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="7.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.90625" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.90625" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.54296875" style="49" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.81640625" style="81" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" style="49" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.36328125" style="49" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.6328125" style="49" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23" style="49" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.90625" style="49" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.08984375" style="49" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.81640625" style="49"/>
-    <col min="25" max="25" width="14.90625" style="49" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="42" style="49" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.81640625" style="49"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" s="72" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
-        <v>522</v>
       </c>
       <c r="B1" s="105"/>
       <c r="C1" s="105"/>
@@ -6902,81 +6561,414 @@
       <c r="T1" s="105"/>
       <c r="U1" s="105"/>
       <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="83"/>
-    </row>
-    <row r="2" spans="1:24" s="64" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
+      <c r="W1" s="106"/>
+    </row>
+    <row r="2" spans="1:23" s="108" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="E2" s="73" t="s">
         <v>499</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="72" t="s">
+        <v>500</v>
+      </c>
+      <c r="H2" s="72" t="s">
+        <v>501</v>
+      </c>
+      <c r="I2" s="72" t="s">
+        <v>502</v>
+      </c>
+      <c r="J2" s="72" t="s">
+        <v>503</v>
+      </c>
+      <c r="K2" s="73" t="s">
+        <v>504</v>
+      </c>
+      <c r="L2" s="72" t="s">
+        <v>505</v>
+      </c>
+      <c r="M2" s="72" t="s">
+        <v>506</v>
+      </c>
+      <c r="N2" s="72" t="s">
+        <v>507</v>
+      </c>
+      <c r="O2" s="72" t="s">
+        <v>508</v>
+      </c>
+      <c r="P2" s="72" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q2" s="72" t="s">
+        <v>510</v>
+      </c>
+      <c r="R2" s="72" t="s">
+        <v>511</v>
+      </c>
+      <c r="S2" s="72" t="s">
+        <v>512</v>
+      </c>
+      <c r="T2" s="107" t="s">
+        <v>364</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>365</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>366</v>
+      </c>
+      <c r="W2" s="72" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" s="74" t="s">
+        <v>357</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>416</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>553</v>
+      </c>
+      <c r="D4" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="74" t="s">
+        <v>514</v>
+      </c>
+      <c r="F4" s="74" t="s">
+        <v>386</v>
+      </c>
+      <c r="G4" s="74">
+        <v>2</v>
+      </c>
+      <c r="H4" s="74" t="s">
+        <v>370</v>
+      </c>
+      <c r="I4" s="74">
+        <v>256</v>
+      </c>
+      <c r="J4" s="74" t="s">
+        <v>371</v>
+      </c>
+      <c r="K4" s="74" t="s">
+        <v>372</v>
+      </c>
+      <c r="L4" s="74" t="s">
+        <v>515</v>
+      </c>
+      <c r="M4" s="74" t="s">
+        <v>373</v>
+      </c>
+      <c r="N4" s="75" t="s">
+        <v>516</v>
+      </c>
+      <c r="O4" s="74" t="s">
+        <v>375</v>
+      </c>
+      <c r="P4" s="74" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q4" s="74" t="s">
+        <v>377</v>
+      </c>
+      <c r="R4" s="74" t="s">
+        <v>378</v>
+      </c>
+      <c r="S4" s="74" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="U4" s="50" t="s">
+        <v>379</v>
+      </c>
+      <c r="V4" s="50" t="s">
+        <v>380</v>
+      </c>
+      <c r="W4" s="50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" s="74" t="s">
+        <v>357</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>416</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="74" t="s">
+        <v>517</v>
+      </c>
+      <c r="F5" s="74" t="s">
+        <v>389</v>
+      </c>
+      <c r="G5" s="74">
+        <v>2</v>
+      </c>
+      <c r="H5" s="74" t="s">
+        <v>395</v>
+      </c>
+      <c r="I5" s="74">
+        <v>256</v>
+      </c>
+      <c r="J5" s="74" t="s">
+        <v>371</v>
+      </c>
+      <c r="K5" s="74" t="s">
+        <v>518</v>
+      </c>
+      <c r="L5" s="74" t="s">
+        <v>519</v>
+      </c>
+      <c r="M5" s="74" t="s">
+        <v>396</v>
+      </c>
+      <c r="N5" s="75" t="s">
+        <v>520</v>
+      </c>
+      <c r="O5" s="74" t="s">
+        <v>397</v>
+      </c>
+      <c r="P5" s="74" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q5" s="74" t="s">
+        <v>377</v>
+      </c>
+      <c r="R5" s="74" t="s">
+        <v>378</v>
+      </c>
+      <c r="S5" s="74" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="U5" s="50" t="s">
+        <v>379</v>
+      </c>
+      <c r="V5" s="50" t="s">
+        <v>380</v>
+      </c>
+      <c r="W5" s="50">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:W1"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R1048576">
+      <formula1>workload_drop</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
+      <formula1>VM_shapes_drop</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576">
+      <formula1>software_drop</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N1048576">
+      <formula1>db_sersion_drop</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K1048576">
+      <formula1>license_type_drop</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" style="76" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" style="49" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.77734375" style="49"/>
+    <col min="25" max="25" width="14.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="42" style="49" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="49"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="71" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="104" t="s">
+        <v>522</v>
+      </c>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="105"/>
+      <c r="W1" s="106"/>
+      <c r="X1" s="78"/>
+    </row>
+    <row r="2" spans="1:24" s="108" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>499</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="72" t="s">
         <v>393</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="I2" s="73" t="s">
+      <c r="I2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="J2" s="73" t="s">
+      <c r="J2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="109" t="s">
         <v>504</v>
       </c>
-      <c r="L2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="M2" s="73" t="s">
+      <c r="M2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="N2" s="73" t="s">
+      <c r="N2" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="O2" s="73" t="s">
+      <c r="O2" s="72" t="s">
         <v>508</v>
       </c>
-      <c r="P2" s="73" t="s">
+      <c r="P2" s="72" t="s">
         <v>509</v>
       </c>
-      <c r="Q2" s="73" t="s">
+      <c r="Q2" s="72" t="s">
         <v>510</v>
       </c>
-      <c r="R2" s="73" t="s">
+      <c r="R2" s="72" t="s">
         <v>511</v>
       </c>
-      <c r="S2" s="73" t="s">
+      <c r="S2" s="72" t="s">
         <v>512</v>
       </c>
-      <c r="T2" s="78" t="s">
+      <c r="T2" s="107" t="s">
         <v>364</v>
       </c>
-      <c r="U2" s="73" t="s">
+      <c r="U2" s="72" t="s">
         <v>365</v>
       </c>
-      <c r="V2" s="73" t="s">
+      <c r="V2" s="72" t="s">
         <v>366</v>
       </c>
-      <c r="W2" s="73" t="s">
+      <c r="W2" s="72" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="59" t="s">
         <v>5</v>
       </c>
@@ -7003,8 +6995,8 @@
       <c r="V3" s="50"/>
       <c r="W3" s="50"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A4" s="79" t="s">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="74" t="s">
         <v>357</v>
       </c>
       <c r="B4" s="35" t="s">
@@ -7013,55 +7005,55 @@
       <c r="C4" s="50" t="s">
         <v>553</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="79" t="s">
+      <c r="E4" s="74" t="s">
         <v>523</v>
       </c>
-      <c r="F4" s="79" t="s">
+      <c r="F4" s="74" t="s">
         <v>394</v>
       </c>
-      <c r="G4" s="79">
+      <c r="G4" s="74">
         <v>2</v>
       </c>
-      <c r="H4" s="79" t="s">
+      <c r="H4" s="74" t="s">
         <v>370</v>
       </c>
-      <c r="I4" s="79">
+      <c r="I4" s="74">
         <v>256</v>
       </c>
-      <c r="J4" s="79" t="s">
+      <c r="J4" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="K4" s="79" t="s">
+      <c r="K4" s="74" t="s">
         <v>372</v>
       </c>
-      <c r="L4" s="79" t="s">
+      <c r="L4" s="74" t="s">
         <v>524</v>
       </c>
-      <c r="M4" s="79" t="s">
+      <c r="M4" s="74" t="s">
         <v>399</v>
       </c>
-      <c r="N4" s="79" t="s">
+      <c r="N4" s="74" t="s">
         <v>374</v>
       </c>
-      <c r="O4" s="79" t="s">
+      <c r="O4" s="74" t="s">
         <v>400</v>
       </c>
-      <c r="P4" s="79" t="s">
+      <c r="P4" s="74" t="s">
         <v>376</v>
       </c>
-      <c r="Q4" s="79" t="s">
+      <c r="Q4" s="74" t="s">
         <v>377</v>
       </c>
-      <c r="R4" s="79" t="s">
+      <c r="R4" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="S4" s="79" t="b">
+      <c r="S4" s="74" t="b">
         <v>0</v>
       </c>
-      <c r="T4" s="79" t="s">
+      <c r="T4" s="74" t="s">
         <v>119</v>
       </c>
       <c r="U4" s="50" t="s">
@@ -7074,8 +7066,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A5" s="79" t="s">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="74" t="s">
         <v>357</v>
       </c>
       <c r="B5" s="35" t="s">
@@ -7084,55 +7076,55 @@
       <c r="C5" s="50" t="s">
         <v>368</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="79" t="s">
+      <c r="E5" s="74" t="s">
         <v>525</v>
       </c>
-      <c r="F5" s="79" t="s">
+      <c r="F5" s="74" t="s">
         <v>398</v>
       </c>
-      <c r="G5" s="79">
+      <c r="G5" s="74">
         <v>2</v>
       </c>
-      <c r="H5" s="79" t="s">
+      <c r="H5" s="74" t="s">
         <v>526</v>
       </c>
-      <c r="I5" s="79">
+      <c r="I5" s="74">
         <v>256</v>
       </c>
-      <c r="J5" s="79" t="s">
+      <c r="J5" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="K5" s="79" t="s">
+      <c r="K5" s="74" t="s">
         <v>518</v>
       </c>
-      <c r="L5" s="79" t="s">
+      <c r="L5" s="74" t="s">
         <v>527</v>
       </c>
-      <c r="M5" s="79" t="s">
+      <c r="M5" s="74" t="s">
         <v>528</v>
       </c>
-      <c r="N5" s="79" t="s">
+      <c r="N5" s="74" t="s">
         <v>529</v>
       </c>
-      <c r="O5" s="79" t="s">
+      <c r="O5" s="74" t="s">
         <v>530</v>
       </c>
-      <c r="P5" s="79" t="s">
+      <c r="P5" s="74" t="s">
         <v>521</v>
       </c>
-      <c r="Q5" s="79" t="s">
+      <c r="Q5" s="74" t="s">
         <v>377</v>
       </c>
-      <c r="R5" s="79" t="s">
+      <c r="R5" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="S5" s="79" t="b">
+      <c r="S5" s="74" t="b">
         <v>1</v>
       </c>
-      <c r="T5" s="79" t="s">
+      <c r="T5" s="74" t="s">
         <v>119</v>
       </c>
       <c r="U5" s="50" t="s">
@@ -7149,49 +7141,25 @@
   <mergeCells count="1">
     <mergeCell ref="A1:W1"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3">
-      <formula1>Shape_Option</formula1>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K1048576">
+      <formula1>license_type_drop</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N1048576">
+      <formula1>db_sersion_drop</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R1048576">
+      <formula1>workload_drop</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576">
+      <formula1>software_drop</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
+      <formula1>bm_shapes_drop</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$F$2:$F$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>F3:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$B$2:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>H3:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$G$2:$G$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>K3:K1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$C$2:$C$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>N3:N1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$D$2:$D$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>R3:R1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7199,43 +7167,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.453125" style="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" style="49" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.54296875" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.54296875" style="49" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.81640625" style="81" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" style="49" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.36328125" style="49" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.6328125" style="49" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.1796875" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" style="76" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.21875" style="49" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="23" style="49" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.90625" style="49" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.08984375" style="49" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.81640625" style="49"/>
-    <col min="25" max="25" width="18.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.81640625" style="49"/>
+    <col min="20" max="20" width="13.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.77734375" style="49"/>
+    <col min="25" max="25" width="18.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.77734375" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="72" customFormat="1" ht="115" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:23" s="71" customFormat="1" ht="115.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="104" t="s">
         <v>531</v>
       </c>
       <c r="B1" s="105"/>
@@ -7259,107 +7227,107 @@
       <c r="T1" s="105"/>
       <c r="U1" s="105"/>
       <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-    </row>
-    <row r="2" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
+      <c r="W1" s="106"/>
+    </row>
+    <row r="2" spans="1:23" s="108" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="77" t="s">
+      <c r="E2" s="72" t="s">
         <v>402</v>
       </c>
-      <c r="F2" s="76" t="s">
+      <c r="F2" s="73" t="s">
         <v>499</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="72" t="s">
         <v>393</v>
       </c>
-      <c r="I2" s="73" t="s">
+      <c r="I2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="J2" s="73" t="s">
+      <c r="J2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="K2" s="76" t="s">
+      <c r="K2" s="73" t="s">
         <v>504</v>
       </c>
-      <c r="L2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="M2" s="73" t="s">
+      <c r="M2" s="72" t="s">
         <v>352</v>
       </c>
-      <c r="N2" s="73" t="s">
+      <c r="N2" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="O2" s="73" t="s">
+      <c r="O2" s="72" t="s">
         <v>508</v>
       </c>
-      <c r="P2" s="73" t="s">
+      <c r="P2" s="72" t="s">
         <v>509</v>
       </c>
-      <c r="Q2" s="73" t="s">
+      <c r="Q2" s="72" t="s">
         <v>510</v>
       </c>
-      <c r="R2" s="73" t="s">
+      <c r="R2" s="72" t="s">
         <v>511</v>
       </c>
-      <c r="S2" s="73" t="s">
+      <c r="S2" s="72" t="s">
         <v>512</v>
       </c>
-      <c r="T2" s="78" t="s">
+      <c r="T2" s="107" t="s">
         <v>364</v>
       </c>
-      <c r="U2" s="73" t="s">
+      <c r="U2" s="72" t="s">
         <v>365</v>
       </c>
-      <c r="V2" s="73" t="s">
+      <c r="V2" s="72" t="s">
         <v>366</v>
       </c>
-      <c r="W2" s="73" t="s">
+      <c r="W2" s="72" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="90" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="87" t="s">
+    <row r="3" spans="1:23" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="86"/>
-      <c r="S3" s="86"/>
-      <c r="T3" s="86"/>
-      <c r="U3" s="86"/>
-      <c r="V3" s="86"/>
-      <c r="W3" s="86"/>
-    </row>
-    <row r="4" spans="1:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="79" t="s">
+      <c r="B3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+    </row>
+    <row r="4" spans="1:23" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="35" t="s">
@@ -7368,55 +7336,55 @@
       <c r="C4" s="35" t="s">
         <v>553</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>368</v>
       </c>
-      <c r="F4" s="79" t="s">
+      <c r="F4" s="74" t="s">
         <v>532</v>
       </c>
-      <c r="G4" s="79" t="s">
+      <c r="G4" s="74" t="s">
         <v>404</v>
       </c>
-      <c r="H4" s="79">
+      <c r="H4" s="74">
         <v>2</v>
       </c>
-      <c r="I4" s="79">
+      <c r="I4" s="74">
         <v>256</v>
       </c>
-      <c r="J4" s="79" t="s">
+      <c r="J4" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="K4" s="79" t="s">
+      <c r="K4" s="74" t="s">
         <v>372</v>
       </c>
-      <c r="L4" s="79" t="s">
+      <c r="L4" s="74" t="s">
         <v>403</v>
       </c>
-      <c r="M4" s="79" t="s">
+      <c r="M4" s="74" t="s">
         <v>373</v>
       </c>
-      <c r="N4" s="79" t="s">
+      <c r="N4" s="74" t="s">
         <v>374</v>
       </c>
-      <c r="O4" s="79" t="s">
+      <c r="O4" s="74" t="s">
         <v>375</v>
       </c>
-      <c r="P4" s="79" t="s">
+      <c r="P4" s="74" t="s">
         <v>376</v>
       </c>
-      <c r="Q4" s="79" t="s">
+      <c r="Q4" s="74" t="s">
         <v>377</v>
       </c>
-      <c r="R4" s="79" t="s">
+      <c r="R4" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="S4" s="79" t="b">
+      <c r="S4" s="74" t="b">
         <v>1</v>
       </c>
-      <c r="T4" s="79" t="s">
+      <c r="T4" s="74" t="s">
         <v>119</v>
       </c>
       <c r="U4" s="50" t="s">
@@ -7429,53 +7397,32 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A5" s="69"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="85"/>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" s="68"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="79"/>
       <c r="K5" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:W1"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5">
-      <formula1>Shape_Option</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G1048576">
+      <formula1>exa_shapes_drop</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N1048576">
+      <formula1>db_sersion_drop</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R1048576">
+      <formula1>workload_drop</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K1048576">
+      <formula1>license_type_drop</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$E$2:$E$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>G3:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$G$2:$G$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>K3:K1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$C$2:$C$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>N3:N1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Database_Dropdown!$D$2:$D$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>R3:R1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7487,45 +7434,45 @@
       <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" style="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="49" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.90625" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.90625" style="49"/>
+    <col min="3" max="3" width="9.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
         <v>384</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="65" t="s">
         <v>533</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="85" t="s">
         <v>534</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="85" t="s">
         <v>363</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>405</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>401</v>
       </c>
-      <c r="G1" s="92" t="s">
+      <c r="G1" s="86" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="74" t="s">
         <v>370</v>
       </c>
       <c r="C2" s="50" t="s">
@@ -7540,15 +7487,15 @@
       <c r="F2" s="50" t="s">
         <v>394</v>
       </c>
-      <c r="G2" s="79" t="s">
+      <c r="G2" s="74" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>385</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="77" t="s">
         <v>536</v>
       </c>
       <c r="C3" s="50" t="s">
@@ -7567,7 +7514,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>386</v>
       </c>
@@ -7584,7 +7531,7 @@
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>383</v>
       </c>
@@ -7601,7 +7548,7 @@
       <c r="F5" s="50"/>
       <c r="G5" s="50"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>387</v>
       </c>
@@ -7616,7 +7563,7 @@
       <c r="F6" s="50"/>
       <c r="G6" s="50"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
         <v>369</v>
       </c>
@@ -7631,7 +7578,7 @@
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
         <v>388</v>
       </c>
@@ -7646,7 +7593,7 @@
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="50" t="s">
         <v>389</v>
       </c>
@@ -7659,7 +7606,7 @@
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="50" t="s">
         <v>390</v>
       </c>
@@ -7672,7 +7619,7 @@
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="50" t="s">
         <v>391</v>
       </c>
@@ -7685,7 +7632,7 @@
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="50" t="s">
         <v>392</v>
       </c>
@@ -7698,7 +7645,7 @@
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50" t="s">
@@ -7709,7 +7656,7 @@
       <c r="F13" s="50"/>
       <c r="G13" s="50"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50" t="s">
@@ -7721,11 +7668,6 @@
       <c r="G14" s="50"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
-      <formula1>$G$2:$G$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7739,21 +7681,21 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="49" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.81640625" style="49" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.77734375" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="57" customFormat="1" ht="55.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:3" s="57" customFormat="1" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="98"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" s="91"/>
+      <c r="C1" s="92"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -7764,14 +7706,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -7782,7 +7724,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>6</v>
       </c>
@@ -7793,7 +7735,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>6</v>
       </c>
@@ -7804,7 +7746,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
         <v>6</v>
       </c>
@@ -7832,28 +7774,28 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="49" customWidth="1"/>
-    <col min="2" max="2" width="17.08984375" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.36328125" style="49" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="49" customWidth="1"/>
     <col min="4" max="4" width="16" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="28.453125" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="28.44140625" style="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="57" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="99" t="s">
+    <row r="1" spans="1:7" s="57" customFormat="1" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="93" t="s">
         <v>413</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="101"/>
-    </row>
-    <row r="2" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="95"/>
+    </row>
+    <row r="2" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -7876,7 +7818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -7887,7 +7829,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -7908,7 +7850,7 @@
       </c>
       <c r="G4" s="50"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -7923,7 +7865,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>6</v>
       </c>
@@ -7946,7 +7888,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
         <v>6</v>
       </c>
@@ -7985,37 +7927,37 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="49" customWidth="1"/>
-    <col min="2" max="2" width="26.6328125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" style="49" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="49" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" style="49" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" style="49" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" style="49" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="49" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" style="49" customWidth="1"/>
-    <col min="10" max="10" width="21.08984375" style="49" customWidth="1"/>
-    <col min="11" max="11" width="26.453125" style="49" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" style="49" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="49" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" style="49" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" style="49" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="49" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" style="49" customWidth="1"/>
+    <col min="10" max="10" width="21.109375" style="49" customWidth="1"/>
+    <col min="11" max="11" width="26.44140625" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="209.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+    <row r="1" spans="1:11" ht="209.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>414</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="104"/>
-    </row>
-    <row r="2" spans="1:11" s="57" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="98"/>
+    </row>
+    <row r="2" spans="1:11" s="57" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
@@ -8050,7 +7992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -8065,7 +8007,7 @@
       <c r="J3" s="50"/>
       <c r="K3" s="50"/>
     </row>
-    <row r="4" spans="1:11" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -8100,7 +8042,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>6</v>
       </c>
@@ -8133,7 +8075,7 @@
       </c>
       <c r="K5" s="50"/>
     </row>
-    <row r="6" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>6</v>
       </c>
@@ -8183,21 +8125,21 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" style="49" customWidth="1"/>
-    <col min="2" max="2" width="41.453125" style="49" customWidth="1"/>
-    <col min="3" max="10" width="9.1796875" style="49" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="49"/>
+    <col min="1" max="1" width="32.21875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" style="49" customWidth="1"/>
+    <col min="3" max="10" width="9.21875" style="49" customWidth="1"/>
+    <col min="11" max="16384" width="9.21875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="57" customFormat="1" ht="142.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+    <row r="1" spans="1:2" s="57" customFormat="1" ht="142.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="104"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="98"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>31</v>
       </c>
@@ -8205,7 +8147,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -8213,13 +8155,13 @@
         <v>456</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="50"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
@@ -8227,7 +8169,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>37</v>
       </c>
@@ -8249,32 +8191,32 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="49" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.453125" style="49" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.54296875" style="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="49" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="49" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" style="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="104"/>
-    </row>
-    <row r="2" spans="1:7" s="57" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="98"/>
+    </row>
+    <row r="2" spans="1:7" s="57" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -8297,7 +8239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>5</v>
       </c>
@@ -8308,7 +8250,7 @@
       <c r="F3" s="50"/>
       <c r="G3" s="50"/>
     </row>
-    <row r="4" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
@@ -8331,7 +8273,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>6</v>
       </c>
@@ -8352,7 +8294,7 @@
       </c>
       <c r="G5" s="50"/>
     </row>
-    <row r="6" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
         <v>6</v>
       </c>
@@ -8387,51 +8329,51 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="49" customWidth="1"/>
-    <col min="2" max="2" width="18.90625" style="49" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="49" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.1796875" style="49" customWidth="1"/>
-    <col min="7" max="7" width="19.54296875" style="49" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.453125" style="49" customWidth="1"/>
-    <col min="11" max="11" width="11.36328125" style="49" customWidth="1"/>
-    <col min="12" max="12" width="14.36328125" style="49" customWidth="1"/>
-    <col min="13" max="13" width="15.81640625" style="49" customWidth="1"/>
-    <col min="14" max="14" width="13.6328125" style="49" customWidth="1"/>
-    <col min="15" max="15" width="11.90625" style="49" customWidth="1"/>
-    <col min="16" max="16" width="14.08984375" style="49" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="49" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" style="49" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.21875" style="49" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="49" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.44140625" style="49" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="49" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" style="49" customWidth="1"/>
+    <col min="13" max="13" width="15.77734375" style="49" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" style="49" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" style="49" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" style="49" customWidth="1"/>
     <col min="17" max="17" width="10" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="172.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+    <row r="1" spans="1:17" ht="172.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="103"/>
-      <c r="Q1" s="104"/>
-    </row>
-    <row r="2" spans="1:17" s="57" customFormat="1" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="98"/>
+    </row>
+    <row r="2" spans="1:17" s="57" customFormat="1" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -8484,7 +8426,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="46" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" s="46" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
         <v>5</v>
       </c>
@@ -8504,8 +8446,8 @@
       <c r="P3" s="45"/>
       <c r="Q3" s="45"/>
     </row>
-    <row r="4" spans="1:17" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
+    <row r="4" spans="1:17" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
@@ -8553,8 +8495,8 @@
       </c>
       <c r="Q4" s="61"/>
     </row>
-    <row r="5" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49" t="s">
+    <row r="5" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
@@ -8600,8 +8542,8 @@
       </c>
       <c r="Q5" s="61"/>
     </row>
-    <row r="6" spans="1:17" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="49" t="s">
+    <row r="6" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
@@ -8647,8 +8589,8 @@
       </c>
       <c r="Q6" s="61"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="49" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="50" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
@@ -8696,8 +8638,8 @@
       </c>
       <c r="Q7" s="61"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="50" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
@@ -8745,8 +8687,8 @@
       </c>
       <c r="Q8" s="61"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="49" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="50" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
@@ -8811,31 +8753,31 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="49" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" style="49" customWidth="1"/>
-    <col min="4" max="4" width="25.08984375" style="49" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" style="49" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="49" customWidth="1"/>
     <col min="5" max="5" width="16" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.81640625" style="49" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1796875" style="49" customWidth="1"/>
+    <col min="6" max="6" width="31.77734375" style="49" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="104"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="98"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Policy - CD3 update
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -1379,12 +1379,6 @@
   </si>
   <si>
     <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
-$ and * in "Policy Statements" will be replaced by "Policy Statement Groups" and "Policy Statement Compartment" respectively;
-If "Compartment Name" is left empty or mentioned 'root', policy will be created in root compartment;
-Enter "Region" as your tenancy's Home Region for Policy Creation</t>
-  </si>
-  <si>
-    <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
  VCN names should be unique and are case-sensitie across sheets; 
 All fields are mandatory for each VCN except "DNS Label" for which the default value is "VCN Name" truncated to 15 chars.
 DNS Label - if specified as n, DNS will not be enabled for the VCN
@@ -1836,6 +1830,12 @@
   </si>
   <si>
     <t>phx-nsg1,phx-nsg2</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+$ and * in "Policy Statements" will be replaced by "Policy Statement Groups" and "Policy Statement Compartment" respectively;
+If "Compartment Name" is mentioned as 'root', policy will be created in root compartment;
+Enter "Region" as your tenancy's Home Region for Policy Creation</t>
   </si>
 </sst>
 </file>
@@ -2383,6 +2383,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2421,17 +2432,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2859,24 +2859,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="98"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="101"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -2962,28 +2962,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="101"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="104"/>
+      <c r="R1" s="104"/>
+      <c r="S1" s="104"/>
+      <c r="T1" s="104"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
@@ -3041,10 +3041,10 @@
         <v>71</v>
       </c>
       <c r="S2" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="T2" s="89" t="s">
         <v>551</v>
-      </c>
-      <c r="T2" s="89" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3076,13 +3076,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>89</v>
@@ -3116,28 +3116,28 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>94</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>91</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I5" s="47" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
@@ -3160,13 +3160,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>89</v>
@@ -3198,13 +3198,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>94</v>
@@ -3262,14 +3262,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="98"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="101"/>
     </row>
     <row r="2" spans="1:6" s="57" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
@@ -3306,7 +3306,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>101</v>
@@ -3326,7 +3326,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>103</v>
@@ -3346,7 +3346,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>105</v>
@@ -3358,7 +3358,7 @@
         <v>102</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -3396,22 +3396,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="98"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="101"/>
     </row>
     <row r="2" spans="1:14" s="57" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
@@ -3480,25 +3480,25 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D4" s="50" t="s">
+        <v>475</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>414</v>
+      </c>
+      <c r="F4" s="50" t="s">
         <v>476</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>415</v>
-      </c>
-      <c r="F4" s="50" t="s">
-        <v>477</v>
       </c>
       <c r="G4" s="50" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I4" s="50" t="s">
         <v>117</v>
@@ -3510,7 +3510,7 @@
         <v>119</v>
       </c>
       <c r="L4" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="M4" s="50"/>
       <c r="N4" s="50" t="s">
@@ -3522,19 +3522,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>120</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G5" s="50" t="b">
         <v>0</v>
@@ -3550,7 +3550,7 @@
         <v>119</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="M5" s="50"/>
       <c r="N5" s="50" t="s">
@@ -3568,10 +3568,10 @@
         <v>65</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F6" s="50" t="s">
         <v>368</v>
@@ -3590,10 +3590,10 @@
         <v>119</v>
       </c>
       <c r="L6" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="M6" s="50" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="N6" s="50"/>
     </row>
@@ -3608,7 +3608,7 @@
         <v>65</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>120</v>
@@ -3630,10 +3630,10 @@
         <v>119</v>
       </c>
       <c r="L7" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="M7" s="50" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="N7" s="50"/>
     </row>
@@ -3666,16 +3666,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="98"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="101"/>
     </row>
     <row r="2" spans="1:8" s="57" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -3723,7 +3723,7 @@
         <v>367</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D4" s="50">
         <v>150</v>
@@ -3732,13 +3732,13 @@
         <v>65</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G4" s="50" t="s">
         <v>128</v>
       </c>
       <c r="H4" s="59" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3749,7 +3749,7 @@
         <v>381</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D5" s="50">
         <v>150</v>
@@ -3758,13 +3758,13 @@
         <v>65</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>128</v>
       </c>
       <c r="H5" s="59" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -3804,24 +3804,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="84.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
+      <c r="P1" s="102"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
@@ -3898,7 +3898,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>104</v>
@@ -3907,7 +3907,7 @@
         <v>142</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32" t="s">
@@ -3926,7 +3926,7 @@
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
       <c r="P4" s="48" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -3981,7 +3981,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>104</v>
@@ -3990,7 +3990,7 @@
         <v>142</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
@@ -4013,7 +4013,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>114</v>
@@ -4022,7 +4022,7 @@
         <v>152</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
@@ -4043,7 +4043,7 @@
       <c r="N8" s="32"/>
       <c r="O8" s="32"/>
       <c r="P8" s="50" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4051,7 +4051,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>114</v>
@@ -4060,7 +4060,7 @@
         <v>156</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
@@ -4087,7 +4087,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>104</v>
@@ -4096,7 +4096,7 @@
         <v>158</v>
       </c>
       <c r="E10" s="48" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -4146,23 +4146,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="99" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
     </row>
     <row r="2" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
@@ -4205,10 +4205,10 @@
         <v>171</v>
       </c>
       <c r="N2" s="43" t="s">
+        <v>492</v>
+      </c>
+      <c r="O2" s="43" t="s">
         <v>493</v>
-      </c>
-      <c r="O2" s="43" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4235,16 +4235,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D4" s="50" t="s">
         <v>172</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F4" s="50" t="b">
         <v>1</v>
@@ -4265,10 +4265,10 @@
         <v>176</v>
       </c>
       <c r="N4" s="50" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="O4" s="87" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -4299,22 +4299,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D6" s="50" t="s">
         <v>178</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F6" s="50" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H6" s="48" t="s">
         <v>179</v>
@@ -4371,24 +4371,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="98"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="101"/>
     </row>
     <row r="2" spans="1:16" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="51" t="s">
@@ -4465,17 +4465,17 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="50" t="s">
         <v>195</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G4" s="50" t="s">
         <v>196</v>
@@ -4519,7 +4519,7 @@
         <v>201</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>196</v>
@@ -4551,17 +4551,17 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
         <v>205</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G6" s="50" t="s">
         <v>196</v>
@@ -4622,26 +4622,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="96" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="95"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="98"/>
     </row>
     <row r="2" spans="1:18" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
@@ -4726,7 +4726,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>222</v>
@@ -4735,7 +4735,7 @@
         <v>223</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
@@ -5188,7 +5188,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C22" s="50" t="s">
         <v>259</v>
@@ -5281,14 +5281,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="57" customFormat="1" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="96" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="95"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="98"/>
     </row>
     <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
@@ -5325,7 +5325,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>263</v>
@@ -5375,7 +5375,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>269</v>
@@ -5420,12 +5420,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="57" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="95"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -5454,10 +5454,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>415</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>416</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>417</v>
       </c>
       <c r="D4" s="50"/>
     </row>
@@ -5466,13 +5466,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
+        <v>417</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>418</v>
       </c>
-      <c r="C5" s="50" t="s">
-        <v>419</v>
-      </c>
       <c r="D5" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -5480,13 +5480,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>419</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>420</v>
       </c>
-      <c r="C6" s="50" t="s">
-        <v>421</v>
-      </c>
       <c r="D6" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -5494,10 +5494,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
+        <v>421</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>422</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>423</v>
       </c>
       <c r="D7" s="50"/>
     </row>
@@ -5506,13 +5506,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -5523,10 +5523,10 @@
         <v>367</v>
       </c>
       <c r="C9" s="50" t="s">
+        <v>424</v>
+      </c>
+      <c r="D9" s="50" t="s">
         <v>425</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -5534,13 +5534,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -5548,13 +5548,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="50" t="s">
+        <v>427</v>
+      </c>
+      <c r="C11" s="50" t="s">
         <v>428</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="D11" s="50" t="s">
         <v>429</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -5587,22 +5587,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="105" t="s">
         <v>272</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="106"/>
     </row>
     <row r="2" spans="1:14" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
@@ -5642,10 +5642,10 @@
         <v>279</v>
       </c>
       <c r="M2" s="43" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="N2" s="43" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -5671,7 +5671,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>195</v>
@@ -5690,16 +5690,16 @@
       </c>
       <c r="H4" s="50"/>
       <c r="I4" s="50" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
       <c r="L4" s="50"/>
       <c r="M4" s="50" t="s">
+        <v>544</v>
+      </c>
+      <c r="N4" s="88" t="s">
         <v>545</v>
-      </c>
-      <c r="N4" s="88" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -5731,7 +5731,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>205</v>
@@ -6123,18 +6123,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
-        <v>490</v>
-      </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="98"/>
+      <c r="A1" s="102" t="s">
+        <v>489</v>
+      </c>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="101"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="54" t="s">
@@ -6187,7 +6187,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C4" s="38" t="s">
         <v>333</v>
@@ -6239,7 +6239,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>340</v>
@@ -6259,13 +6259,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>109</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E7" s="34" t="s">
         <v>342</v>
@@ -6295,7 +6295,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>344</v>
@@ -6391,16 +6391,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
-        <v>495</v>
-      </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="106"/>
+      <c r="A1" s="107" t="s">
+        <v>494</v>
+      </c>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="109"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="65" t="s">
@@ -6445,10 +6445,10 @@
         <v>357</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D4" s="50" t="s">
         <v>358</v>
@@ -6473,10 +6473,10 @@
         <v>357</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>361</v>
@@ -6537,33 +6537,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="71" customFormat="1" ht="101.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
-        <v>498</v>
-      </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="106"/>
-    </row>
-    <row r="2" spans="1:23" s="108" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="107" t="s">
+        <v>497</v>
+      </c>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="108"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="109"/>
+    </row>
+    <row r="2" spans="1:23" s="91" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
@@ -6577,51 +6577,51 @@
         <v>98</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F2" s="72" t="s">
         <v>99</v>
       </c>
       <c r="G2" s="72" t="s">
+        <v>499</v>
+      </c>
+      <c r="H2" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="H2" s="72" t="s">
+      <c r="I2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="J2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="73" t="s">
         <v>503</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="M2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="N2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>508</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>509</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>510</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>511</v>
       </c>
-      <c r="S2" s="72" t="s">
-        <v>512</v>
-      </c>
-      <c r="T2" s="107" t="s">
+      <c r="T2" s="90" t="s">
         <v>364</v>
       </c>
       <c r="U2" s="72" t="s">
@@ -6631,7 +6631,7 @@
         <v>366</v>
       </c>
       <c r="W2" s="72" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -6666,16 +6666,16 @@
         <v>357</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F4" s="74" t="s">
         <v>386</v>
@@ -6696,13 +6696,13 @@
         <v>372</v>
       </c>
       <c r="L4" s="74" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="M4" s="74" t="s">
         <v>373</v>
       </c>
       <c r="N4" s="75" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="O4" s="74" t="s">
         <v>375</v>
@@ -6737,7 +6737,7 @@
         <v>357</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>368</v>
@@ -6746,7 +6746,7 @@
         <v>114</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F5" s="74" t="s">
         <v>389</v>
@@ -6764,22 +6764,22 @@
         <v>371</v>
       </c>
       <c r="K5" s="74" t="s">
+        <v>517</v>
+      </c>
+      <c r="L5" s="74" t="s">
         <v>518</v>
-      </c>
-      <c r="L5" s="74" t="s">
-        <v>519</v>
       </c>
       <c r="M5" s="74" t="s">
         <v>396</v>
       </c>
       <c r="N5" s="75" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="O5" s="74" t="s">
         <v>397</v>
       </c>
       <c r="P5" s="74" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Q5" s="74" t="s">
         <v>377</v>
@@ -6870,34 +6870,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="71" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
-        <v>522</v>
-      </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="106"/>
+      <c r="A1" s="107" t="s">
+        <v>521</v>
+      </c>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="108"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="109"/>
       <c r="X1" s="78"/>
     </row>
-    <row r="2" spans="1:24" s="108" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="91" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>98</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F2" s="72" t="s">
         <v>99</v>
@@ -6920,42 +6920,42 @@
         <v>393</v>
       </c>
       <c r="H2" s="72" t="s">
+        <v>500</v>
+      </c>
+      <c r="I2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="J2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="92" t="s">
         <v>503</v>
       </c>
-      <c r="K2" s="109" t="s">
+      <c r="L2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="M2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="N2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>508</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>509</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>510</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>511</v>
       </c>
-      <c r="S2" s="72" t="s">
-        <v>512</v>
-      </c>
-      <c r="T2" s="107" t="s">
+      <c r="T2" s="90" t="s">
         <v>364</v>
       </c>
       <c r="U2" s="72" t="s">
@@ -6965,7 +6965,7 @@
         <v>366</v>
       </c>
       <c r="W2" s="72" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -7000,16 +7000,16 @@
         <v>357</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F4" s="74" t="s">
         <v>394</v>
@@ -7030,7 +7030,7 @@
         <v>372</v>
       </c>
       <c r="L4" s="74" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="M4" s="74" t="s">
         <v>399</v>
@@ -7071,7 +7071,7 @@
         <v>357</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>368</v>
@@ -7080,7 +7080,7 @@
         <v>65</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F5" s="74" t="s">
         <v>398</v>
@@ -7089,7 +7089,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I5" s="74">
         <v>256</v>
@@ -7098,22 +7098,22 @@
         <v>371</v>
       </c>
       <c r="K5" s="74" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L5" s="74" t="s">
+        <v>526</v>
+      </c>
+      <c r="M5" s="74" t="s">
         <v>527</v>
       </c>
-      <c r="M5" s="74" t="s">
+      <c r="N5" s="74" t="s">
         <v>528</v>
       </c>
-      <c r="N5" s="74" t="s">
+      <c r="O5" s="74" t="s">
         <v>529</v>
       </c>
-      <c r="O5" s="74" t="s">
-        <v>530</v>
-      </c>
       <c r="P5" s="74" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Q5" s="74" t="s">
         <v>377</v>
@@ -7203,33 +7203,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="71" customFormat="1" ht="115.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
-        <v>531</v>
-      </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="106"/>
-    </row>
-    <row r="2" spans="1:23" s="108" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="107" t="s">
+        <v>530</v>
+      </c>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="108"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="109"/>
+    </row>
+    <row r="2" spans="1:23" s="91" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>402</v>
       </c>
       <c r="F2" s="73" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G2" s="72" t="s">
         <v>99</v>
@@ -7255,39 +7255,39 @@
         <v>393</v>
       </c>
       <c r="I2" s="72" t="s">
+        <v>501</v>
+      </c>
+      <c r="J2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="73" t="s">
         <v>503</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>504</v>
-      </c>
-      <c r="L2" s="72" t="s">
-        <v>505</v>
       </c>
       <c r="M2" s="72" t="s">
         <v>352</v>
       </c>
       <c r="N2" s="72" t="s">
+        <v>506</v>
+      </c>
+      <c r="O2" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>508</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>509</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>510</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>511</v>
       </c>
-      <c r="S2" s="72" t="s">
-        <v>512</v>
-      </c>
-      <c r="T2" s="107" t="s">
+      <c r="T2" s="90" t="s">
         <v>364</v>
       </c>
       <c r="U2" s="72" t="s">
@@ -7297,7 +7297,7 @@
         <v>366</v>
       </c>
       <c r="W2" s="72" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="84" customFormat="1" x14ac:dyDescent="0.3">
@@ -7331,10 +7331,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
@@ -7343,7 +7343,7 @@
         <v>368</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G4" s="74" t="s">
         <v>404</v>
@@ -7450,10 +7450,10 @@
         <v>384</v>
       </c>
       <c r="B1" s="65" t="s">
+        <v>532</v>
+      </c>
+      <c r="C1" s="85" t="s">
         <v>533</v>
-      </c>
-      <c r="C1" s="85" t="s">
-        <v>534</v>
       </c>
       <c r="D1" s="85" t="s">
         <v>363</v>
@@ -7465,7 +7465,7 @@
         <v>401</v>
       </c>
       <c r="G1" s="86" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -7476,7 +7476,7 @@
         <v>370</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D2" s="59" t="s">
         <v>378</v>
@@ -7496,13 +7496,13 @@
         <v>385</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C3" s="50" t="s">
         <v>374</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E3" s="50" t="s">
         <v>407</v>
@@ -7511,7 +7511,7 @@
         <v>398</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -7522,7 +7522,7 @@
         <v>395</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="50" t="s">
@@ -7536,10 +7536,10 @@
         <v>383</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
@@ -7554,7 +7554,7 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
@@ -7569,7 +7569,7 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="50" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D7" s="50"/>
       <c r="E7" s="50" t="s">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="50" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="50" t="s">
@@ -7599,7 +7599,7 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="50" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="50"/>
@@ -7612,7 +7612,7 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="50" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D10" s="50"/>
       <c r="E10" s="50"/>
@@ -7625,7 +7625,7 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
@@ -7638,7 +7638,7 @@
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
@@ -7649,7 +7649,7 @@
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="50"/>
@@ -7660,7 +7660,7 @@
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
@@ -7689,11 +7689,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="57" customFormat="1" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="95"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -7718,10 +7718,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>430</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>431</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7729,10 +7729,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
+        <v>432</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>433</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -7740,10 +7740,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>434</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>435</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -7751,10 +7751,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
+        <v>436</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>437</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -7771,7 +7771,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7785,15 +7785,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="57" customFormat="1" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
-        <v>413</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="95"/>
+      <c r="A1" s="96" t="s">
+        <v>554</v>
+      </c>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="98"/>
     </row>
     <row r="2" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -7834,19 +7834,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>439</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>488</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>549</v>
+      </c>
+      <c r="E4" s="50" t="s">
         <v>440</v>
       </c>
-      <c r="C4" s="50" t="s">
-        <v>489</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>550</v>
-      </c>
-      <c r="E4" s="50" t="s">
+      <c r="F4" s="59" t="s">
         <v>441</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>442</v>
       </c>
       <c r="G4" s="50"/>
     </row>
@@ -7856,13 +7856,13 @@
       <c r="C5" s="50"/>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -7870,22 +7870,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>443</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>421</v>
+      </c>
+      <c r="D6" s="50" t="s">
         <v>444</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>422</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>445</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -7893,22 +7893,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G7" s="50" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -7943,19 +7943,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="209.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
-        <v>414</v>
-      </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="98"/>
+      <c r="A1" s="99" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="101"/>
     </row>
     <row r="2" spans="1:11" s="57" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
@@ -8012,7 +8012,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
@@ -8021,7 +8021,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F4" s="50" t="s">
         <v>27</v>
@@ -8033,13 +8033,13 @@
         <v>24</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J4" s="50" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="50" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
@@ -8047,10 +8047,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>26</v>
@@ -8068,7 +8068,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="50" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J5" s="50" t="s">
         <v>28</v>
@@ -8080,10 +8080,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D6" s="50" t="s">
         <v>29</v>
@@ -8101,7 +8101,7 @@
         <v>24</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J6" s="50" t="s">
         <v>28</v>
@@ -8134,10 +8134,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="57" customFormat="1" ht="142.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="98"/>
+      <c r="B1" s="101"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -8152,7 +8152,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -8206,15 +8206,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="98"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" s="57" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -8255,7 +8255,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
@@ -8270,7 +8270,7 @@
         <v>45</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -8278,10 +8278,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>43</v>
@@ -8299,13 +8299,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>46</v>
@@ -8353,25 +8353,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="172.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="98"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="101"/>
     </row>
     <row r="2" spans="1:17" s="57" customFormat="1" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -8451,13 +8451,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>59</v>
@@ -8479,7 +8479,7 @@
         <v>24</v>
       </c>
       <c r="L4" s="60" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="M4" s="60" t="s">
         <v>24</v>
@@ -8500,16 +8500,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D5" s="50" t="s">
+        <v>460</v>
+      </c>
+      <c r="E5" s="50" t="s">
         <v>461</v>
-      </c>
-      <c r="E5" s="50" t="s">
-        <v>462</v>
       </c>
       <c r="F5" s="50" t="s">
         <v>60</v>
@@ -8547,13 +8547,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>64</v>
@@ -8594,16 +8594,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F7" s="50" t="s">
         <v>60</v>
@@ -8612,7 +8612,7 @@
         <v>66</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I7" s="50"/>
       <c r="J7" s="50" t="s">
@@ -8643,16 +8643,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F8" s="50" t="s">
         <v>60</v>
@@ -8661,11 +8661,11 @@
         <v>66</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I8" s="50"/>
       <c r="J8" s="50" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K8" s="50" t="s">
         <v>27</v>
@@ -8692,16 +8692,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D9" s="50" t="s">
+        <v>466</v>
+      </c>
+      <c r="E9" s="50" t="s">
         <v>467</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>468</v>
       </c>
       <c r="F9" s="50" t="s">
         <v>60</v>
@@ -8710,17 +8710,17 @@
         <v>66</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I9" s="50"/>
       <c r="J9" s="50" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K9" s="50" t="s">
         <v>27</v>
       </c>
       <c r="L9" s="60" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="M9" s="60" t="s">
         <v>27</v>
@@ -8766,16 +8766,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="98"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="101"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">

</xml_diff>

<commit_message>
Excel sheet NSG - fix
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="556">
   <si>
     <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
 Leave "Parent Compartment" empty or mention 'root' if it is under 'root' compartment;
@@ -1836,6 +1836,9 @@
 $ and * in "Policy Statements" will be replaced by "Policy Statement Groups" and "Policy Statement Compartment" respectively;
 If "Compartment Name" is mentioned as 'root', policy will be created in root compartment;
 Enter "Region" as your tenancy's Home Region for Policy Creation</t>
+  </si>
+  <si>
+    <t>10.117.0.0/16</t>
   </si>
 </sst>
 </file>
@@ -3218,7 +3221,9 @@
       <c r="H7" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="47"/>
+      <c r="I7" s="47" t="s">
+        <v>555</v>
+      </c>
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
       <c r="L7" s="50"/>

</xml_diff>

<commit_message>
Create Tags - Default Tag value fixes
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -9,31 +9,31 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
     <sheet name="Compartments" sheetId="2" r:id="rId2"/>
     <sheet name="Groups" sheetId="3" r:id="rId3"/>
     <sheet name="Policies" sheetId="4" r:id="rId4"/>
-    <sheet name="VCNs" sheetId="5" r:id="rId5"/>
-    <sheet name="VCN Info" sheetId="6" r:id="rId6"/>
-    <sheet name="DHCP" sheetId="7" r:id="rId7"/>
-    <sheet name="Subnets" sheetId="8" r:id="rId8"/>
-    <sheet name="RouteRulesinOCI" sheetId="9" r:id="rId9"/>
-    <sheet name="SecRulesinOCI" sheetId="10" r:id="rId10"/>
-    <sheet name="NSGs" sheetId="11" r:id="rId11"/>
-    <sheet name="DedicatedVMHosts" sheetId="12" r:id="rId12"/>
-    <sheet name="Instances" sheetId="13" r:id="rId13"/>
-    <sheet name="BlockVols" sheetId="14" r:id="rId14"/>
-    <sheet name="FSS" sheetId="15" r:id="rId15"/>
-    <sheet name="LB-Hostname-Certs" sheetId="16" r:id="rId16"/>
-    <sheet name="BackendSet-BackendServer" sheetId="17" r:id="rId17"/>
-    <sheet name="RuleSet" sheetId="18" r:id="rId18"/>
-    <sheet name="PathRouteSet" sheetId="19" r:id="rId19"/>
-    <sheet name="LB-Listener" sheetId="20" r:id="rId20"/>
-    <sheet name="Rule Set Dropdown" sheetId="21" state="hidden" r:id="rId21"/>
-    <sheet name="Tags" sheetId="22" r:id="rId22"/>
+    <sheet name="Tags" sheetId="22" r:id="rId5"/>
+    <sheet name="VCNs" sheetId="5" r:id="rId6"/>
+    <sheet name="VCN Info" sheetId="6" r:id="rId7"/>
+    <sheet name="DHCP" sheetId="7" r:id="rId8"/>
+    <sheet name="Subnets" sheetId="8" r:id="rId9"/>
+    <sheet name="RouteRulesinOCI" sheetId="9" r:id="rId10"/>
+    <sheet name="SecRulesinOCI" sheetId="10" r:id="rId11"/>
+    <sheet name="NSGs" sheetId="11" r:id="rId12"/>
+    <sheet name="DedicatedVMHosts" sheetId="12" r:id="rId13"/>
+    <sheet name="Instances" sheetId="13" r:id="rId14"/>
+    <sheet name="BlockVols" sheetId="14" r:id="rId15"/>
+    <sheet name="FSS" sheetId="15" r:id="rId16"/>
+    <sheet name="LB-Hostname-Certs" sheetId="16" r:id="rId17"/>
+    <sheet name="BackendSet-BackendServer" sheetId="17" r:id="rId18"/>
+    <sheet name="RuleSet" sheetId="18" r:id="rId19"/>
+    <sheet name="PathRouteSet" sheetId="19" r:id="rId20"/>
+    <sheet name="LB-Listener" sheetId="20" r:id="rId21"/>
+    <sheet name="Rule Set Dropdown" sheetId="21" state="hidden" r:id="rId22"/>
     <sheet name="ADW_ATP" sheetId="23" r:id="rId23"/>
     <sheet name="DB_System_VM" sheetId="24" r:id="rId24"/>
     <sheet name="DB_System_BM" sheetId="25" r:id="rId25"/>
@@ -44,16 +44,16 @@
     <externalReference r:id="rId28"/>
   </externalReferences>
   <definedNames>
-    <definedName name="Action_Values" localSheetId="17">'Rule Set Dropdown'!$A$2:$A$12</definedName>
-    <definedName name="Allowed_Methods" localSheetId="17">'Rule Set Dropdown'!$B$2:$B$41</definedName>
-    <definedName name="Attribute_Names" localSheetId="17">'Rule Set Dropdown'!$D$2:$D$5</definedName>
+    <definedName name="Action_Values" localSheetId="18">'Rule Set Dropdown'!$A$2:$A$12</definedName>
+    <definedName name="Allowed_Methods" localSheetId="18">'Rule Set Dropdown'!$B$2:$B$41</definedName>
+    <definedName name="Attribute_Names" localSheetId="18">'Rule Set Dropdown'!$D$2:$D$5</definedName>
     <definedName name="bm_shapes_drop">Database_Dropdown!$F$2:$F$3</definedName>
     <definedName name="db_sersion_drop">Database_Dropdown!$C$2:$C$14</definedName>
     <definedName name="exa_shapes_drop">Database_Dropdown!$E$2:$E$8</definedName>
     <definedName name="Header_Size">'Rule Set Dropdown'!$F$2:$F$6</definedName>
     <definedName name="license_type_drop">Database_Dropdown!$G$2:$G$3</definedName>
+    <definedName name="Match_Style" localSheetId="19">'Rule Set Dropdown'!$C$2:$C$6</definedName>
     <definedName name="Match_Style" localSheetId="18">'Rule Set Dropdown'!$C$2:$C$6</definedName>
-    <definedName name="Match_Style" localSheetId="17">'Rule Set Dropdown'!$C$2:$C$6</definedName>
     <definedName name="Response_Code">'Rule Set Dropdown'!$E$2:$E$7</definedName>
     <definedName name="Shape_Option" localSheetId="26">#REF!</definedName>
     <definedName name="Shape_Option" localSheetId="24">#REF!</definedName>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="556">
   <si>
     <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
 Leave "Parent Compartment" empty or mention 'root' if it is under 'root' compartment;
@@ -1129,9 +1129,6 @@
     <t>Validator</t>
   </si>
   <si>
-    <t>Default Tag</t>
-  </si>
-  <si>
     <t>Default Tag Value</t>
   </si>
   <si>
@@ -1151,9 +1148,6 @@
   </si>
   <si>
     <t>internal</t>
-  </si>
-  <si>
-    <t>ENUM::"ocs"</t>
   </si>
   <si>
     <t>Operations</t>
@@ -1613,14 +1607,6 @@
     <t>root</t>
   </si>
   <si>
-    <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
- Default Tag Value -  It cannot be left empty if Default Tag field is set to 'TRUE' and must be one of the values entered in Validator field; You can set new default tag values if the Validator field is empty.
-Enter Region as your tenancy's Home Region for Tags Creation
-Enter compartment as 'root' to create the Tags in 'root' compartment
-Is Cost Tracking and Default Tag - defaults to"FALSE", if left empty 
-Validator - For entering values of type "list" use ENUM::&lt;values in double quotes separated by comma&gt; and for type "string" use ENUM::"&lt;value&gt;"</t>
-  </si>
-  <si>
     <t>"DELETE","GET","PUT"</t>
   </si>
   <si>
@@ -1839,6 +1825,20 @@
   </si>
   <si>
     <t>10.117.0.0/16</t>
+  </si>
+  <si>
+    <t>Default Tag Compartment</t>
+  </si>
+  <si>
+    <t>ENUM::"internal-team","ocs-internal"</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+Default Tag Value: To use 'User-Assigned Value' - Leave this field as empty ; To use 'Default Values' - (if the Validator is set) mention one of the values in Validator;(If the Validator is empty) you may enter any value.
+Enter Region as your tenancy's Home Region for Tags Creation
+Enter compartment as 'root' to create the Tags in 'root' compartment
+Is Cost Tracking - defaults to"FALSE", if left empty 
+Validator - For entering values of type "list" use ENUM::&lt;values in double quotes separated by comma&gt; and for type "string" use ENUM::"&lt;value&gt;"</t>
   </si>
 </sst>
 </file>
@@ -2408,12 +2408,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2822,7 +2822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+    <sheetView zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2833,7 +2833,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -2843,6 +2843,73 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" style="49" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="49" customWidth="1"/>
+    <col min="5" max="5" width="16" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.77734375" style="49" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" style="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="101"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -2862,7 +2929,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="99" t="s">
         <v>72</v>
       </c>
       <c r="B1" s="100"/>
@@ -2939,7 +3006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
@@ -3044,10 +3111,10 @@
         <v>71</v>
       </c>
       <c r="S2" s="89" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="T2" s="89" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3079,13 +3146,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>89</v>
@@ -3119,28 +3186,28 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>94</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>91</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="I5" s="47" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
@@ -3163,13 +3230,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>89</v>
@@ -3201,13 +3268,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>94</v>
@@ -3222,7 +3289,7 @@
         <v>92</v>
       </c>
       <c r="I7" s="47" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
@@ -3249,7 +3316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -3267,7 +3334,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="99" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="100"/>
@@ -3311,7 +3378,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>101</v>
@@ -3331,7 +3398,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>103</v>
@@ -3351,7 +3418,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>105</v>
@@ -3363,7 +3430,7 @@
         <v>102</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -3374,7 +3441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
@@ -3401,7 +3468,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="99" t="s">
         <v>106</v>
       </c>
       <c r="B1" s="100"/>
@@ -3485,37 +3552,37 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G4" s="50" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="I4" s="50" t="s">
         <v>117</v>
       </c>
       <c r="J4" s="50" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K4" s="50" t="s">
         <v>119</v>
       </c>
       <c r="L4" s="50" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="M4" s="50"/>
       <c r="N4" s="50" t="s">
@@ -3527,19 +3594,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>120</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G5" s="50" t="b">
         <v>0</v>
@@ -3549,13 +3616,13 @@
         <v>117</v>
       </c>
       <c r="J5" s="50" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K5" s="50" t="s">
         <v>119</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="M5" s="50"/>
       <c r="N5" s="50" t="s">
@@ -3567,19 +3634,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G6" s="50" t="b">
         <v>0</v>
@@ -3595,10 +3662,10 @@
         <v>119</v>
       </c>
       <c r="L6" s="50" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="M6" s="50" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="N6" s="50"/>
     </row>
@@ -3607,19 +3674,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>120</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G7" s="50" t="b">
         <v>0</v>
@@ -3635,10 +3702,10 @@
         <v>119</v>
       </c>
       <c r="L7" s="50" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="M7" s="50" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N7" s="50"/>
     </row>
@@ -3651,7 +3718,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -3671,7 +3738,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="99" t="s">
         <v>123</v>
       </c>
       <c r="B1" s="100"/>
@@ -3725,10 +3792,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D4" s="50">
         <v>150</v>
@@ -3737,13 +3804,13 @@
         <v>65</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G4" s="50" t="s">
         <v>128</v>
       </c>
       <c r="H4" s="59" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3751,10 +3818,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D5" s="50">
         <v>150</v>
@@ -3763,13 +3830,13 @@
         <v>65</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>128</v>
       </c>
       <c r="H5" s="59" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -3781,7 +3848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
@@ -3809,24 +3876,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="84.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
@@ -3903,7 +3970,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>104</v>
@@ -3912,7 +3979,7 @@
         <v>142</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32" t="s">
@@ -3931,7 +3998,7 @@
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
       <c r="P4" s="48" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -3986,7 +4053,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>104</v>
@@ -3995,7 +4062,7 @@
         <v>142</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
@@ -4018,7 +4085,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>114</v>
@@ -4027,7 +4094,7 @@
         <v>152</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
@@ -4048,7 +4115,7 @@
       <c r="N8" s="32"/>
       <c r="O8" s="32"/>
       <c r="P8" s="50" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4056,7 +4123,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>114</v>
@@ -4065,7 +4132,7 @@
         <v>156</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
@@ -4092,7 +4159,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>104</v>
@@ -4101,7 +4168,7 @@
         <v>158</v>
       </c>
       <c r="E10" s="48" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -4128,7 +4195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
@@ -4151,23 +4218,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
     </row>
     <row r="2" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
@@ -4210,10 +4277,10 @@
         <v>171</v>
       </c>
       <c r="N2" s="43" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="O2" s="43" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4240,16 +4307,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D4" s="50" t="s">
         <v>172</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F4" s="50" t="b">
         <v>1</v>
@@ -4270,10 +4337,10 @@
         <v>176</v>
       </c>
       <c r="N4" s="50" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="O4" s="87" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -4304,22 +4371,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D6" s="50" t="s">
         <v>178</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F6" s="50" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H6" s="48" t="s">
         <v>179</v>
@@ -4351,7 +4418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
@@ -4376,7 +4443,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>182</v>
       </c>
       <c r="B1" s="100"/>
@@ -4470,17 +4537,17 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="50" t="s">
         <v>195</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G4" s="50" t="s">
         <v>196</v>
@@ -4524,7 +4591,7 @@
         <v>201</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>196</v>
@@ -4556,17 +4623,17 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
         <v>205</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G6" s="50" t="s">
         <v>196</v>
@@ -4601,7 +4668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R23"/>
   <sheetViews>
@@ -4731,7 +4798,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>222</v>
@@ -4740,7 +4807,7 @@
         <v>223</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
@@ -5193,7 +5260,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C22" s="50" t="s">
         <v>259</v>
@@ -5269,7 +5336,170 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" style="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="57" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="95"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="35"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>413</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>414</v>
+      </c>
+      <c r="D4" s="50"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>415</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>416</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>417</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>418</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>419</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>420</v>
+      </c>
+      <c r="D7" s="50"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>415</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>421</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>365</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>422</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>417</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>424</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>425</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>426</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>427</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -5330,7 +5560,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>263</v>
@@ -5380,7 +5610,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>269</v>
@@ -5408,170 +5638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="49" customWidth="1"/>
-    <col min="3" max="3" width="40.77734375" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5546875" style="49" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="57" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="95"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="35"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>415</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>416</v>
-      </c>
-      <c r="D4" s="50"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>417</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>418</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>419</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>420</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>421</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>422</v>
-      </c>
-      <c r="D7" s="50"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>417</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>423</v>
-      </c>
-      <c r="D8" s="50" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>367</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>424</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>419</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>426</v>
-      </c>
-      <c r="D10" s="50" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="50" t="s">
-        <v>427</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>428</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>429</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
@@ -5647,10 +5714,10 @@
         <v>279</v>
       </c>
       <c r="M2" s="43" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="N2" s="43" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -5676,7 +5743,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>195</v>
@@ -5695,16 +5762,16 @@
       </c>
       <c r="H4" s="50"/>
       <c r="I4" s="50" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
       <c r="L4" s="50"/>
       <c r="M4" s="50" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="N4" s="88" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -5736,7 +5803,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>205</v>
@@ -5780,7 +5847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
@@ -6100,275 +6167,6 @@
       <c r="B41" s="12"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="19.21875" style="49" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" style="49" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="49" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="49" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="49" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="49" customWidth="1"/>
-    <col min="8" max="8" width="21" style="49" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" style="6" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
-        <v>489</v>
-      </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="101"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="53" t="s">
-        <v>325</v>
-      </c>
-      <c r="D2" s="53" t="s">
-        <v>326</v>
-      </c>
-      <c r="E2" s="53" t="s">
-        <v>327</v>
-      </c>
-      <c r="F2" s="53" t="s">
-        <v>328</v>
-      </c>
-      <c r="G2" s="53" t="s">
-        <v>329</v>
-      </c>
-      <c r="H2" s="53" t="s">
-        <v>330</v>
-      </c>
-      <c r="I2" s="54" t="s">
-        <v>331</v>
-      </c>
-      <c r="J2" s="54" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="56"/>
-    </row>
-    <row r="4" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>488</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>333</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>334</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>335</v>
-      </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="33" t="s">
-        <v>336</v>
-      </c>
-      <c r="I4" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="40" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="63"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33" t="s">
-        <v>338</v>
-      </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="33" t="s">
-        <v>339</v>
-      </c>
-      <c r="I5" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="40" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>488</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>340</v>
-      </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34" t="s">
-        <v>341</v>
-      </c>
-      <c r="F6" s="34"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="40"/>
-    </row>
-    <row r="7" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>415</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>547</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>342</v>
-      </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="40"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="63"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34" t="s">
-        <v>343</v>
-      </c>
-      <c r="F8" s="34"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="40"/>
-    </row>
-    <row r="9" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>415</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>344</v>
-      </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33" t="s">
-        <v>345</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>346</v>
-      </c>
-      <c r="G9" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" s="40" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33" t="s">
-        <v>348</v>
-      </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="40"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="63"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33" t="s">
-        <v>349</v>
-      </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="40"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="63"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33" t="s">
-        <v>350</v>
-      </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="40"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -6397,7 +6195,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6415,22 +6213,22 @@
         <v>8</v>
       </c>
       <c r="C2" s="65" t="s">
+        <v>349</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>350</v>
+      </c>
+      <c r="E2" s="66" t="s">
         <v>351</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="F2" s="65" t="s">
         <v>352</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="G2" s="65" t="s">
         <v>353</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="H2" s="65" t="s">
         <v>354</v>
-      </c>
-      <c r="G2" s="65" t="s">
-        <v>355</v>
-      </c>
-      <c r="H2" s="65" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -6447,19 +6245,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
+        <v>355</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>413</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>492</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>356</v>
+      </c>
+      <c r="E4" s="67" t="s">
         <v>357</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>415</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>495</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>358</v>
-      </c>
-      <c r="E4" s="67" t="s">
-        <v>359</v>
       </c>
       <c r="F4" s="50">
         <v>1</v>
@@ -6468,26 +6266,26 @@
         <v>1</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I4" s="70"/>
       <c r="J4" s="64"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
+        <v>355</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>413</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>493</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>359</v>
+      </c>
+      <c r="E5" s="67" t="s">
         <v>357</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>415</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>496</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>361</v>
-      </c>
-      <c r="E5" s="67" t="s">
-        <v>359</v>
       </c>
       <c r="F5" s="50">
         <v>1</v>
@@ -6496,7 +6294,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I5" s="70"/>
       <c r="J5" s="64"/>
@@ -6543,7 +6341,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="71" customFormat="1" ht="101.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6582,61 +6380,61 @@
         <v>98</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="F2" s="72" t="s">
         <v>99</v>
       </c>
       <c r="G2" s="72" t="s">
+        <v>496</v>
+      </c>
+      <c r="H2" s="72" t="s">
+        <v>497</v>
+      </c>
+      <c r="I2" s="72" t="s">
+        <v>498</v>
+      </c>
+      <c r="J2" s="72" t="s">
         <v>499</v>
       </c>
-      <c r="H2" s="72" t="s">
+      <c r="K2" s="73" t="s">
         <v>500</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="L2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="M2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="N2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>508</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>362</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>363</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>364</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>509</v>
-      </c>
-      <c r="R2" s="72" t="s">
-        <v>510</v>
-      </c>
-      <c r="S2" s="72" t="s">
-        <v>511</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>364</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>365</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>366</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -6668,58 +6466,58 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="74" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G4" s="74">
         <v>2</v>
       </c>
       <c r="H4" s="74" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I4" s="74">
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
+        <v>369</v>
+      </c>
+      <c r="K4" s="74" t="s">
+        <v>370</v>
+      </c>
+      <c r="L4" s="74" t="s">
+        <v>511</v>
+      </c>
+      <c r="M4" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="K4" s="74" t="s">
-        <v>372</v>
-      </c>
-      <c r="L4" s="74" t="s">
-        <v>514</v>
-      </c>
-      <c r="M4" s="74" t="s">
+      <c r="N4" s="75" t="s">
+        <v>512</v>
+      </c>
+      <c r="O4" s="74" t="s">
         <v>373</v>
       </c>
-      <c r="N4" s="75" t="s">
-        <v>515</v>
-      </c>
-      <c r="O4" s="74" t="s">
+      <c r="P4" s="74" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q4" s="74" t="s">
         <v>375</v>
       </c>
-      <c r="P4" s="74" t="s">
+      <c r="R4" s="74" t="s">
         <v>376</v>
-      </c>
-      <c r="Q4" s="74" t="s">
-        <v>377</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>378</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>1</v>
@@ -6728,10 +6526,10 @@
         <v>119</v>
       </c>
       <c r="U4" s="50" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="V4" s="50" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="W4" s="50">
         <v>15</v>
@@ -6739,58 +6537,58 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="74" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>114</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G5" s="74">
         <v>2</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I5" s="74">
         <v>256</v>
       </c>
       <c r="J5" s="74" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K5" s="74" t="s">
+        <v>514</v>
+      </c>
+      <c r="L5" s="74" t="s">
+        <v>515</v>
+      </c>
+      <c r="M5" s="74" t="s">
+        <v>394</v>
+      </c>
+      <c r="N5" s="75" t="s">
+        <v>516</v>
+      </c>
+      <c r="O5" s="74" t="s">
+        <v>395</v>
+      </c>
+      <c r="P5" s="74" t="s">
         <v>517</v>
       </c>
-      <c r="L5" s="74" t="s">
-        <v>518</v>
-      </c>
-      <c r="M5" s="74" t="s">
-        <v>396</v>
-      </c>
-      <c r="N5" s="75" t="s">
-        <v>519</v>
-      </c>
-      <c r="O5" s="74" t="s">
-        <v>397</v>
-      </c>
-      <c r="P5" s="74" t="s">
-        <v>520</v>
-      </c>
       <c r="Q5" s="74" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="R5" s="74" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="S5" s="74" t="b">
         <v>0</v>
@@ -6799,10 +6597,10 @@
         <v>119</v>
       </c>
       <c r="U5" s="50" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="V5" s="50" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="W5" s="50">
         <v>15</v>
@@ -6876,7 +6674,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="71" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6916,61 +6714,61 @@
         <v>98</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="F2" s="72" t="s">
         <v>99</v>
       </c>
       <c r="G2" s="72" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H2" s="72" t="s">
+        <v>497</v>
+      </c>
+      <c r="I2" s="72" t="s">
+        <v>498</v>
+      </c>
+      <c r="J2" s="72" t="s">
+        <v>499</v>
+      </c>
+      <c r="K2" s="92" t="s">
         <v>500</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="L2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="M2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="K2" s="92" t="s">
+      <c r="N2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>508</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>362</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>363</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>364</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>509</v>
-      </c>
-      <c r="R2" s="72" t="s">
-        <v>510</v>
-      </c>
-      <c r="S2" s="72" t="s">
-        <v>511</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>364</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>365</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>366</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -7002,58 +6800,58 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="74" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G4" s="74">
         <v>2</v>
       </c>
       <c r="H4" s="74" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I4" s="74">
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K4" s="74" t="s">
+        <v>370</v>
+      </c>
+      <c r="L4" s="74" t="s">
+        <v>520</v>
+      </c>
+      <c r="M4" s="74" t="s">
+        <v>397</v>
+      </c>
+      <c r="N4" s="74" t="s">
         <v>372</v>
       </c>
-      <c r="L4" s="74" t="s">
-        <v>523</v>
-      </c>
-      <c r="M4" s="74" t="s">
-        <v>399</v>
-      </c>
-      <c r="N4" s="74" t="s">
+      <c r="O4" s="74" t="s">
+        <v>398</v>
+      </c>
+      <c r="P4" s="74" t="s">
         <v>374</v>
       </c>
-      <c r="O4" s="74" t="s">
-        <v>400</v>
-      </c>
-      <c r="P4" s="74" t="s">
+      <c r="Q4" s="74" t="s">
+        <v>375</v>
+      </c>
+      <c r="R4" s="74" t="s">
         <v>376</v>
-      </c>
-      <c r="Q4" s="74" t="s">
-        <v>377</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>378</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>0</v>
@@ -7062,10 +6860,10 @@
         <v>119</v>
       </c>
       <c r="U4" s="50" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="V4" s="50" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="W4" s="50">
         <v>15</v>
@@ -7073,58 +6871,58 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="74" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G5" s="74">
         <v>2</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="I5" s="74">
         <v>256</v>
       </c>
       <c r="J5" s="74" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K5" s="74" t="s">
+        <v>514</v>
+      </c>
+      <c r="L5" s="74" t="s">
+        <v>523</v>
+      </c>
+      <c r="M5" s="74" t="s">
+        <v>524</v>
+      </c>
+      <c r="N5" s="74" t="s">
+        <v>525</v>
+      </c>
+      <c r="O5" s="74" t="s">
+        <v>526</v>
+      </c>
+      <c r="P5" s="74" t="s">
         <v>517</v>
       </c>
-      <c r="L5" s="74" t="s">
-        <v>526</v>
-      </c>
-      <c r="M5" s="74" t="s">
-        <v>527</v>
-      </c>
-      <c r="N5" s="74" t="s">
-        <v>528</v>
-      </c>
-      <c r="O5" s="74" t="s">
-        <v>529</v>
-      </c>
-      <c r="P5" s="74" t="s">
-        <v>520</v>
-      </c>
       <c r="Q5" s="74" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="R5" s="74" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="S5" s="74" t="b">
         <v>1</v>
@@ -7133,10 +6931,10 @@
         <v>119</v>
       </c>
       <c r="U5" s="50" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="V5" s="50" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="W5" s="50">
         <v>15</v>
@@ -7209,7 +7007,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="71" customFormat="1" ht="115.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -7248,61 +7046,61 @@
         <v>98</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F2" s="73" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="G2" s="72" t="s">
         <v>99</v>
       </c>
       <c r="H2" s="72" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I2" s="72" t="s">
+        <v>498</v>
+      </c>
+      <c r="J2" s="72" t="s">
+        <v>499</v>
+      </c>
+      <c r="K2" s="73" t="s">
+        <v>500</v>
+      </c>
+      <c r="L2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="J2" s="72" t="s">
-        <v>502</v>
-      </c>
-      <c r="K2" s="73" t="s">
+      <c r="M2" s="72" t="s">
+        <v>350</v>
+      </c>
+      <c r="N2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="M2" s="72" t="s">
-        <v>352</v>
-      </c>
-      <c r="N2" s="72" t="s">
+      <c r="P2" s="72" t="s">
+        <v>505</v>
+      </c>
+      <c r="Q2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>508</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>362</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>363</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>364</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>509</v>
-      </c>
-      <c r="R2" s="72" t="s">
-        <v>510</v>
-      </c>
-      <c r="S2" s="72" t="s">
-        <v>511</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>364</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>365</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>366</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="84" customFormat="1" x14ac:dyDescent="0.3">
@@ -7336,22 +7134,22 @@
         <v>6</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H4" s="74">
         <v>2</v>
@@ -7360,31 +7158,31 @@
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
+        <v>369</v>
+      </c>
+      <c r="K4" s="74" t="s">
+        <v>370</v>
+      </c>
+      <c r="L4" s="74" t="s">
+        <v>401</v>
+      </c>
+      <c r="M4" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="N4" s="74" t="s">
         <v>372</v>
       </c>
-      <c r="L4" s="74" t="s">
-        <v>403</v>
-      </c>
-      <c r="M4" s="74" t="s">
+      <c r="O4" s="74" t="s">
         <v>373</v>
       </c>
-      <c r="N4" s="74" t="s">
+      <c r="P4" s="74" t="s">
         <v>374</v>
       </c>
-      <c r="O4" s="74" t="s">
+      <c r="Q4" s="74" t="s">
         <v>375</v>
       </c>
-      <c r="P4" s="74" t="s">
+      <c r="R4" s="74" t="s">
         <v>376</v>
-      </c>
-      <c r="Q4" s="74" t="s">
-        <v>377</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>378</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>1</v>
@@ -7393,10 +7191,10 @@
         <v>119</v>
       </c>
       <c r="U4" s="50" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="V4" s="50" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="W4" s="50">
         <v>10</v>
@@ -7452,25 +7250,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="65" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B1" s="65" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C1" s="85" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D1" s="85" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G1" s="86" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -7478,133 +7276,133 @@
         <v>118</v>
       </c>
       <c r="B2" s="74" t="s">
+        <v>368</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>531</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>376</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>404</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>392</v>
+      </c>
+      <c r="G2" s="74" t="s">
         <v>370</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>534</v>
-      </c>
-      <c r="D2" s="59" t="s">
-        <v>378</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>406</v>
-      </c>
-      <c r="F2" s="50" t="s">
-        <v>394</v>
-      </c>
-      <c r="G2" s="74" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="50" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="50"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="50"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="50" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D7" s="50"/>
       <c r="E7" s="50" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="50" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="50" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="50" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="50" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="50"/>
@@ -7613,11 +7411,11 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="50" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="50" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D10" s="50"/>
       <c r="E10" s="50"/>
@@ -7626,11 +7424,11 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="50" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
@@ -7639,11 +7437,11 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="50" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
@@ -7654,7 +7452,7 @@
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="50"/>
@@ -7665,7 +7463,7 @@
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
@@ -7723,10 +7521,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7734,10 +7532,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -7745,10 +7543,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -7756,10 +7554,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -7791,7 +7589,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="57" customFormat="1" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="96" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -7839,19 +7637,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>437</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>486</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>546</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>438</v>
+      </c>
+      <c r="F4" s="59" t="s">
         <v>439</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>488</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>549</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>440</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>441</v>
       </c>
       <c r="G4" s="50"/>
     </row>
@@ -7861,13 +7659,13 @@
       <c r="C5" s="50"/>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -7875,22 +7673,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -7898,22 +7696,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G7" s="50" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -7925,6 +7723,275 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J1:J1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="19.21875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="49" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="49" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="49" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="49" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="49" customWidth="1"/>
+    <col min="8" max="8" width="21" style="49" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="21.109375" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
+        <v>555</v>
+      </c>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="101"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>325</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>327</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>328</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>329</v>
+      </c>
+      <c r="H2" s="53" t="s">
+        <v>330</v>
+      </c>
+      <c r="I2" s="54" t="s">
+        <v>553</v>
+      </c>
+      <c r="J2" s="54" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="56"/>
+    </row>
+    <row r="4" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>486</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>413</v>
+      </c>
+      <c r="J4" s="40" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="63"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>554</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>413</v>
+      </c>
+      <c r="J5" s="40"/>
+    </row>
+    <row r="6" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>486</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>338</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34" t="s">
+        <v>339</v>
+      </c>
+      <c r="F6" s="34"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="40"/>
+    </row>
+    <row r="7" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>413</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>544</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>340</v>
+      </c>
+      <c r="F7" s="34"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="40"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="63"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="F8" s="34"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="40"/>
+    </row>
+    <row r="9" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>413</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>342</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>344</v>
+      </c>
+      <c r="G9" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="33"/>
+      <c r="I9" s="50" t="s">
+        <v>417</v>
+      </c>
+      <c r="J9" s="40" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="40"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="63"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33" t="s">
+        <v>347</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="40"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="63"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33" t="s">
+        <v>348</v>
+      </c>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="50" t="s">
+        <v>417</v>
+      </c>
+      <c r="J12" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -7948,8 +8015,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="209.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
-        <v>413</v>
+      <c r="A1" s="102" t="s">
+        <v>411</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -8017,7 +8084,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
@@ -8026,7 +8093,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F4" s="50" t="s">
         <v>27</v>
@@ -8038,13 +8105,13 @@
         <v>24</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J4" s="50" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="50" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
@@ -8052,10 +8119,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>26</v>
@@ -8073,7 +8140,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="50" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J5" s="50" t="s">
         <v>28</v>
@@ -8085,10 +8152,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D6" s="50" t="s">
         <v>29</v>
@@ -8106,7 +8173,7 @@
         <v>24</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="J6" s="50" t="s">
         <v>28</v>
@@ -8122,7 +8189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -8139,7 +8206,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="57" customFormat="1" ht="142.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="101"/>
@@ -8157,7 +8224,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -8191,7 +8258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -8211,7 +8278,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="99" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="100"/>
@@ -8260,7 +8327,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
@@ -8275,7 +8342,7 @@
         <v>45</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -8283,10 +8350,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>43</v>
@@ -8304,13 +8371,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>46</v>
@@ -8329,7 +8396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
@@ -8358,7 +8425,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="172.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="102" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="100"/>
@@ -8456,13 +8523,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>59</v>
@@ -8484,7 +8551,7 @@
         <v>24</v>
       </c>
       <c r="L4" s="60" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M4" s="60" t="s">
         <v>24</v>
@@ -8505,16 +8572,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F5" s="50" t="s">
         <v>60</v>
@@ -8552,13 +8619,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>64</v>
@@ -8599,16 +8666,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F7" s="50" t="s">
         <v>60</v>
@@ -8617,7 +8684,7 @@
         <v>66</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I7" s="50"/>
       <c r="J7" s="50" t="s">
@@ -8648,16 +8715,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D8" s="50" t="s">
+        <v>460</v>
+      </c>
+      <c r="E8" s="50" t="s">
         <v>462</v>
-      </c>
-      <c r="E8" s="50" t="s">
-        <v>464</v>
       </c>
       <c r="F8" s="50" t="s">
         <v>60</v>
@@ -8666,11 +8733,11 @@
         <v>66</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I8" s="50"/>
       <c r="J8" s="50" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K8" s="50" t="s">
         <v>27</v>
@@ -8697,16 +8764,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E9" s="50" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F9" s="50" t="s">
         <v>60</v>
@@ -8715,17 +8782,17 @@
         <v>66</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I9" s="50"/>
       <c r="J9" s="50" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K9" s="50" t="s">
         <v>27</v>
       </c>
       <c r="L9" s="60" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M9" s="60" t="s">
         <v>27</v>
@@ -8748,71 +8815,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="49" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" style="49" customWidth="1"/>
-    <col min="5" max="5" width="16" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.77734375" style="49" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" style="49" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="101"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
SetUpOCI - menu alignment CD3 - Tags example values change
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -5340,8 +5340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7574,7 +7574,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7727,7 +7727,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7932,7 +7932,7 @@
       </c>
       <c r="H9" s="33"/>
       <c r="I9" s="50" t="s">
-        <v>417</v>
+        <v>445</v>
       </c>
       <c r="J9" s="40" t="s">
         <v>345</v>
@@ -7978,7 +7978,7 @@
       <c r="G12" s="33"/>
       <c r="H12" s="33"/>
       <c r="I12" s="50" t="s">
-        <v>417</v>
+        <v>445</v>
       </c>
       <c r="J12" s="40"/>
     </row>

</xml_diff>

<commit_message>
Description space change, CD3 typo corrected, LBR added if loop to templates to avoid modification
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -474,10 +474,6 @@
     <t>VM.Standard.E3.Flex::5</t>
   </si>
   <si>
-    <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
-# Make sure to enter exact name in "Attached To Instance" column as entered in "Hostname" of Instances sheet;"Backup Policy" column can be left blank at the time of block volume creation and can be filled up later on while attaching backup policy to the boot abd block volumes together;</t>
-  </si>
-  <si>
     <t>Block Name</t>
   </si>
   <si>
@@ -1839,6 +1835,11 @@
 Enter compartment as 'root' to create the Tags in 'root' compartment
 Is Cost Tracking - defaults to"FALSE", if left empty 
 Validator - For entering values of type "list" use ENUM::&lt;values in double quotes separated by comma&gt; and for type "string" use ENUM::"&lt;value&gt;"</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+# Make sure to enter exact name in "Attached To Instance" column as entered in "Hostname" of Instances sheet;
+Leave  "Backup Policy" value as empty if you do not need any policy to be attached to the volumes.</t>
   </si>
 </sst>
 </file>
@@ -2833,7 +2834,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -3111,10 +3112,10 @@
         <v>71</v>
       </c>
       <c r="S2" s="89" t="s">
+        <v>546</v>
+      </c>
+      <c r="T2" s="89" t="s">
         <v>547</v>
-      </c>
-      <c r="T2" s="89" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3146,13 +3147,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>89</v>
@@ -3186,28 +3187,28 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>94</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>91</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I5" s="47" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
@@ -3230,13 +3231,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>89</v>
@@ -3268,13 +3269,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>94</v>
@@ -3289,7 +3290,7 @@
         <v>92</v>
       </c>
       <c r="I7" s="47" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
@@ -3378,7 +3379,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>101</v>
@@ -3398,7 +3399,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>103</v>
@@ -3418,7 +3419,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>105</v>
@@ -3430,7 +3431,7 @@
         <v>102</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -3552,37 +3553,37 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D4" s="50" t="s">
+        <v>472</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>411</v>
+      </c>
+      <c r="F4" s="50" t="s">
         <v>473</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>412</v>
-      </c>
-      <c r="F4" s="50" t="s">
-        <v>474</v>
       </c>
       <c r="G4" s="50" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I4" s="50" t="s">
         <v>117</v>
       </c>
       <c r="J4" s="50" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K4" s="50" t="s">
         <v>119</v>
       </c>
       <c r="L4" s="50" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M4" s="50"/>
       <c r="N4" s="50" t="s">
@@ -3594,19 +3595,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>120</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G5" s="50" t="b">
         <v>0</v>
@@ -3616,13 +3617,13 @@
         <v>117</v>
       </c>
       <c r="J5" s="50" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K5" s="50" t="s">
         <v>119</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M5" s="50"/>
       <c r="N5" s="50" t="s">
@@ -3634,19 +3635,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G6" s="50" t="b">
         <v>0</v>
@@ -3662,10 +3663,10 @@
         <v>119</v>
       </c>
       <c r="L6" s="50" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M6" s="50" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="N6" s="50"/>
     </row>
@@ -3674,19 +3675,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>120</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G7" s="50" t="b">
         <v>0</v>
@@ -3702,10 +3703,10 @@
         <v>119</v>
       </c>
       <c r="L7" s="50" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M7" s="50" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N7" s="50"/>
     </row>
@@ -3739,7 +3740,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>123</v>
+        <v>555</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -3757,19 +3758,19 @@
         <v>8</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>98</v>
       </c>
       <c r="F2" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>126</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>127</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>111</v>
@@ -3792,10 +3793,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D4" s="50">
         <v>150</v>
@@ -3804,13 +3805,13 @@
         <v>65</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H4" s="59" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3818,10 +3819,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D5" s="50">
         <v>150</v>
@@ -3830,13 +3831,13 @@
         <v>65</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H5" s="59" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -3877,7 +3878,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="84.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -3906,40 +3907,40 @@
         <v>98</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="O2" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>141</v>
       </c>
       <c r="P2" s="14" t="s">
         <v>112</v>
@@ -3970,26 +3971,26 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>104</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="I4" s="32" t="s">
         <v>144</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>145</v>
       </c>
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
@@ -3998,7 +3999,7 @@
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
       <c r="P4" s="48" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -4011,13 +4012,13 @@
       <c r="G5" s="32"/>
       <c r="H5" s="32"/>
       <c r="I5" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="J5" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="K5" s="32" t="s">
         <v>146</v>
-      </c>
-      <c r="K5" s="32" t="s">
-        <v>147</v>
       </c>
       <c r="L5" s="32"/>
       <c r="M5" s="32"/>
@@ -4034,13 +4035,13 @@
       <c r="G6" s="32"/>
       <c r="H6" s="32"/>
       <c r="I6" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J6" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="K6" s="32" t="s">
         <v>148</v>
-      </c>
-      <c r="K6" s="32" t="s">
-        <v>149</v>
       </c>
       <c r="L6" s="32"/>
       <c r="M6" s="32"/>
@@ -4053,24 +4054,24 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>104</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
       <c r="H7" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="I7" s="32" t="s">
         <v>150</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>151</v>
       </c>
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
@@ -4085,37 +4086,37 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>114</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
       <c r="H8" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="I8" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="J8" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="J8" s="32" t="s">
-        <v>155</v>
-      </c>
       <c r="K8" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L8" s="32"/>
       <c r="M8" s="32"/>
       <c r="N8" s="32"/>
       <c r="O8" s="32"/>
       <c r="P8" s="50" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4123,30 +4124,30 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>114</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="I9" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="I9" s="32" t="s">
-        <v>154</v>
-      </c>
       <c r="J9" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K9" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L9" s="32"/>
       <c r="M9" s="32"/>
@@ -4159,24 +4160,24 @@
         <v>6</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>104</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E10" s="48" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
       <c r="H10" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="I10" s="32" t="s">
         <v>159</v>
-      </c>
-      <c r="I10" s="32" t="s">
-        <v>160</v>
       </c>
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
@@ -4219,7 +4220,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="102" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" s="102"/>
       <c r="C1" s="102"/>
@@ -4244,43 +4245,43 @@
         <v>8</v>
       </c>
       <c r="C2" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="E2" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="F2" s="42" t="s">
         <v>164</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>165</v>
       </c>
       <c r="G2" s="43" t="s">
         <v>112</v>
       </c>
       <c r="H2" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="J2" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="K2" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="L2" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="L2" s="43" t="s">
+      <c r="M2" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="M2" s="43" t="s">
-        <v>171</v>
-      </c>
       <c r="N2" s="43" t="s">
+        <v>488</v>
+      </c>
+      <c r="O2" s="43" t="s">
         <v>489</v>
-      </c>
-      <c r="O2" s="43" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4307,40 +4308,40 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F4" s="50" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="50"/>
       <c r="H4" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="I4" s="50" t="s">
         <v>173</v>
-      </c>
-      <c r="I4" s="50" t="s">
-        <v>174</v>
       </c>
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
       <c r="L4" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="M4" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="M4" s="48" t="s">
-        <v>176</v>
-      </c>
       <c r="N4" s="50" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="O4" s="87" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -4353,15 +4354,15 @@
       <c r="G5" s="50"/>
       <c r="H5" s="48"/>
       <c r="I5" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
       <c r="L5" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="M5" s="48" t="s">
         <v>175</v>
-      </c>
-      <c r="M5" s="48" t="s">
-        <v>176</v>
       </c>
       <c r="N5" s="50"/>
       <c r="O5" s="50"/>
@@ -4371,40 +4372,40 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F6" s="50" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H6" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="I6" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="I6" s="50" t="s">
+      <c r="J6" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="K6" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="J6" s="50" t="s">
-        <v>175</v>
-      </c>
-      <c r="K6" s="50" t="s">
-        <v>181</v>
-      </c>
       <c r="L6" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M6" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N6" s="50"/>
       <c r="O6" s="50"/>
@@ -4444,7 +4445,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="102" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -4470,46 +4471,46 @@
         <v>8</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E2" s="51" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="G2" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="H2" s="51" t="s">
         <v>185</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="I2" s="51" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="J2" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="K2" s="51" t="s">
         <v>188</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="L2" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="L2" s="51" t="s">
+      <c r="M2" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="M2" s="51" t="s">
+      <c r="N2" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="N2" s="51" t="s">
+      <c r="O2" s="51" t="s">
         <v>192</v>
       </c>
-      <c r="O2" s="51" t="s">
+      <c r="P2" s="15" t="s">
         <v>193</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -4537,41 +4538,41 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>482</v>
+      </c>
+      <c r="G4" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="F4" s="50" t="s">
-        <v>483</v>
-      </c>
-      <c r="G4" s="50" t="s">
+      <c r="H4" s="50" t="s">
         <v>196</v>
-      </c>
-      <c r="H4" s="50" t="s">
-        <v>197</v>
       </c>
       <c r="I4" s="50">
         <v>80</v>
       </c>
       <c r="J4" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="K4" s="50" t="s">
         <v>198</v>
       </c>
-      <c r="K4" s="50" t="s">
+      <c r="L4" s="50" t="s">
         <v>199</v>
-      </c>
-      <c r="L4" s="50" t="s">
-        <v>200</v>
       </c>
       <c r="M4" s="50" t="b">
         <v>1</v>
       </c>
       <c r="N4" s="50" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O4" s="50" t="s">
         <v>27</v>
@@ -4585,29 +4586,29 @@
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
       <c r="D5" s="50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>483</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5" s="50" t="s">
         <v>201</v>
-      </c>
-      <c r="F5" s="50" t="s">
-        <v>484</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>196</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>202</v>
       </c>
       <c r="I5" s="50">
         <v>443</v>
       </c>
       <c r="J5" s="50"/>
       <c r="K5" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="L5" s="50" t="s">
         <v>203</v>
-      </c>
-      <c r="L5" s="50" t="s">
-        <v>204</v>
       </c>
       <c r="M5" s="50" t="b">
         <v>1</v>
@@ -4623,29 +4624,29 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G6" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="H6" s="50" t="s">
         <v>196</v>
-      </c>
-      <c r="H6" s="50" t="s">
-        <v>197</v>
       </c>
       <c r="I6" s="50">
         <v>80</v>
       </c>
       <c r="J6" s="50" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K6" s="50" t="s">
         <v>27</v>
@@ -4695,7 +4696,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="96" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -4720,52 +4721,52 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="O2" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="P2" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="Q2" s="14" t="s">
         <v>220</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>221</v>
       </c>
       <c r="R2" s="14" t="s">
         <v>32</v>
@@ -4798,16 +4799,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C4" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="D4" s="50" t="s">
-        <v>223</v>
-      </c>
       <c r="E4" s="50" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
@@ -4831,7 +4832,7 @@
       <c r="C5" s="50"/>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="50"/>
@@ -4853,7 +4854,7 @@
       <c r="C6" s="50"/>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="50"/>
@@ -4875,7 +4876,7 @@
       <c r="C7" s="50"/>
       <c r="D7" s="50"/>
       <c r="E7" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -4897,7 +4898,7 @@
       <c r="C8" s="50"/>
       <c r="D8" s="50"/>
       <c r="E8" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
@@ -4918,7 +4919,7 @@
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
       <c r="D9" s="50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="50" t="b">
@@ -4944,19 +4945,19 @@
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
       <c r="D10" s="50" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E10" s="50"/>
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
       <c r="H10" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="I10" s="50" t="s">
         <v>231</v>
       </c>
-      <c r="I10" s="50" t="s">
+      <c r="J10" s="50" t="s">
         <v>232</v>
-      </c>
-      <c r="J10" s="50" t="s">
-        <v>233</v>
       </c>
       <c r="K10" s="50"/>
       <c r="L10" s="50"/>
@@ -4972,27 +4973,27 @@
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
       <c r="D11" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E11" s="50"/>
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>
       <c r="H11" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="I11" s="50" t="s">
         <v>235</v>
-      </c>
-      <c r="I11" s="50" t="s">
-        <v>236</v>
       </c>
       <c r="J11" s="50"/>
       <c r="K11" s="50" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L11" s="50"/>
       <c r="M11" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="N11" s="50" t="s">
         <v>238</v>
-      </c>
-      <c r="N11" s="50" t="s">
-        <v>239</v>
       </c>
       <c r="O11" s="50">
         <v>302</v>
@@ -5006,27 +5007,27 @@
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
       <c r="D12" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
       <c r="H12" s="50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I12" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J12" s="50"/>
       <c r="K12" s="50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L12" s="50"/>
       <c r="M12" s="50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N12" s="50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O12" s="50">
         <v>303</v>
@@ -5040,7 +5041,7 @@
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
       <c r="D13" s="50" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
@@ -5050,13 +5051,13 @@
       <c r="J13" s="50"/>
       <c r="K13" s="50"/>
       <c r="L13" s="50" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M13" s="50"/>
       <c r="N13" s="50"/>
       <c r="O13" s="50"/>
       <c r="P13" s="50" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Q13" s="50"/>
       <c r="R13" s="50"/>
@@ -5066,7 +5067,7 @@
       <c r="B14" s="50"/>
       <c r="C14" s="50"/>
       <c r="D14" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E14" s="50"/>
       <c r="F14" s="50"/>
@@ -5076,7 +5077,7 @@
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
       <c r="L14" s="50" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M14" s="50"/>
       <c r="N14" s="50"/>
@@ -5084,7 +5085,7 @@
       <c r="P14" s="50"/>
       <c r="Q14" s="50"/>
       <c r="R14" s="50" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -5092,7 +5093,7 @@
       <c r="B15" s="50"/>
       <c r="C15" s="50"/>
       <c r="D15" s="50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="50"/>
@@ -5102,7 +5103,7 @@
       <c r="J15" s="50"/>
       <c r="K15" s="50"/>
       <c r="L15" s="50" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M15" s="50"/>
       <c r="N15" s="50"/>
@@ -5116,7 +5117,7 @@
       <c r="B16" s="50"/>
       <c r="C16" s="50"/>
       <c r="D16" s="50" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E16" s="50"/>
       <c r="F16" s="50"/>
@@ -5126,7 +5127,7 @@
       <c r="J16" s="50"/>
       <c r="K16" s="50"/>
       <c r="L16" s="50" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M16" s="50"/>
       <c r="N16" s="50"/>
@@ -5134,7 +5135,7 @@
       <c r="P16" s="50"/>
       <c r="Q16" s="50"/>
       <c r="R16" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
@@ -5142,7 +5143,7 @@
       <c r="B17" s="50"/>
       <c r="C17" s="50"/>
       <c r="D17" s="50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E17" s="50"/>
       <c r="F17" s="50"/>
@@ -5152,7 +5153,7 @@
       <c r="J17" s="50"/>
       <c r="K17" s="50"/>
       <c r="L17" s="50" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M17" s="50"/>
       <c r="N17" s="50"/>
@@ -5166,7 +5167,7 @@
       <c r="B18" s="50"/>
       <c r="C18" s="50"/>
       <c r="D18" s="50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E18" s="50"/>
       <c r="F18" s="50"/>
@@ -5176,13 +5177,13 @@
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
       <c r="L18" s="50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M18" s="50"/>
       <c r="N18" s="50"/>
       <c r="O18" s="50"/>
       <c r="P18" s="50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q18" s="50"/>
       <c r="R18" s="50"/>
@@ -5211,13 +5212,13 @@
       <c r="A20" s="50"/>
       <c r="B20" s="50"/>
       <c r="C20" s="50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D20" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="E20" s="50" t="s">
         <v>223</v>
-      </c>
-      <c r="E20" s="50" t="s">
-        <v>224</v>
       </c>
       <c r="F20" s="50"/>
       <c r="G20" s="50"/>
@@ -5239,7 +5240,7 @@
       <c r="C21" s="50"/>
       <c r="D21" s="50"/>
       <c r="E21" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="50"/>
@@ -5260,16 +5261,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D22" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="E22" s="50" t="s">
         <v>223</v>
-      </c>
-      <c r="E22" s="50" t="s">
-        <v>224</v>
       </c>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
@@ -5291,7 +5292,7 @@
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
       <c r="E23" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F23" s="50"/>
       <c r="G23" s="50"/>
@@ -5387,10 +5388,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>412</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>413</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>414</v>
       </c>
       <c r="D4" s="50"/>
     </row>
@@ -5399,13 +5400,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
+        <v>414</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>415</v>
       </c>
-      <c r="C5" s="50" t="s">
-        <v>416</v>
-      </c>
       <c r="D5" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -5413,13 +5414,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>416</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>417</v>
       </c>
-      <c r="C6" s="50" t="s">
-        <v>418</v>
-      </c>
       <c r="D6" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -5427,10 +5428,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
+        <v>418</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>419</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>420</v>
       </c>
       <c r="D7" s="50"/>
     </row>
@@ -5439,13 +5440,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -5453,13 +5454,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C9" s="50" t="s">
+        <v>421</v>
+      </c>
+      <c r="D9" s="50" t="s">
         <v>422</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -5467,13 +5468,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -5481,13 +5482,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="50" t="s">
+        <v>424</v>
+      </c>
+      <c r="C11" s="50" t="s">
         <v>425</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="D11" s="50" t="s">
         <v>426</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -5517,7 +5518,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="57" customFormat="1" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="96" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -5530,19 +5531,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>261</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -5560,19 +5561,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C4" s="50" t="s">
+        <v>262</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="50" t="s">
         <v>263</v>
       </c>
-      <c r="D4" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>264</v>
-      </c>
       <c r="F4" s="50" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -5580,29 +5581,29 @@
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
       <c r="D5" s="50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="50"/>
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="50" t="s">
         <v>266</v>
       </c>
-      <c r="D6" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="E6" s="50" t="s">
+      <c r="F6" s="50" t="s">
         <v>267</v>
-      </c>
-      <c r="F6" s="50" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5610,19 +5611,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C7" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7" s="50" t="s">
         <v>269</v>
       </c>
-      <c r="D7" s="50" t="s">
-        <v>205</v>
-      </c>
-      <c r="E7" s="50" t="s">
+      <c r="F7" s="50" t="s">
         <v>270</v>
-      </c>
-      <c r="F7" s="50" t="s">
-        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -5660,7 +5661,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="105" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B1" s="106"/>
       <c r="C1" s="106"/>
@@ -5681,43 +5682,43 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="L2" s="22" t="s">
-        <v>279</v>
-      </c>
       <c r="M2" s="43" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="N2" s="43" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -5743,49 +5744,49 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G4" s="50" t="s">
         <v>27</v>
       </c>
       <c r="H4" s="50"/>
       <c r="I4" s="50" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
       <c r="L4" s="50"/>
       <c r="M4" s="50" t="s">
+        <v>540</v>
+      </c>
+      <c r="N4" s="88" t="s">
         <v>541</v>
-      </c>
-      <c r="N4" s="88" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
       <c r="C5" s="50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>27</v>
@@ -5803,31 +5804,31 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D6" s="50" t="s">
+        <v>280</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="F6" s="50" t="s">
         <v>281</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>269</v>
-      </c>
-      <c r="F6" s="50" t="s">
-        <v>282</v>
       </c>
       <c r="G6" s="50" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J6" s="50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K6" s="50">
         <v>80</v>
@@ -5867,36 +5868,36 @@
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="24" t="s">
         <v>285</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="28" t="s">
         <v>288</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E2" s="27">
         <v>301</v>
@@ -5907,16 +5908,16 @@
     </row>
     <row r="3" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E3" s="36">
         <v>302</v>
@@ -5927,16 +5928,16 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B4" s="36" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" t="s">
         <v>292</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="D4" t="s">
-        <v>293</v>
       </c>
       <c r="E4" s="36">
         <v>303</v>
@@ -5947,13 +5948,13 @@
     </row>
     <row r="5" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D5" s="58"/>
       <c r="E5" s="36">
@@ -5965,10 +5966,10 @@
     </row>
     <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C6" s="26"/>
       <c r="E6" s="36">
@@ -5978,189 +5979,189 @@
     </row>
     <row r="7" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
       <c r="B12" s="36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="36" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="36" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="36" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="36" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="36" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="36" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="36" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="36" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="36" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -6195,7 +6196,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6213,22 +6214,22 @@
         <v>8</v>
       </c>
       <c r="C2" s="65" t="s">
+        <v>348</v>
+      </c>
+      <c r="D2" s="65" t="s">
         <v>349</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="E2" s="66" t="s">
         <v>350</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="F2" s="65" t="s">
         <v>351</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="G2" s="65" t="s">
         <v>352</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="H2" s="65" t="s">
         <v>353</v>
-      </c>
-      <c r="H2" s="65" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -6245,19 +6246,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
+        <v>354</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>412</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>491</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>355</v>
       </c>
-      <c r="B4" s="50" t="s">
-        <v>413</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>492</v>
-      </c>
-      <c r="D4" s="50" t="s">
+      <c r="E4" s="67" t="s">
         <v>356</v>
-      </c>
-      <c r="E4" s="67" t="s">
-        <v>357</v>
       </c>
       <c r="F4" s="50">
         <v>1</v>
@@ -6266,26 +6267,26 @@
         <v>1</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I4" s="70"/>
       <c r="J4" s="64"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E5" s="67" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F5" s="50">
         <v>1</v>
@@ -6294,7 +6295,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I5" s="70"/>
       <c r="J5" s="64"/>
@@ -6341,7 +6342,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="71" customFormat="1" ht="101.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6380,61 +6381,61 @@
         <v>98</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F2" s="72" t="s">
         <v>99</v>
       </c>
       <c r="G2" s="72" t="s">
+        <v>495</v>
+      </c>
+      <c r="H2" s="72" t="s">
         <v>496</v>
       </c>
-      <c r="H2" s="72" t="s">
+      <c r="I2" s="72" t="s">
         <v>497</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="J2" s="72" t="s">
         <v>498</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="73" t="s">
         <v>499</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="M2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="N2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="S2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>361</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>362</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>363</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>508</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>362</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>363</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>364</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -6466,58 +6467,58 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="74" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G4" s="74">
         <v>2</v>
       </c>
       <c r="H4" s="74" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I4" s="74">
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
+        <v>368</v>
+      </c>
+      <c r="K4" s="74" t="s">
         <v>369</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="L4" s="74" t="s">
+        <v>510</v>
+      </c>
+      <c r="M4" s="74" t="s">
         <v>370</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="N4" s="75" t="s">
         <v>511</v>
       </c>
-      <c r="M4" s="74" t="s">
-        <v>371</v>
-      </c>
-      <c r="N4" s="75" t="s">
-        <v>512</v>
-      </c>
       <c r="O4" s="74" t="s">
+        <v>372</v>
+      </c>
+      <c r="P4" s="74" t="s">
         <v>373</v>
       </c>
-      <c r="P4" s="74" t="s">
+      <c r="Q4" s="74" t="s">
         <v>374</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="R4" s="74" t="s">
         <v>375</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>376</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>1</v>
@@ -6526,10 +6527,10 @@
         <v>119</v>
       </c>
       <c r="U4" s="50" t="s">
+        <v>376</v>
+      </c>
+      <c r="V4" s="50" t="s">
         <v>377</v>
-      </c>
-      <c r="V4" s="50" t="s">
-        <v>378</v>
       </c>
       <c r="W4" s="50">
         <v>15</v>
@@ -6537,58 +6538,58 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="74" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>114</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G5" s="74">
         <v>2</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I5" s="74">
         <v>256</v>
       </c>
       <c r="J5" s="74" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K5" s="74" t="s">
+        <v>513</v>
+      </c>
+      <c r="L5" s="74" t="s">
         <v>514</v>
       </c>
-      <c r="L5" s="74" t="s">
+      <c r="M5" s="74" t="s">
+        <v>393</v>
+      </c>
+      <c r="N5" s="75" t="s">
         <v>515</v>
       </c>
-      <c r="M5" s="74" t="s">
+      <c r="O5" s="74" t="s">
         <v>394</v>
       </c>
-      <c r="N5" s="75" t="s">
+      <c r="P5" s="74" t="s">
         <v>516</v>
       </c>
-      <c r="O5" s="74" t="s">
-        <v>395</v>
-      </c>
-      <c r="P5" s="74" t="s">
-        <v>517</v>
-      </c>
       <c r="Q5" s="74" t="s">
+        <v>374</v>
+      </c>
+      <c r="R5" s="74" t="s">
         <v>375</v>
-      </c>
-      <c r="R5" s="74" t="s">
-        <v>376</v>
       </c>
       <c r="S5" s="74" t="b">
         <v>0</v>
@@ -6597,10 +6598,10 @@
         <v>119</v>
       </c>
       <c r="U5" s="50" t="s">
+        <v>376</v>
+      </c>
+      <c r="V5" s="50" t="s">
         <v>377</v>
-      </c>
-      <c r="V5" s="50" t="s">
-        <v>378</v>
       </c>
       <c r="W5" s="50">
         <v>15</v>
@@ -6674,7 +6675,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="71" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6714,61 +6715,61 @@
         <v>98</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F2" s="72" t="s">
         <v>99</v>
       </c>
       <c r="G2" s="72" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H2" s="72" t="s">
+        <v>496</v>
+      </c>
+      <c r="I2" s="72" t="s">
         <v>497</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="J2" s="72" t="s">
         <v>498</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="92" t="s">
         <v>499</v>
       </c>
-      <c r="K2" s="92" t="s">
+      <c r="L2" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="M2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="N2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="S2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>361</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>362</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>363</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>508</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>362</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>363</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>364</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -6800,58 +6801,58 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="74" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G4" s="74">
         <v>2</v>
       </c>
       <c r="H4" s="74" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I4" s="74">
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
+        <v>368</v>
+      </c>
+      <c r="K4" s="74" t="s">
         <v>369</v>
       </c>
-      <c r="K4" s="74" t="s">
-        <v>370</v>
-      </c>
       <c r="L4" s="74" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="M4" s="74" t="s">
+        <v>396</v>
+      </c>
+      <c r="N4" s="74" t="s">
+        <v>371</v>
+      </c>
+      <c r="O4" s="74" t="s">
         <v>397</v>
       </c>
-      <c r="N4" s="74" t="s">
-        <v>372</v>
-      </c>
-      <c r="O4" s="74" t="s">
-        <v>398</v>
-      </c>
       <c r="P4" s="74" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q4" s="74" t="s">
         <v>374</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="R4" s="74" t="s">
         <v>375</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>376</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>0</v>
@@ -6860,10 +6861,10 @@
         <v>119</v>
       </c>
       <c r="U4" s="50" t="s">
+        <v>376</v>
+      </c>
+      <c r="V4" s="50" t="s">
         <v>377</v>
-      </c>
-      <c r="V4" s="50" t="s">
-        <v>378</v>
       </c>
       <c r="W4" s="50">
         <v>15</v>
@@ -6871,58 +6872,58 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="74" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G5" s="74">
         <v>2</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I5" s="74">
         <v>256</v>
       </c>
       <c r="J5" s="74" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K5" s="74" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L5" s="74" t="s">
+        <v>522</v>
+      </c>
+      <c r="M5" s="74" t="s">
         <v>523</v>
       </c>
-      <c r="M5" s="74" t="s">
+      <c r="N5" s="74" t="s">
         <v>524</v>
       </c>
-      <c r="N5" s="74" t="s">
+      <c r="O5" s="74" t="s">
         <v>525</v>
       </c>
-      <c r="O5" s="74" t="s">
-        <v>526</v>
-      </c>
       <c r="P5" s="74" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="Q5" s="74" t="s">
+        <v>374</v>
+      </c>
+      <c r="R5" s="74" t="s">
         <v>375</v>
-      </c>
-      <c r="R5" s="74" t="s">
-        <v>376</v>
       </c>
       <c r="S5" s="74" t="b">
         <v>1</v>
@@ -6931,10 +6932,10 @@
         <v>119</v>
       </c>
       <c r="U5" s="50" t="s">
+        <v>376</v>
+      </c>
+      <c r="V5" s="50" t="s">
         <v>377</v>
-      </c>
-      <c r="V5" s="50" t="s">
-        <v>378</v>
       </c>
       <c r="W5" s="50">
         <v>15</v>
@@ -7007,7 +7008,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="71" customFormat="1" ht="115.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -7046,61 +7047,61 @@
         <v>98</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F2" s="73" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G2" s="72" t="s">
         <v>99</v>
       </c>
       <c r="H2" s="72" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I2" s="72" t="s">
+        <v>497</v>
+      </c>
+      <c r="J2" s="72" t="s">
         <v>498</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="73" t="s">
         <v>499</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="L2" s="72" t="s">
-        <v>501</v>
-      </c>
       <c r="M2" s="72" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N2" s="72" t="s">
+        <v>502</v>
+      </c>
+      <c r="O2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="S2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>361</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>362</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>363</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>508</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>362</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>363</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>364</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="84" customFormat="1" x14ac:dyDescent="0.3">
@@ -7134,22 +7135,22 @@
         <v>6</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H4" s="74">
         <v>2</v>
@@ -7158,31 +7159,31 @@
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
+        <v>368</v>
+      </c>
+      <c r="K4" s="74" t="s">
         <v>369</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="L4" s="74" t="s">
+        <v>400</v>
+      </c>
+      <c r="M4" s="74" t="s">
         <v>370</v>
       </c>
-      <c r="L4" s="74" t="s">
-        <v>401</v>
-      </c>
-      <c r="M4" s="74" t="s">
+      <c r="N4" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="N4" s="74" t="s">
+      <c r="O4" s="74" t="s">
         <v>372</v>
       </c>
-      <c r="O4" s="74" t="s">
+      <c r="P4" s="74" t="s">
         <v>373</v>
       </c>
-      <c r="P4" s="74" t="s">
+      <c r="Q4" s="74" t="s">
         <v>374</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="R4" s="74" t="s">
         <v>375</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>376</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>1</v>
@@ -7191,10 +7192,10 @@
         <v>119</v>
       </c>
       <c r="U4" s="50" t="s">
+        <v>376</v>
+      </c>
+      <c r="V4" s="50" t="s">
         <v>377</v>
-      </c>
-      <c r="V4" s="50" t="s">
-        <v>378</v>
       </c>
       <c r="W4" s="50">
         <v>10</v>
@@ -7250,25 +7251,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="65" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B1" s="65" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1" s="85" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="85" t="s">
-        <v>530</v>
-      </c>
       <c r="D1" s="85" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G1" s="86" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -7276,133 +7277,133 @@
         <v>118</v>
       </c>
       <c r="B2" s="74" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F2" s="50" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G2" s="74" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="50" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="50"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="50"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="50" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D7" s="50"/>
       <c r="E7" s="50" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="50" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="50" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="50" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="50" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="50"/>
@@ -7411,11 +7412,11 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="50" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="50" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D10" s="50"/>
       <c r="E10" s="50"/>
@@ -7424,11 +7425,11 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="50" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
@@ -7437,11 +7438,11 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="50" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
@@ -7452,7 +7453,7 @@
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="50"/>
@@ -7463,7 +7464,7 @@
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
@@ -7521,10 +7522,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>427</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>428</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7532,10 +7533,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
+        <v>429</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>430</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -7543,10 +7544,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>431</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>432</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -7554,10 +7555,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
+        <v>433</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>434</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -7589,7 +7590,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="57" customFormat="1" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="96" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -7637,19 +7638,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>436</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>485</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>545</v>
+      </c>
+      <c r="E4" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="C4" s="50" t="s">
-        <v>486</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>546</v>
-      </c>
-      <c r="E4" s="50" t="s">
+      <c r="F4" s="59" t="s">
         <v>438</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>439</v>
       </c>
       <c r="G4" s="50"/>
     </row>
@@ -7659,13 +7660,13 @@
       <c r="C5" s="50"/>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -7673,22 +7674,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>440</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>418</v>
+      </c>
+      <c r="D6" s="50" t="s">
         <v>441</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>419</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>442</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -7696,22 +7697,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G7" s="50" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -7746,7 +7747,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -7766,28 +7767,28 @@
         <v>8</v>
       </c>
       <c r="C2" s="53" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2" s="53" t="s">
         <v>325</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="E2" s="53" t="s">
         <v>326</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="F2" s="53" t="s">
         <v>327</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="G2" s="53" t="s">
         <v>328</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="H2" s="53" t="s">
         <v>329</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="I2" s="54" t="s">
+        <v>552</v>
+      </c>
+      <c r="J2" s="54" t="s">
         <v>330</v>
-      </c>
-      <c r="I2" s="54" t="s">
-        <v>553</v>
-      </c>
-      <c r="J2" s="54" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -7809,29 +7810,29 @@
         <v>6</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C4" s="38" t="s">
+        <v>331</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="E4" s="33" t="s">
         <v>333</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>334</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>412</v>
+      </c>
+      <c r="J4" s="40" t="s">
         <v>335</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>413</v>
-      </c>
-      <c r="J4" s="40" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -7840,17 +7841,17 @@
       <c r="C5" s="38"/>
       <c r="D5" s="33"/>
       <c r="E5" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F5" s="33"/>
       <c r="G5" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J5" s="40"/>
     </row>
@@ -7859,14 +7860,14 @@
         <v>6</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D6" s="33"/>
       <c r="E6" s="34" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="33"/>
@@ -7879,16 +7880,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>109</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="33"/>
@@ -7902,7 +7903,7 @@
       <c r="C8" s="38"/>
       <c r="D8" s="33"/>
       <c r="E8" s="34" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F8" s="34"/>
       <c r="G8" s="33"/>
@@ -7915,27 +7916,27 @@
         <v>6</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="33" t="s">
+        <v>342</v>
+      </c>
+      <c r="F9" s="33" t="s">
         <v>343</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>344</v>
       </c>
       <c r="G9" s="33" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="33"/>
       <c r="I9" s="50" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J9" s="40" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -7944,7 +7945,7 @@
       <c r="C10" s="38"/>
       <c r="D10" s="33"/>
       <c r="E10" s="33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F10" s="33"/>
       <c r="G10" s="33"/>
@@ -7958,7 +7959,7 @@
       <c r="C11" s="41"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F11" s="33"/>
       <c r="G11" s="33"/>
@@ -7972,13 +7973,13 @@
       <c r="C12" s="41"/>
       <c r="D12" s="33"/>
       <c r="E12" s="33" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F12" s="33"/>
       <c r="G12" s="33"/>
       <c r="H12" s="33"/>
       <c r="I12" s="50" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J12" s="40"/>
     </row>
@@ -8016,7 +8017,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="209.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="102" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -8084,7 +8085,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
@@ -8093,7 +8094,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F4" s="50" t="s">
         <v>27</v>
@@ -8105,13 +8106,13 @@
         <v>24</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J4" s="50" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
@@ -8119,10 +8120,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>26</v>
@@ -8140,7 +8141,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="50" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J5" s="50" t="s">
         <v>28</v>
@@ -8152,10 +8153,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D6" s="50" t="s">
         <v>29</v>
@@ -8173,7 +8174,7 @@
         <v>24</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J6" s="50" t="s">
         <v>28</v>
@@ -8224,7 +8225,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -8327,7 +8328,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
@@ -8342,7 +8343,7 @@
         <v>45</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -8350,10 +8351,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>43</v>
@@ -8371,13 +8372,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>46</v>
@@ -8523,13 +8524,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>59</v>
@@ -8551,7 +8552,7 @@
         <v>24</v>
       </c>
       <c r="L4" s="60" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="M4" s="60" t="s">
         <v>24</v>
@@ -8572,16 +8573,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D5" s="50" t="s">
+        <v>457</v>
+      </c>
+      <c r="E5" s="50" t="s">
         <v>458</v>
-      </c>
-      <c r="E5" s="50" t="s">
-        <v>459</v>
       </c>
       <c r="F5" s="50" t="s">
         <v>60</v>
@@ -8619,13 +8620,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>64</v>
@@ -8666,16 +8667,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F7" s="50" t="s">
         <v>60</v>
@@ -8684,7 +8685,7 @@
         <v>66</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I7" s="50"/>
       <c r="J7" s="50" t="s">
@@ -8715,16 +8716,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F8" s="50" t="s">
         <v>60</v>
@@ -8733,11 +8734,11 @@
         <v>66</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I8" s="50"/>
       <c r="J8" s="50" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K8" s="50" t="s">
         <v>27</v>
@@ -8764,16 +8765,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D9" s="50" t="s">
+        <v>463</v>
+      </c>
+      <c r="E9" s="50" t="s">
         <v>464</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>465</v>
       </c>
       <c r="F9" s="50" t="s">
         <v>60</v>
@@ -8782,17 +8783,17 @@
         <v>66</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I9" s="50"/>
       <c r="J9" s="50" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K9" s="50" t="s">
         <v>27</v>
       </c>
       <c r="L9" s="60" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="M9" s="60" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
NSG - comment added Excel Sheet changes
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -355,10 +355,6 @@
     <t>ICMPCode</t>
   </si>
   <si>
-    <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
-Valid values for sourcetype or destinationtype are: cidr(for CIDR_BLOCK), nsg(for NETWORK_SECURITY_GROUP) and service(for SERVICE_CIDR_BLOCK)</t>
-  </si>
-  <si>
     <t>NSG Name</t>
   </si>
   <si>
@@ -1840,6 +1836,11 @@
     <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
 # Make sure to enter exact name in "Attached To Instance" column as entered in "Hostname" of Instances sheet;
 Leave  "Backup Policy" value as empty if you do not need any policy to be attached to the volumes.</t>
+  </si>
+  <si>
+    <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+Valid values for sourcetype or destinationtype are: cidr(for CIDR_BLOCK), nsg(for NETWORK_SECURITY_GROUP) and service(for SERVICE_CIDR_BLOCK)
+DO NOT change or re-arrange the columns/column names.</t>
   </si>
 </sst>
 </file>
@@ -2834,7 +2835,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -3032,9 +3033,9 @@
     <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="103" t="s">
-        <v>85</v>
+        <v>555</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -3067,10 +3068,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>86</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>87</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>75</v>
@@ -3079,7 +3080,7 @@
         <v>76</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>77</v>
@@ -3112,10 +3113,10 @@
         <v>71</v>
       </c>
       <c r="S2" s="89" t="s">
+        <v>545</v>
+      </c>
+      <c r="T2" s="89" t="s">
         <v>546</v>
-      </c>
-      <c r="T2" s="89" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3147,27 +3148,27 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E4" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="G4" s="50" t="s">
         <v>90</v>
-      </c>
-      <c r="G4" s="50" t="s">
-        <v>91</v>
       </c>
       <c r="H4" s="50"/>
       <c r="I4" s="47"/>
       <c r="J4" s="50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K4" s="50" t="s">
         <v>35</v>
@@ -3187,28 +3188,28 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="50" t="s">
+        <v>466</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="50" t="s">
         <v>467</v>
       </c>
-      <c r="E5" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="F5" s="50" t="s">
+      <c r="G5" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="50" t="s">
         <v>468</v>
       </c>
-      <c r="G5" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>469</v>
-      </c>
       <c r="I5" s="47" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
@@ -3231,28 +3232,28 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E6" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="G6" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="50" t="s">
+      <c r="J6" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="J6" s="50" t="s">
+      <c r="K6" s="47" t="s">
         <v>92</v>
-      </c>
-      <c r="K6" s="47" t="s">
-        <v>93</v>
       </c>
       <c r="L6" s="50"/>
       <c r="M6" s="50"/>
@@ -3269,28 +3270,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E7" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="50" t="s">
-        <v>95</v>
-      </c>
       <c r="G7" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="H7" s="50" t="s">
-        <v>92</v>
-      </c>
       <c r="I7" s="47" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
@@ -3336,7 +3337,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -3352,16 +3353,16 @@
         <v>8</v>
       </c>
       <c r="C2" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="E2" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="F2" s="43" t="s">
         <v>99</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3379,19 +3380,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" s="50" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3399,19 +3400,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C5" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="50" t="s">
-        <v>104</v>
-      </c>
       <c r="E5" s="50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3419,19 +3420,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" s="50" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -3470,7 +3471,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -3494,40 +3495,40 @@
         <v>8</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="I2" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="J2" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="J2" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" s="42" t="s">
+      <c r="L2" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="M2" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="M2" s="42" t="s">
+      <c r="N2" s="42" t="s">
         <v>112</v>
-      </c>
-      <c r="N2" s="42" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3553,41 +3554,41 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D4" s="50" t="s">
+        <v>471</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>410</v>
+      </c>
+      <c r="F4" s="50" t="s">
         <v>472</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>411</v>
-      </c>
-      <c r="F4" s="50" t="s">
-        <v>473</v>
       </c>
       <c r="G4" s="50" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J4" s="50" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K4" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L4" s="50" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="M4" s="50"/>
       <c r="N4" s="50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -3595,39 +3596,39 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G5" s="50" t="b">
         <v>0</v>
       </c>
       <c r="H5" s="50"/>
       <c r="I5" s="50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J5" s="50" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K5" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="M5" s="50"/>
       <c r="N5" s="50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -3635,38 +3636,38 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G6" s="50" t="b">
         <v>0</v>
       </c>
       <c r="H6" s="59"/>
       <c r="I6" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="J6" s="62" t="s">
-        <v>122</v>
-      </c>
       <c r="K6" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L6" s="50" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="M6" s="50" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N6" s="50"/>
     </row>
@@ -3675,38 +3676,38 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G7" s="50" t="b">
         <v>0</v>
       </c>
       <c r="H7" s="59"/>
       <c r="I7" s="50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J7" s="62" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K7" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L7" s="50" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="M7" s="50" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="N7" s="50"/>
     </row>
@@ -3740,7 +3741,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -3758,22 +3759,22 @@
         <v>8</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>126</v>
-      </c>
       <c r="H2" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3793,10 +3794,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D4" s="50">
         <v>150</v>
@@ -3805,13 +3806,13 @@
         <v>65</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H4" s="59" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3819,10 +3820,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D5" s="50">
         <v>150</v>
@@ -3831,13 +3832,13 @@
         <v>65</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H5" s="59" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -3878,7 +3879,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="84.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -3904,46 +3905,46 @@
         <v>8</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="O2" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="O2" s="14" t="s">
-        <v>140</v>
-      </c>
       <c r="P2" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -3971,26 +3972,26 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="I4" s="32" t="s">
         <v>143</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>144</v>
       </c>
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
@@ -3999,7 +4000,7 @@
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
       <c r="P4" s="48" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -4012,13 +4013,13 @@
       <c r="G5" s="32"/>
       <c r="H5" s="32"/>
       <c r="I5" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="J5" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="K5" s="32" t="s">
         <v>145</v>
-      </c>
-      <c r="K5" s="32" t="s">
-        <v>146</v>
       </c>
       <c r="L5" s="32"/>
       <c r="M5" s="32"/>
@@ -4035,13 +4036,13 @@
       <c r="G6" s="32"/>
       <c r="H6" s="32"/>
       <c r="I6" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J6" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="K6" s="32" t="s">
         <v>147</v>
-      </c>
-      <c r="K6" s="32" t="s">
-        <v>148</v>
       </c>
       <c r="L6" s="32"/>
       <c r="M6" s="32"/>
@@ -4054,24 +4055,24 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
       <c r="H7" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="I7" s="32" t="s">
         <v>149</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>150</v>
       </c>
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
@@ -4086,37 +4087,37 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
       <c r="H8" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="J8" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="J8" s="32" t="s">
-        <v>154</v>
-      </c>
       <c r="K8" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L8" s="32"/>
       <c r="M8" s="32"/>
       <c r="N8" s="32"/>
       <c r="O8" s="32"/>
       <c r="P8" s="50" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4124,30 +4125,30 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="I9" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="I9" s="32" t="s">
-        <v>153</v>
-      </c>
       <c r="J9" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K9" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L9" s="32"/>
       <c r="M9" s="32"/>
@@ -4160,24 +4161,24 @@
         <v>6</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E10" s="48" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
       <c r="H10" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="I10" s="32" t="s">
         <v>158</v>
-      </c>
-      <c r="I10" s="32" t="s">
-        <v>159</v>
       </c>
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
@@ -4220,7 +4221,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="102" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B1" s="102"/>
       <c r="C1" s="102"/>
@@ -4245,43 +4246,43 @@
         <v>8</v>
       </c>
       <c r="C2" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="E2" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="F2" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="G2" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="43" t="s">
+      <c r="I2" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="J2" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="K2" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="L2" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="L2" s="43" t="s">
+      <c r="M2" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="43" t="s">
-        <v>170</v>
-      </c>
       <c r="N2" s="43" t="s">
+        <v>487</v>
+      </c>
+      <c r="O2" s="43" t="s">
         <v>488</v>
-      </c>
-      <c r="O2" s="43" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4308,40 +4309,40 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F4" s="50" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="50"/>
       <c r="H4" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4" s="50" t="s">
         <v>172</v>
-      </c>
-      <c r="I4" s="50" t="s">
-        <v>173</v>
       </c>
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
       <c r="L4" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="M4" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="M4" s="48" t="s">
-        <v>175</v>
-      </c>
       <c r="N4" s="50" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="O4" s="87" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -4354,15 +4355,15 @@
       <c r="G5" s="50"/>
       <c r="H5" s="48"/>
       <c r="I5" s="50" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
       <c r="L5" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="M5" s="48" t="s">
         <v>174</v>
-      </c>
-      <c r="M5" s="48" t="s">
-        <v>175</v>
       </c>
       <c r="N5" s="50"/>
       <c r="O5" s="50"/>
@@ -4372,40 +4373,40 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F6" s="50" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H6" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="I6" s="50" t="s">
         <v>178</v>
       </c>
-      <c r="I6" s="50" t="s">
+      <c r="J6" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="K6" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="J6" s="50" t="s">
-        <v>174</v>
-      </c>
-      <c r="K6" s="50" t="s">
-        <v>180</v>
-      </c>
       <c r="L6" s="50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M6" s="50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N6" s="50"/>
       <c r="O6" s="50"/>
@@ -4445,7 +4446,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="102" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -4471,46 +4472,46 @@
         <v>8</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E2" s="51" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="G2" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="H2" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="I2" s="51" t="s">
         <v>185</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="J2" s="51" t="s">
         <v>186</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="K2" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="L2" s="51" t="s">
         <v>188</v>
       </c>
-      <c r="L2" s="51" t="s">
+      <c r="M2" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="M2" s="51" t="s">
+      <c r="N2" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="N2" s="51" t="s">
+      <c r="O2" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="O2" s="51" t="s">
+      <c r="P2" s="15" t="s">
         <v>192</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -4538,47 +4539,47 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>481</v>
+      </c>
+      <c r="G4" s="50" t="s">
         <v>194</v>
       </c>
-      <c r="F4" s="50" t="s">
-        <v>482</v>
-      </c>
-      <c r="G4" s="50" t="s">
+      <c r="H4" s="50" t="s">
         <v>195</v>
-      </c>
-      <c r="H4" s="50" t="s">
-        <v>196</v>
       </c>
       <c r="I4" s="50">
         <v>80</v>
       </c>
       <c r="J4" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="K4" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="K4" s="50" t="s">
+      <c r="L4" s="50" t="s">
         <v>198</v>
-      </c>
-      <c r="L4" s="50" t="s">
-        <v>199</v>
       </c>
       <c r="M4" s="50" t="b">
         <v>1</v>
       </c>
       <c r="N4" s="50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O4" s="50" t="s">
         <v>27</v>
       </c>
       <c r="P4" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -4586,29 +4587,29 @@
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
       <c r="D5" s="50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E5" s="50" t="s">
+        <v>199</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>482</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="H5" s="50" t="s">
         <v>200</v>
-      </c>
-      <c r="F5" s="50" t="s">
-        <v>483</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>201</v>
       </c>
       <c r="I5" s="50">
         <v>443</v>
       </c>
       <c r="J5" s="50"/>
       <c r="K5" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="L5" s="50" t="s">
         <v>202</v>
-      </c>
-      <c r="L5" s="50" t="s">
-        <v>203</v>
       </c>
       <c r="M5" s="50" t="b">
         <v>1</v>
@@ -4624,29 +4625,29 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G6" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="H6" s="50" t="s">
         <v>195</v>
-      </c>
-      <c r="H6" s="50" t="s">
-        <v>196</v>
       </c>
       <c r="I6" s="50">
         <v>80</v>
       </c>
       <c r="J6" s="50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K6" s="50" t="s">
         <v>27</v>
@@ -4696,7 +4697,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="96" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -4721,52 +4722,52 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="O2" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="P2" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="Q2" s="14" t="s">
         <v>219</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>220</v>
       </c>
       <c r="R2" s="14" t="s">
         <v>32</v>
@@ -4799,16 +4800,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C4" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="D4" s="50" t="s">
-        <v>222</v>
-      </c>
       <c r="E4" s="50" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
@@ -4832,7 +4833,7 @@
       <c r="C5" s="50"/>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="50"/>
@@ -4854,7 +4855,7 @@
       <c r="C6" s="50"/>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="50"/>
@@ -4876,7 +4877,7 @@
       <c r="C7" s="50"/>
       <c r="D7" s="50"/>
       <c r="E7" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -4898,7 +4899,7 @@
       <c r="C8" s="50"/>
       <c r="D8" s="50"/>
       <c r="E8" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
@@ -4919,7 +4920,7 @@
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
       <c r="D9" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="50" t="b">
@@ -4945,19 +4946,19 @@
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
       <c r="D10" s="50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E10" s="50"/>
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
       <c r="H10" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="I10" s="50" t="s">
         <v>230</v>
       </c>
-      <c r="I10" s="50" t="s">
+      <c r="J10" s="50" t="s">
         <v>231</v>
-      </c>
-      <c r="J10" s="50" t="s">
-        <v>232</v>
       </c>
       <c r="K10" s="50"/>
       <c r="L10" s="50"/>
@@ -4973,27 +4974,27 @@
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
       <c r="D11" s="50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E11" s="50"/>
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>
       <c r="H11" s="50" t="s">
+        <v>233</v>
+      </c>
+      <c r="I11" s="50" t="s">
         <v>234</v>
-      </c>
-      <c r="I11" s="50" t="s">
-        <v>235</v>
       </c>
       <c r="J11" s="50"/>
       <c r="K11" s="50" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L11" s="50"/>
       <c r="M11" s="50" t="s">
+        <v>236</v>
+      </c>
+      <c r="N11" s="50" t="s">
         <v>237</v>
-      </c>
-      <c r="N11" s="50" t="s">
-        <v>238</v>
       </c>
       <c r="O11" s="50">
         <v>302</v>
@@ -5007,27 +5008,27 @@
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
       <c r="D12" s="50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
       <c r="H12" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I12" s="50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J12" s="50"/>
       <c r="K12" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L12" s="50"/>
       <c r="M12" s="50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N12" s="50" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O12" s="50">
         <v>303</v>
@@ -5041,7 +5042,7 @@
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
       <c r="D13" s="50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
@@ -5051,13 +5052,13 @@
       <c r="J13" s="50"/>
       <c r="K13" s="50"/>
       <c r="L13" s="50" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M13" s="50"/>
       <c r="N13" s="50"/>
       <c r="O13" s="50"/>
       <c r="P13" s="50" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q13" s="50"/>
       <c r="R13" s="50"/>
@@ -5067,7 +5068,7 @@
       <c r="B14" s="50"/>
       <c r="C14" s="50"/>
       <c r="D14" s="50" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E14" s="50"/>
       <c r="F14" s="50"/>
@@ -5077,7 +5078,7 @@
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
       <c r="L14" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M14" s="50"/>
       <c r="N14" s="50"/>
@@ -5085,7 +5086,7 @@
       <c r="P14" s="50"/>
       <c r="Q14" s="50"/>
       <c r="R14" s="50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -5093,7 +5094,7 @@
       <c r="B15" s="50"/>
       <c r="C15" s="50"/>
       <c r="D15" s="50" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="50"/>
@@ -5103,7 +5104,7 @@
       <c r="J15" s="50"/>
       <c r="K15" s="50"/>
       <c r="L15" s="50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M15" s="50"/>
       <c r="N15" s="50"/>
@@ -5117,7 +5118,7 @@
       <c r="B16" s="50"/>
       <c r="C16" s="50"/>
       <c r="D16" s="50" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E16" s="50"/>
       <c r="F16" s="50"/>
@@ -5127,7 +5128,7 @@
       <c r="J16" s="50"/>
       <c r="K16" s="50"/>
       <c r="L16" s="50" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M16" s="50"/>
       <c r="N16" s="50"/>
@@ -5135,7 +5136,7 @@
       <c r="P16" s="50"/>
       <c r="Q16" s="50"/>
       <c r="R16" s="50" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
@@ -5143,7 +5144,7 @@
       <c r="B17" s="50"/>
       <c r="C17" s="50"/>
       <c r="D17" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E17" s="50"/>
       <c r="F17" s="50"/>
@@ -5153,7 +5154,7 @@
       <c r="J17" s="50"/>
       <c r="K17" s="50"/>
       <c r="L17" s="50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M17" s="50"/>
       <c r="N17" s="50"/>
@@ -5167,7 +5168,7 @@
       <c r="B18" s="50"/>
       <c r="C18" s="50"/>
       <c r="D18" s="50" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E18" s="50"/>
       <c r="F18" s="50"/>
@@ -5177,13 +5178,13 @@
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
       <c r="L18" s="50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M18" s="50"/>
       <c r="N18" s="50"/>
       <c r="O18" s="50"/>
       <c r="P18" s="50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q18" s="50"/>
       <c r="R18" s="50"/>
@@ -5212,13 +5213,13 @@
       <c r="A20" s="50"/>
       <c r="B20" s="50"/>
       <c r="C20" s="50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D20" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="E20" s="50" t="s">
         <v>222</v>
-      </c>
-      <c r="E20" s="50" t="s">
-        <v>223</v>
       </c>
       <c r="F20" s="50"/>
       <c r="G20" s="50"/>
@@ -5240,7 +5241,7 @@
       <c r="C21" s="50"/>
       <c r="D21" s="50"/>
       <c r="E21" s="50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="50"/>
@@ -5261,16 +5262,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D22" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="E22" s="50" t="s">
         <v>222</v>
-      </c>
-      <c r="E22" s="50" t="s">
-        <v>223</v>
       </c>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
@@ -5292,7 +5293,7 @@
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
       <c r="E23" s="50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F23" s="50"/>
       <c r="G23" s="50"/>
@@ -5388,10 +5389,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>411</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>412</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>413</v>
       </c>
       <c r="D4" s="50"/>
     </row>
@@ -5400,13 +5401,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
+        <v>413</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>414</v>
       </c>
-      <c r="C5" s="50" t="s">
-        <v>415</v>
-      </c>
       <c r="D5" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -5414,13 +5415,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>415</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>416</v>
       </c>
-      <c r="C6" s="50" t="s">
-        <v>417</v>
-      </c>
       <c r="D6" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -5428,10 +5429,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
+        <v>417</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>418</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>419</v>
       </c>
       <c r="D7" s="50"/>
     </row>
@@ -5440,13 +5441,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -5454,13 +5455,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C9" s="50" t="s">
+        <v>420</v>
+      </c>
+      <c r="D9" s="50" t="s">
         <v>421</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -5468,13 +5469,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -5482,13 +5483,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="50" t="s">
+        <v>423</v>
+      </c>
+      <c r="C11" s="50" t="s">
         <v>424</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="D11" s="50" t="s">
         <v>425</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -5518,7 +5519,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="57" customFormat="1" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="96" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -5531,19 +5532,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>260</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -5561,19 +5562,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C4" s="50" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="50" t="s">
         <v>262</v>
       </c>
-      <c r="D4" s="50" t="s">
-        <v>194</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>263</v>
-      </c>
       <c r="F4" s="50" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -5581,29 +5582,29 @@
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
       <c r="D5" s="50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="50"/>
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
+        <v>264</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" s="50" t="s">
         <v>265</v>
       </c>
-      <c r="D6" s="50" t="s">
-        <v>194</v>
-      </c>
-      <c r="E6" s="50" t="s">
+      <c r="F6" s="50" t="s">
         <v>266</v>
-      </c>
-      <c r="F6" s="50" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5611,19 +5612,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C7" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>203</v>
+      </c>
+      <c r="E7" s="50" t="s">
         <v>268</v>
       </c>
-      <c r="D7" s="50" t="s">
-        <v>204</v>
-      </c>
-      <c r="E7" s="50" t="s">
+      <c r="F7" s="50" t="s">
         <v>269</v>
-      </c>
-      <c r="F7" s="50" t="s">
-        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -5661,7 +5662,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="105" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B1" s="106"/>
       <c r="C1" s="106"/>
@@ -5682,43 +5683,43 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="L2" s="22" t="s">
-        <v>278</v>
-      </c>
       <c r="M2" s="43" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N2" s="43" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -5744,49 +5745,49 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G4" s="50" t="s">
         <v>27</v>
       </c>
       <c r="H4" s="50"/>
       <c r="I4" s="50" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
       <c r="L4" s="50"/>
       <c r="M4" s="50" t="s">
+        <v>539</v>
+      </c>
+      <c r="N4" s="88" t="s">
         <v>540</v>
-      </c>
-      <c r="N4" s="88" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
       <c r="C5" s="50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>27</v>
@@ -5804,31 +5805,31 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D6" s="50" t="s">
+        <v>279</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="F6" s="50" t="s">
         <v>280</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>268</v>
-      </c>
-      <c r="F6" s="50" t="s">
-        <v>281</v>
       </c>
       <c r="G6" s="50" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J6" s="50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K6" s="50">
         <v>80</v>
@@ -5868,36 +5869,36 @@
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="24" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="29" t="s">
         <v>285</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="28" t="s">
         <v>287</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E2" s="27">
         <v>301</v>
@@ -5908,16 +5909,16 @@
     </row>
     <row r="3" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E3" s="36">
         <v>302</v>
@@ -5928,16 +5929,16 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B4" s="36" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" t="s">
         <v>291</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="D4" t="s">
-        <v>292</v>
       </c>
       <c r="E4" s="36">
         <v>303</v>
@@ -5948,13 +5949,13 @@
     </row>
     <row r="5" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D5" s="58"/>
       <c r="E5" s="36">
@@ -5966,10 +5967,10 @@
     </row>
     <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C6" s="26"/>
       <c r="E6" s="36">
@@ -5979,189 +5980,189 @@
     </row>
     <row r="7" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
       <c r="B12" s="36" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="36" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="36" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="36" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="36" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="36" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="36" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="36" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="36" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="36" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -6196,7 +6197,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6214,22 +6215,22 @@
         <v>8</v>
       </c>
       <c r="C2" s="65" t="s">
+        <v>347</v>
+      </c>
+      <c r="D2" s="65" t="s">
         <v>348</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="E2" s="66" t="s">
         <v>349</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="F2" s="65" t="s">
         <v>350</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="G2" s="65" t="s">
         <v>351</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="H2" s="65" t="s">
         <v>352</v>
-      </c>
-      <c r="H2" s="65" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -6246,19 +6247,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
+        <v>353</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>411</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>490</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>354</v>
       </c>
-      <c r="B4" s="50" t="s">
-        <v>412</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>491</v>
-      </c>
-      <c r="D4" s="50" t="s">
+      <c r="E4" s="67" t="s">
         <v>355</v>
-      </c>
-      <c r="E4" s="67" t="s">
-        <v>356</v>
       </c>
       <c r="F4" s="50">
         <v>1</v>
@@ -6267,26 +6268,26 @@
         <v>1</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I4" s="70"/>
       <c r="J4" s="64"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E5" s="67" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F5" s="50">
         <v>1</v>
@@ -6295,7 +6296,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I5" s="70"/>
       <c r="J5" s="64"/>
@@ -6342,7 +6343,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="71" customFormat="1" ht="101.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6378,64 +6379,64 @@
         <v>48</v>
       </c>
       <c r="D2" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>493</v>
+      </c>
+      <c r="F2" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="G2" s="72" t="s">
         <v>494</v>
       </c>
-      <c r="F2" s="72" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" s="72" t="s">
+      <c r="H2" s="72" t="s">
         <v>495</v>
       </c>
-      <c r="H2" s="72" t="s">
+      <c r="I2" s="72" t="s">
         <v>496</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="J2" s="72" t="s">
         <v>497</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="73" t="s">
         <v>498</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>499</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="M2" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="N2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="S2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>360</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>361</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>362</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>507</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>361</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>362</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>363</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -6467,70 +6468,70 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="74" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G4" s="74">
         <v>2</v>
       </c>
       <c r="H4" s="74" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I4" s="74">
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
+        <v>367</v>
+      </c>
+      <c r="K4" s="74" t="s">
         <v>368</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="L4" s="74" t="s">
+        <v>509</v>
+      </c>
+      <c r="M4" s="74" t="s">
         <v>369</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="N4" s="75" t="s">
         <v>510</v>
       </c>
-      <c r="M4" s="74" t="s">
-        <v>370</v>
-      </c>
-      <c r="N4" s="75" t="s">
-        <v>511</v>
-      </c>
       <c r="O4" s="74" t="s">
+        <v>371</v>
+      </c>
+      <c r="P4" s="74" t="s">
         <v>372</v>
       </c>
-      <c r="P4" s="74" t="s">
+      <c r="Q4" s="74" t="s">
         <v>373</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="R4" s="74" t="s">
         <v>374</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>375</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>1</v>
       </c>
       <c r="T4" s="74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U4" s="50" t="s">
+        <v>375</v>
+      </c>
+      <c r="V4" s="50" t="s">
         <v>376</v>
-      </c>
-      <c r="V4" s="50" t="s">
-        <v>377</v>
       </c>
       <c r="W4" s="50">
         <v>15</v>
@@ -6538,70 +6539,70 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="74" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D5" s="74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G5" s="74">
         <v>2</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I5" s="74">
         <v>256</v>
       </c>
       <c r="J5" s="74" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K5" s="74" t="s">
+        <v>512</v>
+      </c>
+      <c r="L5" s="74" t="s">
         <v>513</v>
       </c>
-      <c r="L5" s="74" t="s">
+      <c r="M5" s="74" t="s">
+        <v>392</v>
+      </c>
+      <c r="N5" s="75" t="s">
         <v>514</v>
       </c>
-      <c r="M5" s="74" t="s">
+      <c r="O5" s="74" t="s">
         <v>393</v>
       </c>
-      <c r="N5" s="75" t="s">
+      <c r="P5" s="74" t="s">
         <v>515</v>
       </c>
-      <c r="O5" s="74" t="s">
-        <v>394</v>
-      </c>
-      <c r="P5" s="74" t="s">
-        <v>516</v>
-      </c>
       <c r="Q5" s="74" t="s">
+        <v>373</v>
+      </c>
+      <c r="R5" s="74" t="s">
         <v>374</v>
-      </c>
-      <c r="R5" s="74" t="s">
-        <v>375</v>
       </c>
       <c r="S5" s="74" t="b">
         <v>0</v>
       </c>
       <c r="T5" s="74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U5" s="50" t="s">
+        <v>375</v>
+      </c>
+      <c r="V5" s="50" t="s">
         <v>376</v>
-      </c>
-      <c r="V5" s="50" t="s">
-        <v>377</v>
       </c>
       <c r="W5" s="50">
         <v>15</v>
@@ -6675,7 +6676,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="71" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6712,64 +6713,64 @@
         <v>48</v>
       </c>
       <c r="D2" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>493</v>
+      </c>
+      <c r="F2" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="73" t="s">
-        <v>494</v>
-      </c>
-      <c r="F2" s="72" t="s">
-        <v>99</v>
-      </c>
       <c r="G2" s="72" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H2" s="72" t="s">
+        <v>495</v>
+      </c>
+      <c r="I2" s="72" t="s">
         <v>496</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="J2" s="72" t="s">
         <v>497</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="92" t="s">
         <v>498</v>
       </c>
-      <c r="K2" s="92" t="s">
+      <c r="L2" s="72" t="s">
         <v>499</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="M2" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="N2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="S2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>360</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>361</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>362</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>507</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>361</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>362</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>363</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -6801,70 +6802,70 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="74" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G4" s="74">
         <v>2</v>
       </c>
       <c r="H4" s="74" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I4" s="74">
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
+        <v>367</v>
+      </c>
+      <c r="K4" s="74" t="s">
         <v>368</v>
       </c>
-      <c r="K4" s="74" t="s">
-        <v>369</v>
-      </c>
       <c r="L4" s="74" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="M4" s="74" t="s">
+        <v>395</v>
+      </c>
+      <c r="N4" s="74" t="s">
+        <v>370</v>
+      </c>
+      <c r="O4" s="74" t="s">
         <v>396</v>
       </c>
-      <c r="N4" s="74" t="s">
-        <v>371</v>
-      </c>
-      <c r="O4" s="74" t="s">
-        <v>397</v>
-      </c>
       <c r="P4" s="74" t="s">
+        <v>372</v>
+      </c>
+      <c r="Q4" s="74" t="s">
         <v>373</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="R4" s="74" t="s">
         <v>374</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>375</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>0</v>
       </c>
       <c r="T4" s="74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U4" s="50" t="s">
+        <v>375</v>
+      </c>
+      <c r="V4" s="50" t="s">
         <v>376</v>
-      </c>
-      <c r="V4" s="50" t="s">
-        <v>377</v>
       </c>
       <c r="W4" s="50">
         <v>15</v>
@@ -6872,70 +6873,70 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="74" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G5" s="74">
         <v>2</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I5" s="74">
         <v>256</v>
       </c>
       <c r="J5" s="74" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K5" s="74" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L5" s="74" t="s">
+        <v>521</v>
+      </c>
+      <c r="M5" s="74" t="s">
         <v>522</v>
       </c>
-      <c r="M5" s="74" t="s">
+      <c r="N5" s="74" t="s">
         <v>523</v>
       </c>
-      <c r="N5" s="74" t="s">
+      <c r="O5" s="74" t="s">
         <v>524</v>
       </c>
-      <c r="O5" s="74" t="s">
-        <v>525</v>
-      </c>
       <c r="P5" s="74" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="Q5" s="74" t="s">
+        <v>373</v>
+      </c>
+      <c r="R5" s="74" t="s">
         <v>374</v>
-      </c>
-      <c r="R5" s="74" t="s">
-        <v>375</v>
       </c>
       <c r="S5" s="74" t="b">
         <v>1</v>
       </c>
       <c r="T5" s="74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U5" s="50" t="s">
+        <v>375</v>
+      </c>
+      <c r="V5" s="50" t="s">
         <v>376</v>
-      </c>
-      <c r="V5" s="50" t="s">
-        <v>377</v>
       </c>
       <c r="W5" s="50">
         <v>15</v>
@@ -7008,7 +7009,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="71" customFormat="1" ht="115.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -7044,64 +7045,64 @@
         <v>48</v>
       </c>
       <c r="D2" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="72" t="s">
+        <v>398</v>
+      </c>
+      <c r="F2" s="73" t="s">
+        <v>493</v>
+      </c>
+      <c r="G2" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="72" t="s">
-        <v>399</v>
-      </c>
-      <c r="F2" s="73" t="s">
-        <v>494</v>
-      </c>
-      <c r="G2" s="72" t="s">
-        <v>99</v>
-      </c>
       <c r="H2" s="72" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I2" s="72" t="s">
+        <v>496</v>
+      </c>
+      <c r="J2" s="72" t="s">
         <v>497</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="73" t="s">
         <v>498</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>499</v>
       </c>
-      <c r="L2" s="72" t="s">
-        <v>500</v>
-      </c>
       <c r="M2" s="72" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N2" s="72" t="s">
+        <v>501</v>
+      </c>
+      <c r="O2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>506</v>
       </c>
-      <c r="S2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>360</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>361</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>362</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>507</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>361</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>362</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>363</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="84" customFormat="1" x14ac:dyDescent="0.3">
@@ -7135,22 +7136,22 @@
         <v>6</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H4" s="74">
         <v>2</v>
@@ -7159,43 +7160,43 @@
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
+        <v>367</v>
+      </c>
+      <c r="K4" s="74" t="s">
         <v>368</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="L4" s="74" t="s">
+        <v>399</v>
+      </c>
+      <c r="M4" s="74" t="s">
         <v>369</v>
       </c>
-      <c r="L4" s="74" t="s">
-        <v>400</v>
-      </c>
-      <c r="M4" s="74" t="s">
+      <c r="N4" s="74" t="s">
         <v>370</v>
       </c>
-      <c r="N4" s="74" t="s">
+      <c r="O4" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="O4" s="74" t="s">
+      <c r="P4" s="74" t="s">
         <v>372</v>
       </c>
-      <c r="P4" s="74" t="s">
+      <c r="Q4" s="74" t="s">
         <v>373</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="R4" s="74" t="s">
         <v>374</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>375</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>1</v>
       </c>
       <c r="T4" s="74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U4" s="50" t="s">
+        <v>375</v>
+      </c>
+      <c r="V4" s="50" t="s">
         <v>376</v>
-      </c>
-      <c r="V4" s="50" t="s">
-        <v>377</v>
       </c>
       <c r="W4" s="50">
         <v>10</v>
@@ -7251,159 +7252,159 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="65" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B1" s="65" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1" s="85" t="s">
         <v>528</v>
       </c>
-      <c r="C1" s="85" t="s">
-        <v>529</v>
-      </c>
       <c r="D1" s="85" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G1" s="86" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" s="74" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F2" s="50" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G2" s="74" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="50" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="50"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="50"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="50" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D7" s="50"/>
       <c r="E7" s="50" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="50" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="50" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="50" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="50" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="50"/>
@@ -7412,11 +7413,11 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="50" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="50" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D10" s="50"/>
       <c r="E10" s="50"/>
@@ -7425,11 +7426,11 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="50" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
@@ -7438,11 +7439,11 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="50" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
@@ -7453,7 +7454,7 @@
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="50"/>
@@ -7464,7 +7465,7 @@
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
@@ -7522,10 +7523,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>426</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>427</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7533,10 +7534,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
+        <v>428</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>429</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -7544,10 +7545,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>430</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>431</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -7555,10 +7556,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
+        <v>432</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>433</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -7590,7 +7591,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="57" customFormat="1" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="96" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -7638,19 +7639,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>435</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>484</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>544</v>
+      </c>
+      <c r="E4" s="50" t="s">
         <v>436</v>
       </c>
-      <c r="C4" s="50" t="s">
-        <v>485</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>545</v>
-      </c>
-      <c r="E4" s="50" t="s">
+      <c r="F4" s="59" t="s">
         <v>437</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>438</v>
       </c>
       <c r="G4" s="50"/>
     </row>
@@ -7660,13 +7661,13 @@
       <c r="C5" s="50"/>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -7674,22 +7675,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>439</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>417</v>
+      </c>
+      <c r="D6" s="50" t="s">
         <v>440</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>418</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>441</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -7697,22 +7698,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G7" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -7747,7 +7748,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -7767,28 +7768,28 @@
         <v>8</v>
       </c>
       <c r="C2" s="53" t="s">
+        <v>323</v>
+      </c>
+      <c r="D2" s="53" t="s">
         <v>324</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="E2" s="53" t="s">
         <v>325</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="F2" s="53" t="s">
         <v>326</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="G2" s="53" t="s">
         <v>327</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="H2" s="53" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="I2" s="54" t="s">
+        <v>551</v>
+      </c>
+      <c r="J2" s="54" t="s">
         <v>329</v>
-      </c>
-      <c r="I2" s="54" t="s">
-        <v>552</v>
-      </c>
-      <c r="J2" s="54" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -7810,29 +7811,29 @@
         <v>6</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C4" s="38" t="s">
+        <v>330</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="E4" s="33" t="s">
         <v>332</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>333</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>411</v>
+      </c>
+      <c r="J4" s="40" t="s">
         <v>334</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>412</v>
-      </c>
-      <c r="J4" s="40" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -7841,17 +7842,17 @@
       <c r="C5" s="38"/>
       <c r="D5" s="33"/>
       <c r="E5" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F5" s="33"/>
       <c r="G5" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J5" s="40"/>
     </row>
@@ -7860,14 +7861,14 @@
         <v>6</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D6" s="33"/>
       <c r="E6" s="34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="33"/>
@@ -7880,16 +7881,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="33"/>
@@ -7903,7 +7904,7 @@
       <c r="C8" s="38"/>
       <c r="D8" s="33"/>
       <c r="E8" s="34" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F8" s="34"/>
       <c r="G8" s="33"/>
@@ -7916,27 +7917,27 @@
         <v>6</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="F9" s="33" t="s">
         <v>342</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>343</v>
       </c>
       <c r="G9" s="33" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="33"/>
       <c r="I9" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J9" s="40" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -7945,7 +7946,7 @@
       <c r="C10" s="38"/>
       <c r="D10" s="33"/>
       <c r="E10" s="33" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F10" s="33"/>
       <c r="G10" s="33"/>
@@ -7959,7 +7960,7 @@
       <c r="C11" s="41"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F11" s="33"/>
       <c r="G11" s="33"/>
@@ -7973,13 +7974,13 @@
       <c r="C12" s="41"/>
       <c r="D12" s="33"/>
       <c r="E12" s="33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F12" s="33"/>
       <c r="G12" s="33"/>
       <c r="H12" s="33"/>
       <c r="I12" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J12" s="40"/>
     </row>
@@ -8017,7 +8018,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="209.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="102" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -8085,7 +8086,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
@@ -8094,7 +8095,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F4" s="50" t="s">
         <v>27</v>
@@ -8106,13 +8107,13 @@
         <v>24</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J4" s="50" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="50" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
@@ -8120,10 +8121,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>26</v>
@@ -8141,7 +8142,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J5" s="50" t="s">
         <v>28</v>
@@ -8153,10 +8154,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D6" s="50" t="s">
         <v>29</v>
@@ -8174,7 +8175,7 @@
         <v>24</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J6" s="50" t="s">
         <v>28</v>
@@ -8225,7 +8226,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -8328,7 +8329,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
@@ -8343,7 +8344,7 @@
         <v>45</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -8351,10 +8352,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>43</v>
@@ -8372,13 +8373,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>46</v>
@@ -8524,13 +8525,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>59</v>
@@ -8552,7 +8553,7 @@
         <v>24</v>
       </c>
       <c r="L4" s="60" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="M4" s="60" t="s">
         <v>24</v>
@@ -8573,16 +8574,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D5" s="50" t="s">
+        <v>456</v>
+      </c>
+      <c r="E5" s="50" t="s">
         <v>457</v>
-      </c>
-      <c r="E5" s="50" t="s">
-        <v>458</v>
       </c>
       <c r="F5" s="50" t="s">
         <v>60</v>
@@ -8620,13 +8621,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>64</v>
@@ -8667,16 +8668,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F7" s="50" t="s">
         <v>60</v>
@@ -8685,7 +8686,7 @@
         <v>66</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I7" s="50"/>
       <c r="J7" s="50" t="s">
@@ -8716,16 +8717,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F8" s="50" t="s">
         <v>60</v>
@@ -8734,11 +8735,11 @@
         <v>66</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I8" s="50"/>
       <c r="J8" s="50" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K8" s="50" t="s">
         <v>27</v>
@@ -8765,16 +8766,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D9" s="50" t="s">
+        <v>462</v>
+      </c>
+      <c r="E9" s="50" t="s">
         <v>463</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>464</v>
       </c>
       <c r="F9" s="50" t="s">
         <v>60</v>
@@ -8783,17 +8784,17 @@
         <v>66</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I9" s="50"/>
       <c r="J9" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K9" s="50" t="s">
         <v>27</v>
       </c>
       <c r="L9" s="60" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="M9" s="60" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Excel sheet added example
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="561">
   <si>
     <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
 Leave "Parent Compartment" empty or mention 'root' if it is under 'root' compartment;
@@ -1848,6 +1848,15 @@
 Group "Name" is mandatory field;
 "Matching Rule" - Specify the matching rule for creating Dynamic Groups; else leave it empty.
 Enter "Region" as your tenancy's Home Region for Group Creation.</t>
+  </si>
+  <si>
+    <t>DevOCS_dyngrp</t>
+  </si>
+  <si>
+    <t>any {ALL {instance.compartment.id = 'ocid1.compartment.oc1..aaaaaaaa4ufdfsdytjlbgd7q6bi6fzssum62cqc5yyvatr346hhpkzkri3wq'},ALL {instance.compartment.id = 'ocid1.compartment.oc1..aaaaaaaao5pv3wnyma2fyj6mik3cnuuiya2dnwkm5mhxnjqjebpmfmao45fa'}}</t>
+  </si>
+  <si>
+    <t>Dynamic Group for developer servers</t>
   </si>
 </sst>
 </file>
@@ -2487,6 +2496,7 @@
       <sheetName val="TagServer"/>
       <sheetName val="TagVolume"/>
       <sheetName val="NSGs"/>
+      <sheetName val="Sheet 2"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -2537,6 +2547,7 @@
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
+      <sheetData sheetId="21" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7489,10 +7500,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7500,7 +7511,7 @@
     <col min="1" max="1" width="9.21875" style="49" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" style="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.77734375" style="49" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="57" customFormat="1" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -7581,12 +7592,26 @@
       </c>
       <c r="D7" s="50"/>
     </row>
+    <row r="8" spans="1:4" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>558</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>560</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>559</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SSL-HTTPS changed - LBR
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ocifromnewgit\oci_tenancy\SetUpOCI_Via_TF\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ATK7.0-Demo\code\oci_tenancy\SetUpOCI_Via_TF\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -954,9 +954,6 @@
     <t>Listener Name</t>
   </si>
   <si>
-    <t>Listener Protocol (HTTPS|HTTP|TCP)</t>
-  </si>
-  <si>
     <t>Listener Port</t>
   </si>
   <si>
@@ -1857,6 +1854,9 @@
   </si>
   <si>
     <t>Dynamic Group for developer servers</t>
+  </si>
+  <si>
+    <t>Listener Protocol (HTTP|TCP)</t>
   </si>
 </sst>
 </file>
@@ -2853,7 +2853,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -3031,7 +3031,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView zoomScale="91" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3053,7 +3053,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="103" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -3131,10 +3131,10 @@
         <v>70</v>
       </c>
       <c r="S2" s="89" t="s">
+        <v>543</v>
+      </c>
+      <c r="T2" s="89" t="s">
         <v>544</v>
-      </c>
-      <c r="T2" s="89" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3166,13 +3166,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>87</v>
@@ -3206,28 +3206,28 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>92</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>89</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I5" s="47" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
@@ -3250,13 +3250,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>87</v>
@@ -3288,13 +3288,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>92</v>
@@ -3309,7 +3309,7 @@
         <v>90</v>
       </c>
       <c r="I7" s="47" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
@@ -3398,7 +3398,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>99</v>
@@ -3418,7 +3418,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>101</v>
@@ -3438,7 +3438,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>103</v>
@@ -3450,7 +3450,7 @@
         <v>100</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -3516,7 +3516,7 @@
         <v>96</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E2" s="43" t="s">
         <v>98</v>
@@ -3572,37 +3572,37 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="50" t="s">
+        <v>469</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>408</v>
+      </c>
+      <c r="F4" s="50" t="s">
         <v>470</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>409</v>
-      </c>
-      <c r="F4" s="50" t="s">
-        <v>471</v>
       </c>
       <c r="G4" s="50" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I4" s="50" t="s">
         <v>115</v>
       </c>
       <c r="J4" s="50" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K4" s="50" t="s">
         <v>117</v>
       </c>
       <c r="L4" s="50" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="M4" s="50"/>
       <c r="N4" s="50" t="s">
@@ -3614,19 +3614,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>118</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G5" s="50" t="b">
         <v>0</v>
@@ -3636,13 +3636,13 @@
         <v>115</v>
       </c>
       <c r="J5" s="50" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K5" s="50" t="s">
         <v>117</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="M5" s="50"/>
       <c r="N5" s="50" t="s">
@@ -3654,19 +3654,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G6" s="50" t="b">
         <v>0</v>
@@ -3682,10 +3682,10 @@
         <v>117</v>
       </c>
       <c r="L6" s="50" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="M6" s="50" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="N6" s="50"/>
     </row>
@@ -3694,19 +3694,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>64</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>118</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G7" s="50" t="b">
         <v>0</v>
@@ -3722,10 +3722,10 @@
         <v>117</v>
       </c>
       <c r="L7" s="50" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="M7" s="50" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="N7" s="50"/>
     </row>
@@ -3759,7 +3759,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="100" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -3812,10 +3812,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D4" s="50">
         <v>150</v>
@@ -3824,13 +3824,13 @@
         <v>64</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G4" s="50" t="s">
         <v>125</v>
       </c>
       <c r="H4" s="59" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3838,10 +3838,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D5" s="50">
         <v>150</v>
@@ -3850,13 +3850,13 @@
         <v>64</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>125</v>
       </c>
       <c r="H5" s="59" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -3990,7 +3990,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>102</v>
@@ -3999,7 +3999,7 @@
         <v>139</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="32" t="s">
@@ -4018,7 +4018,7 @@
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
       <c r="P4" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -4073,7 +4073,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>102</v>
@@ -4082,7 +4082,7 @@
         <v>139</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
@@ -4105,7 +4105,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>112</v>
@@ -4114,7 +4114,7 @@
         <v>149</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
@@ -4135,7 +4135,7 @@
       <c r="N8" s="32"/>
       <c r="O8" s="32"/>
       <c r="P8" s="50" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4143,7 +4143,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>112</v>
@@ -4152,7 +4152,7 @@
         <v>153</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
@@ -4179,7 +4179,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>102</v>
@@ -4188,7 +4188,7 @@
         <v>155</v>
       </c>
       <c r="E10" s="48" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -4297,10 +4297,10 @@
         <v>168</v>
       </c>
       <c r="N2" s="43" t="s">
+        <v>485</v>
+      </c>
+      <c r="O2" s="43" t="s">
         <v>486</v>
-      </c>
-      <c r="O2" s="43" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4327,16 +4327,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D4" s="50" t="s">
         <v>169</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F4" s="50" t="b">
         <v>1</v>
@@ -4357,10 +4357,10 @@
         <v>173</v>
       </c>
       <c r="N4" s="50" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="O4" s="87" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -4391,22 +4391,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D6" s="50" t="s">
         <v>175</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F6" s="50" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H6" s="48" t="s">
         <v>176</v>
@@ -4557,17 +4557,17 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="50" t="s">
         <v>192</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G4" s="50" t="s">
         <v>193</v>
@@ -4611,7 +4611,7 @@
         <v>198</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G5" s="50" t="s">
         <v>193</v>
@@ -4643,17 +4643,17 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
         <v>202</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G6" s="50" t="s">
         <v>193</v>
@@ -4818,7 +4818,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>219</v>
@@ -4827,7 +4827,7 @@
         <v>220</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
@@ -5280,7 +5280,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C22" s="50" t="s">
         <v>256</v>
@@ -5407,10 +5407,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>409</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>410</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>411</v>
       </c>
       <c r="D4" s="50"/>
     </row>
@@ -5419,13 +5419,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
+        <v>411</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>412</v>
       </c>
-      <c r="C5" s="50" t="s">
-        <v>413</v>
-      </c>
       <c r="D5" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -5433,13 +5433,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>413</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>414</v>
       </c>
-      <c r="C6" s="50" t="s">
-        <v>415</v>
-      </c>
       <c r="D6" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -5447,10 +5447,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
+        <v>415</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>416</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>417</v>
       </c>
       <c r="D7" s="50"/>
     </row>
@@ -5459,13 +5459,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -5473,13 +5473,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C9" s="50" t="s">
+        <v>418</v>
+      </c>
+      <c r="D9" s="50" t="s">
         <v>419</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -5487,13 +5487,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -5501,13 +5501,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="50" t="s">
+        <v>421</v>
+      </c>
+      <c r="C11" s="50" t="s">
         <v>422</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="D11" s="50" t="s">
         <v>423</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -5580,7 +5580,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>260</v>
@@ -5630,7 +5630,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>266</v>
@@ -5663,7 +5663,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5725,19 +5725,19 @@
         <v>273</v>
       </c>
       <c r="J2" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="L2" s="22" t="s">
-        <v>276</v>
-      </c>
       <c r="M2" s="43" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N2" s="43" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -5763,13 +5763,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>192</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>260</v>
@@ -5782,16 +5782,16 @@
       </c>
       <c r="H4" s="50"/>
       <c r="I4" s="50" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
       <c r="L4" s="50"/>
       <c r="M4" s="50" t="s">
+        <v>537</v>
+      </c>
+      <c r="N4" s="88" t="s">
         <v>538</v>
-      </c>
-      <c r="N4" s="88" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -5812,7 +5812,7 @@
       </c>
       <c r="H5" s="50"/>
       <c r="I5" s="50" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="J5" s="50"/>
       <c r="K5" s="50"/>
@@ -5825,19 +5825,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>202</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>266</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G6" s="50" t="s">
         <v>23</v>
@@ -5846,7 +5846,7 @@
         <v>177</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J6" s="50" t="s">
         <v>194</v>
@@ -5889,22 +5889,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>281</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="29" t="s">
         <v>283</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="24" t="s">
         <v>284</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="28" t="s">
         <v>285</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.35">
@@ -5912,7 +5912,7 @@
         <v>243</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>234</v>
@@ -5932,7 +5932,7 @@
         <v>247</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>268</v>
@@ -5952,13 +5952,13 @@
         <v>227</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>238</v>
       </c>
       <c r="D4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E4" s="36">
         <v>303</v>
@@ -5972,7 +5972,7 @@
         <v>220</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>265</v>
@@ -5990,7 +5990,7 @@
         <v>240</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" s="26"/>
       <c r="E6" s="36">
@@ -6003,7 +6003,7 @@
         <v>252</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E7" s="12"/>
     </row>
@@ -6028,7 +6028,7 @@
         <v>245</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -6036,118 +6036,118 @@
         <v>250</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
       <c r="B12" s="36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="36" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="36" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="36" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="36" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="36" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="36" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="36" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="36" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -6157,7 +6157,7 @@
     </row>
     <row r="35" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="36" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -6167,7 +6167,7 @@
     </row>
     <row r="37" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -6177,12 +6177,12 @@
     </row>
     <row r="39" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="36" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -6217,7 +6217,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6235,22 +6235,22 @@
         <v>7</v>
       </c>
       <c r="C2" s="65" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2" s="65" t="s">
         <v>346</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="E2" s="66" t="s">
         <v>347</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="F2" s="65" t="s">
         <v>348</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="G2" s="65" t="s">
         <v>349</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="H2" s="65" t="s">
         <v>350</v>
-      </c>
-      <c r="H2" s="65" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -6267,19 +6267,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
+        <v>351</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>409</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>488</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>352</v>
       </c>
-      <c r="B4" s="50" t="s">
-        <v>410</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>489</v>
-      </c>
-      <c r="D4" s="50" t="s">
+      <c r="E4" s="67" t="s">
         <v>353</v>
-      </c>
-      <c r="E4" s="67" t="s">
-        <v>354</v>
       </c>
       <c r="F4" s="50">
         <v>1</v>
@@ -6288,26 +6288,26 @@
         <v>1</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I4" s="70"/>
       <c r="J4" s="64"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E5" s="67" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F5" s="50">
         <v>1</v>
@@ -6316,7 +6316,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I5" s="70"/>
       <c r="J5" s="64"/>
@@ -6363,7 +6363,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="71" customFormat="1" ht="101.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6402,61 +6402,61 @@
         <v>96</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F2" s="72" t="s">
         <v>97</v>
       </c>
       <c r="G2" s="72" t="s">
+        <v>492</v>
+      </c>
+      <c r="H2" s="72" t="s">
         <v>493</v>
       </c>
-      <c r="H2" s="72" t="s">
+      <c r="I2" s="72" t="s">
         <v>494</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="J2" s="72" t="s">
         <v>495</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="73" t="s">
         <v>496</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>497</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="M2" s="72" t="s">
         <v>498</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="N2" s="72" t="s">
         <v>499</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="S2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>359</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>360</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>505</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>359</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>360</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>361</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -6488,58 +6488,58 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="74" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>64</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G4" s="74">
         <v>2</v>
       </c>
       <c r="H4" s="74" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I4" s="74">
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
+        <v>365</v>
+      </c>
+      <c r="K4" s="74" t="s">
         <v>366</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="L4" s="74" t="s">
+        <v>507</v>
+      </c>
+      <c r="M4" s="74" t="s">
         <v>367</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="N4" s="75" t="s">
         <v>508</v>
       </c>
-      <c r="M4" s="74" t="s">
-        <v>368</v>
-      </c>
-      <c r="N4" s="75" t="s">
-        <v>509</v>
-      </c>
       <c r="O4" s="74" t="s">
+        <v>369</v>
+      </c>
+      <c r="P4" s="74" t="s">
         <v>370</v>
       </c>
-      <c r="P4" s="74" t="s">
+      <c r="Q4" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="R4" s="74" t="s">
         <v>372</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>373</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>1</v>
@@ -6548,10 +6548,10 @@
         <v>117</v>
       </c>
       <c r="U4" s="50" t="s">
+        <v>373</v>
+      </c>
+      <c r="V4" s="50" t="s">
         <v>374</v>
-      </c>
-      <c r="V4" s="50" t="s">
-        <v>375</v>
       </c>
       <c r="W4" s="50">
         <v>15</v>
@@ -6559,58 +6559,58 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="74" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>112</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G5" s="74">
         <v>2</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I5" s="74">
         <v>256</v>
       </c>
       <c r="J5" s="74" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K5" s="74" t="s">
+        <v>510</v>
+      </c>
+      <c r="L5" s="74" t="s">
         <v>511</v>
       </c>
-      <c r="L5" s="74" t="s">
+      <c r="M5" s="74" t="s">
+        <v>390</v>
+      </c>
+      <c r="N5" s="75" t="s">
         <v>512</v>
       </c>
-      <c r="M5" s="74" t="s">
+      <c r="O5" s="74" t="s">
         <v>391</v>
       </c>
-      <c r="N5" s="75" t="s">
+      <c r="P5" s="74" t="s">
         <v>513</v>
       </c>
-      <c r="O5" s="74" t="s">
-        <v>392</v>
-      </c>
-      <c r="P5" s="74" t="s">
-        <v>514</v>
-      </c>
       <c r="Q5" s="74" t="s">
+        <v>371</v>
+      </c>
+      <c r="R5" s="74" t="s">
         <v>372</v>
-      </c>
-      <c r="R5" s="74" t="s">
-        <v>373</v>
       </c>
       <c r="S5" s="74" t="b">
         <v>0</v>
@@ -6619,10 +6619,10 @@
         <v>117</v>
       </c>
       <c r="U5" s="50" t="s">
+        <v>373</v>
+      </c>
+      <c r="V5" s="50" t="s">
         <v>374</v>
-      </c>
-      <c r="V5" s="50" t="s">
-        <v>375</v>
       </c>
       <c r="W5" s="50">
         <v>15</v>
@@ -6696,7 +6696,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="71" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -6736,61 +6736,61 @@
         <v>96</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F2" s="72" t="s">
         <v>97</v>
       </c>
       <c r="G2" s="72" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H2" s="72" t="s">
+        <v>493</v>
+      </c>
+      <c r="I2" s="72" t="s">
         <v>494</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="J2" s="72" t="s">
         <v>495</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="92" t="s">
         <v>496</v>
       </c>
-      <c r="K2" s="92" t="s">
+      <c r="L2" s="72" t="s">
         <v>497</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="M2" s="72" t="s">
         <v>498</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="N2" s="72" t="s">
         <v>499</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="O2" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="S2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>359</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>360</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>505</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>359</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>360</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>361</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -6822,58 +6822,58 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="74" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>64</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G4" s="74">
         <v>2</v>
       </c>
       <c r="H4" s="74" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I4" s="74">
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
+        <v>365</v>
+      </c>
+      <c r="K4" s="74" t="s">
         <v>366</v>
       </c>
-      <c r="K4" s="74" t="s">
-        <v>367</v>
-      </c>
       <c r="L4" s="74" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="M4" s="74" t="s">
+        <v>393</v>
+      </c>
+      <c r="N4" s="74" t="s">
+        <v>368</v>
+      </c>
+      <c r="O4" s="74" t="s">
         <v>394</v>
       </c>
-      <c r="N4" s="74" t="s">
-        <v>369</v>
-      </c>
-      <c r="O4" s="74" t="s">
-        <v>395</v>
-      </c>
       <c r="P4" s="74" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q4" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="R4" s="74" t="s">
         <v>372</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>373</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>0</v>
@@ -6882,10 +6882,10 @@
         <v>117</v>
       </c>
       <c r="U4" s="50" t="s">
+        <v>373</v>
+      </c>
+      <c r="V4" s="50" t="s">
         <v>374</v>
-      </c>
-      <c r="V4" s="50" t="s">
-        <v>375</v>
       </c>
       <c r="W4" s="50">
         <v>15</v>
@@ -6893,58 +6893,58 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="74" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>64</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G5" s="74">
         <v>2</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I5" s="74">
         <v>256</v>
       </c>
       <c r="J5" s="74" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K5" s="74" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L5" s="74" t="s">
+        <v>519</v>
+      </c>
+      <c r="M5" s="74" t="s">
         <v>520</v>
       </c>
-      <c r="M5" s="74" t="s">
+      <c r="N5" s="74" t="s">
         <v>521</v>
       </c>
-      <c r="N5" s="74" t="s">
+      <c r="O5" s="74" t="s">
         <v>522</v>
       </c>
-      <c r="O5" s="74" t="s">
-        <v>523</v>
-      </c>
       <c r="P5" s="74" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="Q5" s="74" t="s">
+        <v>371</v>
+      </c>
+      <c r="R5" s="74" t="s">
         <v>372</v>
-      </c>
-      <c r="R5" s="74" t="s">
-        <v>373</v>
       </c>
       <c r="S5" s="74" t="b">
         <v>1</v>
@@ -6953,10 +6953,10 @@
         <v>117</v>
       </c>
       <c r="U5" s="50" t="s">
+        <v>373</v>
+      </c>
+      <c r="V5" s="50" t="s">
         <v>374</v>
-      </c>
-      <c r="V5" s="50" t="s">
-        <v>375</v>
       </c>
       <c r="W5" s="50">
         <v>15</v>
@@ -7029,7 +7029,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="71" customFormat="1" ht="115.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="108"/>
@@ -7068,61 +7068,61 @@
         <v>96</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F2" s="73" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G2" s="72" t="s">
         <v>97</v>
       </c>
       <c r="H2" s="72" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I2" s="72" t="s">
+        <v>494</v>
+      </c>
+      <c r="J2" s="72" t="s">
         <v>495</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="K2" s="73" t="s">
         <v>496</v>
       </c>
-      <c r="K2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>497</v>
       </c>
-      <c r="L2" s="72" t="s">
-        <v>498</v>
-      </c>
       <c r="M2" s="72" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N2" s="72" t="s">
+        <v>499</v>
+      </c>
+      <c r="O2" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>501</v>
       </c>
-      <c r="P2" s="72" t="s">
+      <c r="Q2" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="Q2" s="72" t="s">
+      <c r="R2" s="72" t="s">
         <v>503</v>
       </c>
-      <c r="R2" s="72" t="s">
+      <c r="S2" s="72" t="s">
         <v>504</v>
       </c>
-      <c r="S2" s="72" t="s">
+      <c r="T2" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="U2" s="72" t="s">
+        <v>359</v>
+      </c>
+      <c r="V2" s="72" t="s">
+        <v>360</v>
+      </c>
+      <c r="W2" s="72" t="s">
         <v>505</v>
-      </c>
-      <c r="T2" s="90" t="s">
-        <v>359</v>
-      </c>
-      <c r="U2" s="72" t="s">
-        <v>360</v>
-      </c>
-      <c r="V2" s="72" t="s">
-        <v>361</v>
-      </c>
-      <c r="W2" s="72" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="84" customFormat="1" x14ac:dyDescent="0.3">
@@ -7156,22 +7156,22 @@
         <v>6</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>64</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F4" s="74" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H4" s="74">
         <v>2</v>
@@ -7180,31 +7180,31 @@
         <v>256</v>
       </c>
       <c r="J4" s="74" t="s">
+        <v>365</v>
+      </c>
+      <c r="K4" s="74" t="s">
         <v>366</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="L4" s="74" t="s">
+        <v>397</v>
+      </c>
+      <c r="M4" s="74" t="s">
         <v>367</v>
       </c>
-      <c r="L4" s="74" t="s">
-        <v>398</v>
-      </c>
-      <c r="M4" s="74" t="s">
+      <c r="N4" s="74" t="s">
         <v>368</v>
       </c>
-      <c r="N4" s="74" t="s">
+      <c r="O4" s="74" t="s">
         <v>369</v>
       </c>
-      <c r="O4" s="74" t="s">
+      <c r="P4" s="74" t="s">
         <v>370</v>
       </c>
-      <c r="P4" s="74" t="s">
+      <c r="Q4" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="R4" s="74" t="s">
         <v>372</v>
-      </c>
-      <c r="R4" s="74" t="s">
-        <v>373</v>
       </c>
       <c r="S4" s="74" t="b">
         <v>1</v>
@@ -7213,10 +7213,10 @@
         <v>117</v>
       </c>
       <c r="U4" s="50" t="s">
+        <v>373</v>
+      </c>
+      <c r="V4" s="50" t="s">
         <v>374</v>
-      </c>
-      <c r="V4" s="50" t="s">
-        <v>375</v>
       </c>
       <c r="W4" s="50">
         <v>10</v>
@@ -7272,25 +7272,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="65" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B1" s="65" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1" s="85" t="s">
         <v>526</v>
       </c>
-      <c r="C1" s="85" t="s">
-        <v>527</v>
-      </c>
       <c r="D1" s="85" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G1" s="86" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -7298,133 +7298,133 @@
         <v>116</v>
       </c>
       <c r="B2" s="74" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F2" s="50" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G2" s="74" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="50" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="50"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="50" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="50"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="50" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D7" s="50"/>
       <c r="E7" s="50" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="50" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="50" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="50" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="50"/>
@@ -7433,11 +7433,11 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="50" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="50" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D10" s="50"/>
       <c r="E10" s="50"/>
@@ -7446,11 +7446,11 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="50" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
@@ -7459,11 +7459,11 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="50" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
@@ -7474,7 +7474,7 @@
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="50"/>
@@ -7485,7 +7485,7 @@
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
@@ -7516,7 +7516,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="57" customFormat="1" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="96" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B1" s="96"/>
       <c r="C1" s="96"/>
@@ -7533,7 +7533,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -7549,10 +7549,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>424</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>425</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>426</v>
       </c>
       <c r="D4" s="50"/>
     </row>
@@ -7561,10 +7561,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
+        <v>426</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>427</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>428</v>
       </c>
       <c r="D5" s="50"/>
     </row>
@@ -7573,10 +7573,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>428</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>429</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>430</v>
       </c>
       <c r="D6" s="50"/>
     </row>
@@ -7585,10 +7585,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
+        <v>430</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>431</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>432</v>
       </c>
       <c r="D7" s="50"/>
     </row>
@@ -7597,13 +7597,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="59" t="s">
+        <v>557</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>559</v>
+      </c>
+      <c r="D8" s="48" t="s">
         <v>558</v>
-      </c>
-      <c r="C8" s="59" t="s">
-        <v>560</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -7635,7 +7635,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="57" customFormat="1" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="97" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B1" s="98"/>
       <c r="C1" s="98"/>
@@ -7683,19 +7683,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>433</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>482</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>542</v>
+      </c>
+      <c r="E4" s="50" t="s">
         <v>434</v>
       </c>
-      <c r="C4" s="50" t="s">
-        <v>483</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>543</v>
-      </c>
-      <c r="E4" s="50" t="s">
+      <c r="F4" s="59" t="s">
         <v>435</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>436</v>
       </c>
       <c r="G4" s="50"/>
     </row>
@@ -7705,13 +7705,13 @@
       <c r="C5" s="50"/>
       <c r="D5" s="50"/>
       <c r="E5" s="50" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -7719,22 +7719,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>437</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>415</v>
+      </c>
+      <c r="D6" s="50" t="s">
         <v>438</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>416</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>439</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -7742,22 +7742,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G7" s="50" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -7792,7 +7792,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="100" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -7812,28 +7812,28 @@
         <v>7</v>
       </c>
       <c r="C2" s="53" t="s">
+        <v>321</v>
+      </c>
+      <c r="D2" s="53" t="s">
         <v>322</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="E2" s="53" t="s">
         <v>323</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="F2" s="53" t="s">
         <v>324</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="G2" s="53" t="s">
         <v>325</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="H2" s="53" t="s">
         <v>326</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="I2" s="54" t="s">
+        <v>549</v>
+      </c>
+      <c r="J2" s="54" t="s">
         <v>327</v>
-      </c>
-      <c r="I2" s="54" t="s">
-        <v>550</v>
-      </c>
-      <c r="J2" s="54" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -7855,29 +7855,29 @@
         <v>6</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C4" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>329</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="E4" s="33" t="s">
         <v>330</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>331</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>409</v>
+      </c>
+      <c r="J4" s="40" t="s">
         <v>332</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>410</v>
-      </c>
-      <c r="J4" s="40" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -7886,17 +7886,17 @@
       <c r="C5" s="38"/>
       <c r="D5" s="33"/>
       <c r="E5" s="33" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F5" s="33"/>
       <c r="G5" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J5" s="40"/>
     </row>
@@ -7905,14 +7905,14 @@
         <v>6</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D6" s="33"/>
       <c r="E6" s="34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="33"/>
@@ -7925,16 +7925,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>107</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="33"/>
@@ -7948,7 +7948,7 @@
       <c r="C8" s="38"/>
       <c r="D8" s="33"/>
       <c r="E8" s="34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F8" s="34"/>
       <c r="G8" s="33"/>
@@ -7961,27 +7961,27 @@
         <v>6</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="F9" s="33" t="s">
         <v>340</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>341</v>
       </c>
       <c r="G9" s="33" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="33"/>
       <c r="I9" s="50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J9" s="40" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -7990,7 +7990,7 @@
       <c r="C10" s="38"/>
       <c r="D10" s="33"/>
       <c r="E10" s="33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F10" s="33"/>
       <c r="G10" s="33"/>
@@ -8004,7 +8004,7 @@
       <c r="C11" s="41"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F11" s="33"/>
       <c r="G11" s="33"/>
@@ -8018,13 +8018,13 @@
       <c r="C12" s="41"/>
       <c r="D12" s="33"/>
       <c r="E12" s="33" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F12" s="33"/>
       <c r="G12" s="33"/>
       <c r="H12" s="33"/>
       <c r="I12" s="50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J12" s="40"/>
     </row>
@@ -8062,7 +8062,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="209.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="96" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -8130,7 +8130,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>21</v>
@@ -8139,7 +8139,7 @@
         <v>22</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F4" s="50" t="s">
         <v>26</v>
@@ -8151,13 +8151,13 @@
         <v>23</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J4" s="50" t="s">
         <v>24</v>
       </c>
       <c r="K4" s="50" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
@@ -8165,10 +8165,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>25</v>
@@ -8186,7 +8186,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="50" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J5" s="50" t="s">
         <v>27</v>
@@ -8198,10 +8198,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D6" s="50" t="s">
         <v>28</v>
@@ -8219,7 +8219,7 @@
         <v>23</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J6" s="50" t="s">
         <v>27</v>
@@ -8270,7 +8270,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -8373,7 +8373,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>21</v>
@@ -8388,7 +8388,7 @@
         <v>44</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -8396,10 +8396,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>42</v>
@@ -8417,13 +8417,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>45</v>
@@ -8569,13 +8569,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>58</v>
@@ -8597,7 +8597,7 @@
         <v>23</v>
       </c>
       <c r="L4" s="60" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="M4" s="60" t="s">
         <v>23</v>
@@ -8618,16 +8618,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D5" s="50" t="s">
+        <v>454</v>
+      </c>
+      <c r="E5" s="50" t="s">
         <v>455</v>
-      </c>
-      <c r="E5" s="50" t="s">
-        <v>456</v>
       </c>
       <c r="F5" s="50" t="s">
         <v>59</v>
@@ -8665,13 +8665,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E6" s="50" t="s">
         <v>63</v>
@@ -8712,16 +8712,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F7" s="50" t="s">
         <v>59</v>
@@ -8730,7 +8730,7 @@
         <v>65</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I7" s="50"/>
       <c r="J7" s="50" t="s">
@@ -8761,16 +8761,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F8" s="50" t="s">
         <v>59</v>
@@ -8779,11 +8779,11 @@
         <v>65</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I8" s="50"/>
       <c r="J8" s="50" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K8" s="50" t="s">
         <v>26</v>
@@ -8810,16 +8810,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D9" s="50" t="s">
+        <v>460</v>
+      </c>
+      <c r="E9" s="50" t="s">
         <v>461</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>462</v>
       </c>
       <c r="F9" s="50" t="s">
         <v>59</v>
@@ -8828,17 +8828,17 @@
         <v>65</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I9" s="50"/>
       <c r="J9" s="50" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K9" s="50" t="s">
         <v>26</v>
       </c>
       <c r="L9" s="60" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="M9" s="60" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Password related info in CD3 ADW/ATP
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-template.xlsx
@@ -4451,100 +4451,6 @@
   </si>
   <si>
     <r>
-      <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"DB Name"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Should Not be more than 14 character and should contain only Alpha-Numeric Characters.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"ADW or ATP" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- Specify ADW/ATP in this column to create the respective Autonomous database.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Defined Tags"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
-                             Multiple Tag Key , Values can be specified using semi colon (;) as the delimeter. 
-                             </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Example: Operations.CostCenter=01;Users.Name=user01</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
 </t>
     </r>
@@ -5436,6 +5342,123 @@
       </rPr>
       <t>Leave it empty to not attach any backup policy to the boot volume.
                                    Values can be either of the following: Gold | Silver | Bronze</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"DB Name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Should Not be more than 14 character and should contain only Alpha-Numeric Characters.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"ADW or ATP" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Specify ADW/ATP in this column to create the respective Autonomous database.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Admin Password"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Password must be 9 to 30 characters and contain at least 2 uppercase, 2 lowercase, 2 special, and 2 numeric 
+                                  characters. The special characters must be _, #, or -.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Defined Tags"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
+                             Multiple Tag Key , Values can be specified using semi colon (;) as the delimeter. 
+                             </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example: Operations.CostCenter=01;Users.Name=user01</t>
     </r>
   </si>
 </sst>
@@ -6572,7 +6595,7 @@
     <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:1" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="91" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
   </sheetData>
@@ -7241,7 +7264,7 @@
       <c r="F1" s="101"/>
       <c r="G1" s="102"/>
       <c r="H1" s="100" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I1" s="101"/>
       <c r="J1" s="101"/>
@@ -7517,7 +7540,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="92" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B1" s="92"/>
       <c r="C1" s="92"/>
@@ -7665,7 +7688,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="100" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -10030,9 +10053,9 @@
     <col min="10" max="16384" width="8.88671875" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="110" t="s">
-        <v>562</v>
+        <v>574</v>
       </c>
       <c r="B1" s="110"/>
       <c r="C1" s="110"/>
@@ -10148,6 +10171,7 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10185,7 +10209,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="68" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="93" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94"/>
@@ -10529,7 +10553,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="68" customFormat="1" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="92" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B1" s="92"/>
       <c r="C1" s="92"/>
@@ -10869,7 +10893,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="68" customFormat="1" ht="165.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="92" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B1" s="92"/>
       <c r="C1" s="92"/>
@@ -11276,7 +11300,7 @@
       </c>
       <c r="D9" s="49"/>
       <c r="E9" s="49" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F9" s="49"/>
       <c r="G9" s="49"/>
@@ -11291,7 +11315,7 @@
       </c>
       <c r="D10" s="49"/>
       <c r="E10" s="49" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F10" s="49"/>
       <c r="G10" s="49"/>
@@ -11306,7 +11330,7 @@
       </c>
       <c r="D11" s="49"/>
       <c r="E11" s="49" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F11" s="49"/>
       <c r="G11" s="49"/>
@@ -11947,7 +11971,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="48" customFormat="1" ht="187.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="93" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94"/>
@@ -11955,7 +11979,7 @@
       <c r="E1" s="94"/>
       <c r="F1" s="95"/>
       <c r="G1" s="93" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H1" s="94"/>
       <c r="I1" s="94"/>

</xml_diff>